<commit_message>
Fix date cell formats
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maheug\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708DB72B-3F12-4963-B9E8-5C68D7DBA1BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AF68CC-9649-4EE3-9E09-E077CDCBBB2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1069,12 +1069,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="166" formatCode="mmm\-yyyy"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -2825,21 +2826,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2931,68 +2917,83 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3737,16 +3738,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="218" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
       <c r="G1" s="1"/>
-      <c r="J1" s="253" t="s">
+      <c r="J1" s="248" t="s">
         <v>336</v>
       </c>
     </row>
@@ -3758,32 +3759,32 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
-      <c r="J2" s="253" t="s">
+      <c r="J2" s="248" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="225" t="s">
+      <c r="A3" s="220" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="226"/>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226"/>
-      <c r="E3" s="226"/>
-      <c r="F3" s="226"/>
+      <c r="B3" s="221"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="225" t="s">
+      <c r="A4" s="220" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="226"/>
-      <c r="C4" s="226"/>
+      <c r="B4" s="221"/>
+      <c r="C4" s="221"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="1"/>
-      <c r="J4" s="253" t="s">
+      <c r="J4" s="248" t="s">
         <v>336</v>
       </c>
     </row>
@@ -3795,100 +3796,100 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="1"/>
-      <c r="J5" s="253" t="s">
+      <c r="J5" s="248" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="227" t="s">
+      <c r="A6" s="222" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="254" t="str">
+      <c r="B6" s="251" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="254"/>
-      <c r="D6" s="228" t="s">
+      <c r="C6" s="251"/>
+      <c r="D6" s="223" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="254" t="str">
+      <c r="E6" s="251" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="254"/>
+      <c r="F6" s="251"/>
       <c r="G6" s="1"/>
-      <c r="J6" s="253" t="s">
+      <c r="J6" s="248" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="227" t="s">
+      <c r="A7" s="222" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="255"/>
-      <c r="C7" s="255"/>
-      <c r="D7" s="228" t="s">
+      <c r="B7" s="249"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="223" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="255" t="str">
+      <c r="E7" s="249" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="255"/>
+      <c r="F7" s="249"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="227" t="s">
+      <c r="A8" s="222" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="228" t="s">
+      <c r="B8" s="249"/>
+      <c r="C8" s="249"/>
+      <c r="D8" s="223" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="255" t="str">
+      <c r="E8" s="249" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="255"/>
+      <c r="F8" s="249"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="227" t="s">
+      <c r="A9" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="255"/>
-      <c r="C9" s="255"/>
-      <c r="D9" s="228" t="s">
+      <c r="B9" s="249"/>
+      <c r="C9" s="249"/>
+      <c r="D9" s="223" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="255" t="str">
+      <c r="E9" s="249" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="255"/>
+      <c r="F9" s="249"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="228" t="s">
+      <c r="D10" s="223" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="256" t="str">
+      <c r="E10" s="250" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="256"/>
+      <c r="F10" s="250"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="227" t="s">
+      <c r="A11" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="254"/>
-      <c r="C11" s="254"/>
+      <c r="B11" s="251"/>
+      <c r="C11" s="251"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -3897,10 +3898,10 @@
     <row r="12" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="D12" s="228" t="s">
+      <c r="D12" s="223" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="229">
+      <c r="E12" s="224">
         <f>Sheet1!P7</f>
         <v>0</v>
       </c>
@@ -3908,26 +3909,26 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="230" t="s">
+      <c r="A13" s="225" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="254" t="s">
+      <c r="B13" s="251" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="254"/>
-      <c r="D13" s="228" t="s">
+      <c r="C13" s="251"/>
+      <c r="D13" s="223" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="231"/>
+      <c r="E13" s="226"/>
       <c r="F13" s="2"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="230" t="s">
+      <c r="A14" s="225" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="232"/>
-      <c r="C14" s="232"/>
+      <c r="B14" s="227"/>
+      <c r="C14" s="227"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -3943,17 +3944,17 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="233" t="s">
+      <c r="A16" s="228" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="233"/>
-      <c r="C16" s="234" t="s">
+      <c r="B16" s="228"/>
+      <c r="C16" s="229" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="228" t="s">
+      <c r="E16" s="223" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="234" t="s">
+      <c r="F16" s="229" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="1"/>
@@ -3964,92 +3965,92 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="232"/>
+      <c r="F17" s="227"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="236" t="s">
+      <c r="B18" s="231" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="235"/>
-      <c r="E18" s="236" t="s">
+      <c r="C18" s="230"/>
+      <c r="E18" s="231" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="235"/>
+      <c r="F18" s="230"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="236" t="s">
+      <c r="B19" s="231" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="235" t="str">
+      <c r="C19" s="230" t="str">
         <f>Sheet1!L138</f>
         <v/>
       </c>
-      <c r="E19" s="236" t="s">
+      <c r="E19" s="231" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="235"/>
+      <c r="F19" s="230"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="236" t="s">
+      <c r="B20" s="231" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="235" t="str">
+      <c r="C20" s="230" t="str">
         <f>Sheet1!L141</f>
         <v/>
       </c>
-      <c r="E20" s="236" t="s">
+      <c r="E20" s="231" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="235"/>
+      <c r="F20" s="230"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="236" t="s">
+      <c r="B21" s="231" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="235" t="str">
+      <c r="C21" s="230" t="str">
         <f>Sheet1!L140</f>
         <v/>
       </c>
-      <c r="E21" s="236" t="s">
+      <c r="E21" s="231" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="235"/>
+      <c r="F21" s="230"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="236" t="s">
+      <c r="B22" s="231" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="235"/>
-      <c r="E22" s="236" t="s">
+      <c r="C22" s="230"/>
+      <c r="E22" s="231" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="235"/>
+      <c r="F22" s="230"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="236" t="s">
+      <c r="B23" s="231" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="235" t="str">
+      <c r="C23" s="230" t="str">
         <f>Sheet1!K171</f>
         <v/>
       </c>
-      <c r="E23" s="236" t="s">
+      <c r="E23" s="231" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="235"/>
+      <c r="F23" s="230"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="236" t="s">
+      <c r="B24" s="231" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="235" t="str">
+      <c r="C24" s="230" t="str">
         <f>Sheet1!F191</f>
         <v/>
       </c>
@@ -4059,10 +4060,10 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="236" t="s">
+      <c r="B25" s="231" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="235" t="str">
+      <c r="C25" s="230" t="str">
         <f>Sheet1!H152</f>
         <v/>
       </c>
@@ -4072,10 +4073,10 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="236" t="s">
+      <c r="B26" s="231" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="235" t="str">
+      <c r="C26" s="230" t="str">
         <f>Sheet1!C187</f>
         <v/>
       </c>
@@ -4085,30 +4086,30 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="236" t="s">
+      <c r="B27" s="231" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="235"/>
+      <c r="C27" s="230"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="236" t="s">
+      <c r="B28" s="231" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="235"/>
+      <c r="C28" s="230"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="236" t="s">
+      <c r="B29" s="231" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="235"/>
+      <c r="C29" s="230"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -4124,7 +4125,7 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="230" t="s">
+      <c r="A31" s="225" t="s">
         <v>40</v>
       </c>
       <c r="B31" s="2"/>
@@ -4135,99 +4136,99 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="237"/>
-      <c r="B32" s="238"/>
-      <c r="C32" s="238"/>
-      <c r="D32" s="238"/>
-      <c r="E32" s="238"/>
-      <c r="F32" s="239"/>
+      <c r="A32" s="232"/>
+      <c r="B32" s="233"/>
+      <c r="C32" s="233"/>
+      <c r="D32" s="233"/>
+      <c r="E32" s="233"/>
+      <c r="F32" s="234"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="240"/>
-      <c r="B33" s="241"/>
-      <c r="C33" s="241"/>
-      <c r="D33" s="241"/>
-      <c r="E33" s="241"/>
-      <c r="F33" s="242"/>
+      <c r="A33" s="235"/>
+      <c r="B33" s="236"/>
+      <c r="C33" s="236"/>
+      <c r="D33" s="236"/>
+      <c r="E33" s="236"/>
+      <c r="F33" s="237"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="240"/>
-      <c r="B34" s="241"/>
-      <c r="C34" s="241"/>
-      <c r="D34" s="241"/>
-      <c r="E34" s="241"/>
-      <c r="F34" s="242"/>
+      <c r="A34" s="235"/>
+      <c r="B34" s="236"/>
+      <c r="C34" s="236"/>
+      <c r="D34" s="236"/>
+      <c r="E34" s="236"/>
+      <c r="F34" s="237"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="240"/>
-      <c r="B35" s="241"/>
-      <c r="C35" s="241"/>
-      <c r="D35" s="241"/>
-      <c r="E35" s="241"/>
-      <c r="F35" s="242"/>
+      <c r="A35" s="235"/>
+      <c r="B35" s="236"/>
+      <c r="C35" s="236"/>
+      <c r="D35" s="236"/>
+      <c r="E35" s="236"/>
+      <c r="F35" s="237"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="240"/>
-      <c r="B36" s="241"/>
-      <c r="C36" s="241"/>
-      <c r="D36" s="241"/>
-      <c r="E36" s="241"/>
-      <c r="F36" s="242"/>
+      <c r="A36" s="235"/>
+      <c r="B36" s="236"/>
+      <c r="C36" s="236"/>
+      <c r="D36" s="236"/>
+      <c r="E36" s="236"/>
+      <c r="F36" s="237"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="240"/>
-      <c r="B37" s="241"/>
-      <c r="C37" s="241"/>
-      <c r="D37" s="241"/>
-      <c r="E37" s="241"/>
-      <c r="F37" s="242"/>
+      <c r="A37" s="235"/>
+      <c r="B37" s="236"/>
+      <c r="C37" s="236"/>
+      <c r="D37" s="236"/>
+      <c r="E37" s="236"/>
+      <c r="F37" s="237"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="240"/>
-      <c r="B38" s="241"/>
-      <c r="C38" s="241"/>
-      <c r="D38" s="241"/>
-      <c r="E38" s="241"/>
-      <c r="F38" s="242"/>
+      <c r="A38" s="235"/>
+      <c r="B38" s="236"/>
+      <c r="C38" s="236"/>
+      <c r="D38" s="236"/>
+      <c r="E38" s="236"/>
+      <c r="F38" s="237"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="240"/>
-      <c r="B39" s="241"/>
-      <c r="C39" s="241"/>
-      <c r="D39" s="241"/>
-      <c r="E39" s="241"/>
-      <c r="F39" s="242"/>
+      <c r="A39" s="235"/>
+      <c r="B39" s="236"/>
+      <c r="C39" s="236"/>
+      <c r="D39" s="236"/>
+      <c r="E39" s="236"/>
+      <c r="F39" s="237"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="243"/>
-      <c r="B40" s="244"/>
-      <c r="C40" s="244"/>
-      <c r="D40" s="244"/>
-      <c r="E40" s="244"/>
-      <c r="F40" s="245"/>
+      <c r="A40" s="238"/>
+      <c r="B40" s="239"/>
+      <c r="C40" s="239"/>
+      <c r="D40" s="239"/>
+      <c r="E40" s="239"/>
+      <c r="F40" s="240"/>
       <c r="G40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -4250,9 +4251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23:L23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4409,7 +4408,7 @@
       <c r="O7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="218"/>
+      <c r="P7" s="270"/>
       <c r="W7" s="17" t="s">
         <v>50</v>
       </c>
@@ -4443,19 +4442,19 @@
       <c r="O8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="219" t="str">
+      <c r="P8" s="271" t="str">
         <f>IF(AB8="","",AB8)</f>
         <v/>
       </c>
       <c r="AA8" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="AB8" s="221"/>
+      <c r="AB8" s="272"/>
       <c r="AC8" s="42" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AD8" s="222" t="str">
+      <c r="AD8" s="273" t="str">
         <f>IF(P7="","",P7)</f>
         <v/>
       </c>
@@ -4516,19 +4515,19 @@
       <c r="E10" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="257" t="str">
+      <c r="F10" s="265" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="257"/>
+      <c r="G10" s="265"/>
       <c r="J10" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="257" t="str">
+      <c r="K10" s="265" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="257"/>
+      <c r="L10" s="265"/>
       <c r="M10" s="25"/>
       <c r="O10" s="26"/>
       <c r="Q10" s="30" t="s">
@@ -4569,19 +4568,19 @@
       <c r="E11" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="258" t="str">
+      <c r="F11" s="268" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="258"/>
+      <c r="G11" s="268"/>
       <c r="J11" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="257" t="str">
+      <c r="K11" s="265" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="257"/>
+      <c r="L11" s="265"/>
       <c r="M11" s="25"/>
       <c r="O11" s="26"/>
       <c r="Q11" s="30" t="s">
@@ -4622,19 +4621,19 @@
       <c r="E12" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="258" t="str">
+      <c r="F12" s="268" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="258"/>
+      <c r="G12" s="268"/>
       <c r="J12" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="259" t="str">
+      <c r="K12" s="269" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="259"/>
+      <c r="L12" s="269"/>
       <c r="M12" s="25"/>
       <c r="O12" s="26"/>
       <c r="Q12" s="30" t="s">
@@ -4675,19 +4674,19 @@
       <c r="E13" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="258" t="str">
+      <c r="F13" s="268" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="258"/>
+      <c r="G13" s="268"/>
       <c r="J13" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="257" t="str">
+      <c r="K13" s="265" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="257"/>
+      <c r="L13" s="265"/>
       <c r="M13" s="25"/>
       <c r="O13" s="26"/>
       <c r="Q13" s="30" t="s">
@@ -4785,19 +4784,19 @@
       <c r="E16" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="257" t="str">
+      <c r="F16" s="265" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="257"/>
+      <c r="G16" s="265"/>
       <c r="J16" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="259" t="str">
+      <c r="K16" s="269" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="259"/>
+      <c r="L16" s="269"/>
       <c r="M16" s="25"/>
       <c r="O16" s="26"/>
       <c r="P16" s="58" t="s">
@@ -4825,19 +4824,19 @@
       <c r="E17" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="258" t="str">
+      <c r="F17" s="268" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="258"/>
+      <c r="G17" s="268"/>
       <c r="J17" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="257" t="str">
+      <c r="K17" s="265" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="257"/>
+      <c r="L17" s="265"/>
       <c r="M17" s="25"/>
       <c r="O17" s="26"/>
       <c r="Q17" s="30" t="s">
@@ -4878,11 +4877,11 @@
       <c r="J18" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="257" t="str">
+      <c r="K18" s="265" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="257"/>
+      <c r="L18" s="265"/>
       <c r="M18" s="25"/>
       <c r="O18" s="26"/>
       <c r="Q18" s="30" t="s">
@@ -4954,11 +4953,11 @@
       <c r="E20" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="257" t="str">
+      <c r="F20" s="265" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="257"/>
+      <c r="G20" s="265"/>
       <c r="I20" s="61" t="s">
         <v>76</v>
       </c>
@@ -4983,19 +4982,19 @@
       <c r="E21" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="260" t="str">
+      <c r="F21" s="267" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="260"/>
+      <c r="G21" s="267"/>
       <c r="J21" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="257" t="str">
+      <c r="K21" s="265" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="257"/>
+      <c r="L21" s="265"/>
       <c r="M21" s="25"/>
       <c r="O21" s="26"/>
       <c r="Q21" s="30" t="s">
@@ -5034,11 +5033,11 @@
       <c r="J22" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="257" t="str">
+      <c r="K22" s="265" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="257"/>
+      <c r="L22" s="265"/>
       <c r="M22" s="25"/>
       <c r="O22" s="26"/>
       <c r="Q22" s="30" t="s">
@@ -5079,19 +5078,19 @@
       <c r="E23" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="257" t="str">
+      <c r="F23" s="265" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="257"/>
+      <c r="G23" s="265"/>
       <c r="J23" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="257" t="str">
+      <c r="K23" s="265" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="257"/>
+      <c r="L23" s="265"/>
       <c r="M23" s="25"/>
       <c r="O23" s="26"/>
       <c r="P23" s="58" t="s">
@@ -5127,11 +5126,11 @@
       <c r="E24" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="257" t="str">
+      <c r="F24" s="265" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="257"/>
+      <c r="G24" s="265"/>
       <c r="M24" s="25"/>
       <c r="O24" s="26"/>
       <c r="Q24" s="30" t="s">
@@ -5172,11 +5171,11 @@
       <c r="E25" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="257" t="str">
+      <c r="F25" s="265" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="257"/>
+      <c r="G25" s="265"/>
       <c r="J25" s="57" t="s">
         <v>82</v>
       </c>
@@ -5216,11 +5215,11 @@
       <c r="J26" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="257" t="str">
+      <c r="K26" s="265" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="257"/>
+      <c r="L26" s="265"/>
       <c r="M26" s="25"/>
       <c r="O26" s="26"/>
       <c r="Q26" s="30" t="s">
@@ -5248,19 +5247,19 @@
       <c r="E27" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="257" t="str">
+      <c r="F27" s="265" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="257"/>
+      <c r="G27" s="265"/>
       <c r="J27" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="257" t="str">
+      <c r="K27" s="265" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="257"/>
+      <c r="L27" s="265"/>
       <c r="M27" s="25"/>
       <c r="O27" s="26"/>
       <c r="P27" s="58" t="s">
@@ -5287,11 +5286,11 @@
       <c r="E28" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="257" t="str">
+      <c r="F28" s="265" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="257"/>
+      <c r="G28" s="265"/>
       <c r="M28" s="25"/>
       <c r="O28" s="26"/>
       <c r="Q28" s="30" t="s">
@@ -5332,11 +5331,11 @@
       <c r="E29" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="257" t="str">
+      <c r="F29" s="265" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="257"/>
+      <c r="G29" s="265"/>
       <c r="M29" s="25"/>
       <c r="O29" s="26"/>
       <c r="Q29" s="30" t="s">
@@ -5446,10 +5445,10 @@
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
-      <c r="L32" s="261" t="s">
+      <c r="L32" s="266" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="261"/>
+      <c r="M32" s="266"/>
       <c r="AA32" s="30" t="s">
         <v>70</v>
       </c>
@@ -6529,7 +6528,7 @@
       <c r="C65" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D65" s="220" t="str">
+      <c r="D65" s="274" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -6819,23 +6818,23 @@
       <c r="P72" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="Q72" s="246" t="str">
+      <c r="Q72" s="241" t="str">
         <f t="shared" ref="Q72:Q88" si="15">IF(Q91&lt;&gt;"",Q91,IF(AB43="","",AB43))</f>
         <v/>
       </c>
-      <c r="R72" s="246" t="str">
+      <c r="R72" s="241" t="str">
         <f t="shared" ref="R72:R88" si="16">IF(R91&lt;&gt;"",R91,IF(AB61="","",AB61))</f>
         <v/>
       </c>
-      <c r="S72" s="246" t="str">
+      <c r="S72" s="241" t="str">
         <f t="shared" ref="S72:S88" si="17">IF(S91&lt;&gt;"",S91,IF(AB79="","",AB79))</f>
         <v/>
       </c>
-      <c r="T72" s="246" t="str">
+      <c r="T72" s="241" t="str">
         <f t="shared" ref="T72:T88" si="18">IF(T91&lt;&gt;"",T91,IF(AB97="","",AB97))</f>
         <v/>
       </c>
-      <c r="U72" s="246" t="str">
+      <c r="U72" s="241" t="str">
         <f t="shared" ref="U72:U88" si="19">IF(U91&lt;&gt;"",U91,IF(AB115="","",AB115))</f>
         <v/>
       </c>
@@ -6886,23 +6885,23 @@
       <c r="P73" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="Q73" s="247" t="str">
+      <c r="Q73" s="242" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R73" s="247" t="str">
+      <c r="R73" s="242" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S73" s="247" t="str">
+      <c r="S73" s="242" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T73" s="247" t="str">
+      <c r="T73" s="242" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U73" s="247" t="str">
+      <c r="U73" s="242" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -6953,23 +6952,23 @@
       <c r="P74" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="Q74" s="246" t="str">
+      <c r="Q74" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R74" s="246" t="str">
+      <c r="R74" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S74" s="246" t="str">
+      <c r="S74" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T74" s="246" t="str">
+      <c r="T74" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U74" s="246" t="str">
+      <c r="U74" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7020,23 +7019,23 @@
       <c r="P75" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="Q75" s="246" t="str">
+      <c r="Q75" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R75" s="246" t="str">
+      <c r="R75" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S75" s="246" t="str">
+      <c r="S75" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T75" s="246" t="str">
+      <c r="T75" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U75" s="246" t="str">
+      <c r="U75" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7087,23 +7086,23 @@
       <c r="P76" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="Q76" s="246" t="str">
+      <c r="Q76" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R76" s="246" t="str">
+      <c r="R76" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S76" s="246" t="str">
+      <c r="S76" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T76" s="246" t="str">
+      <c r="T76" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U76" s="246" t="str">
+      <c r="U76" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7154,23 +7153,23 @@
       <c r="P77" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="Q77" s="246" t="str">
+      <c r="Q77" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R77" s="246" t="str">
+      <c r="R77" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S77" s="246" t="str">
+      <c r="S77" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T77" s="246" t="str">
+      <c r="T77" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U77" s="246" t="str">
+      <c r="U77" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7221,23 +7220,23 @@
       <c r="P78" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="Q78" s="246" t="str">
+      <c r="Q78" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R78" s="246" t="str">
+      <c r="R78" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S78" s="246" t="str">
+      <c r="S78" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T78" s="246" t="str">
+      <c r="T78" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U78" s="246" t="str">
+      <c r="U78" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7282,23 +7281,23 @@
       <c r="P79" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="Q79" s="246" t="str">
+      <c r="Q79" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R79" s="246" t="str">
+      <c r="R79" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S79" s="246" t="str">
+      <c r="S79" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T79" s="246" t="str">
+      <c r="T79" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U79" s="246" t="str">
+      <c r="U79" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7349,23 +7348,23 @@
       <c r="P80" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q80" s="246" t="str">
+      <c r="Q80" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R80" s="246" t="str">
+      <c r="R80" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S80" s="246" t="str">
+      <c r="S80" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T80" s="246" t="str">
+      <c r="T80" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U80" s="246" t="str">
+      <c r="U80" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7416,23 +7415,23 @@
       <c r="P81" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="Q81" s="246" t="str">
+      <c r="Q81" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R81" s="246" t="str">
+      <c r="R81" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S81" s="246" t="str">
+      <c r="S81" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T81" s="246" t="str">
+      <c r="T81" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U81" s="246" t="str">
+      <c r="U81" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7483,23 +7482,23 @@
       <c r="P82" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="Q82" s="246" t="str">
+      <c r="Q82" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R82" s="246" t="str">
+      <c r="R82" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S82" s="246" t="str">
+      <c r="S82" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T82" s="246" t="str">
+      <c r="T82" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U82" s="246" t="str">
+      <c r="U82" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7550,23 +7549,23 @@
       <c r="P83" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="Q83" s="246" t="str">
+      <c r="Q83" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R83" s="246" t="str">
+      <c r="R83" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S83" s="246" t="str">
+      <c r="S83" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T83" s="246" t="str">
+      <c r="T83" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U83" s="246" t="str">
+      <c r="U83" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7617,23 +7616,23 @@
       <c r="P84" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="Q84" s="246" t="str">
+      <c r="Q84" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R84" s="246" t="str">
+      <c r="R84" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S84" s="246" t="str">
+      <c r="S84" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T84" s="246" t="str">
+      <c r="T84" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U84" s="246" t="str">
+      <c r="U84" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7684,23 +7683,23 @@
       <c r="P85" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="Q85" s="246" t="str">
+      <c r="Q85" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R85" s="246" t="str">
+      <c r="R85" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S85" s="246" t="str">
+      <c r="S85" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T85" s="246" t="str">
+      <c r="T85" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U85" s="246" t="str">
+      <c r="U85" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7751,23 +7750,23 @@
       <c r="P86" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="Q86" s="246" t="str">
+      <c r="Q86" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R86" s="246" t="str">
+      <c r="R86" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S86" s="246" t="str">
+      <c r="S86" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T86" s="246" t="str">
+      <c r="T86" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U86" s="246" t="str">
+      <c r="U86" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7818,23 +7817,23 @@
       <c r="P87" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="Q87" s="246" t="str">
+      <c r="Q87" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R87" s="246" t="str">
+      <c r="R87" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S87" s="246" t="str">
+      <c r="S87" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T87" s="246" t="str">
+      <c r="T87" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U87" s="246" t="str">
+      <c r="U87" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -7885,23 +7884,23 @@
       <c r="P88" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="Q88" s="246" t="str">
+      <c r="Q88" s="241" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="R88" s="246" t="str">
+      <c r="R88" s="241" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="S88" s="246" t="str">
+      <c r="S88" s="241" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="T88" s="246" t="str">
+      <c r="T88" s="241" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="U88" s="246" t="str">
+      <c r="U88" s="241" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
@@ -8005,25 +8004,25 @@
       </c>
       <c r="B91" s="23"/>
       <c r="E91" s="71"/>
-      <c r="F91" s="267" t="s">
+      <c r="F91" s="258" t="s">
         <v>151</v>
       </c>
-      <c r="G91" s="267"/>
-      <c r="H91" s="267"/>
-      <c r="I91" s="268" t="s">
+      <c r="G91" s="258"/>
+      <c r="H91" s="258"/>
+      <c r="I91" s="259" t="s">
         <v>152</v>
       </c>
-      <c r="J91" s="268"/>
+      <c r="J91" s="259"/>
       <c r="M91" s="25"/>
       <c r="O91" s="26"/>
       <c r="P91" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="Q91" s="248"/>
-      <c r="R91" s="248"/>
-      <c r="S91" s="248"/>
-      <c r="T91" s="248"/>
-      <c r="U91" s="248"/>
+      <c r="Q91" s="243"/>
+      <c r="R91" s="243"/>
+      <c r="S91" s="243"/>
+      <c r="T91" s="243"/>
+      <c r="U91" s="243"/>
       <c r="Y91" s="27"/>
       <c r="AA91" s="30" t="s">
         <v>135</v>
@@ -8067,23 +8066,23 @@
       <c r="P92" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="Q92" s="249" t="str">
+      <c r="Q92" s="244" t="str">
         <f>IF(OR(Q93="",Q95=""),"",Q93/Q95)</f>
         <v/>
       </c>
-      <c r="R92" s="249" t="str">
+      <c r="R92" s="244" t="str">
         <f>IF(OR(R93="",R95=""),"",R93/R95)</f>
         <v/>
       </c>
-      <c r="S92" s="249" t="str">
+      <c r="S92" s="244" t="str">
         <f>IF(OR(S93="",S95=""),"",S93/S95)</f>
         <v/>
       </c>
-      <c r="T92" s="249" t="str">
+      <c r="T92" s="244" t="str">
         <f>IF(OR(T93="",T95=""),"",T93/T95)</f>
         <v/>
       </c>
-      <c r="U92" s="249" t="str">
+      <c r="U92" s="244" t="str">
         <f>IF(OR(U93="",U95=""),"",U93/U95)</f>
         <v/>
       </c>
@@ -8138,23 +8137,23 @@
       <c r="P93" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="Q93" s="248" t="str">
+      <c r="Q93" s="243" t="str">
         <f>IF(OR(Q94="",Q103=""),"",Q94*Q103)</f>
         <v/>
       </c>
-      <c r="R93" s="248" t="str">
+      <c r="R93" s="243" t="str">
         <f>IF(OR(R94="",R103=""),"",R94*R103)</f>
         <v/>
       </c>
-      <c r="S93" s="248" t="str">
+      <c r="S93" s="243" t="str">
         <f>IF(OR(S94="",S103=""),"",S94*S103)</f>
         <v/>
       </c>
-      <c r="T93" s="248" t="str">
+      <c r="T93" s="243" t="str">
         <f>IF(OR(T94="",T103=""),"",T94*T103)</f>
         <v/>
       </c>
-      <c r="U93" s="248" t="str">
+      <c r="U93" s="243" t="str">
         <f>IF(OR(U94="",U103=""),"",U94*U103)</f>
         <v/>
       </c>
@@ -8177,10 +8176,10 @@
         <v>28</v>
       </c>
       <c r="B94" s="23"/>
-      <c r="D94" s="269" t="s">
+      <c r="D94" s="260" t="s">
         <v>161</v>
       </c>
-      <c r="E94" s="269" t="s">
+      <c r="E94" s="260" t="s">
         <v>161</v>
       </c>
       <c r="F94" s="97" t="str">
@@ -8214,11 +8213,11 @@
       <c r="P94" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="Q94" s="248"/>
-      <c r="R94" s="248"/>
-      <c r="S94" s="248"/>
-      <c r="T94" s="248"/>
-      <c r="U94" s="248"/>
+      <c r="Q94" s="243"/>
+      <c r="R94" s="243"/>
+      <c r="S94" s="243"/>
+      <c r="T94" s="243"/>
+      <c r="U94" s="243"/>
       <c r="Y94" s="27"/>
       <c r="AA94" s="30" t="s">
         <v>143</v>
@@ -8238,8 +8237,8 @@
         <v>29</v>
       </c>
       <c r="B95" s="23"/>
-      <c r="D95" s="269"/>
-      <c r="E95" s="269"/>
+      <c r="D95" s="260"/>
+      <c r="E95" s="260"/>
       <c r="F95" s="102" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -8271,11 +8270,11 @@
       <c r="P95" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="Q95" s="248"/>
-      <c r="R95" s="248"/>
-      <c r="S95" s="248"/>
-      <c r="T95" s="248"/>
-      <c r="U95" s="248"/>
+      <c r="Q95" s="243"/>
+      <c r="R95" s="243"/>
+      <c r="S95" s="243"/>
+      <c r="T95" s="243"/>
+      <c r="U95" s="243"/>
       <c r="Y95" s="27"/>
       <c r="AA95" s="30" t="s">
         <v>145</v>
@@ -8295,8 +8294,8 @@
         <v>30</v>
       </c>
       <c r="B96" s="23"/>
-      <c r="D96" s="269"/>
-      <c r="E96" s="269"/>
+      <c r="D96" s="260"/>
+      <c r="E96" s="260"/>
       <c r="F96" s="107" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -8330,11 +8329,11 @@
       <c r="P96" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="Q96" s="248"/>
-      <c r="R96" s="248"/>
-      <c r="S96" s="248"/>
-      <c r="T96" s="248"/>
-      <c r="U96" s="248"/>
+      <c r="Q96" s="243"/>
+      <c r="R96" s="243"/>
+      <c r="S96" s="243"/>
+      <c r="T96" s="243"/>
+      <c r="U96" s="243"/>
       <c r="Y96" s="27"/>
       <c r="AA96" s="38" t="s">
         <v>164</v>
@@ -8382,11 +8381,11 @@
       <c r="P97" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="Q97" s="248"/>
-      <c r="R97" s="248"/>
-      <c r="S97" s="248"/>
-      <c r="T97" s="248"/>
-      <c r="U97" s="248"/>
+      <c r="Q97" s="243"/>
+      <c r="R97" s="243"/>
+      <c r="S97" s="243"/>
+      <c r="T97" s="243"/>
+      <c r="U97" s="243"/>
       <c r="Y97" s="27"/>
       <c r="AA97" s="30" t="s">
         <v>107</v>
@@ -8443,11 +8442,11 @@
       <c r="P98" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="Q98" s="248"/>
-      <c r="R98" s="248"/>
-      <c r="S98" s="248"/>
-      <c r="T98" s="248"/>
-      <c r="U98" s="248"/>
+      <c r="Q98" s="243"/>
+      <c r="R98" s="243"/>
+      <c r="S98" s="243"/>
+      <c r="T98" s="243"/>
+      <c r="U98" s="243"/>
       <c r="Y98" s="27"/>
       <c r="AA98" s="30" t="s">
         <v>109</v>
@@ -8503,11 +8502,11 @@
       <c r="P99" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q99" s="248"/>
-      <c r="R99" s="248"/>
-      <c r="S99" s="248"/>
-      <c r="T99" s="248"/>
-      <c r="U99" s="248"/>
+      <c r="Q99" s="243"/>
+      <c r="R99" s="243"/>
+      <c r="S99" s="243"/>
+      <c r="T99" s="243"/>
+      <c r="U99" s="243"/>
       <c r="Y99" s="27"/>
       <c r="AA99" s="30" t="s">
         <v>111</v>
@@ -8563,11 +8562,11 @@
       <c r="P100" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="Q100" s="248"/>
-      <c r="R100" s="248"/>
-      <c r="S100" s="248"/>
-      <c r="T100" s="248"/>
-      <c r="U100" s="248"/>
+      <c r="Q100" s="243"/>
+      <c r="R100" s="243"/>
+      <c r="S100" s="243"/>
+      <c r="T100" s="243"/>
+      <c r="U100" s="243"/>
       <c r="Y100" s="27"/>
       <c r="AA100" s="30" t="s">
         <v>112</v>
@@ -8615,11 +8614,11 @@
       <c r="P101" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="Q101" s="248"/>
-      <c r="R101" s="248"/>
-      <c r="S101" s="248"/>
-      <c r="T101" s="248"/>
-      <c r="U101" s="248"/>
+      <c r="Q101" s="243"/>
+      <c r="R101" s="243"/>
+      <c r="S101" s="243"/>
+      <c r="T101" s="243"/>
+      <c r="U101" s="243"/>
       <c r="Y101" s="27"/>
       <c r="AA101" s="30" t="s">
         <v>114</v>
@@ -8669,23 +8668,23 @@
       <c r="P102" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="Q102" s="248" t="str">
+      <c r="Q102" s="243" t="str">
         <f>IF(OR(Q100="",Q101="",Q103=""),"",(Q101*Q100)*Q103)</f>
         <v/>
       </c>
-      <c r="R102" s="248" t="str">
+      <c r="R102" s="243" t="str">
         <f>IF(OR(R100="",R101="",R103=""),"",(R101*R100)*R103)</f>
         <v/>
       </c>
-      <c r="S102" s="248" t="str">
+      <c r="S102" s="243" t="str">
         <f>IF(OR(S100="",S101="",S103=""),"",(S101*S100)*S103)</f>
         <v/>
       </c>
-      <c r="T102" s="248" t="str">
+      <c r="T102" s="243" t="str">
         <f>IF(OR(T100="",T101="",T103=""),"",(T101*T100)*T103)</f>
         <v/>
       </c>
-      <c r="U102" s="248" t="str">
+      <c r="U102" s="243" t="str">
         <f>IF(OR(U100="",U101="",U103=""),"",(U101*U100)*U103)</f>
         <v/>
       </c>
@@ -8738,11 +8737,11 @@
       <c r="P103" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="Q103" s="248"/>
-      <c r="R103" s="248"/>
-      <c r="S103" s="248"/>
-      <c r="T103" s="248"/>
-      <c r="U103" s="248"/>
+      <c r="Q103" s="243"/>
+      <c r="R103" s="243"/>
+      <c r="S103" s="243"/>
+      <c r="T103" s="243"/>
+      <c r="U103" s="243"/>
       <c r="Y103" s="27"/>
       <c r="AA103" s="30" t="s">
         <v>118</v>
@@ -8781,11 +8780,11 @@
       <c r="P104" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="Q104" s="248"/>
-      <c r="R104" s="248"/>
-      <c r="S104" s="248"/>
-      <c r="T104" s="248"/>
-      <c r="U104" s="248"/>
+      <c r="Q104" s="243"/>
+      <c r="R104" s="243"/>
+      <c r="S104" s="243"/>
+      <c r="T104" s="243"/>
+      <c r="U104" s="243"/>
       <c r="Y104" s="27"/>
       <c r="AA104" s="30" t="s">
         <v>120</v>
@@ -8821,11 +8820,11 @@
       <c r="P105" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="Q105" s="248"/>
-      <c r="R105" s="248"/>
-      <c r="S105" s="248"/>
-      <c r="T105" s="248"/>
-      <c r="U105" s="248"/>
+      <c r="Q105" s="243"/>
+      <c r="R105" s="243"/>
+      <c r="S105" s="243"/>
+      <c r="T105" s="243"/>
+      <c r="U105" s="243"/>
       <c r="Y105" s="27"/>
       <c r="AA105" s="30" t="s">
         <v>123</v>
@@ -8858,11 +8857,11 @@
       <c r="P106" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="Q106" s="248"/>
-      <c r="R106" s="248"/>
-      <c r="S106" s="248"/>
-      <c r="T106" s="248"/>
-      <c r="U106" s="248"/>
+      <c r="Q106" s="243"/>
+      <c r="R106" s="243"/>
+      <c r="S106" s="243"/>
+      <c r="T106" s="243"/>
+      <c r="U106" s="243"/>
       <c r="Y106" s="27"/>
       <c r="AA106" s="30" t="s">
         <v>126</v>
@@ -8890,11 +8889,11 @@
       <c r="P107" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="Q107" s="248"/>
-      <c r="R107" s="248"/>
-      <c r="S107" s="248"/>
-      <c r="T107" s="248"/>
-      <c r="U107" s="248"/>
+      <c r="Q107" s="243"/>
+      <c r="R107" s="243"/>
+      <c r="S107" s="243"/>
+      <c r="T107" s="243"/>
+      <c r="U107" s="243"/>
       <c r="Y107" s="27"/>
       <c r="AA107" s="30" t="s">
         <v>129</v>
@@ -9100,34 +9099,34 @@
       <c r="D112" s="50" t="s">
         <v>334</v>
       </c>
-      <c r="E112" s="250" t="str">
+      <c r="E112" s="245" t="str">
         <f>IF(Q137="","",Q137)</f>
         <v/>
       </c>
-      <c r="F112" s="251" t="str">
+      <c r="F112" s="246" t="str">
         <f t="shared" ref="F112:H112" si="27">IF(R137="","",R137)</f>
         <v/>
       </c>
-      <c r="G112" s="251" t="str">
+      <c r="G112" s="246" t="str">
         <f t="shared" si="27"/>
         <v/>
       </c>
-      <c r="H112" s="252" t="str">
+      <c r="H112" s="247" t="str">
         <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="J112" s="22"/>
       <c r="M112" s="25"/>
       <c r="O112" s="26"/>
-      <c r="Q112" s="270" t="s">
+      <c r="Q112" s="261" t="s">
         <v>151</v>
       </c>
-      <c r="R112" s="270"/>
-      <c r="S112" s="270"/>
-      <c r="T112" s="272" t="s">
+      <c r="R112" s="261"/>
+      <c r="S112" s="261"/>
+      <c r="T112" s="253" t="s">
         <v>152</v>
       </c>
-      <c r="U112" s="272"/>
+      <c r="U112" s="253"/>
       <c r="W112" s="58" t="s">
         <v>158</v>
       </c>
@@ -9265,10 +9264,10 @@
       </c>
       <c r="J115" s="22"/>
       <c r="M115" s="25"/>
-      <c r="O115" s="273" t="s">
+      <c r="O115" s="254" t="s">
         <v>161</v>
       </c>
-      <c r="P115" s="273" t="s">
+      <c r="P115" s="254" t="s">
         <v>161</v>
       </c>
       <c r="Q115" s="141"/>
@@ -9308,8 +9307,8 @@
       <c r="H116" s="22"/>
       <c r="J116" s="22"/>
       <c r="M116" s="25"/>
-      <c r="O116" s="273"/>
-      <c r="P116" s="273"/>
+      <c r="O116" s="254"/>
+      <c r="P116" s="254"/>
       <c r="Q116" s="144"/>
       <c r="R116" s="145"/>
       <c r="S116" s="146"/>
@@ -9349,8 +9348,8 @@
       <c r="H117" s="22"/>
       <c r="J117" s="22"/>
       <c r="M117" s="25"/>
-      <c r="O117" s="273"/>
-      <c r="P117" s="273"/>
+      <c r="O117" s="254"/>
+      <c r="P117" s="254"/>
       <c r="Q117" s="148"/>
       <c r="R117" s="149"/>
       <c r="S117" s="150"/>
@@ -9991,7 +9990,7 @@
       <c r="C131" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D131" s="220" t="str">
+      <c r="D131" s="274" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -10103,7 +10102,7 @@
         <v>CT System Compliance Inspection</v>
       </c>
       <c r="O134" s="26"/>
-      <c r="P134" s="274" t="s">
+      <c r="P134" s="255" t="s">
         <v>181</v>
       </c>
       <c r="Q134" s="175"/>
@@ -10143,7 +10142,7 @@
       <c r="L135" s="15"/>
       <c r="M135" s="16"/>
       <c r="O135" s="26"/>
-      <c r="P135" s="274"/>
+      <c r="P135" s="255"/>
       <c r="Q135" s="175"/>
       <c r="R135" s="176"/>
       <c r="S135" s="176"/>
@@ -10191,7 +10190,7 @@
       </c>
       <c r="M136" s="25"/>
       <c r="O136" s="26"/>
-      <c r="P136" s="274"/>
+      <c r="P136" s="255"/>
       <c r="Q136" s="178"/>
       <c r="R136" s="179"/>
       <c r="S136" s="179"/>
@@ -11031,10 +11030,10 @@
         <v>150</v>
       </c>
       <c r="W154" s="190"/>
-      <c r="X154" s="265" t="s">
+      <c r="X154" s="256" t="s">
         <v>226</v>
       </c>
-      <c r="Y154" s="265"/>
+      <c r="Y154" s="256"/>
       <c r="AA154" s="30"/>
       <c r="AB154" s="187"/>
       <c r="AD154" s="187"/>
@@ -11576,14 +11575,14 @@
       <c r="B168" s="23"/>
       <c r="C168" s="55"/>
       <c r="D168" s="71"/>
-      <c r="E168" s="266" t="s">
+      <c r="E168" s="257" t="s">
         <v>151</v>
       </c>
-      <c r="F168" s="266"/>
-      <c r="G168" s="266" t="s">
+      <c r="F168" s="257"/>
+      <c r="G168" s="257" t="s">
         <v>152</v>
       </c>
-      <c r="H168" s="266"/>
+      <c r="H168" s="257"/>
       <c r="M168" s="25"/>
       <c r="O168" s="189"/>
       <c r="P168" s="30" t="s">
@@ -11983,14 +11982,14 @@
       </c>
       <c r="M178" s="25"/>
       <c r="O178" s="26"/>
-      <c r="P178" s="271" t="s">
+      <c r="P178" s="252" t="s">
         <v>151</v>
       </c>
-      <c r="Q178" s="271"/>
-      <c r="R178" s="271" t="s">
+      <c r="Q178" s="252"/>
+      <c r="R178" s="252" t="s">
         <v>152</v>
       </c>
-      <c r="S178" s="271"/>
+      <c r="S178" s="252"/>
       <c r="Y178" s="27"/>
       <c r="AA178" s="30"/>
       <c r="AB178" s="187"/>
@@ -12669,7 +12668,7 @@
       <c r="C197" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D197" s="220" t="str">
+      <c r="D197" s="274" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -14654,7 +14653,7 @@
       <c r="C263" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D263" s="220" t="str">
+      <c r="D263" s="274" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -14687,11 +14686,39 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="P178:Q178"/>
-    <mergeCell ref="R178:S178"/>
-    <mergeCell ref="T112:U112"/>
-    <mergeCell ref="O115:P117"/>
-    <mergeCell ref="P134:P136"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="Q89:S89"/>
+    <mergeCell ref="T89:U89"/>
     <mergeCell ref="X154:Y154"/>
     <mergeCell ref="E168:F168"/>
     <mergeCell ref="G168:H168"/>
@@ -14699,39 +14726,11 @@
     <mergeCell ref="I91:J91"/>
     <mergeCell ref="D94:E96"/>
     <mergeCell ref="Q112:S112"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="T70:U70"/>
-    <mergeCell ref="Q89:S89"/>
-    <mergeCell ref="T89:U89"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="P178:Q178"/>
+    <mergeCell ref="R178:S178"/>
+    <mergeCell ref="T112:U112"/>
+    <mergeCell ref="O115:P117"/>
+    <mergeCell ref="P134:P136"/>
   </mergeCells>
   <conditionalFormatting sqref="L33:L38 L41:L45 L47:L56 L59:L62">
     <cfRule type="cellIs" dxfId="31" priority="41" operator="equal">
@@ -14906,17 +14905,17 @@
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="271" t="s">
+      <c r="A2" s="252" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="271" t="s">
+      <c r="B2" s="252" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
+      <c r="C2" s="252"/>
+      <c r="D2" s="252"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="271"/>
+      <c r="A3" s="252"/>
       <c r="B3" s="5" t="s">
         <v>292</v>
       </c>
@@ -15088,17 +15087,17 @@
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="271" t="s">
+      <c r="A16" s="252" t="s">
         <v>290</v>
       </c>
-      <c r="B16" s="271" t="s">
+      <c r="B16" s="252" t="s">
         <v>307</v>
       </c>
-      <c r="C16" s="271"/>
-      <c r="D16" s="271"/>
+      <c r="C16" s="252"/>
+      <c r="D16" s="252"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="271"/>
+      <c r="A17" s="252"/>
       <c r="B17" s="5" t="s">
         <v>292</v>
       </c>
@@ -15334,16 +15333,16 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="271" t="s">
+      <c r="A35" s="252" t="s">
         <v>290</v>
       </c>
-      <c r="B35" s="271" t="s">
+      <c r="B35" s="252" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="271"/>
+      <c r="C35" s="252"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="271"/>
+      <c r="A36" s="252"/>
       <c r="B36" s="5" t="s">
         <v>293</v>
       </c>
@@ -15429,16 +15428,16 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="271" t="s">
+      <c r="A45" s="252" t="s">
         <v>290</v>
       </c>
-      <c r="B45" s="271" t="s">
+      <c r="B45" s="252" t="s">
         <v>315</v>
       </c>
-      <c r="C45" s="271"/>
+      <c r="C45" s="252"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="271"/>
+      <c r="A46" s="252"/>
       <c r="B46" s="5" t="s">
         <v>293</v>
       </c>
@@ -15524,16 +15523,16 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="271" t="s">
+      <c r="A55" s="252" t="s">
         <v>290</v>
       </c>
-      <c r="B55" s="271" t="s">
+      <c r="B55" s="252" t="s">
         <v>322</v>
       </c>
-      <c r="C55" s="271"/>
+      <c r="C55" s="252"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="271"/>
+      <c r="A56" s="252"/>
       <c r="B56" s="5" t="s">
         <v>293</v>
       </c>
@@ -15619,16 +15618,16 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="271" t="s">
+      <c r="A65" s="252" t="s">
         <v>290</v>
       </c>
-      <c r="B65" s="271" t="s">
+      <c r="B65" s="252" t="s">
         <v>327</v>
       </c>
-      <c r="C65" s="271"/>
+      <c r="C65" s="252"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="271"/>
+      <c r="A66" s="252"/>
       <c r="B66" s="5" t="s">
         <v>293</v>
       </c>
@@ -15759,18 +15758,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="A65:A66"/>
     <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="69" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fix page break on summary page
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maheug\Documents\GitHub\EquipTestingSpreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AF68CC-9649-4EE3-9E09-E077CDCBBB2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -24,6 +23,7 @@
     <definedName name="CTReport" localSheetId="1">"First,CTDI,ACRPhantom,Comments"</definedName>
     <definedName name="First">Sheet1!$B$1:$M$66</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$B$1:$M$198</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$A$1:$F$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1068,14 +1068,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="166" formatCode="mmm\-yyyy"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -2177,7 +2177,7 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="275">
+  <cellXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2917,13 +2917,70 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2938,72 +2995,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Fail" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Heading" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Heading1" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Fail" xfId="6"/>
+    <cellStyle name="Heading" xfId="3"/>
+    <cellStyle name="Heading1" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pass" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Result" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Pass" xfId="5"/>
+    <cellStyle name="Result" xfId="1"/>
+    <cellStyle name="Result2" xfId="2"/>
   </cellStyles>
   <dxfs count="32">
     <dxf>
@@ -3717,27 +3744,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
     <col min="5" max="5" width="16" style="6" customWidth="1"/>
     <col min="6" max="6" width="22" style="6" customWidth="1"/>
     <col min="7" max="1020" width="9.6640625" style="6" customWidth="1"/>
-    <col min="1021" max="1025" width="12.77734375" style="6" customWidth="1"/>
+    <col min="1021" max="1025" width="12.83203125" style="6" customWidth="1"/>
     <col min="1026" max="16384" width="9.33203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="218" t="s">
         <v>0</v>
       </c>
@@ -3763,7 +3790,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="220" t="s">
         <v>1</v>
       </c>
@@ -3800,74 +3827,74 @@
         <v>337</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="222" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="251" t="str">
+      <c r="B6" s="254" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="251"/>
+      <c r="C6" s="254"/>
       <c r="D6" s="223" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="251" t="str">
+      <c r="E6" s="254" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="251"/>
+      <c r="F6" s="254"/>
       <c r="G6" s="1"/>
       <c r="J6" s="248" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="222" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
+      <c r="B7" s="255"/>
+      <c r="C7" s="255"/>
       <c r="D7" s="223" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="249" t="str">
+      <c r="E7" s="255" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="249"/>
+      <c r="F7" s="255"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="222" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="249"/>
-      <c r="C8" s="249"/>
+      <c r="B8" s="255"/>
+      <c r="C8" s="255"/>
       <c r="D8" s="223" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="249" t="str">
+      <c r="E8" s="255" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="249"/>
+      <c r="F8" s="255"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="249"/>
-      <c r="C9" s="249"/>
+      <c r="B9" s="255"/>
+      <c r="C9" s="255"/>
       <c r="D9" s="223" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="249" t="str">
+      <c r="E9" s="255" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="249"/>
+      <c r="F9" s="255"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3877,19 +3904,19 @@
       <c r="D10" s="223" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="250" t="str">
+      <c r="E10" s="256" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="250"/>
+      <c r="F10" s="256"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="251"/>
-      <c r="C11" s="251"/>
+      <c r="B11" s="254"/>
+      <c r="C11" s="254"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -3912,10 +3939,10 @@
       <c r="A13" s="225" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="251" t="s">
+      <c r="B13" s="254" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="251"/>
+      <c r="C13" s="254"/>
       <c r="D13" s="223" t="s">
         <v>16</v>
       </c>
@@ -3943,7 +3970,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="228" t="s">
         <v>18</v>
       </c>
@@ -3968,7 +3995,7 @@
       <c r="F17" s="227"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="231" t="s">
         <v>22</v>
       </c>
@@ -3979,7 +4006,7 @@
       <c r="F18" s="230"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="231" t="s">
         <v>24</v>
       </c>
@@ -3993,7 +4020,7 @@
       <c r="F19" s="230"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="231" t="s">
         <v>26</v>
       </c>
@@ -4007,7 +4034,7 @@
       <c r="F20" s="230"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="231" t="s">
         <v>28</v>
       </c>
@@ -4021,7 +4048,7 @@
       <c r="F21" s="230"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="231" t="s">
         <v>30</v>
       </c>
@@ -4032,7 +4059,7 @@
       <c r="F22" s="230"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="231" t="s">
         <v>32</v>
       </c>
@@ -4135,7 +4162,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="232"/>
       <c r="B32" s="233"/>
       <c r="C32" s="233"/>
@@ -4144,7 +4171,7 @@
       <c r="F32" s="234"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="235"/>
       <c r="B33" s="236"/>
       <c r="C33" s="236"/>
@@ -4153,7 +4180,7 @@
       <c r="F33" s="237"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="235"/>
       <c r="B34" s="236"/>
       <c r="C34" s="236"/>
@@ -4162,7 +4189,7 @@
       <c r="F34" s="237"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="235"/>
       <c r="B35" s="236"/>
       <c r="C35" s="236"/>
@@ -4171,7 +4198,7 @@
       <c r="F35" s="237"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="235"/>
       <c r="B36" s="236"/>
       <c r="C36" s="236"/>
@@ -4180,7 +4207,7 @@
       <c r="F36" s="237"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="235"/>
       <c r="B37" s="236"/>
       <c r="C37" s="236"/>
@@ -4189,7 +4216,7 @@
       <c r="F37" s="237"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="235"/>
       <c r="B38" s="236"/>
       <c r="C38" s="236"/>
@@ -4198,7 +4225,7 @@
       <c r="F38" s="237"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="235"/>
       <c r="B39" s="236"/>
       <c r="C39" s="236"/>
@@ -4207,7 +4234,7 @@
       <c r="F39" s="237"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="238"/>
       <c r="B40" s="239"/>
       <c r="C40" s="239"/>
@@ -4218,23 +4245,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29">
       <formula1>$J$1:$J$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F23">
       <formula1>$J$4:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -4248,23 +4275,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72:J88"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="11" customWidth="1"/>
-    <col min="2" max="2" width="2.77734375" style="17" customWidth="1"/>
-    <col min="3" max="13" width="12.77734375" style="17" customWidth="1"/>
-    <col min="14" max="14" width="2.77734375" style="17" customWidth="1"/>
-    <col min="15" max="30" width="12.77734375" style="17" customWidth="1"/>
-    <col min="31" max="32" width="12.77734375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" style="17" customWidth="1"/>
+    <col min="3" max="13" width="12.83203125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" style="17" customWidth="1"/>
+    <col min="15" max="30" width="12.83203125" style="17" customWidth="1"/>
+    <col min="31" max="32" width="12.83203125" style="22" customWidth="1"/>
     <col min="33" max="16384" width="9.33203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11">
         <v>1</v>
       </c>
@@ -4297,7 +4326,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>2</v>
       </c>
@@ -4315,7 +4344,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>3</v>
       </c>
@@ -4334,7 +4363,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>4</v>
       </c>
@@ -4349,7 +4378,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>5</v>
       </c>
@@ -4364,7 +4393,7 @@
       </c>
       <c r="Y5" s="27"/>
     </row>
-    <row r="6" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>6</v>
       </c>
@@ -4401,14 +4430,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>7</v>
       </c>
       <c r="O7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="270"/>
+      <c r="P7" s="249"/>
       <c r="W7" s="17" t="s">
         <v>50</v>
       </c>
@@ -4432,7 +4461,7 @@
         <v>First,CTDI,ACRPhantom</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>8</v>
       </c>
@@ -4442,24 +4471,24 @@
       <c r="O8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="271" t="str">
+      <c r="P8" s="250" t="str">
         <f>IF(AB8="","",AB8)</f>
         <v/>
       </c>
       <c r="AA8" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="AB8" s="272"/>
+      <c r="AB8" s="251"/>
       <c r="AC8" s="42" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AD8" s="273" t="str">
+      <c r="AD8" s="252" t="str">
         <f>IF(P7="","",P7)</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>9</v>
       </c>
@@ -4507,7 +4536,7 @@
         <v>Eugene Mah</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>10</v>
       </c>
@@ -4515,19 +4544,19 @@
       <c r="E10" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="265" t="str">
+      <c r="F10" s="257" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="265"/>
+      <c r="G10" s="257"/>
       <c r="J10" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="265" t="str">
+      <c r="K10" s="257" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="265"/>
+      <c r="L10" s="257"/>
       <c r="M10" s="25"/>
       <c r="O10" s="26"/>
       <c r="Q10" s="30" t="s">
@@ -4560,7 +4589,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>11</v>
       </c>
@@ -4568,19 +4597,19 @@
       <c r="E11" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="268" t="str">
+      <c r="F11" s="258" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="268"/>
+      <c r="G11" s="258"/>
       <c r="J11" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="265" t="str">
+      <c r="K11" s="257" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="265"/>
+      <c r="L11" s="257"/>
       <c r="M11" s="25"/>
       <c r="O11" s="26"/>
       <c r="Q11" s="30" t="s">
@@ -4613,7 +4642,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>12</v>
       </c>
@@ -4621,19 +4650,19 @@
       <c r="E12" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="268" t="str">
+      <c r="F12" s="258" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="268"/>
+      <c r="G12" s="258"/>
       <c r="J12" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="269" t="str">
+      <c r="K12" s="259" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="269"/>
+      <c r="L12" s="259"/>
       <c r="M12" s="25"/>
       <c r="O12" s="26"/>
       <c r="Q12" s="30" t="s">
@@ -4666,7 +4695,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>13</v>
       </c>
@@ -4674,19 +4703,19 @@
       <c r="E13" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="268" t="str">
+      <c r="F13" s="258" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="268"/>
+      <c r="G13" s="258"/>
       <c r="J13" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="265" t="str">
+      <c r="K13" s="257" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="265"/>
+      <c r="L13" s="257"/>
       <c r="M13" s="25"/>
       <c r="O13" s="26"/>
       <c r="Q13" s="30" t="s">
@@ -4719,7 +4748,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>14</v>
       </c>
@@ -4752,7 +4781,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>15</v>
       </c>
@@ -4776,7 +4805,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>16</v>
       </c>
@@ -4784,19 +4813,19 @@
       <c r="E16" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="265" t="str">
+      <c r="F16" s="257" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="265"/>
+      <c r="G16" s="257"/>
       <c r="J16" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="269" t="str">
+      <c r="K16" s="259" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="269"/>
+      <c r="L16" s="259"/>
       <c r="M16" s="25"/>
       <c r="O16" s="26"/>
       <c r="P16" s="58" t="s">
@@ -4816,7 +4845,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>17</v>
       </c>
@@ -4824,19 +4853,19 @@
       <c r="E17" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="268" t="str">
+      <c r="F17" s="258" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="268"/>
+      <c r="G17" s="258"/>
       <c r="J17" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="265" t="str">
+      <c r="K17" s="257" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="265"/>
+      <c r="L17" s="257"/>
       <c r="M17" s="25"/>
       <c r="O17" s="26"/>
       <c r="Q17" s="30" t="s">
@@ -4869,7 +4898,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>18</v>
       </c>
@@ -4877,11 +4906,11 @@
       <c r="J18" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="265" t="str">
+      <c r="K18" s="257" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="265"/>
+      <c r="L18" s="257"/>
       <c r="M18" s="25"/>
       <c r="O18" s="26"/>
       <c r="Q18" s="30" t="s">
@@ -4914,7 +4943,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>19</v>
       </c>
@@ -4945,7 +4974,7 @@
       <c r="AC19" s="22"/>
       <c r="AD19" s="22"/>
     </row>
-    <row r="20" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>20</v>
       </c>
@@ -4953,11 +4982,11 @@
       <c r="E20" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="265" t="str">
+      <c r="F20" s="257" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="265"/>
+      <c r="G20" s="257"/>
       <c r="I20" s="61" t="s">
         <v>76</v>
       </c>
@@ -4974,7 +5003,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>21</v>
       </c>
@@ -4982,19 +5011,19 @@
       <c r="E21" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="267" t="str">
+      <c r="F21" s="260" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="267"/>
+      <c r="G21" s="260"/>
       <c r="J21" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="265" t="str">
+      <c r="K21" s="257" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="265"/>
+      <c r="L21" s="257"/>
       <c r="M21" s="25"/>
       <c r="O21" s="26"/>
       <c r="Q21" s="30" t="s">
@@ -5022,7 +5051,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>22</v>
       </c>
@@ -5033,11 +5062,11 @@
       <c r="J22" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="265" t="str">
+      <c r="K22" s="257" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="265"/>
+      <c r="L22" s="257"/>
       <c r="M22" s="25"/>
       <c r="O22" s="26"/>
       <c r="Q22" s="30" t="s">
@@ -5070,7 +5099,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>23</v>
       </c>
@@ -5078,19 +5107,19 @@
       <c r="E23" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="265" t="str">
+      <c r="F23" s="257" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="265"/>
+      <c r="G23" s="257"/>
       <c r="J23" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="265" t="str">
+      <c r="K23" s="257" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="265"/>
+      <c r="L23" s="257"/>
       <c r="M23" s="25"/>
       <c r="O23" s="26"/>
       <c r="P23" s="58" t="s">
@@ -5118,7 +5147,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>24</v>
       </c>
@@ -5126,11 +5155,11 @@
       <c r="E24" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="265" t="str">
+      <c r="F24" s="257" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="265"/>
+      <c r="G24" s="257"/>
       <c r="M24" s="25"/>
       <c r="O24" s="26"/>
       <c r="Q24" s="30" t="s">
@@ -5163,7 +5192,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>25</v>
       </c>
@@ -5171,11 +5200,11 @@
       <c r="E25" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="265" t="str">
+      <c r="F25" s="257" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="265"/>
+      <c r="G25" s="257"/>
       <c r="J25" s="57" t="s">
         <v>82</v>
       </c>
@@ -5203,7 +5232,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>26</v>
       </c>
@@ -5215,11 +5244,11 @@
       <c r="J26" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="265" t="str">
+      <c r="K26" s="257" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="265"/>
+      <c r="L26" s="257"/>
       <c r="M26" s="25"/>
       <c r="O26" s="26"/>
       <c r="Q26" s="30" t="s">
@@ -5239,7 +5268,7 @@
       <c r="AC26" s="22"/>
       <c r="AD26" s="22"/>
     </row>
-    <row r="27" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>27</v>
       </c>
@@ -5247,19 +5276,19 @@
       <c r="E27" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="265" t="str">
+      <c r="F27" s="257" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="265"/>
+      <c r="G27" s="257"/>
       <c r="J27" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="265" t="str">
+      <c r="K27" s="257" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="265"/>
+      <c r="L27" s="257"/>
       <c r="M27" s="25"/>
       <c r="O27" s="26"/>
       <c r="P27" s="58" t="s">
@@ -5278,7 +5307,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>28</v>
       </c>
@@ -5286,11 +5315,11 @@
       <c r="E28" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="265" t="str">
+      <c r="F28" s="257" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="265"/>
+      <c r="G28" s="257"/>
       <c r="M28" s="25"/>
       <c r="O28" s="26"/>
       <c r="Q28" s="30" t="s">
@@ -5323,7 +5352,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>29</v>
       </c>
@@ -5331,11 +5360,11 @@
       <c r="E29" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="265" t="str">
+      <c r="F29" s="257" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="265"/>
+      <c r="G29" s="257"/>
       <c r="M29" s="25"/>
       <c r="O29" s="26"/>
       <c r="Q29" s="30" t="s">
@@ -5360,7 +5389,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>30</v>
       </c>
@@ -5399,7 +5428,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>31</v>
       </c>
@@ -5427,7 +5456,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>32</v>
       </c>
@@ -5445,10 +5474,10 @@
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
-      <c r="L32" s="266" t="s">
+      <c r="L32" s="261" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="266"/>
+      <c r="M32" s="261"/>
       <c r="AA32" s="30" t="s">
         <v>70</v>
       </c>
@@ -5462,7 +5491,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>33</v>
       </c>
@@ -5498,7 +5527,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>34</v>
       </c>
@@ -5543,7 +5572,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>35</v>
       </c>
@@ -5575,7 +5604,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>36</v>
       </c>
@@ -5612,7 +5641,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>37</v>
       </c>
@@ -5647,7 +5676,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>38</v>
       </c>
@@ -5682,7 +5711,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <v>39</v>
       </c>
@@ -5708,7 +5737,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
         <v>40</v>
       </c>
@@ -5737,7 +5766,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>41</v>
       </c>
@@ -5763,7 +5792,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
         <v>42</v>
       </c>
@@ -5789,7 +5818,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
         <v>43</v>
       </c>
@@ -5821,7 +5850,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>44</v>
       </c>
@@ -5856,7 +5885,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>45</v>
       </c>
@@ -5891,7 +5920,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>46</v>
       </c>
@@ -5917,7 +5946,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
         <v>47</v>
       </c>
@@ -5952,7 +5981,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>48</v>
       </c>
@@ -5987,7 +6016,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>49</v>
       </c>
@@ -6022,7 +6051,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>50</v>
       </c>
@@ -6054,7 +6083,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
         <v>51</v>
       </c>
@@ -6091,7 +6120,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11">
         <v>52</v>
       </c>
@@ -6128,7 +6157,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11">
         <v>53</v>
       </c>
@@ -6165,7 +6194,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
         <v>54</v>
       </c>
@@ -6202,7 +6231,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11">
         <v>55</v>
       </c>
@@ -6239,7 +6268,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
         <v>56</v>
       </c>
@@ -6274,7 +6303,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11">
         <v>57</v>
       </c>
@@ -6300,7 +6329,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11">
         <v>58</v>
       </c>
@@ -6329,7 +6358,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
         <v>59</v>
       </c>
@@ -6364,7 +6393,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>60</v>
       </c>
@@ -6390,7 +6419,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
         <v>61</v>
       </c>
@@ -6422,7 +6451,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>62</v>
       </c>
@@ -6457,7 +6486,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>63</v>
       </c>
@@ -6484,7 +6513,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>64</v>
       </c>
@@ -6521,14 +6550,14 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
         <v>65</v>
       </c>
       <c r="C65" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D65" s="274" t="str">
+      <c r="D65" s="253" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -6560,7 +6589,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11">
         <v>66</v>
       </c>
@@ -6599,7 +6628,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>1</v>
       </c>
@@ -6631,7 +6660,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>2</v>
       </c>
@@ -6655,7 +6684,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:30" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:30" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>3</v>
       </c>
@@ -6689,7 +6718,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11">
         <v>4</v>
       </c>
@@ -6733,7 +6762,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>5</v>
       </c>
@@ -6785,7 +6814,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="11">
         <v>6</v>
       </c>
@@ -6793,23 +6822,23 @@
       <c r="E72" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="F72" s="79" t="str">
+      <c r="F72" s="275" t="str">
         <f t="shared" ref="F72:F88" si="10">IF(Q72="","",Q72)</f>
         <v/>
       </c>
-      <c r="G72" s="80" t="str">
+      <c r="G72" s="276" t="str">
         <f t="shared" ref="G72:G88" si="11">IF(R72="","",R72)</f>
         <v/>
       </c>
-      <c r="H72" s="80" t="str">
+      <c r="H72" s="276" t="str">
         <f t="shared" ref="H72:H88" si="12">IF(S72="","",S72)</f>
         <v/>
       </c>
-      <c r="I72" s="80" t="str">
+      <c r="I72" s="276" t="str">
         <f t="shared" ref="I72:I88" si="13">IF(T72="","",T72)</f>
         <v/>
       </c>
-      <c r="J72" s="81" t="str">
+      <c r="J72" s="277" t="str">
         <f t="shared" ref="J72:J88" si="14">IF(U72="","",U72)</f>
         <v/>
       </c>
@@ -6852,7 +6881,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11">
         <v>7</v>
       </c>
@@ -6860,23 +6889,23 @@
       <c r="E73" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="F73" s="82" t="str">
+      <c r="F73" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G73" s="83" t="str">
+      <c r="G73" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H73" s="83" t="str">
+      <c r="H73" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I73" s="83" t="str">
+      <c r="I73" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J73" s="84" t="str">
+      <c r="J73" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -6919,7 +6948,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
         <v>8</v>
       </c>
@@ -6927,23 +6956,23 @@
       <c r="E74" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="F74" s="82" t="str">
+      <c r="F74" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G74" s="83" t="str">
+      <c r="G74" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H74" s="83" t="str">
+      <c r="H74" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I74" s="83" t="str">
+      <c r="I74" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J74" s="84" t="str">
+      <c r="J74" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -6986,7 +7015,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11">
         <v>9</v>
       </c>
@@ -6994,23 +7023,23 @@
       <c r="E75" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="F75" s="82" t="str">
+      <c r="F75" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G75" s="83" t="str">
+      <c r="G75" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H75" s="83" t="str">
+      <c r="H75" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I75" s="83" t="str">
+      <c r="I75" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J75" s="84" t="str">
+      <c r="J75" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7053,7 +7082,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11">
         <v>10</v>
       </c>
@@ -7061,23 +7090,23 @@
       <c r="E76" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="F76" s="82" t="str">
+      <c r="F76" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G76" s="83" t="str">
+      <c r="G76" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H76" s="83" t="str">
+      <c r="H76" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I76" s="83" t="str">
+      <c r="I76" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J76" s="84" t="str">
+      <c r="J76" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7120,7 +7149,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11">
         <v>11</v>
       </c>
@@ -7128,23 +7157,23 @@
       <c r="E77" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="F77" s="82" t="str">
+      <c r="F77" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G77" s="83" t="str">
+      <c r="G77" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H77" s="83" t="str">
+      <c r="H77" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I77" s="83" t="str">
+      <c r="I77" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J77" s="84" t="str">
+      <c r="J77" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7187,7 +7216,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="11">
         <v>12</v>
       </c>
@@ -7195,23 +7224,23 @@
       <c r="E78" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="F78" s="82" t="str">
+      <c r="F78" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G78" s="83" t="str">
+      <c r="G78" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H78" s="83" t="str">
+      <c r="H78" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I78" s="83" t="str">
+      <c r="I78" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J78" s="84" t="str">
+      <c r="J78" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7248,7 +7277,7 @@
       <c r="AC78" s="22"/>
       <c r="AD78" s="22"/>
     </row>
-    <row r="79" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="11">
         <v>13</v>
       </c>
@@ -7256,23 +7285,23 @@
       <c r="E79" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="82" t="str">
+      <c r="F79" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G79" s="83" t="str">
+      <c r="G79" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H79" s="83" t="str">
+      <c r="H79" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I79" s="83" t="str">
+      <c r="I79" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J79" s="84" t="str">
+      <c r="J79" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7315,7 +7344,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="11">
         <v>14</v>
       </c>
@@ -7323,23 +7352,23 @@
       <c r="E80" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="F80" s="82" t="str">
+      <c r="F80" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G80" s="83" t="str">
+      <c r="G80" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H80" s="83" t="str">
+      <c r="H80" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I80" s="83" t="str">
+      <c r="I80" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J80" s="84" t="str">
+      <c r="J80" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7382,7 +7411,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11">
         <v>15</v>
       </c>
@@ -7390,23 +7419,23 @@
       <c r="E81" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="F81" s="82" t="str">
+      <c r="F81" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G81" s="83" t="str">
+      <c r="G81" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H81" s="83" t="str">
+      <c r="H81" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I81" s="83" t="str">
+      <c r="I81" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J81" s="84" t="str">
+      <c r="J81" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7449,7 +7478,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11">
         <v>16</v>
       </c>
@@ -7457,23 +7486,23 @@
       <c r="E82" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="F82" s="82" t="str">
+      <c r="F82" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G82" s="83" t="str">
+      <c r="G82" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H82" s="83" t="str">
+      <c r="H82" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I82" s="83" t="str">
+      <c r="I82" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J82" s="84" t="str">
+      <c r="J82" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7516,7 +7545,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11">
         <v>17</v>
       </c>
@@ -7524,23 +7553,23 @@
       <c r="E83" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="F83" s="82" t="str">
+      <c r="F83" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G83" s="83" t="str">
+      <c r="G83" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H83" s="83" t="str">
+      <c r="H83" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I83" s="83" t="str">
+      <c r="I83" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J83" s="84" t="str">
+      <c r="J83" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7583,7 +7612,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="11">
         <v>18</v>
       </c>
@@ -7591,23 +7620,23 @@
       <c r="E84" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="F84" s="82" t="str">
+      <c r="F84" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G84" s="83" t="str">
+      <c r="G84" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H84" s="83" t="str">
+      <c r="H84" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I84" s="83" t="str">
+      <c r="I84" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J84" s="84" t="str">
+      <c r="J84" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7650,7 +7679,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11">
         <v>19</v>
       </c>
@@ -7658,23 +7687,23 @@
       <c r="E85" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="F85" s="82" t="str">
+      <c r="F85" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G85" s="83" t="str">
+      <c r="G85" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H85" s="83" t="str">
+      <c r="H85" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I85" s="83" t="str">
+      <c r="I85" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J85" s="84" t="str">
+      <c r="J85" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7717,7 +7746,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11">
         <v>20</v>
       </c>
@@ -7725,23 +7754,23 @@
       <c r="E86" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="F86" s="82" t="str">
+      <c r="F86" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G86" s="83" t="str">
+      <c r="G86" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H86" s="83" t="str">
+      <c r="H86" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I86" s="83" t="str">
+      <c r="I86" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J86" s="84" t="str">
+      <c r="J86" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7784,7 +7813,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11">
         <v>21</v>
       </c>
@@ -7792,23 +7821,23 @@
       <c r="E87" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="F87" s="82" t="str">
+      <c r="F87" s="278" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G87" s="83" t="str">
+      <c r="G87" s="279" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H87" s="83" t="str">
+      <c r="H87" s="279" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I87" s="83" t="str">
+      <c r="I87" s="279" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J87" s="84" t="str">
+      <c r="J87" s="280" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7851,7 +7880,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
         <v>22</v>
       </c>
@@ -7859,23 +7888,23 @@
       <c r="E88" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="F88" s="85" t="str">
+      <c r="F88" s="281" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="G88" s="86" t="str">
+      <c r="G88" s="282" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H88" s="86" t="str">
+      <c r="H88" s="282" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I88" s="86" t="str">
+      <c r="I88" s="282" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J88" s="87" t="str">
+      <c r="J88" s="283" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7918,7 +7947,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11">
         <v>23</v>
       </c>
@@ -7959,7 +7988,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>24</v>
       </c>
@@ -7998,21 +8027,21 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11">
         <v>25</v>
       </c>
       <c r="B91" s="23"/>
       <c r="E91" s="71"/>
-      <c r="F91" s="258" t="s">
+      <c r="F91" s="267" t="s">
         <v>151</v>
       </c>
-      <c r="G91" s="258"/>
-      <c r="H91" s="258"/>
-      <c r="I91" s="259" t="s">
+      <c r="G91" s="267"/>
+      <c r="H91" s="267"/>
+      <c r="I91" s="268" t="s">
         <v>152</v>
       </c>
-      <c r="J91" s="259"/>
+      <c r="J91" s="268"/>
       <c r="M91" s="25"/>
       <c r="O91" s="26"/>
       <c r="P91" s="30" t="s">
@@ -8037,7 +8066,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11">
         <v>26</v>
       </c>
@@ -8100,7 +8129,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11">
         <v>27</v>
       </c>
@@ -8171,15 +8200,15 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11">
         <v>28</v>
       </c>
       <c r="B94" s="23"/>
-      <c r="D94" s="260" t="s">
+      <c r="D94" s="269" t="s">
         <v>161</v>
       </c>
-      <c r="E94" s="260" t="s">
+      <c r="E94" s="269" t="s">
         <v>161</v>
       </c>
       <c r="F94" s="97" t="str">
@@ -8232,13 +8261,13 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <v>29</v>
       </c>
       <c r="B95" s="23"/>
-      <c r="D95" s="260"/>
-      <c r="E95" s="260"/>
+      <c r="D95" s="269"/>
+      <c r="E95" s="269"/>
       <c r="F95" s="102" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -8289,13 +8318,13 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <v>30</v>
       </c>
       <c r="B96" s="23"/>
-      <c r="D96" s="260"/>
-      <c r="E96" s="260"/>
+      <c r="D96" s="269"/>
+      <c r="E96" s="269"/>
       <c r="F96" s="107" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -8339,7 +8368,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="11">
         <v>31</v>
       </c>
@@ -8400,7 +8429,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11">
         <v>32</v>
       </c>
@@ -8461,7 +8490,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
         <v>33</v>
       </c>
@@ -8521,7 +8550,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11">
         <v>34</v>
       </c>
@@ -8581,7 +8610,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="11">
         <v>35</v>
       </c>
@@ -8633,7 +8662,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="11">
         <v>36</v>
       </c>
@@ -8702,7 +8731,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11">
         <v>37</v>
       </c>
@@ -8756,7 +8785,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11">
         <v>38</v>
       </c>
@@ -8799,7 +8828,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="11">
         <v>39</v>
       </c>
@@ -8839,7 +8868,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11">
         <v>40</v>
       </c>
@@ -8876,7 +8905,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11">
         <v>41</v>
       </c>
@@ -8908,7 +8937,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11">
         <v>42</v>
       </c>
@@ -8958,7 +8987,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="11">
         <v>43</v>
       </c>
@@ -8997,7 +9026,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
         <v>44</v>
       </c>
@@ -9039,7 +9068,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="11">
         <v>45</v>
       </c>
@@ -9091,7 +9120,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="11">
         <v>46</v>
       </c>
@@ -9118,15 +9147,15 @@
       <c r="J112" s="22"/>
       <c r="M112" s="25"/>
       <c r="O112" s="26"/>
-      <c r="Q112" s="261" t="s">
+      <c r="Q112" s="270" t="s">
         <v>151</v>
       </c>
-      <c r="R112" s="261"/>
-      <c r="S112" s="261"/>
-      <c r="T112" s="253" t="s">
+      <c r="R112" s="270"/>
+      <c r="S112" s="270"/>
+      <c r="T112" s="272" t="s">
         <v>152</v>
       </c>
-      <c r="U112" s="253"/>
+      <c r="U112" s="272"/>
       <c r="W112" s="58" t="s">
         <v>158</v>
       </c>
@@ -9144,7 +9173,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="11">
         <v>47</v>
       </c>
@@ -9189,7 +9218,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="11">
         <v>48</v>
       </c>
@@ -9250,7 +9279,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="115" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="11">
         <v>49</v>
       </c>
@@ -9264,10 +9293,10 @@
       </c>
       <c r="J115" s="22"/>
       <c r="M115" s="25"/>
-      <c r="O115" s="254" t="s">
+      <c r="O115" s="273" t="s">
         <v>161</v>
       </c>
-      <c r="P115" s="254" t="s">
+      <c r="P115" s="273" t="s">
         <v>161</v>
       </c>
       <c r="Q115" s="141"/>
@@ -9295,7 +9324,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="11">
         <v>50</v>
       </c>
@@ -9307,8 +9336,8 @@
       <c r="H116" s="22"/>
       <c r="J116" s="22"/>
       <c r="M116" s="25"/>
-      <c r="O116" s="254"/>
-      <c r="P116" s="254"/>
+      <c r="O116" s="273"/>
+      <c r="P116" s="273"/>
       <c r="Q116" s="144"/>
       <c r="R116" s="145"/>
       <c r="S116" s="146"/>
@@ -9336,7 +9365,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="11">
         <v>51</v>
       </c>
@@ -9348,8 +9377,8 @@
       <c r="H117" s="22"/>
       <c r="J117" s="22"/>
       <c r="M117" s="25"/>
-      <c r="O117" s="254"/>
-      <c r="P117" s="254"/>
+      <c r="O117" s="273"/>
+      <c r="P117" s="273"/>
       <c r="Q117" s="148"/>
       <c r="R117" s="149"/>
       <c r="S117" s="150"/>
@@ -9377,7 +9406,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="11">
         <v>52</v>
       </c>
@@ -9435,7 +9464,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="11">
         <v>53</v>
       </c>
@@ -9478,7 +9507,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11">
         <v>54</v>
       </c>
@@ -9515,7 +9544,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="11">
         <v>55</v>
       </c>
@@ -9562,7 +9591,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="11">
         <v>56</v>
       </c>
@@ -9617,7 +9646,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11">
         <v>57</v>
       </c>
@@ -9664,7 +9693,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="11">
         <v>58</v>
       </c>
@@ -9713,7 +9742,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="11">
         <v>59</v>
       </c>
@@ -9775,7 +9804,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="11">
         <v>60</v>
       </c>
@@ -9840,7 +9869,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="11">
         <v>61</v>
       </c>
@@ -9888,7 +9917,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="11">
         <v>62</v>
       </c>
@@ -9920,7 +9949,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11">
         <v>63</v>
       </c>
@@ -9945,7 +9974,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11">
         <v>64</v>
       </c>
@@ -9983,14 +10012,14 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A131" s="11">
         <v>65</v>
       </c>
       <c r="C131" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D131" s="274" t="str">
+      <c r="D131" s="253" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -10029,7 +10058,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="11">
         <v>66</v>
       </c>
@@ -10060,7 +10089,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="133" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="11">
         <v>1</v>
       </c>
@@ -10090,7 +10119,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="11">
         <v>2</v>
       </c>
@@ -10102,7 +10131,7 @@
         <v>CT System Compliance Inspection</v>
       </c>
       <c r="O134" s="26"/>
-      <c r="P134" s="255" t="s">
+      <c r="P134" s="274" t="s">
         <v>181</v>
       </c>
       <c r="Q134" s="175"/>
@@ -10123,7 +10152,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A135" s="11">
         <v>3</v>
       </c>
@@ -10142,7 +10171,7 @@
       <c r="L135" s="15"/>
       <c r="M135" s="16"/>
       <c r="O135" s="26"/>
-      <c r="P135" s="255"/>
+      <c r="P135" s="274"/>
       <c r="Q135" s="175"/>
       <c r="R135" s="176"/>
       <c r="S135" s="176"/>
@@ -10161,7 +10190,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="11">
         <v>4</v>
       </c>
@@ -10190,7 +10219,7 @@
       </c>
       <c r="M136" s="25"/>
       <c r="O136" s="26"/>
-      <c r="P136" s="255"/>
+      <c r="P136" s="274"/>
       <c r="Q136" s="178"/>
       <c r="R136" s="179"/>
       <c r="S136" s="179"/>
@@ -10209,7 +10238,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="11">
         <v>5</v>
       </c>
@@ -10250,7 +10279,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="11">
         <v>6</v>
       </c>
@@ -10300,7 +10329,7 @@
       <c r="AC138" s="22"/>
       <c r="AD138" s="22"/>
     </row>
-    <row r="139" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="11">
         <v>7</v>
       </c>
@@ -10350,7 +10379,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="11">
         <v>8</v>
       </c>
@@ -10400,7 +10429,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="11">
         <v>9</v>
       </c>
@@ -10442,7 +10471,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="11">
         <v>10</v>
       </c>
@@ -10470,7 +10499,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="11">
         <v>11</v>
       </c>
@@ -10489,7 +10518,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="11">
         <v>12</v>
       </c>
@@ -10528,7 +10557,7 @@
       <c r="AC144" s="22"/>
       <c r="AD144" s="22"/>
     </row>
-    <row r="145" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="11">
         <v>13</v>
       </c>
@@ -10592,7 +10621,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="11">
         <v>14</v>
       </c>
@@ -10655,7 +10684,7 @@
       <c r="AC146" s="22"/>
       <c r="AD146" s="187"/>
     </row>
-    <row r="147" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="11">
         <v>15</v>
       </c>
@@ -10706,7 +10735,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="11">
         <v>16</v>
       </c>
@@ -10761,7 +10790,7 @@
       <c r="AC148" s="22"/>
       <c r="AD148" s="187"/>
     </row>
-    <row r="149" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="11">
         <v>17</v>
       </c>
@@ -10825,7 +10854,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="11">
         <v>18</v>
       </c>
@@ -10880,7 +10909,7 @@
       <c r="AB150" s="187"/>
       <c r="AD150" s="187"/>
     </row>
-    <row r="151" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A151" s="11">
         <v>19</v>
       </c>
@@ -10938,7 +10967,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="11">
         <v>20</v>
       </c>
@@ -10963,7 +10992,7 @@
       <c r="AB152" s="187"/>
       <c r="AD152" s="187"/>
     </row>
-    <row r="153" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="11">
         <v>21</v>
       </c>
@@ -10993,7 +11022,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="11">
         <v>22</v>
       </c>
@@ -11030,15 +11059,15 @@
         <v>150</v>
       </c>
       <c r="W154" s="190"/>
-      <c r="X154" s="256" t="s">
+      <c r="X154" s="265" t="s">
         <v>226</v>
       </c>
-      <c r="Y154" s="256"/>
+      <c r="Y154" s="265"/>
       <c r="AA154" s="30"/>
       <c r="AB154" s="187"/>
       <c r="AD154" s="187"/>
     </row>
-    <row r="155" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="11">
         <v>23</v>
       </c>
@@ -11073,7 +11102,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="11">
         <v>24</v>
       </c>
@@ -11105,7 +11134,7 @@
       <c r="AB156" s="187"/>
       <c r="AD156" s="187"/>
     </row>
-    <row r="157" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="11">
         <v>25</v>
       </c>
@@ -11165,7 +11194,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="11">
         <v>26</v>
       </c>
@@ -11218,7 +11247,7 @@
       <c r="AB158" s="187"/>
       <c r="AD158" s="187"/>
     </row>
-    <row r="159" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="11">
         <v>27</v>
       </c>
@@ -11278,7 +11307,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="11">
         <v>28</v>
       </c>
@@ -11331,7 +11360,7 @@
       <c r="AB160" s="187"/>
       <c r="AD160" s="31"/>
     </row>
-    <row r="161" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="11">
         <v>29</v>
       </c>
@@ -11384,7 +11413,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="11">
         <v>30</v>
       </c>
@@ -11427,7 +11456,7 @@
       <c r="AB162" s="187"/>
       <c r="AD162" s="187"/>
     </row>
-    <row r="163" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="11">
         <v>31</v>
       </c>
@@ -11476,7 +11505,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="11">
         <v>32</v>
       </c>
@@ -11499,7 +11528,7 @@
       <c r="AB164" s="187"/>
       <c r="AD164" s="187"/>
     </row>
-    <row r="165" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="11">
         <v>33</v>
       </c>
@@ -11523,7 +11552,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="11">
         <v>34</v>
       </c>
@@ -11538,7 +11567,7 @@
       <c r="AB166" s="187"/>
       <c r="AD166" s="187"/>
     </row>
-    <row r="167" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="11">
         <v>35</v>
       </c>
@@ -11568,21 +11597,21 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="11">
         <v>36</v>
       </c>
       <c r="B168" s="23"/>
       <c r="C168" s="55"/>
       <c r="D168" s="71"/>
-      <c r="E168" s="257" t="s">
+      <c r="E168" s="266" t="s">
         <v>151</v>
       </c>
-      <c r="F168" s="257"/>
-      <c r="G168" s="257" t="s">
+      <c r="F168" s="266"/>
+      <c r="G168" s="266" t="s">
         <v>152</v>
       </c>
-      <c r="H168" s="257"/>
+      <c r="H168" s="266"/>
       <c r="M168" s="25"/>
       <c r="O168" s="189"/>
       <c r="P168" s="30" t="s">
@@ -11598,7 +11627,7 @@
       <c r="AB168" s="187"/>
       <c r="AD168" s="187"/>
     </row>
-    <row r="169" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A169" s="11">
         <v>37</v>
       </c>
@@ -11639,7 +11668,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A170" s="11">
         <v>38</v>
       </c>
@@ -11701,7 +11730,7 @@
       <c r="AB170" s="187"/>
       <c r="AD170" s="187"/>
     </row>
-    <row r="171" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="11">
         <v>39</v>
       </c>
@@ -11755,7 +11784,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A172" s="11">
         <v>40</v>
       </c>
@@ -11795,7 +11824,7 @@
       <c r="AB172" s="187"/>
       <c r="AD172" s="187"/>
     </row>
-    <row r="173" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A173" s="11">
         <v>41</v>
       </c>
@@ -11857,7 +11886,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="11">
         <v>42</v>
       </c>
@@ -11895,7 +11924,7 @@
       <c r="AB174" s="187"/>
       <c r="AD174" s="187"/>
     </row>
-    <row r="175" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="11">
         <v>43</v>
       </c>
@@ -11925,7 +11954,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="11">
         <v>44</v>
       </c>
@@ -11944,7 +11973,7 @@
       <c r="AB176" s="187"/>
       <c r="AD176" s="31"/>
     </row>
-    <row r="177" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="11">
         <v>45</v>
       </c>
@@ -11970,7 +11999,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="11">
         <v>46</v>
       </c>
@@ -11982,20 +12011,20 @@
       </c>
       <c r="M178" s="25"/>
       <c r="O178" s="26"/>
-      <c r="P178" s="252" t="s">
+      <c r="P178" s="271" t="s">
         <v>151</v>
       </c>
-      <c r="Q178" s="252"/>
-      <c r="R178" s="252" t="s">
+      <c r="Q178" s="271"/>
+      <c r="R178" s="271" t="s">
         <v>152</v>
       </c>
-      <c r="S178" s="252"/>
+      <c r="S178" s="271"/>
       <c r="Y178" s="27"/>
       <c r="AA178" s="30"/>
       <c r="AB178" s="187"/>
       <c r="AD178" s="31"/>
     </row>
-    <row r="179" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A179" s="11">
         <v>47</v>
       </c>
@@ -12033,7 +12062,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A180" s="11">
         <v>48</v>
       </c>
@@ -12081,7 +12110,7 @@
       <c r="AB180" s="187"/>
       <c r="AD180" s="31"/>
     </row>
-    <row r="181" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="11">
         <v>49</v>
       </c>
@@ -12137,7 +12166,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="11">
         <v>50</v>
       </c>
@@ -12182,7 +12211,7 @@
       </c>
       <c r="Y182" s="27"/>
     </row>
-    <row r="183" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="11">
         <v>51</v>
       </c>
@@ -12237,7 +12266,7 @@
       </c>
       <c r="Y183" s="27"/>
     </row>
-    <row r="184" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="11">
         <v>52</v>
       </c>
@@ -12292,7 +12321,7 @@
       </c>
       <c r="Y184" s="27"/>
     </row>
-    <row r="185" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="11">
         <v>53</v>
       </c>
@@ -12326,7 +12355,7 @@
       <c r="O185" s="26"/>
       <c r="Y185" s="27"/>
     </row>
-    <row r="186" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="11">
         <v>54</v>
       </c>
@@ -12350,7 +12379,7 @@
       </c>
       <c r="Y186" s="27"/>
     </row>
-    <row r="187" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="11">
         <v>55</v>
       </c>
@@ -12387,7 +12416,7 @@
       <c r="V187" s="22"/>
       <c r="Y187" s="27"/>
     </row>
-    <row r="188" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="11">
         <v>56</v>
       </c>
@@ -12417,7 +12446,7 @@
       <c r="X188" s="22"/>
       <c r="Y188" s="27"/>
     </row>
-    <row r="189" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="11">
         <v>57</v>
       </c>
@@ -12447,7 +12476,7 @@
       <c r="V189" s="22"/>
       <c r="Y189" s="27"/>
     </row>
-    <row r="190" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A190" s="11">
         <v>58</v>
       </c>
@@ -12481,7 +12510,7 @@
       <c r="V190" s="22"/>
       <c r="Y190" s="27"/>
     </row>
-    <row r="191" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="11">
         <v>59</v>
       </c>
@@ -12527,7 +12556,7 @@
       <c r="V191" s="22"/>
       <c r="Y191" s="27"/>
     </row>
-    <row r="192" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="11">
         <v>60</v>
       </c>
@@ -12571,7 +12600,7 @@
       <c r="V192" s="22"/>
       <c r="Y192" s="27"/>
     </row>
-    <row r="193" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="11">
         <v>61</v>
       </c>
@@ -12591,7 +12620,7 @@
       </c>
       <c r="Y193" s="27"/>
     </row>
-    <row r="194" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="11">
         <v>62</v>
       </c>
@@ -12604,7 +12633,7 @@
       </c>
       <c r="Y194" s="27"/>
     </row>
-    <row r="195" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="11">
         <v>63</v>
       </c>
@@ -12628,7 +12657,7 @@
       <c r="R195" s="7"/>
       <c r="Y195" s="27"/>
     </row>
-    <row r="196" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="11">
         <v>64</v>
       </c>
@@ -12661,14 +12690,14 @@
       </c>
       <c r="Y196" s="27"/>
     </row>
-    <row r="197" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="11">
         <v>65</v>
       </c>
       <c r="C197" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D197" s="274" t="str">
+      <c r="D197" s="253" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -12694,7 +12723,7 @@
       </c>
       <c r="Y197" s="27"/>
     </row>
-    <row r="198" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="11">
         <v>66</v>
       </c>
@@ -12715,7 +12744,7 @@
       <c r="O198" s="26"/>
       <c r="Y198" s="27"/>
     </row>
-    <row r="199" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="11">
         <v>1</v>
       </c>
@@ -12728,7 +12757,7 @@
       </c>
       <c r="Y199" s="27"/>
     </row>
-    <row r="200" spans="1:25" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:25" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A200" s="11">
         <v>2</v>
       </c>
@@ -12746,7 +12775,7 @@
       <c r="U200" s="22"/>
       <c r="Y200" s="27"/>
     </row>
-    <row r="201" spans="1:25" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A201" s="11">
         <v>3</v>
       </c>
@@ -12773,7 +12802,7 @@
       <c r="T201" s="145"/>
       <c r="Y201" s="27"/>
     </row>
-    <row r="202" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="11">
         <v>4</v>
       </c>
@@ -12802,7 +12831,7 @@
       <c r="T202" s="145"/>
       <c r="Y202" s="27"/>
     </row>
-    <row r="203" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="11">
         <v>5</v>
       </c>
@@ -12831,7 +12860,7 @@
       <c r="T203" s="145"/>
       <c r="Y203" s="27"/>
     </row>
-    <row r="204" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="11">
         <v>6</v>
       </c>
@@ -12865,7 +12894,7 @@
       <c r="X204" s="22"/>
       <c r="Y204" s="27"/>
     </row>
-    <row r="205" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="11">
         <v>7</v>
       </c>
@@ -12899,7 +12928,7 @@
       <c r="X205" s="22"/>
       <c r="Y205" s="27"/>
     </row>
-    <row r="206" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="11">
         <v>8</v>
       </c>
@@ -12938,7 +12967,7 @@
       <c r="X206" s="22"/>
       <c r="Y206" s="27"/>
     </row>
-    <row r="207" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="11">
         <v>9</v>
       </c>
@@ -12975,7 +13004,7 @@
       <c r="X207" s="22"/>
       <c r="Y207" s="27"/>
     </row>
-    <row r="208" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="11">
         <v>10</v>
       </c>
@@ -13010,7 +13039,7 @@
       <c r="X208" s="36"/>
       <c r="Y208" s="37"/>
     </row>
-    <row r="209" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="11">
         <v>11</v>
       </c>
@@ -13040,7 +13069,7 @@
       <c r="X209" s="22"/>
       <c r="Y209" s="22"/>
     </row>
-    <row r="210" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="11">
         <v>12</v>
       </c>
@@ -13062,7 +13091,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="211" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="11">
         <v>13</v>
       </c>
@@ -13094,7 +13123,7 @@
       <c r="X211" s="19"/>
       <c r="Y211" s="20"/>
     </row>
-    <row r="212" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="11">
         <v>14</v>
       </c>
@@ -13128,7 +13157,7 @@
       <c r="X212" s="209"/>
       <c r="Y212" s="27"/>
     </row>
-    <row r="213" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="11">
         <v>15</v>
       </c>
@@ -13165,7 +13194,7 @@
       <c r="X213" s="213"/>
       <c r="Y213" s="27"/>
     </row>
-    <row r="214" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="11">
         <v>16</v>
       </c>
@@ -13199,7 +13228,7 @@
       <c r="X214" s="209"/>
       <c r="Y214" s="27"/>
     </row>
-    <row r="215" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="11">
         <v>17</v>
       </c>
@@ -13236,7 +13265,7 @@
       <c r="X215" s="213"/>
       <c r="Y215" s="27"/>
     </row>
-    <row r="216" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="11">
         <v>18</v>
       </c>
@@ -13270,7 +13299,7 @@
       <c r="X216" s="209"/>
       <c r="Y216" s="27"/>
     </row>
-    <row r="217" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="11">
         <v>19</v>
       </c>
@@ -13307,7 +13336,7 @@
       <c r="X217" s="213"/>
       <c r="Y217" s="27"/>
     </row>
-    <row r="218" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="11">
         <v>20</v>
       </c>
@@ -13341,7 +13370,7 @@
       <c r="X218" s="209"/>
       <c r="Y218" s="27"/>
     </row>
-    <row r="219" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="11">
         <v>21</v>
       </c>
@@ -13378,7 +13407,7 @@
       <c r="X219" s="213"/>
       <c r="Y219" s="27"/>
     </row>
-    <row r="220" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="11">
         <v>22</v>
       </c>
@@ -13412,7 +13441,7 @@
       <c r="X220" s="209"/>
       <c r="Y220" s="27"/>
     </row>
-    <row r="221" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="11">
         <v>23</v>
       </c>
@@ -13449,7 +13478,7 @@
       <c r="X221" s="213"/>
       <c r="Y221" s="27"/>
     </row>
-    <row r="222" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="11">
         <v>24</v>
       </c>
@@ -13483,7 +13512,7 @@
       <c r="X222" s="209"/>
       <c r="Y222" s="27"/>
     </row>
-    <row r="223" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="11">
         <v>25</v>
       </c>
@@ -13518,7 +13547,7 @@
       <c r="X223" s="213"/>
       <c r="Y223" s="27"/>
     </row>
-    <row r="224" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="11">
         <v>26</v>
       </c>
@@ -13552,7 +13581,7 @@
       <c r="X224" s="209"/>
       <c r="Y224" s="27"/>
     </row>
-    <row r="225" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="11">
         <v>27</v>
       </c>
@@ -13587,7 +13616,7 @@
       <c r="X225" s="213"/>
       <c r="Y225" s="27"/>
     </row>
-    <row r="226" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="11">
         <v>28</v>
       </c>
@@ -13621,7 +13650,7 @@
       <c r="X226" s="209"/>
       <c r="Y226" s="27"/>
     </row>
-    <row r="227" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="11">
         <v>29</v>
       </c>
@@ -13656,7 +13685,7 @@
       <c r="X227" s="213"/>
       <c r="Y227" s="27"/>
     </row>
-    <row r="228" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="11">
         <v>30</v>
       </c>
@@ -13690,7 +13719,7 @@
       <c r="X228" s="209"/>
       <c r="Y228" s="27"/>
     </row>
-    <row r="229" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="11">
         <v>31</v>
       </c>
@@ -13725,7 +13754,7 @@
       <c r="X229" s="213"/>
       <c r="Y229" s="27"/>
     </row>
-    <row r="230" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="11">
         <v>32</v>
       </c>
@@ -13759,7 +13788,7 @@
       <c r="X230" s="209"/>
       <c r="Y230" s="27"/>
     </row>
-    <row r="231" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="11">
         <v>33</v>
       </c>
@@ -13794,7 +13823,7 @@
       <c r="X231" s="213"/>
       <c r="Y231" s="27"/>
     </row>
-    <row r="232" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="11">
         <v>34</v>
       </c>
@@ -13828,7 +13857,7 @@
       <c r="X232" s="209"/>
       <c r="Y232" s="27"/>
     </row>
-    <row r="233" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="11">
         <v>35</v>
       </c>
@@ -13863,7 +13892,7 @@
       <c r="X233" s="213"/>
       <c r="Y233" s="27"/>
     </row>
-    <row r="234" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="11">
         <v>36</v>
       </c>
@@ -13897,7 +13926,7 @@
       <c r="X234" s="209"/>
       <c r="Y234" s="27"/>
     </row>
-    <row r="235" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="11">
         <v>37</v>
       </c>
@@ -13932,7 +13961,7 @@
       <c r="X235" s="213"/>
       <c r="Y235" s="27"/>
     </row>
-    <row r="236" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="11">
         <v>38</v>
       </c>
@@ -13966,7 +13995,7 @@
       <c r="X236" s="209"/>
       <c r="Y236" s="27"/>
     </row>
-    <row r="237" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="11">
         <v>39</v>
       </c>
@@ -14001,7 +14030,7 @@
       <c r="X237" s="213"/>
       <c r="Y237" s="27"/>
     </row>
-    <row r="238" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="11">
         <v>40</v>
       </c>
@@ -14035,7 +14064,7 @@
       <c r="X238" s="209"/>
       <c r="Y238" s="27"/>
     </row>
-    <row r="239" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="11">
         <v>41</v>
       </c>
@@ -14070,7 +14099,7 @@
       <c r="X239" s="213"/>
       <c r="Y239" s="27"/>
     </row>
-    <row r="240" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="11">
         <v>42</v>
       </c>
@@ -14104,7 +14133,7 @@
       <c r="X240" s="209"/>
       <c r="Y240" s="27"/>
     </row>
-    <row r="241" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="11">
         <v>43</v>
       </c>
@@ -14139,7 +14168,7 @@
       <c r="X241" s="213"/>
       <c r="Y241" s="27"/>
     </row>
-    <row r="242" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="11">
         <v>44</v>
       </c>
@@ -14173,7 +14202,7 @@
       <c r="X242" s="209"/>
       <c r="Y242" s="27"/>
     </row>
-    <row r="243" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="11">
         <v>45</v>
       </c>
@@ -14208,7 +14237,7 @@
       <c r="X243" s="213"/>
       <c r="Y243" s="27"/>
     </row>
-    <row r="244" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="11">
         <v>46</v>
       </c>
@@ -14242,7 +14271,7 @@
       <c r="X244" s="209"/>
       <c r="Y244" s="27"/>
     </row>
-    <row r="245" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="11">
         <v>47</v>
       </c>
@@ -14277,7 +14306,7 @@
       <c r="X245" s="213"/>
       <c r="Y245" s="27"/>
     </row>
-    <row r="246" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="11">
         <v>48</v>
       </c>
@@ -14311,7 +14340,7 @@
       <c r="X246" s="209"/>
       <c r="Y246" s="27"/>
     </row>
-    <row r="247" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="11">
         <v>49</v>
       </c>
@@ -14346,7 +14375,7 @@
       <c r="X247" s="213"/>
       <c r="Y247" s="27"/>
     </row>
-    <row r="248" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="11">
         <v>50</v>
       </c>
@@ -14380,7 +14409,7 @@
       <c r="X248" s="209"/>
       <c r="Y248" s="27"/>
     </row>
-    <row r="249" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="11">
         <v>51</v>
       </c>
@@ -14415,7 +14444,7 @@
       <c r="X249" s="213"/>
       <c r="Y249" s="27"/>
     </row>
-    <row r="250" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="11">
         <v>52</v>
       </c>
@@ -14445,7 +14474,7 @@
       <c r="X250" s="36"/>
       <c r="Y250" s="37"/>
     </row>
-    <row r="251" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="11">
         <v>53</v>
       </c>
@@ -14475,7 +14504,7 @@
       <c r="X251" s="22"/>
       <c r="Y251" s="22"/>
     </row>
-    <row r="252" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="11">
         <v>54</v>
       </c>
@@ -14494,7 +14523,7 @@
       <c r="L252" s="200"/>
       <c r="M252" s="25"/>
     </row>
-    <row r="253" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="11">
         <v>55</v>
       </c>
@@ -14513,7 +14542,7 @@
       <c r="L253" s="198"/>
       <c r="M253" s="25"/>
     </row>
-    <row r="254" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="11">
         <v>56</v>
       </c>
@@ -14532,7 +14561,7 @@
       <c r="L254" s="200"/>
       <c r="M254" s="25"/>
     </row>
-    <row r="255" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="11">
         <v>57</v>
       </c>
@@ -14551,7 +14580,7 @@
       <c r="L255" s="200"/>
       <c r="M255" s="25"/>
     </row>
-    <row r="256" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="11">
         <v>58</v>
       </c>
@@ -14570,7 +14599,7 @@
       <c r="L256" s="198"/>
       <c r="M256" s="25"/>
     </row>
-    <row r="257" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="11">
         <v>59</v>
       </c>
@@ -14589,7 +14618,7 @@
       <c r="L257" s="200"/>
       <c r="M257" s="25"/>
     </row>
-    <row r="258" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="11">
         <v>60</v>
       </c>
@@ -14608,28 +14637,28 @@
       <c r="L258" s="200"/>
       <c r="M258" s="25"/>
     </row>
-    <row r="259" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="11">
         <v>61</v>
       </c>
       <c r="B259" s="23"/>
       <c r="M259" s="25"/>
     </row>
-    <row r="260" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="11">
         <v>62</v>
       </c>
       <c r="B260" s="23"/>
       <c r="M260" s="25"/>
     </row>
-    <row r="261" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="11">
         <v>63</v>
       </c>
       <c r="B261" s="23"/>
       <c r="M261" s="25"/>
     </row>
-    <row r="262" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="11">
         <v>64</v>
       </c>
@@ -14646,14 +14675,14 @@
       <c r="L262" s="33"/>
       <c r="M262" s="34"/>
     </row>
-    <row r="263" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="11">
         <v>65</v>
       </c>
       <c r="C263" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D263" s="274" t="str">
+      <c r="D263" s="253" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -14665,7 +14694,7 @@
         <v>Eugene Mah</v>
       </c>
     </row>
-    <row r="264" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="11">
         <v>66</v>
       </c>
@@ -14686,39 +14715,11 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="T70:U70"/>
-    <mergeCell ref="Q89:S89"/>
-    <mergeCell ref="T89:U89"/>
+    <mergeCell ref="P178:Q178"/>
+    <mergeCell ref="R178:S178"/>
+    <mergeCell ref="T112:U112"/>
+    <mergeCell ref="O115:P117"/>
+    <mergeCell ref="P134:P136"/>
     <mergeCell ref="X154:Y154"/>
     <mergeCell ref="E168:F168"/>
     <mergeCell ref="G168:H168"/>
@@ -14726,11 +14727,39 @@
     <mergeCell ref="I91:J91"/>
     <mergeCell ref="D94:E96"/>
     <mergeCell ref="Q112:S112"/>
-    <mergeCell ref="P178:Q178"/>
-    <mergeCell ref="R178:S178"/>
-    <mergeCell ref="T112:U112"/>
-    <mergeCell ref="O115:P117"/>
-    <mergeCell ref="P134:P136"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="Q89:S89"/>
+    <mergeCell ref="T89:U89"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <conditionalFormatting sqref="L33:L38 L41:L45 L47:L56 L59:L62">
     <cfRule type="cellIs" dxfId="31" priority="41" operator="equal">
@@ -14886,17 +14915,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1012" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1012" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>289</v>
       </c>
@@ -14904,18 +14933,18 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="252" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="271" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="252" t="s">
+      <c r="B2" s="271" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="252"/>
-      <c r="D2" s="252"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="252"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="271"/>
       <c r="B3" s="5" t="s">
         <v>292</v>
       </c>
@@ -14926,7 +14955,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>295</v>
       </c>
@@ -14940,7 +14969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>297</v>
       </c>
@@ -14954,7 +14983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>298</v>
       </c>
@@ -14968,7 +14997,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>300</v>
       </c>
@@ -14982,7 +15011,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>301</v>
       </c>
@@ -14996,7 +15025,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>302</v>
       </c>
@@ -15010,7 +15039,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>303</v>
       </c>
@@ -15024,7 +15053,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>304</v>
       </c>
@@ -15038,7 +15067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>304</v>
       </c>
@@ -15052,7 +15081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>305</v>
       </c>
@@ -15066,7 +15095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>306</v>
       </c>
@@ -15080,24 +15109,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="252" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="271" t="s">
         <v>290</v>
       </c>
-      <c r="B16" s="252" t="s">
+      <c r="B16" s="271" t="s">
         <v>307</v>
       </c>
-      <c r="C16" s="252"/>
-      <c r="D16" s="252"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="252"/>
+      <c r="C16" s="271"/>
+      <c r="D16" s="271"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="271"/>
       <c r="B17" s="5" t="s">
         <v>292</v>
       </c>
@@ -15108,7 +15137,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>295</v>
       </c>
@@ -15122,7 +15151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>297</v>
       </c>
@@ -15136,7 +15165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>298</v>
       </c>
@@ -15150,7 +15179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>300</v>
       </c>
@@ -15164,7 +15193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>301</v>
       </c>
@@ -15178,7 +15207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>300</v>
       </c>
@@ -15192,7 +15221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>308</v>
       </c>
@@ -15206,7 +15235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>303</v>
       </c>
@@ -15220,7 +15249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>309</v>
       </c>
@@ -15234,7 +15263,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>306</v>
       </c>
@@ -15248,7 +15277,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>305</v>
       </c>
@@ -15262,7 +15291,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>310</v>
       </c>
@@ -15276,7 +15305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>304</v>
       </c>
@@ -15290,7 +15319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>302</v>
       </c>
@@ -15304,7 +15333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>311</v>
       </c>
@@ -15318,7 +15347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>302</v>
       </c>
@@ -15332,17 +15361,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="252" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="271" t="s">
         <v>290</v>
       </c>
-      <c r="B35" s="252" t="s">
+      <c r="B35" s="271" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="252"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="252"/>
+      <c r="C35" s="271"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="271"/>
       <c r="B36" s="5" t="s">
         <v>293</v>
       </c>
@@ -15350,7 +15379,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>310</v>
       </c>
@@ -15361,7 +15390,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>313</v>
       </c>
@@ -15372,7 +15401,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>303</v>
       </c>
@@ -15383,7 +15412,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>301</v>
       </c>
@@ -15394,7 +15423,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>297</v>
       </c>
@@ -15405,7 +15434,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>295</v>
       </c>
@@ -15416,7 +15445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>314</v>
       </c>
@@ -15427,17 +15456,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="252" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="271" t="s">
         <v>290</v>
       </c>
-      <c r="B45" s="252" t="s">
+      <c r="B45" s="271" t="s">
         <v>315</v>
       </c>
-      <c r="C45" s="252"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="252"/>
+      <c r="C45" s="271"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="271"/>
       <c r="B46" s="5" t="s">
         <v>293</v>
       </c>
@@ -15445,7 +15474,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>316</v>
       </c>
@@ -15456,7 +15485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>317</v>
       </c>
@@ -15467,7 +15496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>318</v>
       </c>
@@ -15478,7 +15507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>319</v>
       </c>
@@ -15489,7 +15518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>320</v>
       </c>
@@ -15500,7 +15529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>295</v>
       </c>
@@ -15511,7 +15540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>321</v>
       </c>
@@ -15522,17 +15551,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="252" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="271" t="s">
         <v>290</v>
       </c>
-      <c r="B55" s="252" t="s">
+      <c r="B55" s="271" t="s">
         <v>322</v>
       </c>
-      <c r="C55" s="252"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="252"/>
+      <c r="C55" s="271"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="271"/>
       <c r="B56" s="5" t="s">
         <v>293</v>
       </c>
@@ -15540,7 +15569,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>323</v>
       </c>
@@ -15551,7 +15580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>324</v>
       </c>
@@ -15562,7 +15591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>325</v>
       </c>
@@ -15573,7 +15602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>320</v>
       </c>
@@ -15584,7 +15613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>303</v>
       </c>
@@ -15595,7 +15624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>326</v>
       </c>
@@ -15606,7 +15635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>311</v>
       </c>
@@ -15617,17 +15646,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="252" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="271" t="s">
         <v>290</v>
       </c>
-      <c r="B65" s="252" t="s">
+      <c r="B65" s="271" t="s">
         <v>327</v>
       </c>
-      <c r="C65" s="252"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="252"/>
+      <c r="C65" s="271"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="271"/>
       <c r="B66" s="5" t="s">
         <v>293</v>
       </c>
@@ -15635,7 +15664,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>295</v>
       </c>
@@ -15646,7 +15675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>328</v>
       </c>
@@ -15657,7 +15686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>297</v>
       </c>
@@ -15668,7 +15697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>301</v>
       </c>
@@ -15679,7 +15708,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>303</v>
       </c>
@@ -15690,7 +15719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>329</v>
       </c>
@@ -15701,7 +15730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>330</v>
       </c>
@@ -15712,7 +15741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>331</v>
       </c>
@@ -15723,7 +15752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>306</v>
       </c>
@@ -15734,7 +15763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>332</v>
       </c>
@@ -15745,7 +15774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>333</v>
       </c>
@@ -15758,18 +15787,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:C65"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:C65"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="69" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Add conditional highlighting to CT number section
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -25,7 +25,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$B$1:$M$198</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$A$1:$F$40</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="342">
   <si>
     <t>Medical Physicist CT Survey Report</t>
   </si>
@@ -1063,6 +1063,9 @@
   </si>
   <si>
     <t>First,CTDI,ACRPhantom</t>
+  </si>
+  <si>
+    <t>Siemens CT Beam Profiles http://128.23.56.214/MPwiki/index.php?title=Siemens_CT_Beam_Profiles</t>
   </si>
 </sst>
 </file>
@@ -2959,13 +2962,55 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2979,48 +3024,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3032,7 +3035,67 @@
     <cellStyle name="Result" xfId="1"/>
     <cellStyle name="Result2" xfId="2"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="207">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3105,6 +3168,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -3135,6 +3218,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3175,6 +3268,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -3225,6 +3338,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -3245,6 +3378,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -3255,6 +3418,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3265,6 +3458,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3275,6 +3478,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3285,6 +3498,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3295,6 +3518,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3305,6 +3538,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -3335,6 +3588,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3345,6 +3608,156 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -3355,6 +3768,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3445,6 +3888,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -3475,6 +3938,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3550,6 +4023,646 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4471,19 +5584,19 @@
       <c r="A6" s="222" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="265" t="str">
+      <c r="B6" s="263" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="265"/>
+      <c r="C6" s="263"/>
       <c r="D6" s="223" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="265" t="str">
+      <c r="E6" s="263" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="263"/>
       <c r="G6" s="1"/>
       <c r="J6" s="248" t="s">
         <v>338</v>
@@ -4493,48 +5606,48 @@
       <c r="A7" s="222" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="263"/>
-      <c r="C7" s="263"/>
+      <c r="B7" s="264"/>
+      <c r="C7" s="264"/>
       <c r="D7" s="223" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="263" t="str">
+      <c r="E7" s="264" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="263"/>
+      <c r="F7" s="264"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="222" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="263"/>
-      <c r="C8" s="263"/>
+      <c r="B8" s="264"/>
+      <c r="C8" s="264"/>
       <c r="D8" s="223" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="263" t="str">
+      <c r="E8" s="264" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="263"/>
+      <c r="F8" s="264"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="263"/>
-      <c r="C9" s="263"/>
+      <c r="B9" s="264"/>
+      <c r="C9" s="264"/>
       <c r="D9" s="223" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="263" t="str">
+      <c r="E9" s="264" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="263"/>
+      <c r="F9" s="264"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4544,19 +5657,19 @@
       <c r="D10" s="223" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="264" t="str">
+      <c r="E10" s="265" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="264"/>
+      <c r="F10" s="265"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="265"/>
-      <c r="C11" s="265"/>
+      <c r="B11" s="263"/>
+      <c r="C11" s="263"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4579,10 +5692,10 @@
       <c r="A13" s="225" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="265" t="s">
+      <c r="B13" s="263" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="265"/>
+      <c r="C13" s="263"/>
       <c r="D13" s="223" t="s">
         <v>16</v>
       </c>
@@ -4885,17 +5998,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29">
@@ -4918,8 +6031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q123" sqref="Q123:U123"/>
+    <sheetView tabSelected="1" topLeftCell="I154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P165" sqref="P165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5184,19 +6297,19 @@
       <c r="E10" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="279" t="str">
+      <c r="F10" s="266" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="279"/>
+      <c r="G10" s="266"/>
       <c r="J10" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="279" t="str">
+      <c r="K10" s="266" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="279"/>
+      <c r="L10" s="266"/>
       <c r="M10" s="25"/>
       <c r="O10" s="26"/>
       <c r="Q10" s="30" t="s">
@@ -5237,19 +6350,19 @@
       <c r="E11" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="282" t="str">
+      <c r="F11" s="267" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="282"/>
+      <c r="G11" s="267"/>
       <c r="J11" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="279" t="str">
+      <c r="K11" s="266" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="279"/>
+      <c r="L11" s="266"/>
       <c r="M11" s="25"/>
       <c r="O11" s="26"/>
       <c r="Q11" s="30" t="s">
@@ -5290,19 +6403,19 @@
       <c r="E12" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="282" t="str">
+      <c r="F12" s="267" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="282"/>
+      <c r="G12" s="267"/>
       <c r="J12" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="283" t="str">
+      <c r="K12" s="268" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="283"/>
+      <c r="L12" s="268"/>
       <c r="M12" s="25"/>
       <c r="O12" s="26"/>
       <c r="Q12" s="30" t="s">
@@ -5343,19 +6456,19 @@
       <c r="E13" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="282" t="str">
+      <c r="F13" s="267" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="282"/>
+      <c r="G13" s="267"/>
       <c r="J13" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="279" t="str">
+      <c r="K13" s="266" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="279"/>
+      <c r="L13" s="266"/>
       <c r="M13" s="25"/>
       <c r="O13" s="26"/>
       <c r="Q13" s="30" t="s">
@@ -5453,19 +6566,19 @@
       <c r="E16" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="279" t="str">
+      <c r="F16" s="266" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="279"/>
+      <c r="G16" s="266"/>
       <c r="J16" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="283" t="str">
+      <c r="K16" s="268" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="283"/>
+      <c r="L16" s="268"/>
       <c r="M16" s="25"/>
       <c r="O16" s="26"/>
       <c r="P16" s="58" t="s">
@@ -5493,19 +6606,19 @@
       <c r="E17" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="282" t="str">
+      <c r="F17" s="267" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="282"/>
+      <c r="G17" s="267"/>
       <c r="J17" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="279" t="str">
+      <c r="K17" s="266" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="279"/>
+      <c r="L17" s="266"/>
       <c r="M17" s="25"/>
       <c r="O17" s="26"/>
       <c r="Q17" s="30" t="s">
@@ -5546,11 +6659,11 @@
       <c r="J18" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="279" t="str">
+      <c r="K18" s="266" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="279"/>
+      <c r="L18" s="266"/>
       <c r="M18" s="25"/>
       <c r="O18" s="26"/>
       <c r="Q18" s="30" t="s">
@@ -5622,11 +6735,11 @@
       <c r="E20" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="279" t="str">
+      <c r="F20" s="266" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="279"/>
+      <c r="G20" s="266"/>
       <c r="I20" s="61" t="s">
         <v>76</v>
       </c>
@@ -5651,19 +6764,19 @@
       <c r="E21" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="281" t="str">
+      <c r="F21" s="269" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="281"/>
+      <c r="G21" s="269"/>
       <c r="J21" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="279" t="str">
+      <c r="K21" s="266" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="279"/>
+      <c r="L21" s="266"/>
       <c r="M21" s="25"/>
       <c r="O21" s="26"/>
       <c r="Q21" s="30" t="s">
@@ -5702,11 +6815,11 @@
       <c r="J22" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="279" t="str">
+      <c r="K22" s="266" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="279"/>
+      <c r="L22" s="266"/>
       <c r="M22" s="25"/>
       <c r="O22" s="26"/>
       <c r="Q22" s="30" t="s">
@@ -5747,19 +6860,19 @@
       <c r="E23" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="279" t="str">
+      <c r="F23" s="266" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="279"/>
+      <c r="G23" s="266"/>
       <c r="J23" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="279" t="str">
+      <c r="K23" s="266" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="279"/>
+      <c r="L23" s="266"/>
       <c r="M23" s="25"/>
       <c r="O23" s="26"/>
       <c r="P23" s="58" t="s">
@@ -5795,11 +6908,11 @@
       <c r="E24" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="279" t="str">
+      <c r="F24" s="266" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="279"/>
+      <c r="G24" s="266"/>
       <c r="M24" s="25"/>
       <c r="O24" s="26"/>
       <c r="Q24" s="30" t="s">
@@ -5840,11 +6953,11 @@
       <c r="E25" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="279" t="str">
+      <c r="F25" s="266" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="279"/>
+      <c r="G25" s="266"/>
       <c r="J25" s="57" t="s">
         <v>82</v>
       </c>
@@ -5884,11 +6997,11 @@
       <c r="J26" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="279" t="str">
+      <c r="K26" s="266" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="279"/>
+      <c r="L26" s="266"/>
       <c r="M26" s="25"/>
       <c r="O26" s="26"/>
       <c r="Q26" s="30" t="s">
@@ -5916,19 +7029,19 @@
       <c r="E27" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="279" t="str">
+      <c r="F27" s="266" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="279"/>
+      <c r="G27" s="266"/>
       <c r="J27" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="279" t="str">
+      <c r="K27" s="266" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="279"/>
+      <c r="L27" s="266"/>
       <c r="M27" s="25"/>
       <c r="O27" s="26"/>
       <c r="P27" s="58" t="s">
@@ -5955,11 +7068,11 @@
       <c r="E28" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="279" t="str">
+      <c r="F28" s="266" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="279"/>
+      <c r="G28" s="266"/>
       <c r="M28" s="25"/>
       <c r="O28" s="26"/>
       <c r="Q28" s="30" t="s">
@@ -6000,11 +7113,11 @@
       <c r="E29" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="279" t="str">
+      <c r="F29" s="266" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="279"/>
+      <c r="G29" s="266"/>
       <c r="M29" s="25"/>
       <c r="O29" s="26"/>
       <c r="Q29" s="30" t="s">
@@ -6114,10 +7227,10 @@
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
-      <c r="L32" s="280" t="s">
+      <c r="L32" s="270" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="280"/>
+      <c r="M32" s="270"/>
       <c r="AA32" s="30" t="s">
         <v>70</v>
       </c>
@@ -7364,27 +8477,27 @@
       </c>
       <c r="B70" s="23"/>
       <c r="E70" s="71"/>
-      <c r="F70" s="276" t="s">
+      <c r="F70" s="271" t="s">
         <v>151</v>
       </c>
-      <c r="G70" s="276"/>
-      <c r="H70" s="276"/>
-      <c r="I70" s="276" t="s">
+      <c r="G70" s="271"/>
+      <c r="H70" s="271"/>
+      <c r="I70" s="271" t="s">
         <v>152</v>
       </c>
-      <c r="J70" s="276"/>
+      <c r="J70" s="271"/>
       <c r="M70" s="25"/>
       <c r="O70" s="46"/>
       <c r="P70" s="19"/>
-      <c r="Q70" s="277" t="s">
+      <c r="Q70" s="272" t="s">
         <v>151</v>
       </c>
-      <c r="R70" s="277"/>
-      <c r="S70" s="277"/>
-      <c r="T70" s="277" t="s">
+      <c r="R70" s="272"/>
+      <c r="S70" s="272"/>
+      <c r="T70" s="272" t="s">
         <v>152</v>
       </c>
-      <c r="U70" s="277"/>
+      <c r="U70" s="272"/>
       <c r="V70" s="19"/>
       <c r="W70" s="19"/>
       <c r="X70" s="19"/>
@@ -8605,15 +9718,15 @@
       <c r="M89" s="89"/>
       <c r="O89" s="26"/>
       <c r="P89" s="55"/>
-      <c r="Q89" s="278" t="s">
+      <c r="Q89" s="273" t="s">
         <v>151</v>
       </c>
-      <c r="R89" s="278"/>
-      <c r="S89" s="278"/>
-      <c r="T89" s="278" t="s">
+      <c r="R89" s="273"/>
+      <c r="S89" s="273"/>
+      <c r="T89" s="273" t="s">
         <v>152</v>
       </c>
-      <c r="U89" s="278"/>
+      <c r="U89" s="273"/>
       <c r="Y89" s="27"/>
       <c r="AA89" s="30" t="s">
         <v>129</v>
@@ -8673,15 +9786,15 @@
       </c>
       <c r="B91" s="23"/>
       <c r="E91" s="71"/>
-      <c r="F91" s="272" t="s">
+      <c r="F91" s="276" t="s">
         <v>151</v>
       </c>
-      <c r="G91" s="272"/>
-      <c r="H91" s="272"/>
-      <c r="I91" s="273" t="s">
+      <c r="G91" s="276"/>
+      <c r="H91" s="276"/>
+      <c r="I91" s="277" t="s">
         <v>152</v>
       </c>
-      <c r="J91" s="273"/>
+      <c r="J91" s="277"/>
       <c r="M91" s="25"/>
       <c r="O91" s="26"/>
       <c r="P91" s="30" t="s">
@@ -8845,10 +9958,10 @@
         <v>28</v>
       </c>
       <c r="B94" s="23"/>
-      <c r="D94" s="274" t="s">
+      <c r="D94" s="278" t="s">
         <v>161</v>
       </c>
-      <c r="E94" s="274" t="s">
+      <c r="E94" s="278" t="s">
         <v>161</v>
       </c>
       <c r="F94" s="97" t="str">
@@ -8906,8 +10019,8 @@
         <v>29</v>
       </c>
       <c r="B95" s="23"/>
-      <c r="D95" s="274"/>
-      <c r="E95" s="274"/>
+      <c r="D95" s="278"/>
+      <c r="E95" s="278"/>
       <c r="F95" s="102" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -8963,8 +10076,8 @@
         <v>30</v>
       </c>
       <c r="B96" s="23"/>
-      <c r="D96" s="274"/>
-      <c r="E96" s="274"/>
+      <c r="D96" s="278"/>
+      <c r="E96" s="278"/>
       <c r="F96" s="107" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -9787,15 +10900,15 @@
       <c r="J112" s="22"/>
       <c r="M112" s="25"/>
       <c r="O112" s="26"/>
-      <c r="Q112" s="275" t="s">
+      <c r="Q112" s="279" t="s">
         <v>151</v>
       </c>
-      <c r="R112" s="275"/>
-      <c r="S112" s="275"/>
-      <c r="T112" s="267" t="s">
+      <c r="R112" s="279"/>
+      <c r="S112" s="279"/>
+      <c r="T112" s="281" t="s">
         <v>152</v>
       </c>
-      <c r="U112" s="267"/>
+      <c r="U112" s="281"/>
       <c r="W112" s="58" t="s">
         <v>158</v>
       </c>
@@ -9933,10 +11046,10 @@
       </c>
       <c r="J115" s="22"/>
       <c r="M115" s="25"/>
-      <c r="O115" s="268" t="s">
+      <c r="O115" s="282" t="s">
         <v>161</v>
       </c>
-      <c r="P115" s="268" t="s">
+      <c r="P115" s="282" t="s">
         <v>161</v>
       </c>
       <c r="Q115" s="141"/>
@@ -9976,8 +11089,8 @@
       <c r="H116" s="22"/>
       <c r="J116" s="22"/>
       <c r="M116" s="25"/>
-      <c r="O116" s="268"/>
-      <c r="P116" s="268"/>
+      <c r="O116" s="282"/>
+      <c r="P116" s="282"/>
       <c r="Q116" s="144"/>
       <c r="R116" s="145"/>
       <c r="S116" s="146"/>
@@ -10017,8 +11130,8 @@
       <c r="H117" s="22"/>
       <c r="J117" s="22"/>
       <c r="M117" s="25"/>
-      <c r="O117" s="268"/>
-      <c r="P117" s="268"/>
+      <c r="O117" s="282"/>
+      <c r="P117" s="282"/>
       <c r="Q117" s="148"/>
       <c r="R117" s="149"/>
       <c r="S117" s="150"/>
@@ -10771,7 +11884,7 @@
         <v>CT System Compliance Inspection</v>
       </c>
       <c r="O134" s="26"/>
-      <c r="P134" s="269" t="s">
+      <c r="P134" s="283" t="s">
         <v>181</v>
       </c>
       <c r="Q134" s="175"/>
@@ -10811,7 +11924,7 @@
       <c r="L135" s="15"/>
       <c r="M135" s="16"/>
       <c r="O135" s="26"/>
-      <c r="P135" s="269"/>
+      <c r="P135" s="283"/>
       <c r="Q135" s="175"/>
       <c r="R135" s="176"/>
       <c r="S135" s="176"/>
@@ -10859,7 +11972,7 @@
       </c>
       <c r="M136" s="25"/>
       <c r="O136" s="26"/>
-      <c r="P136" s="269"/>
+      <c r="P136" s="283"/>
       <c r="Q136" s="178"/>
       <c r="R136" s="179"/>
       <c r="S136" s="179"/>
@@ -11699,10 +12812,10 @@
         <v>150</v>
       </c>
       <c r="W154" s="190"/>
-      <c r="X154" s="270" t="s">
+      <c r="X154" s="274" t="s">
         <v>226</v>
       </c>
-      <c r="Y154" s="270"/>
+      <c r="Y154" s="274"/>
       <c r="AA154" s="30"/>
       <c r="AB154" s="187"/>
       <c r="AD154" s="187"/>
@@ -12244,14 +13357,14 @@
       <c r="B168" s="23"/>
       <c r="C168" s="55"/>
       <c r="D168" s="71"/>
-      <c r="E168" s="271" t="s">
+      <c r="E168" s="275" t="s">
         <v>151</v>
       </c>
-      <c r="F168" s="271"/>
-      <c r="G168" s="271" t="s">
+      <c r="F168" s="275"/>
+      <c r="G168" s="275" t="s">
         <v>152</v>
       </c>
-      <c r="H168" s="271"/>
+      <c r="H168" s="275"/>
       <c r="M168" s="25"/>
       <c r="O168" s="189"/>
       <c r="P168" s="30" t="s">
@@ -12651,14 +13764,14 @@
       </c>
       <c r="M178" s="25"/>
       <c r="O178" s="26"/>
-      <c r="P178" s="266" t="s">
+      <c r="P178" s="280" t="s">
         <v>151</v>
       </c>
-      <c r="Q178" s="266"/>
-      <c r="R178" s="266" t="s">
+      <c r="Q178" s="280"/>
+      <c r="R178" s="280" t="s">
         <v>152</v>
       </c>
-      <c r="S178" s="266"/>
+      <c r="S178" s="280"/>
       <c r="Y178" s="27"/>
       <c r="AA178" s="30"/>
       <c r="AB178" s="187"/>
@@ -15355,39 +16468,11 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="T70:U70"/>
-    <mergeCell ref="Q89:S89"/>
-    <mergeCell ref="T89:U89"/>
+    <mergeCell ref="P178:Q178"/>
+    <mergeCell ref="R178:S178"/>
+    <mergeCell ref="T112:U112"/>
+    <mergeCell ref="O115:P117"/>
+    <mergeCell ref="P134:P136"/>
     <mergeCell ref="X154:Y154"/>
     <mergeCell ref="E168:F168"/>
     <mergeCell ref="G168:H168"/>
@@ -15395,148 +16480,206 @@
     <mergeCell ref="I91:J91"/>
     <mergeCell ref="D94:E96"/>
     <mergeCell ref="Q112:S112"/>
-    <mergeCell ref="P178:Q178"/>
-    <mergeCell ref="R178:S178"/>
-    <mergeCell ref="T112:U112"/>
-    <mergeCell ref="O115:P117"/>
-    <mergeCell ref="P134:P136"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="Q89:S89"/>
+    <mergeCell ref="T89:U89"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <conditionalFormatting sqref="L33:L38 L41:L45 L47:L56 L59:L62">
-    <cfRule type="cellIs" dxfId="63" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="46" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q124:U124 F102:J102">
-    <cfRule type="cellIs" dxfId="62" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q138:T138 E114:H114">
-    <cfRule type="cellIs" dxfId="61" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122">
-    <cfRule type="cellIs" dxfId="60" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="40" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="41" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C125:C127">
-    <cfRule type="cellIs" dxfId="58" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="38" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H152">
-    <cfRule type="cellIs" dxfId="57" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F163:J163 Q173:U173 K170:K171 F191:F192 Q196:Q197">
-    <cfRule type="cellIs" dxfId="56" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T208 F127">
-    <cfRule type="cellIs" dxfId="55" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="33" operator="greaterThan">
       <formula>0.15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q123:U123">
-    <cfRule type="cellIs" dxfId="32" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="lessThan">
       <formula>0.2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="31" operator="greaterThan">
       <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q122:U122">
-    <cfRule type="cellIs" dxfId="54" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="28" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="29" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M33:M38 M41:M45 M47:M56 M59:M62">
-    <cfRule type="cellIs" dxfId="52" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L138:L141">
-    <cfRule type="cellIs" dxfId="51" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q196:Q197">
-    <cfRule type="cellIs" dxfId="50" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="18" operator="equal">
-      <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R188:S192">
-    <cfRule type="cellIs" dxfId="48" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H181:H185">
-    <cfRule type="cellIs" dxfId="46" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T188:T192">
-    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
       <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="13" operator="equal">
-      <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P157:V157">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
+      <formula>-5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThan">
       <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="lessThan">
-      <formula>-5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X180">
-    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
-      <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P184:Q184">
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R184">
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S184">
-    <cfRule type="cellIs" dxfId="35" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R156:T156">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+      <formula>$X$156</formula>
+      <formula>$Y$156</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R157:T157">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+      <formula>$X$157</formula>
+      <formula>$Y$157</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R159:T159">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+      <formula>$X$158</formula>
+      <formula>$Y$158</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R160:T160">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>$X$159</formula>
+      <formula>$Y$159</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R161:T161">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>$X$160</formula>
+      <formula>$Y$160</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -15556,7 +16699,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
@@ -15566,100 +16709,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="266" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="280" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="266" t="s">
+      <c r="B4" s="280" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="266"/>
-      <c r="D2" s="266"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="266"/>
-      <c r="B3" s="5" t="s">
+      <c r="C4" s="280"/>
+      <c r="D4" s="280"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="280"/>
+      <c r="B5" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="C4" s="12">
-        <v>3.5</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="C5" s="12">
-        <v>6</v>
-      </c>
-      <c r="D5" s="12">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C6" s="12">
-        <v>10.5</v>
+        <v>3.5</v>
       </c>
       <c r="D6" s="12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C7" s="12">
-        <v>11.5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C8" s="12">
-        <v>11.1</v>
+        <v>10.5</v>
       </c>
       <c r="D8" s="12">
         <v>1.5</v>
@@ -15667,13 +16787,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>299</v>
       </c>
       <c r="C9" s="12">
-        <v>18.8</v>
+        <v>11.5</v>
       </c>
       <c r="D9" s="12">
         <v>1.5</v>
@@ -15681,13 +16801,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>296</v>
       </c>
       <c r="C10" s="12">
-        <v>19.399999999999999</v>
+        <v>11.1</v>
       </c>
       <c r="D10" s="12">
         <v>1.5</v>
@@ -15695,41 +16815,41 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C11" s="12">
-        <v>24.4</v>
+        <v>18.8</v>
       </c>
       <c r="D11" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C12" s="12">
-        <v>27.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="D12" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>296</v>
       </c>
       <c r="C13" s="12">
-        <v>44</v>
+        <v>24.4</v>
       </c>
       <c r="D13" s="12">
         <v>2</v>
@@ -15737,83 +16857,83 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>299</v>
       </c>
       <c r="C14" s="12">
-        <v>45.5</v>
+        <v>27.4</v>
       </c>
       <c r="D14" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C15" s="12">
+        <v>44</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C16" s="12">
+        <v>45.5</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="280" t="s">
         <v>290</v>
       </c>
-      <c r="B16" s="266" t="s">
+      <c r="B18" s="280" t="s">
         <v>307</v>
       </c>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="266"/>
-      <c r="B17" s="5" t="s">
+      <c r="C18" s="280"/>
+      <c r="D18" s="280"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="280"/>
+      <c r="B19" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="C18" s="12">
-        <v>4.7</v>
-      </c>
-      <c r="D18" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="C19" s="12">
-        <v>6.6</v>
-      </c>
-      <c r="D19" s="12">
-        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C20" s="12">
-        <v>11.2</v>
+        <v>4.7</v>
       </c>
       <c r="D20" s="12">
         <v>1</v>
@@ -15821,13 +16941,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>296</v>
       </c>
       <c r="C21" s="12">
-        <v>8.5</v>
+        <v>6.6</v>
       </c>
       <c r="D21" s="12">
         <v>1</v>
@@ -15835,13 +16955,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C22" s="12">
-        <v>11.6</v>
+        <v>11.2</v>
       </c>
       <c r="D22" s="12">
         <v>1</v>
@@ -15852,10 +16972,10 @@
         <v>300</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C23" s="12">
-        <v>11.5</v>
+        <v>8.5</v>
       </c>
       <c r="D23" s="12">
         <v>1</v>
@@ -15863,13 +16983,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>296</v>
       </c>
       <c r="C24" s="12">
-        <v>11.8</v>
+        <v>11.6</v>
       </c>
       <c r="D24" s="12">
         <v>1</v>
@@ -15877,13 +16997,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C25" s="12">
-        <v>19.8</v>
+        <v>11.5</v>
       </c>
       <c r="D25" s="12">
         <v>1</v>
@@ -15891,41 +17011,41 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>296</v>
       </c>
       <c r="C26" s="12">
-        <v>41</v>
+        <v>11.8</v>
       </c>
       <c r="D26" s="12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C27" s="12">
-        <v>45.5</v>
+        <v>19.8</v>
       </c>
       <c r="D27" s="12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>296</v>
       </c>
       <c r="C28" s="12">
-        <v>43.5</v>
+        <v>41</v>
       </c>
       <c r="D28" s="12">
         <v>1.5</v>
@@ -15933,41 +17053,41 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C29" s="12">
-        <v>23.5</v>
+        <v>45.5</v>
       </c>
       <c r="D29" s="12">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C30" s="12">
-        <v>28</v>
+        <v>43.5</v>
       </c>
       <c r="D30" s="12">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>296</v>
       </c>
       <c r="C31" s="12">
-        <v>18</v>
+        <v>23.5</v>
       </c>
       <c r="D31" s="12">
         <v>1</v>
@@ -15975,13 +17095,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C32" s="12">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D32" s="12">
         <v>1</v>
@@ -15992,61 +17112,67 @@
         <v>302</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C33" s="12">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D33" s="12">
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C34" s="12">
+        <v>25</v>
+      </c>
+      <c r="D34" s="12">
+        <v>1</v>
+      </c>
+    </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="266" t="s">
+      <c r="A35" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35" s="12">
+        <v>20</v>
+      </c>
+      <c r="D35" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="280" t="s">
         <v>290</v>
       </c>
-      <c r="B35" s="266" t="s">
+      <c r="B37" s="280" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="266"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="266"/>
-      <c r="B36" s="5" t="s">
+      <c r="C37" s="280"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="280"/>
+      <c r="B38" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="B37" s="12">
-        <v>22.5</v>
-      </c>
-      <c r="C37" s="12">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="B38" s="12">
-        <v>33.5</v>
-      </c>
-      <c r="C38" s="12">
-        <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="B39" s="12">
-        <v>19.5</v>
+        <v>22.5</v>
       </c>
       <c r="C39" s="12">
         <v>1.5</v>
@@ -16054,10 +17180,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="B40" s="12">
-        <v>11.5</v>
+        <v>33.5</v>
       </c>
       <c r="C40" s="12">
         <v>1.5</v>
@@ -16065,10 +17191,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B41" s="12">
-        <v>6.5</v>
+        <v>19.5</v>
       </c>
       <c r="C41" s="12">
         <v>1.5</v>
@@ -16076,72 +17202,72 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B42" s="12">
-        <v>4</v>
+        <v>11.5</v>
       </c>
       <c r="C42" s="12">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B43" s="12">
+        <v>6.5</v>
+      </c>
+      <c r="C43" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B44" s="12">
+        <v>4</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B45" s="12">
         <v>7</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C45" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="266" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="280" t="s">
         <v>290</v>
       </c>
-      <c r="B45" s="266" t="s">
+      <c r="B47" s="280" t="s">
         <v>315</v>
       </c>
-      <c r="C45" s="266"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="266"/>
-      <c r="B46" s="5" t="s">
+      <c r="C47" s="280"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="280"/>
+      <c r="B48" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="B47" s="12">
-        <v>30.5</v>
-      </c>
-      <c r="C47" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B48" s="12">
-        <v>18.5</v>
-      </c>
-      <c r="C48" s="12">
-        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B49" s="12">
-        <v>24.5</v>
+        <v>30.5</v>
       </c>
       <c r="C49" s="12">
         <v>1</v>
@@ -16149,10 +17275,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B50" s="12">
-        <v>15.5</v>
+        <v>18.5</v>
       </c>
       <c r="C50" s="12">
         <v>1</v>
@@ -16160,10 +17286,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B51" s="12">
-        <v>12.5</v>
+        <v>24.5</v>
       </c>
       <c r="C51" s="12">
         <v>1</v>
@@ -16171,10 +17297,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="B52" s="12">
-        <v>3.5</v>
+        <v>15.5</v>
       </c>
       <c r="C52" s="12">
         <v>1</v>
@@ -16182,61 +17308,61 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B53" s="12">
-        <v>3</v>
+        <v>12.5</v>
       </c>
       <c r="C53" s="12">
         <v>1</v>
       </c>
     </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B54" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="C54" s="12">
+        <v>1</v>
+      </c>
+    </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="266" t="s">
+      <c r="A55" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B55" s="12">
+        <v>3</v>
+      </c>
+      <c r="C55" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="280" t="s">
         <v>290</v>
       </c>
-      <c r="B55" s="266" t="s">
+      <c r="B57" s="280" t="s">
         <v>322</v>
       </c>
-      <c r="C55" s="266"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="266"/>
-      <c r="B56" s="5" t="s">
+      <c r="C57" s="280"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="280"/>
+      <c r="B58" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B57" s="12">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C57" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B58" s="12">
-        <v>12.6</v>
-      </c>
-      <c r="C58" s="12">
-        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B59" s="12">
-        <v>14.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C59" s="12">
         <v>1</v>
@@ -16244,7 +17370,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B60" s="12">
         <v>12.6</v>
@@ -16255,10 +17381,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="B61" s="12">
-        <v>18.5</v>
+        <v>14.5</v>
       </c>
       <c r="C61" s="12">
         <v>1</v>
@@ -16266,10 +17392,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B62" s="12">
-        <v>18.5</v>
+        <v>12.6</v>
       </c>
       <c r="C62" s="12">
         <v>1</v>
@@ -16277,61 +17403,61 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="B63" s="12">
-        <v>24.2</v>
+        <v>18.5</v>
       </c>
       <c r="C63" s="12">
         <v>1</v>
       </c>
     </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B64" s="12">
+        <v>18.5</v>
+      </c>
+      <c r="C64" s="12">
+        <v>1</v>
+      </c>
+    </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="266" t="s">
+      <c r="A65" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B65" s="12">
+        <v>24.2</v>
+      </c>
+      <c r="C65" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="280" t="s">
         <v>290</v>
       </c>
-      <c r="B65" s="266" t="s">
+      <c r="B67" s="280" t="s">
         <v>327</v>
       </c>
-      <c r="C65" s="266"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="266"/>
-      <c r="B66" s="5" t="s">
+      <c r="C67" s="280"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="280"/>
+      <c r="B68" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B67" s="13">
-        <v>3</v>
-      </c>
-      <c r="C67" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="B68" s="13">
-        <v>7</v>
-      </c>
-      <c r="C68" s="13">
-        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B69" s="13">
-        <v>7.5</v>
+        <v>3</v>
       </c>
       <c r="C69" s="13">
         <v>1</v>
@@ -16339,43 +17465,43 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>301</v>
+        <v>328</v>
       </c>
       <c r="B70" s="13">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C70" s="13">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B71" s="13">
-        <v>24</v>
+        <v>7.5</v>
       </c>
       <c r="C71" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>329</v>
+        <v>301</v>
       </c>
       <c r="B72" s="13">
-        <v>22.5</v>
+        <v>12</v>
       </c>
       <c r="C72" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="B73" s="13">
-        <v>24.5</v>
+        <v>24</v>
       </c>
       <c r="C73" s="13">
         <v>2</v>
@@ -16383,10 +17509,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B74" s="13">
-        <v>28.5</v>
+        <v>22.5</v>
       </c>
       <c r="C74" s="13">
         <v>2</v>
@@ -16394,10 +17520,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>306</v>
+        <v>330</v>
       </c>
       <c r="B75" s="13">
-        <v>47.5</v>
+        <v>24.5</v>
       </c>
       <c r="C75" s="13">
         <v>2</v>
@@ -16405,10 +17531,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B76" s="13">
-        <v>66</v>
+        <v>28.5</v>
       </c>
       <c r="C76" s="13">
         <v>2</v>
@@ -16416,29 +17542,51 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
       <c r="B77" s="13">
-        <v>67</v>
+        <v>47.5</v>
       </c>
       <c r="C77" s="13">
         <v>2</v>
       </c>
     </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B78" s="13">
+        <v>66</v>
+      </c>
+      <c r="C78" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B79" s="13">
+        <v>67</v>
+      </c>
+      <c r="C79" s="13">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="69" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Remove test data that got saved into the template
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="350">
   <si>
     <t>Medical Physicist CT Survey Report</t>
   </si>
@@ -1083,13 +1083,13 @@
     <t>Serial #:</t>
   </si>
   <si>
-    <t>CB2-17090320</t>
-  </si>
-  <si>
     <t>Calibration Date:</t>
   </si>
   <si>
     <t>Calibration Due:</t>
+  </si>
+  <si>
+    <t>Somatom Confidence</t>
   </si>
 </sst>
 </file>
@@ -2228,7 +2228,7 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="295">
+  <cellXfs count="298">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3010,6 +3010,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="21" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="21" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3019,92 +3052,68 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="170" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="21" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="21" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3965,19 +3974,19 @@
       <c r="A6" s="219" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="265" t="str">
+      <c r="B6" s="276" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="265"/>
+      <c r="C6" s="276"/>
       <c r="D6" s="220" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="265" t="str">
+      <c r="E6" s="276" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="265"/>
+      <c r="F6" s="276"/>
       <c r="G6" s="1"/>
       <c r="J6" s="245" t="s">
         <v>337</v>
@@ -3987,48 +3996,48 @@
       <c r="A7" s="219" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="263"/>
-      <c r="C7" s="263"/>
+      <c r="B7" s="274"/>
+      <c r="C7" s="274"/>
       <c r="D7" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="263" t="str">
+      <c r="E7" s="274" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="263"/>
+      <c r="F7" s="274"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="219" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="263"/>
-      <c r="C8" s="263"/>
+      <c r="B8" s="274"/>
+      <c r="C8" s="274"/>
       <c r="D8" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="263" t="str">
+      <c r="E8" s="274" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="263"/>
+      <c r="F8" s="274"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="219" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="263"/>
-      <c r="C9" s="263"/>
+      <c r="B9" s="274"/>
+      <c r="C9" s="274"/>
       <c r="D9" s="220" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="263" t="str">
+      <c r="E9" s="274" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="263"/>
+      <c r="F9" s="274"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4038,19 +4047,19 @@
       <c r="D10" s="220" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="264" t="str">
+      <c r="E10" s="275" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="264"/>
+      <c r="F10" s="275"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="219" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="265"/>
-      <c r="C11" s="265"/>
+      <c r="B11" s="276"/>
+      <c r="C11" s="276"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4073,10 +4082,10 @@
       <c r="A13" s="222" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="265" t="s">
+      <c r="B13" s="276" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="265"/>
+      <c r="C13" s="276"/>
       <c r="D13" s="220" t="s">
         <v>16</v>
       </c>
@@ -4412,9 +4421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K190" sqref="K190"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4678,19 +4685,19 @@
       <c r="E10" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="277" t="str">
+      <c r="F10" s="289" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="277"/>
+      <c r="G10" s="289"/>
       <c r="J10" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="277" t="str">
+      <c r="K10" s="289" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="277"/>
+      <c r="L10" s="289"/>
       <c r="M10" s="23"/>
       <c r="O10" s="24"/>
       <c r="Q10" s="28" t="s">
@@ -4731,19 +4738,19 @@
       <c r="E11" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="280" t="str">
+      <c r="F11" s="292" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="280"/>
+      <c r="G11" s="292"/>
       <c r="J11" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="277" t="str">
+      <c r="K11" s="289" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="277"/>
+      <c r="L11" s="289"/>
       <c r="M11" s="23"/>
       <c r="O11" s="24"/>
       <c r="Q11" s="28" t="s">
@@ -4784,19 +4791,19 @@
       <c r="E12" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="280" t="str">
+      <c r="F12" s="292" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="280"/>
+      <c r="G12" s="292"/>
       <c r="J12" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="281" t="str">
+      <c r="K12" s="293" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="281"/>
+      <c r="L12" s="293"/>
       <c r="M12" s="23"/>
       <c r="O12" s="24"/>
       <c r="Q12" s="28" t="s">
@@ -4837,19 +4844,19 @@
       <c r="E13" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="280" t="str">
+      <c r="F13" s="292" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="280"/>
+      <c r="G13" s="292"/>
       <c r="J13" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="277" t="str">
+      <c r="K13" s="289" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="277"/>
+      <c r="L13" s="289"/>
       <c r="M13" s="23"/>
       <c r="O13" s="24"/>
       <c r="Q13" s="28" t="s">
@@ -4947,19 +4954,19 @@
       <c r="E16" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="277" t="str">
+      <c r="F16" s="289" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="277"/>
+      <c r="G16" s="289"/>
       <c r="J16" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="281" t="str">
+      <c r="K16" s="293" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="281"/>
+      <c r="L16" s="293"/>
       <c r="M16" s="23"/>
       <c r="O16" s="24"/>
       <c r="P16" s="56" t="s">
@@ -4987,19 +4994,19 @@
       <c r="E17" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="280" t="str">
+      <c r="F17" s="292" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="280"/>
+      <c r="G17" s="292"/>
       <c r="J17" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="277" t="str">
+      <c r="K17" s="289" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="277"/>
+      <c r="L17" s="289"/>
       <c r="M17" s="23"/>
       <c r="O17" s="24"/>
       <c r="Q17" s="28" t="s">
@@ -5040,11 +5047,11 @@
       <c r="J18" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="277" t="str">
+      <c r="K18" s="289" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="277"/>
+      <c r="L18" s="289"/>
       <c r="M18" s="23"/>
       <c r="O18" s="24"/>
       <c r="Q18" s="28" t="s">
@@ -5116,11 +5123,11 @@
       <c r="E20" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="277" t="str">
+      <c r="F20" s="289" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="277"/>
+      <c r="G20" s="289"/>
       <c r="I20" s="59" t="s">
         <v>76</v>
       </c>
@@ -5145,19 +5152,19 @@
       <c r="E21" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="279" t="str">
+      <c r="F21" s="291" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="279"/>
+      <c r="G21" s="291"/>
       <c r="J21" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="277" t="str">
+      <c r="K21" s="289" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="277"/>
+      <c r="L21" s="289"/>
       <c r="M21" s="23"/>
       <c r="O21" s="24"/>
       <c r="Q21" s="28" t="s">
@@ -5196,11 +5203,11 @@
       <c r="J22" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="277" t="str">
+      <c r="K22" s="289" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="277"/>
+      <c r="L22" s="289"/>
       <c r="M22" s="23"/>
       <c r="O22" s="24"/>
       <c r="Q22" s="28" t="s">
@@ -5241,19 +5248,19 @@
       <c r="E23" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="277" t="str">
+      <c r="F23" s="289" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="277"/>
+      <c r="G23" s="289"/>
       <c r="J23" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="277" t="str">
+      <c r="K23" s="289" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="277"/>
+      <c r="L23" s="289"/>
       <c r="M23" s="23"/>
       <c r="O23" s="24"/>
       <c r="P23" s="56" t="s">
@@ -5289,11 +5296,11 @@
       <c r="E24" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="277" t="str">
+      <c r="F24" s="289" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="277"/>
+      <c r="G24" s="289"/>
       <c r="M24" s="23"/>
       <c r="O24" s="24"/>
       <c r="Q24" s="28" t="s">
@@ -5334,11 +5341,11 @@
       <c r="E25" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="277" t="str">
+      <c r="F25" s="289" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="277"/>
+      <c r="G25" s="289"/>
       <c r="J25" s="55" t="s">
         <v>82</v>
       </c>
@@ -5378,11 +5385,11 @@
       <c r="J26" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="277" t="str">
+      <c r="K26" s="289" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="277"/>
+      <c r="L26" s="289"/>
       <c r="M26" s="23"/>
       <c r="O26" s="24"/>
       <c r="Q26" s="28" t="s">
@@ -5410,19 +5417,19 @@
       <c r="E27" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="277" t="str">
+      <c r="F27" s="289" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="277"/>
+      <c r="G27" s="289"/>
       <c r="J27" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="277" t="str">
+      <c r="K27" s="289" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="277"/>
+      <c r="L27" s="289"/>
       <c r="M27" s="23"/>
       <c r="O27" s="24"/>
       <c r="P27" s="56" t="s">
@@ -5449,11 +5456,11 @@
       <c r="E28" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="277" t="str">
+      <c r="F28" s="289" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="277"/>
+      <c r="G28" s="289"/>
       <c r="M28" s="23"/>
       <c r="O28" s="24"/>
       <c r="Q28" s="28" t="s">
@@ -5494,11 +5501,11 @@
       <c r="E29" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="277" t="str">
+      <c r="F29" s="289" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="277"/>
+      <c r="G29" s="289"/>
       <c r="M29" s="23"/>
       <c r="O29" s="24"/>
       <c r="Q29" s="28" t="s">
@@ -5608,10 +5615,10 @@
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
-      <c r="L32" s="278" t="s">
+      <c r="L32" s="290" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="278"/>
+      <c r="M32" s="290"/>
       <c r="AA32" s="28" t="s">
         <v>70</v>
       </c>
@@ -6202,7 +6209,7 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="O50" s="282"/>
+      <c r="O50" s="263"/>
       <c r="Y50" s="25"/>
       <c r="AA50" s="28" t="s">
         <v>120</v>
@@ -6874,27 +6881,27 @@
       </c>
       <c r="B70" s="21"/>
       <c r="E70" s="69"/>
-      <c r="F70" s="274" t="s">
+      <c r="F70" s="286" t="s">
         <v>150</v>
       </c>
-      <c r="G70" s="274"/>
-      <c r="H70" s="274"/>
-      <c r="I70" s="274" t="s">
+      <c r="G70" s="286"/>
+      <c r="H70" s="286"/>
+      <c r="I70" s="286" t="s">
         <v>151</v>
       </c>
-      <c r="J70" s="274"/>
+      <c r="J70" s="286"/>
       <c r="M70" s="23"/>
       <c r="O70" s="44"/>
       <c r="P70" s="17"/>
-      <c r="Q70" s="275" t="s">
+      <c r="Q70" s="287" t="s">
         <v>150</v>
       </c>
-      <c r="R70" s="275"/>
-      <c r="S70" s="275"/>
-      <c r="T70" s="275" t="s">
+      <c r="R70" s="287"/>
+      <c r="S70" s="287"/>
+      <c r="T70" s="287" t="s">
         <v>151</v>
       </c>
-      <c r="U70" s="275"/>
+      <c r="U70" s="287"/>
       <c r="V70" s="17"/>
       <c r="W70" s="17"/>
       <c r="X70" s="17"/>
@@ -8115,15 +8122,15 @@
       <c r="M89" s="87"/>
       <c r="O89" s="24"/>
       <c r="P89" s="53"/>
-      <c r="Q89" s="276" t="s">
+      <c r="Q89" s="288" t="s">
         <v>150</v>
       </c>
-      <c r="R89" s="276"/>
-      <c r="S89" s="276"/>
-      <c r="T89" s="276" t="s">
+      <c r="R89" s="288"/>
+      <c r="S89" s="288"/>
+      <c r="T89" s="288" t="s">
         <v>151</v>
       </c>
-      <c r="U89" s="276"/>
+      <c r="U89" s="288"/>
       <c r="Y89" s="25"/>
       <c r="AA89" s="28" t="s">
         <v>129</v>
@@ -8189,12 +8196,12 @@
         <f>IF(P112="","",P112)</f>
         <v>Piranha</v>
       </c>
-      <c r="G91" s="284" t="s">
-        <v>348</v>
-      </c>
-      <c r="H91" s="294">
+      <c r="G91" s="264" t="s">
+        <v>347</v>
+      </c>
+      <c r="H91" s="273" t="str">
         <f>IF(S112="","",S112)</f>
-        <v>43014</v>
+        <v/>
       </c>
       <c r="M91" s="23"/>
       <c r="O91" s="24"/>
@@ -8228,34 +8235,25 @@
       <c r="C92" s="48" t="s">
         <v>346</v>
       </c>
-      <c r="D92" s="293" t="str">
+      <c r="D92" s="272" t="str">
         <f>IF(P113="","",P113)</f>
-        <v>CB2-17090320</v>
-      </c>
-      <c r="G92" s="284" t="s">
-        <v>349</v>
-      </c>
-      <c r="H92" s="294">
+        <v/>
+      </c>
+      <c r="G92" s="264" t="s">
+        <v>348</v>
+      </c>
+      <c r="H92" s="273" t="str">
         <f>IF(S113="","",S113)</f>
-        <v>43744</v>
+        <v/>
       </c>
       <c r="M92" s="23"/>
       <c r="O92" s="24"/>
       <c r="P92" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="Q92" s="241" t="str">
-        <f>IF(OR(Q93="",Q95=""),"",Q93/Q95)</f>
-        <v/>
-      </c>
-      <c r="R92" s="241" t="str">
-        <f>IF(OR(R93="",R95=""),"",R93/R95)</f>
-        <v/>
-      </c>
-      <c r="S92" s="241" t="str">
-        <f>IF(OR(S93="",S95=""),"",S93/S95)</f>
-        <v/>
-      </c>
+      <c r="Q92" s="241"/>
+      <c r="R92" s="241"/>
+      <c r="S92" s="241"/>
       <c r="T92" s="241" t="str">
         <f>IF(OR(T93="",T95=""),"",T93/T95)</f>
         <v/>
@@ -8288,18 +8286,9 @@
       <c r="P93" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="Q93" s="240" t="str">
-        <f>IF(OR(Q94="",Q103=""),"",Q94*Q103)</f>
-        <v/>
-      </c>
-      <c r="R93" s="240" t="str">
-        <f>IF(OR(R94="",R103=""),"",R94*R103)</f>
-        <v/>
-      </c>
-      <c r="S93" s="240" t="str">
-        <f>IF(OR(S94="",S103=""),"",S94*S103)</f>
-        <v/>
-      </c>
+      <c r="Q93" s="240"/>
+      <c r="R93" s="240"/>
+      <c r="S93" s="240"/>
       <c r="T93" s="240" t="str">
         <f>IF(OR(T94="",T103=""),"",T94*T103)</f>
         <v/>
@@ -8328,15 +8317,15 @@
       </c>
       <c r="B94" s="21"/>
       <c r="E94" s="69"/>
-      <c r="F94" s="270" t="s">
+      <c r="F94" s="279" t="s">
         <v>150</v>
       </c>
-      <c r="G94" s="270"/>
-      <c r="H94" s="270"/>
-      <c r="I94" s="271" t="s">
+      <c r="G94" s="279"/>
+      <c r="H94" s="279"/>
+      <c r="I94" s="280" t="s">
         <v>151</v>
       </c>
-      <c r="J94" s="271"/>
+      <c r="J94" s="280"/>
       <c r="M94" s="23"/>
       <c r="O94" s="24"/>
       <c r="P94" s="28" t="s">
@@ -8461,28 +8450,28 @@
         <v>31</v>
       </c>
       <c r="B97" s="21"/>
-      <c r="D97" s="272" t="s">
+      <c r="D97" s="284" t="s">
         <v>160</v>
       </c>
-      <c r="E97" s="292"/>
+      <c r="E97" s="285"/>
       <c r="F97" s="95" t="str">
-        <f>IF(Q118="","",Q118)</f>
+        <f t="shared" ref="F97:J102" si="24">IF(Q118="","",Q118)</f>
         <v/>
       </c>
       <c r="G97" s="96" t="str">
-        <f>IF(R118="","",R118)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="H97" s="97" t="str">
-        <f>IF(S118="","",S118)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I97" s="96" t="str">
-        <f>IF(T118="","",T118)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="J97" s="97" t="str">
-        <f>IF(U118="","",U118)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="K97" s="20"/>
@@ -8507,11 +8496,11 @@
       </c>
       <c r="AB97" s="39"/>
       <c r="AC97" s="40" t="str">
-        <f t="shared" ref="AC97:AC113" si="24">IF(AB97&lt;&gt;AD97,"Change","")</f>
+        <f t="shared" ref="AC97:AC113" si="25">IF(AB97&lt;&gt;AD97,"Change","")</f>
         <v/>
       </c>
       <c r="AD97" s="47" t="str">
-        <f t="shared" ref="AD97:AD113" si="25">IF(T72="","",T72)</f>
+        <f t="shared" ref="AD97:AD113" si="26">IF(T72="","",T72)</f>
         <v/>
       </c>
     </row>
@@ -8520,26 +8509,26 @@
         <v>32</v>
       </c>
       <c r="B98" s="21"/>
-      <c r="D98" s="272"/>
-      <c r="E98" s="292"/>
+      <c r="D98" s="284"/>
+      <c r="E98" s="285"/>
       <c r="F98" s="100" t="str">
-        <f>IF(Q119="","",Q119)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="G98" s="101" t="str">
-        <f>IF(R119="","",R119)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="H98" s="102" t="str">
-        <f>IF(S119="","",S119)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I98" s="101" t="str">
-        <f>IF(T119="","",T119)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="J98" s="102" t="str">
-        <f>IF(U119="","",U119)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="K98" s="20"/>
@@ -8564,11 +8553,11 @@
       </c>
       <c r="AB98" s="39"/>
       <c r="AC98" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD98" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -8577,26 +8566,26 @@
         <v>33</v>
       </c>
       <c r="B99" s="21"/>
-      <c r="D99" s="272"/>
-      <c r="E99" s="292"/>
+      <c r="D99" s="284"/>
+      <c r="E99" s="285"/>
       <c r="F99" s="105" t="str">
-        <f>IF(Q120="","",Q120)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="G99" s="106" t="str">
-        <f>IF(R120="","",R120)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="H99" s="107" t="str">
-        <f>IF(S120="","",S120)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I99" s="106" t="str">
-        <f>IF(T120="","",T120)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="J99" s="107" t="str">
-        <f>IF(U120="","",U120)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="K99" s="108" t="s">
@@ -8623,11 +8612,11 @@
       </c>
       <c r="AB99" s="39"/>
       <c r="AC99" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD99" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -8641,23 +8630,23 @@
         <v>164</v>
       </c>
       <c r="F100" s="111" t="str">
-        <f>IF(Q121="","",Q121)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="G100" s="112" t="str">
-        <f>IF(R121="","",R121)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="H100" s="113" t="str">
-        <f>IF(S121="","",S121)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I100" s="114" t="str">
-        <f>IF(T121="","",T121)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="J100" s="115" t="str">
-        <f>IF(U121="","",U121)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="K100" s="116" t="s">
@@ -8684,11 +8673,11 @@
       </c>
       <c r="AB100" s="39"/>
       <c r="AC100" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD100" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -8702,23 +8691,23 @@
         <v>166</v>
       </c>
       <c r="F101" s="77" t="str">
-        <f>IF(Q122="","",Q122)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="G101" s="78" t="str">
-        <f>IF(R122="","",R122)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="H101" s="79" t="str">
-        <f>IF(S122="","",S122)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I101" s="78" t="str">
-        <f>IF(T122="","",T122)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="J101" s="79" t="str">
-        <f>IF(U122="","",U122)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="K101" s="116" t="s">
@@ -8745,11 +8734,11 @@
       </c>
       <c r="AB101" s="39"/>
       <c r="AC101" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD101" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -8762,23 +8751,23 @@
         <v>168</v>
       </c>
       <c r="F102" s="83" t="str">
-        <f>IF(Q123="","",Q123)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="G102" s="84" t="str">
-        <f>IF(R123="","",R123)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="H102" s="85" t="str">
-        <f>IF(S123="","",S123)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I102" s="84" t="str">
-        <f>IF(T123="","",T123)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="J102" s="85" t="str">
-        <f>IF(U123="","",U123)</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="K102" s="116" t="s">
@@ -8794,18 +8783,9 @@
       <c r="P102" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="Q102" s="240" t="str">
-        <f>IF(OR(Q100="",Q101="",Q103=""),"",(Q101*Q100)*Q103)</f>
-        <v/>
-      </c>
-      <c r="R102" s="240" t="str">
-        <f>IF(OR(R100="",R101="",R103=""),"",(R101*R100)*R103)</f>
-        <v/>
-      </c>
-      <c r="S102" s="240" t="str">
-        <f>IF(OR(S100="",S101="",S103=""),"",(S101*S100)*S103)</f>
-        <v/>
-      </c>
+      <c r="Q102" s="240"/>
+      <c r="R102" s="240"/>
+      <c r="S102" s="240"/>
       <c r="T102" s="240" t="str">
         <f>IF(OR(T100="",T101="",T103=""),"",(T101*T100)*T103)</f>
         <v/>
@@ -8820,11 +8800,11 @@
       </c>
       <c r="AB102" s="39"/>
       <c r="AC102" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD102" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -8837,23 +8817,23 @@
         <v>170</v>
       </c>
       <c r="F103" s="119" t="str">
-        <f>IF(Q125="","",Q125)</f>
+        <f t="shared" ref="F103:J106" si="27">IF(Q125="","",Q125)</f>
         <v/>
       </c>
       <c r="G103" s="120" t="str">
-        <f>IF(R125="","",R125)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="H103" s="121" t="str">
-        <f>IF(S125="","",S125)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="I103" s="120" t="str">
-        <f>IF(T125="","",T125)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="J103" s="121" t="str">
-        <f>IF(U125="","",U125)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="K103" s="122" t="s">
@@ -8880,11 +8860,11 @@
       </c>
       <c r="AB103" s="39"/>
       <c r="AC103" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD103" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -8897,23 +8877,23 @@
         <v>172</v>
       </c>
       <c r="F104" s="125" t="str">
-        <f>IF(Q126="","",Q126)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="G104" s="126" t="str">
-        <f>IF(R126="","",R126)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="H104" s="127" t="str">
-        <f>IF(S126="","",S126)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="I104" s="126" t="str">
-        <f>IF(T126="","",T126)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="J104" s="127" t="str">
-        <f>IF(U126="","",U126)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="M104" s="23"/>
@@ -8932,11 +8912,11 @@
       </c>
       <c r="AB104" s="39"/>
       <c r="AC104" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD104" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -8951,23 +8931,23 @@
         <v>173</v>
       </c>
       <c r="F105" s="92" t="str">
-        <f>IF(Q127="","",Q127)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="G105" s="93" t="str">
-        <f>IF(R127="","",R127)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="H105" s="94" t="str">
-        <f>IF(S127="","",S127)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="I105" s="93" t="str">
-        <f>IF(T127="","",T127)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="J105" s="94" t="str">
-        <f>IF(U127="","",U127)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="M105" s="23"/>
@@ -8986,11 +8966,11 @@
       </c>
       <c r="AB105" s="39"/>
       <c r="AC105" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD105" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9005,23 +8985,23 @@
         <v>174</v>
       </c>
       <c r="F106" s="128" t="str">
-        <f>IF(Q128="","",Q128)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="G106" s="129" t="str">
-        <f>IF(R128="","",R128)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="H106" s="130" t="str">
-        <f>IF(S128="","",S128)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="I106" s="129" t="str">
-        <f>IF(T128="","",T128)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="J106" s="130" t="str">
-        <f>IF(U128="","",U128)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="M106" s="23"/>
@@ -9040,11 +9020,11 @@
       </c>
       <c r="AB106" s="39"/>
       <c r="AC106" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD106" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9083,11 +9063,11 @@
       </c>
       <c r="AB107" s="39"/>
       <c r="AC107" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD107" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9124,11 +9104,11 @@
       </c>
       <c r="AB108" s="39"/>
       <c r="AC108" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD108" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9144,11 +9124,11 @@
       </c>
       <c r="AB109" s="39"/>
       <c r="AC109" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD109" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9170,11 +9150,11 @@
       </c>
       <c r="AB110" s="39"/>
       <c r="AC110" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD110" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9187,19 +9167,19 @@
         <v>176</v>
       </c>
       <c r="E111" s="77" t="str">
-        <f>IF(Q133="","",Q133)</f>
+        <f t="shared" ref="E111:H114" si="28">IF(Q133="","",Q133)</f>
         <v/>
       </c>
       <c r="F111" s="78" t="str">
-        <f>IF(R133="","",R133)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G111" s="78" t="str">
-        <f>IF(S133="","",S133)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H111" s="79" t="str">
-        <f>IF(T133="","",T133)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J111" s="20"/>
@@ -9222,11 +9202,11 @@
       </c>
       <c r="AB111" s="39"/>
       <c r="AC111" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD111" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9239,47 +9219,45 @@
         <v>177</v>
       </c>
       <c r="E112" s="80" t="str">
-        <f>IF(Q134="","",Q134)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="F112" s="81" t="str">
-        <f>IF(R134="","",R134)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G112" s="81" t="str">
-        <f>IF(S134="","",S134)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H112" s="82" t="str">
-        <f>IF(T134="","",T134)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J112" s="20"/>
       <c r="M112" s="23"/>
-      <c r="O112" s="286" t="s">
+      <c r="O112" s="266" t="s">
         <v>344</v>
       </c>
-      <c r="P112" s="287" t="s">
+      <c r="P112" s="267" t="s">
         <v>345</v>
       </c>
-      <c r="R112" s="285" t="s">
-        <v>348</v>
-      </c>
-      <c r="S112" s="290">
-        <v>43014</v>
-      </c>
-      <c r="T112" s="289"/>
+      <c r="R112" s="265" t="s">
+        <v>347</v>
+      </c>
+      <c r="S112" s="270"/>
+      <c r="T112" s="269"/>
       <c r="Y112" s="25"/>
       <c r="AA112" s="28" t="s">
         <v>142</v>
       </c>
       <c r="AB112" s="39"/>
       <c r="AC112" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD112" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9292,47 +9270,43 @@
         <v>178</v>
       </c>
       <c r="E113" s="80" t="str">
-        <f>IF(Q135="","",Q135)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="F113" s="81" t="str">
-        <f>IF(R135="","",R135)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G113" s="81" t="str">
-        <f>IF(S135="","",S135)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H113" s="82" t="str">
-        <f>IF(T135="","",T135)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J113" s="20"/>
       <c r="M113" s="23"/>
-      <c r="O113" s="286" t="s">
+      <c r="O113" s="266" t="s">
         <v>346</v>
       </c>
-      <c r="P113" s="288" t="s">
+      <c r="P113" s="268"/>
+      <c r="R113" s="265" t="s">
         <v>347</v>
       </c>
-      <c r="R113" s="285" t="s">
-        <v>348</v>
-      </c>
-      <c r="S113" s="291">
-        <v>43744</v>
-      </c>
-      <c r="T113" s="289"/>
+      <c r="S113" s="271"/>
+      <c r="T113" s="269"/>
       <c r="Y113" s="25"/>
       <c r="AA113" s="28" t="s">
         <v>144</v>
       </c>
       <c r="AB113" s="39"/>
       <c r="AC113" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AD113" s="47" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -9345,19 +9319,19 @@
         <v>179</v>
       </c>
       <c r="E114" s="80" t="str">
-        <f>IF(Q136="","",Q136)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="F114" s="81" t="str">
-        <f>IF(R136="","",R136)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G114" s="81" t="str">
-        <f>IF(S136="","",S136)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H114" s="82" t="str">
-        <f>IF(T136="","",T136)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J114" s="20"/>
@@ -9395,15 +9369,15 @@
       <c r="J115" s="20"/>
       <c r="M115" s="23"/>
       <c r="O115" s="24"/>
-      <c r="Q115" s="273" t="s">
+      <c r="Q115" s="281" t="s">
         <v>150</v>
       </c>
-      <c r="R115" s="273"/>
-      <c r="S115" s="273"/>
-      <c r="T115" s="267" t="s">
+      <c r="R115" s="281"/>
+      <c r="S115" s="281"/>
+      <c r="T115" s="277" t="s">
         <v>151</v>
       </c>
-      <c r="U115" s="267"/>
+      <c r="U115" s="277"/>
       <c r="W115" s="56" t="s">
         <v>157</v>
       </c>
@@ -9413,11 +9387,11 @@
       </c>
       <c r="AB115" s="39"/>
       <c r="AC115" s="40" t="str">
-        <f t="shared" ref="AC115:AC131" si="26">IF(AB115&lt;&gt;AD115,"Change","")</f>
+        <f t="shared" ref="AC115:AC131" si="29">IF(AB115&lt;&gt;AD115,"Change","")</f>
         <v/>
       </c>
       <c r="AD115" s="47" t="str">
-        <f t="shared" ref="AD115:AD131" si="27">IF(U72="","",U72)</f>
+        <f t="shared" ref="AD115:AD131" si="30">IF(U72="","",U72)</f>
         <v/>
       </c>
     </row>
@@ -9458,11 +9432,11 @@
       </c>
       <c r="AB116" s="39"/>
       <c r="AC116" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD116" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9528,11 +9502,11 @@
       </c>
       <c r="AB117" s="39"/>
       <c r="AC117" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD117" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9551,10 +9525,10 @@
       <c r="I118" s="20"/>
       <c r="J118" s="20"/>
       <c r="M118" s="23"/>
-      <c r="O118" s="268" t="s">
+      <c r="O118" s="283" t="s">
         <v>160</v>
       </c>
-      <c r="P118" s="283"/>
+      <c r="P118" s="282"/>
       <c r="Q118" s="138"/>
       <c r="R118" s="139"/>
       <c r="S118" s="140"/>
@@ -9572,11 +9546,11 @@
       </c>
       <c r="AB118" s="39"/>
       <c r="AC118" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD118" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9592,8 +9566,8 @@
       <c r="I119" s="20"/>
       <c r="J119" s="20"/>
       <c r="M119" s="23"/>
-      <c r="O119" s="268"/>
-      <c r="P119" s="283"/>
+      <c r="O119" s="283"/>
+      <c r="P119" s="282"/>
       <c r="Q119" s="141"/>
       <c r="R119" s="142"/>
       <c r="S119" s="143"/>
@@ -9613,11 +9587,11 @@
       </c>
       <c r="AB119" s="39"/>
       <c r="AC119" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD119" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9627,8 +9601,8 @@
       </c>
       <c r="B120" s="21"/>
       <c r="M120" s="23"/>
-      <c r="O120" s="268"/>
-      <c r="P120" s="283"/>
+      <c r="O120" s="283"/>
+      <c r="P120" s="282"/>
       <c r="Q120" s="145"/>
       <c r="R120" s="146"/>
       <c r="S120" s="147"/>
@@ -9648,11 +9622,11 @@
       </c>
       <c r="AB120" s="39"/>
       <c r="AC120" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD120" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9703,11 +9677,11 @@
       </c>
       <c r="AB121" s="39"/>
       <c r="AC121" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD121" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9748,11 +9722,11 @@
       </c>
       <c r="AB122" s="39"/>
       <c r="AC122" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD122" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9785,11 +9759,11 @@
       </c>
       <c r="AB123" s="39"/>
       <c r="AC123" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD123" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9832,11 +9806,11 @@
       </c>
       <c r="AB124" s="39"/>
       <c r="AC124" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD124" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9895,11 +9869,11 @@
       </c>
       <c r="AB125" s="39"/>
       <c r="AC125" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD125" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9960,11 +9934,11 @@
       </c>
       <c r="AB126" s="39"/>
       <c r="AC126" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD126" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9997,11 +9971,11 @@
         <v/>
       </c>
       <c r="R127" s="136" t="str">
-        <f>IF(R121="","",IF(AND(R121&lt;=Y119,R125&lt;=0.05,R126&lt;=0.2),"Pass","Fail"))</f>
+        <f>IF(R121="","",IF(AND(R121&lt;=Y119,R126&lt;=0.2),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="S127" s="137" t="str">
-        <f>IF(S121="","",IF(AND(S121&lt;=Y120,S125&lt;=0.05,S126&lt;=0.2),"Pass","Fail"))</f>
+        <f>IF(S121="","",IF(AND(S121&lt;=Y120,S126&lt;=0.2),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="T127" s="136" t="str">
@@ -10020,11 +9994,11 @@
       </c>
       <c r="AB127" s="39"/>
       <c r="AC127" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD127" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -10066,11 +10040,11 @@
       </c>
       <c r="AB128" s="39"/>
       <c r="AC128" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD128" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -10115,11 +10089,11 @@
       </c>
       <c r="AB129" s="39"/>
       <c r="AC129" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD129" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -10159,11 +10133,11 @@
       </c>
       <c r="AB130" s="39"/>
       <c r="AC130" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD130" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -10203,11 +10177,11 @@
       </c>
       <c r="AB131" s="39"/>
       <c r="AC131" s="40" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD131" s="47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -10404,7 +10378,7 @@
       <c r="C137" s="53"/>
       <c r="M137" s="23"/>
       <c r="O137" s="24"/>
-      <c r="P137" s="283" t="s">
+      <c r="P137" s="282" t="s">
         <v>180</v>
       </c>
       <c r="Q137" s="172"/>
@@ -10448,7 +10422,7 @@
       </c>
       <c r="M138" s="23"/>
       <c r="O138" s="24"/>
-      <c r="P138" s="283"/>
+      <c r="P138" s="282"/>
       <c r="Q138" s="172"/>
       <c r="R138" s="173"/>
       <c r="S138" s="173"/>
@@ -10492,7 +10466,7 @@
       </c>
       <c r="M139" s="23"/>
       <c r="O139" s="24"/>
-      <c r="P139" s="283"/>
+      <c r="P139" s="282"/>
       <c r="Q139" s="175"/>
       <c r="R139" s="176"/>
       <c r="S139" s="176"/>
@@ -10593,15 +10567,15 @@
         <v/>
       </c>
       <c r="R141" s="136" t="str">
-        <f>IF(R140="","",IF(OR(ABS(R136-R140)&lt;=3,ABS(AVERAGE(R137:R139)-R136)/R136&lt;0.3),"Pass","Fail"))</f>
+        <f t="shared" ref="R141:T141" si="31">IF(R140="","",IF(OR(ABS(R136-R140)&lt;=3,ABS(AVERAGE(R137:R139)-R136)/R136&lt;0.3),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="S141" s="136" t="str">
-        <f>IF(S140="","",IF(OR(ABS(S136-S140)&lt;=3,ABS(AVERAGE(S137:S139)-S136)/S136&lt;0.3),"Pass","Fail"))</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="T141" s="137" t="str">
-        <f>IF(T140="","",IF(OR(ABS(T136-T140)&lt;=3,ABS(AVERAGE(T137:T139)-T136)/T136&lt;0.3),"Pass","Fail"))</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="Y141" s="25"/>
@@ -10734,31 +10708,31 @@
         <v>111</v>
       </c>
       <c r="E145" s="80" t="str">
-        <f>IF(P158="","",P158)</f>
+        <f t="shared" ref="E145:K151" si="32">IF(P158="","",P158)</f>
         <v/>
       </c>
       <c r="F145" s="81" t="str">
-        <f>IF(Q158="","",Q158)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G145" s="81" t="str">
-        <f>IF(R158="","",R158)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H145" s="81" t="str">
-        <f>IF(S158="","",S158)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I145" s="81" t="str">
-        <f>IF(T158="","",T158)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J145" s="81" t="str">
-        <f>IF(U158="","",U158)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K145" s="82" t="str">
-        <f>IF(V158="","",V158)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M145" s="23"/>
@@ -10796,31 +10770,31 @@
         <v>215</v>
       </c>
       <c r="E146" s="80" t="str">
-        <f>IF(P159="","",P159)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="F146" s="81" t="str">
-        <f>IF(Q159="","",Q159)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G146" s="81" t="str">
-        <f>IF(R159="","",R159)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H146" s="81" t="str">
-        <f>IF(S159="","",S159)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I146" s="81" t="str">
-        <f>IF(T159="","",T159)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J146" s="81" t="str">
-        <f>IF(U159="","",U159)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K146" s="82" t="str">
-        <f>IF(V159="","",V159)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M146" s="23"/>
@@ -10839,31 +10813,31 @@
         <v>217</v>
       </c>
       <c r="E147" s="80" t="str">
-        <f>IF(P160="","",P160)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="F147" s="81" t="str">
-        <f>IF(Q160="","",Q160)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G147" s="81" t="str">
-        <f>IF(R160="","",R160)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H147" s="81" t="str">
-        <f>IF(S160="","",S160)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I147" s="81" t="str">
-        <f>IF(T160="","",T160)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J147" s="81" t="str">
-        <f>IF(U160="","",U160)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K147" s="82" t="str">
-        <f>IF(V160="","",V160)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M147" s="23"/>
@@ -10891,31 +10865,31 @@
         <v>218</v>
       </c>
       <c r="E148" s="80" t="str">
-        <f>IF(P161="","",P161)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="F148" s="81" t="str">
-        <f>IF(Q161="","",Q161)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G148" s="81" t="str">
-        <f>IF(R161="","",R161)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H148" s="81" t="str">
-        <f>IF(S161="","",S161)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I148" s="81" t="str">
-        <f>IF(T161="","",T161)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J148" s="81" t="str">
-        <f>IF(U161="","",U161)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K148" s="82" t="str">
-        <f>IF(V161="","",V161)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M148" s="23"/>
@@ -10947,31 +10921,31 @@
         <v>220</v>
       </c>
       <c r="E149" s="80" t="str">
-        <f>IF(P162="","",P162)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="F149" s="81" t="str">
-        <f>IF(Q162="","",Q162)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G149" s="81" t="str">
-        <f>IF(R162="","",R162)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H149" s="81" t="str">
-        <f>IF(S162="","",S162)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I149" s="81" t="str">
-        <f>IF(T162="","",T162)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J149" s="81" t="str">
-        <f>IF(U162="","",U162)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K149" s="82" t="str">
-        <f>IF(V162="","",V162)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M149" s="23"/>
@@ -11016,31 +10990,31 @@
         <v>221</v>
       </c>
       <c r="E150" s="80" t="str">
-        <f>IF(P163="","",P163)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="F150" s="81" t="str">
-        <f>IF(Q163="","",Q163)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G150" s="81" t="str">
-        <f>IF(R163="","",R163)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H150" s="81" t="str">
-        <f>IF(S163="","",S163)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I150" s="81" t="str">
-        <f>IF(T163="","",T163)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J150" s="81" t="str">
-        <f>IF(U163="","",U163)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K150" s="82" t="str">
-        <f>IF(V163="","",V163)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M150" s="23"/>
@@ -11060,31 +11034,31 @@
         <v>223</v>
       </c>
       <c r="E151" s="83" t="str">
-        <f>IF(P164="","",P164)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="F151" s="84" t="str">
-        <f>IF(Q164="","",Q164)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G151" s="84" t="str">
-        <f>IF(R164="","",R164)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H151" s="84" t="str">
-        <f>IF(S164="","",S164)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I151" s="84" t="str">
-        <f>IF(T164="","",T164)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J151" s="84" t="str">
-        <f>IF(U164="","",U164)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K151" s="85" t="str">
-        <f>IF(V164="","",V164)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M151" s="23"/>
@@ -11260,23 +11234,23 @@
         <v>229</v>
       </c>
       <c r="F157" s="77" t="str">
-        <f>IF(Q170="","",Q170)</f>
+        <f t="shared" ref="F157:J163" si="33">IF(Q170="","",Q170)</f>
         <v/>
       </c>
       <c r="G157" s="78" t="str">
-        <f>IF(R170="","",R170)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H157" s="78" t="str">
-        <f>IF(S170="","",S170)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I157" s="78" t="str">
-        <f>IF(T170="","",T170)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J157" s="79" t="str">
-        <f>IF(U170="","",U170)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="M157" s="23"/>
@@ -11330,23 +11304,23 @@
         <v>230</v>
       </c>
       <c r="F158" s="80" t="str">
-        <f>IF(Q171="","",Q171)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G158" s="81" t="str">
-        <f>IF(R171="","",R171)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H158" s="81" t="str">
-        <f>IF(S171="","",S171)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I158" s="81" t="str">
-        <f>IF(T171="","",T171)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J158" s="82" t="str">
-        <f>IF(U171="","",U171)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="M158" s="23"/>
@@ -11381,23 +11355,23 @@
         <v>231</v>
       </c>
       <c r="F159" s="80" t="str">
-        <f>IF(Q172="","",Q172)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G159" s="81" t="str">
-        <f>IF(R172="","",R172)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H159" s="81" t="str">
-        <f>IF(S172="","",S172)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I159" s="81" t="str">
-        <f>IF(T172="","",T172)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J159" s="82" t="str">
-        <f>IF(U172="","",U172)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="M159" s="23"/>
@@ -11441,23 +11415,23 @@
         <v>204</v>
       </c>
       <c r="F160" s="80" t="str">
-        <f>IF(Q173="","",Q173)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G160" s="81" t="str">
-        <f>IF(R173="","",R173)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H160" s="81" t="str">
-        <f>IF(S173="","",S173)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I160" s="81" t="str">
-        <f>IF(T173="","",T173)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J160" s="82" t="str">
-        <f>IF(U173="","",U173)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="M160" s="23"/>
@@ -11494,23 +11468,23 @@
         <v>232</v>
       </c>
       <c r="F161" s="80" t="str">
-        <f>IF(Q174="","",Q174)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G161" s="81" t="str">
-        <f>IF(R174="","",R174)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H161" s="81" t="str">
-        <f>IF(S174="","",S174)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I161" s="81" t="str">
-        <f>IF(T174="","",T174)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J161" s="82" t="str">
-        <f>IF(U174="","",U174)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="M161" s="23"/>
@@ -11554,23 +11528,23 @@
         <v>233</v>
       </c>
       <c r="F162" s="83" t="str">
-        <f>IF(Q175="","",Q175)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G162" s="84" t="str">
-        <f>IF(R175="","",R175)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H162" s="84" t="str">
-        <f>IF(S175="","",S175)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I162" s="84" t="str">
-        <f>IF(T175="","",T175)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J162" s="85" t="str">
-        <f>IF(U175="","",U175)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="M162" s="23"/>
@@ -11607,23 +11581,23 @@
         <v>173</v>
       </c>
       <c r="F163" s="92" t="str">
-        <f>IF(Q176="","",Q176)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G163" s="93" t="str">
-        <f>IF(R176="","",R176)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H163" s="93" t="str">
-        <f>IF(S176="","",S176)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I163" s="93" t="str">
-        <f>IF(T176="","",T176)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J163" s="94" t="str">
-        <f>IF(U176="","",U176)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="M163" s="23"/>
@@ -11769,14 +11743,14 @@
       <c r="B168" s="21"/>
       <c r="C168" s="53"/>
       <c r="D168" s="69"/>
-      <c r="E168" s="269" t="s">
+      <c r="E168" s="278" t="s">
         <v>150</v>
       </c>
-      <c r="F168" s="269"/>
-      <c r="G168" s="269" t="s">
+      <c r="F168" s="278"/>
+      <c r="G168" s="278" t="s">
         <v>151</v>
       </c>
-      <c r="H168" s="269"/>
+      <c r="H168" s="278"/>
       <c r="M168" s="23"/>
       <c r="O168" s="24"/>
       <c r="Y168" s="25"/>
@@ -11829,19 +11803,19 @@
         <v>237</v>
       </c>
       <c r="E170" s="77" t="str">
-        <f>IF(P183="","",P183)</f>
+        <f t="shared" ref="E170:H174" si="34">IF(P183="","",P183)</f>
         <v/>
       </c>
       <c r="F170" s="78" t="str">
-        <f>IF(Q183="","",Q183)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="G170" s="78" t="str">
-        <f>IF(R183="","",R183)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="H170" s="79" t="str">
-        <f>IF(S183="","",S183)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="J170" s="48" t="s">
@@ -11876,19 +11850,19 @@
         <v>239</v>
       </c>
       <c r="E171" s="80" t="str">
-        <f>IF(P184="","",P184)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="F171" s="81" t="str">
-        <f>IF(Q184="","",Q184)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="G171" s="81" t="str">
-        <f>IF(R184="","",R184)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="H171" s="82" t="str">
-        <f>IF(S184="","",S184)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="J171" s="48" t="s">
@@ -11930,19 +11904,19 @@
         <v>240</v>
       </c>
       <c r="E172" s="80" t="str">
-        <f>IF(P185="","",P185)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="F172" s="81" t="str">
-        <f>IF(Q185="","",Q185)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="G172" s="81" t="str">
-        <f>IF(R185="","",R185)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="H172" s="82" t="str">
-        <f>IF(S185="","",S185)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="M172" s="23"/>
@@ -11970,19 +11944,19 @@
         <v>241</v>
       </c>
       <c r="E173" s="80" t="str">
-        <f>IF(P186="","",P186)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="F173" s="81" t="str">
-        <f>IF(Q186="","",Q186)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="G173" s="81" t="str">
-        <f>IF(R186="","",R186)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="H173" s="82" t="str">
-        <f>IF(S186="","",S186)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="M173" s="23"/>
@@ -12032,19 +12006,19 @@
         <v>242</v>
       </c>
       <c r="E174" s="105" t="str">
-        <f>IF(P187="","",P187)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="F174" s="106" t="str">
-        <f>IF(Q187="","",Q187)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="G174" s="106" t="str">
-        <f>IF(R187="","",R187)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="H174" s="107" t="str">
-        <f>IF(S187="","",S187)</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="M174" s="23"/>
@@ -12253,23 +12227,23 @@
         <v>250</v>
       </c>
       <c r="D181" s="77" t="str">
-        <f>IF(P191="","",P191)</f>
+        <f t="shared" ref="D181:H185" si="35">IF(P191="","",P191)</f>
         <v/>
       </c>
       <c r="E181" s="79" t="str">
-        <f>IF(Q191="","",Q191)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="F181" s="77" t="str">
-        <f>IF(R191="","",R191)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="G181" s="78" t="str">
-        <f>IF(S191="","",S191)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="H181" s="79" t="str">
-        <f>IF(T191="","",T191)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="I181" s="20"/>
@@ -12305,23 +12279,23 @@
         <v>252</v>
       </c>
       <c r="D182" s="80" t="str">
-        <f>IF(P192="","",P192)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="E182" s="82" t="str">
-        <f>IF(Q192="","",Q192)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="F182" s="80" t="str">
-        <f>IF(R192="","",R192)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="G182" s="81" t="str">
-        <f>IF(S192="","",S192)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="H182" s="82" t="str">
-        <f>IF(T192="","",T192)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="I182" s="20"/>
@@ -12357,23 +12331,23 @@
         <v>255</v>
       </c>
       <c r="D183" s="80" t="str">
-        <f>IF(P193="","",P193)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="E183" s="82" t="str">
-        <f>IF(Q193="","",Q193)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="F183" s="80" t="str">
-        <f>IF(R193="","",R193)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="G183" s="81" t="str">
-        <f>IF(S193="","",S193)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="H183" s="82" t="str">
-        <f>IF(T193="","",T193)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="I183" s="20"/>
@@ -12408,23 +12382,23 @@
         <v>257</v>
       </c>
       <c r="D184" s="80" t="str">
-        <f>IF(P194="","",P194)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="E184" s="82" t="str">
-        <f>IF(Q194="","",Q194)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="F184" s="80" t="str">
-        <f>IF(R194="","",R194)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="G184" s="81" t="str">
-        <f>IF(S194="","",S194)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="H184" s="82" t="str">
-        <f>IF(T194="","",T194)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="I184" s="20"/>
@@ -12454,23 +12428,23 @@
         <v>259</v>
       </c>
       <c r="D185" s="83" t="str">
-        <f>IF(P195="","",P195)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="E185" s="85" t="str">
-        <f>IF(Q195="","",Q195)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="F185" s="83" t="str">
-        <f>IF(R195="","",R195)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="G185" s="84" t="str">
-        <f>IF(S195="","",S195)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="H185" s="85" t="str">
-        <f>IF(T195="","",T195)</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="I185" s="20"/>
@@ -13037,7 +13011,7 @@
       <c r="S204" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="T204" s="142"/>
+      <c r="T204" s="297"/>
       <c r="Y204" s="25"/>
     </row>
     <row r="205" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13066,7 +13040,7 @@
       <c r="S205" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="T205" s="142"/>
+      <c r="T205" s="297"/>
       <c r="Y205" s="25"/>
     </row>
     <row r="206" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13095,7 +13069,7 @@
       <c r="S206" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="T206" s="142"/>
+      <c r="T206" s="297"/>
       <c r="Y206" s="25"/>
     </row>
     <row r="207" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13116,7 +13090,7 @@
       <c r="K207" s="197"/>
       <c r="L207" s="197"/>
       <c r="M207" s="23"/>
-      <c r="O207" s="71"/>
+      <c r="O207" s="296"/>
       <c r="P207" s="15" t="s">
         <v>190</v>
       </c>
@@ -13125,7 +13099,7 @@
       <c r="S207" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="T207" s="142"/>
+      <c r="T207" s="297"/>
       <c r="U207" s="20"/>
       <c r="V207" s="20"/>
       <c r="W207" s="20"/>
@@ -13150,7 +13124,7 @@
       <c r="K208" s="195"/>
       <c r="L208" s="195"/>
       <c r="M208" s="23"/>
-      <c r="O208" s="71"/>
+      <c r="O208" s="296"/>
       <c r="P208" s="15" t="s">
         <v>193</v>
       </c>
@@ -13159,7 +13133,7 @@
       <c r="S208" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="T208" s="142"/>
+      <c r="T208" s="297"/>
       <c r="U208" s="20"/>
       <c r="V208" s="20"/>
       <c r="W208" s="20"/>
@@ -13195,7 +13169,7 @@
       <c r="S209" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="T209" s="117" t="str">
+      <c r="T209" s="150" t="str">
         <f>IF(T204="","",AVERAGE(T204:T208))</f>
         <v/>
       </c>
@@ -14907,6 +14881,7 @@
     <mergeCell ref="T70:U70"/>
     <mergeCell ref="Q89:S89"/>
     <mergeCell ref="T89:U89"/>
+    <mergeCell ref="T115:U115"/>
     <mergeCell ref="E168:F168"/>
     <mergeCell ref="G168:H168"/>
     <mergeCell ref="F94:H94"/>
@@ -14915,7 +14890,6 @@
     <mergeCell ref="P137:P139"/>
     <mergeCell ref="O118:P120"/>
     <mergeCell ref="D97:E99"/>
-    <mergeCell ref="T115:U115"/>
   </mergeCells>
   <conditionalFormatting sqref="L33:L38 L41:L45 L60:L63 L47:L57">
     <cfRule type="cellIs" dxfId="36" priority="46" operator="equal">
@@ -15102,9 +15076,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView topLeftCell="A51" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:A82"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15125,17 +15101,17 @@
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="266" t="s">
+      <c r="A4" s="295" t="s">
         <v>289</v>
       </c>
-      <c r="B4" s="266" t="s">
+      <c r="B4" s="295" t="s">
         <v>290</v>
       </c>
-      <c r="C4" s="266"/>
-      <c r="D4" s="266"/>
+      <c r="C4" s="295"/>
+      <c r="D4" s="295"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="266"/>
+      <c r="A5" s="295"/>
       <c r="B5" s="5" t="s">
         <v>291</v>
       </c>
@@ -15307,17 +15283,17 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="266" t="s">
+      <c r="A18" s="295" t="s">
         <v>289</v>
       </c>
-      <c r="B18" s="266" t="s">
+      <c r="B18" s="295" t="s">
         <v>306</v>
       </c>
-      <c r="C18" s="266"/>
-      <c r="D18" s="266"/>
+      <c r="C18" s="295"/>
+      <c r="D18" s="295"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="266"/>
+      <c r="A19" s="295"/>
       <c r="B19" s="5" t="s">
         <v>291</v>
       </c>
@@ -15553,16 +15529,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="266" t="s">
+      <c r="A37" s="295" t="s">
         <v>289</v>
       </c>
-      <c r="B37" s="266" t="s">
+      <c r="B37" s="295" t="s">
         <v>311</v>
       </c>
-      <c r="C37" s="266"/>
+      <c r="C37" s="295"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="266"/>
+      <c r="A38" s="295"/>
       <c r="B38" s="5" t="s">
         <v>292</v>
       </c>
@@ -15648,16 +15624,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="266" t="s">
+      <c r="A47" s="295" t="s">
         <v>289</v>
       </c>
-      <c r="B47" s="266" t="s">
+      <c r="B47" s="295" t="s">
         <v>314</v>
       </c>
-      <c r="C47" s="266"/>
+      <c r="C47" s="295"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="266"/>
+      <c r="A48" s="295"/>
       <c r="B48" s="5" t="s">
         <v>292</v>
       </c>
@@ -15743,16 +15719,16 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="266" t="s">
+      <c r="A57" s="295" t="s">
         <v>289</v>
       </c>
-      <c r="B57" s="266" t="s">
+      <c r="B57" s="295" t="s">
         <v>321</v>
       </c>
-      <c r="C57" s="266"/>
+      <c r="C57" s="295"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="266"/>
+      <c r="A58" s="295"/>
       <c r="B58" s="5" t="s">
         <v>292</v>
       </c>
@@ -15838,16 +15814,16 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="266" t="s">
+      <c r="A67" s="295" t="s">
         <v>289</v>
       </c>
-      <c r="B67" s="266" t="s">
+      <c r="B67" s="295" t="s">
         <v>326</v>
       </c>
-      <c r="C67" s="266"/>
+      <c r="C67" s="295"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="266"/>
+      <c r="A68" s="295"/>
       <c r="B68" s="5" t="s">
         <v>292</v>
       </c>
@@ -15976,14 +15952,76 @@
         <v>2</v>
       </c>
     </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="294" t="s">
+        <v>289</v>
+      </c>
+      <c r="B81" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="294"/>
+      <c r="B82" t="s">
+        <v>292</v>
+      </c>
+      <c r="C82" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>301</v>
+      </c>
+      <c r="B83">
+        <v>18.8</v>
+      </c>
+      <c r="C83">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>294</v>
+      </c>
+      <c r="B84">
+        <v>3.5</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>302</v>
+      </c>
+      <c r="B85">
+        <v>19.8</v>
+      </c>
+      <c r="C85">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>310</v>
+      </c>
+      <c r="B86">
+        <v>25</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:C37"/>
+    <mergeCell ref="A81:A82"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="A57:A58"/>

</xml_diff>

<commit_message>
Update dosimetry pass/fail criteria
Update dosimetry pass/fail criteria to be ACR pass/fail dose limits, rather than ACR reference dose limits
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -471,24 +471,12 @@
     <t>Dose reduction techniques</t>
   </si>
   <si>
-    <t>Routine head protocol CTDI is below ACR reference level of 75 mGy</t>
-  </si>
-  <si>
     <t>Indiated CTDIvol (mGy)</t>
   </si>
   <si>
-    <t>Routine body protocol CTDI is below ACR reference level of 25 mGy</t>
-  </si>
-  <si>
     <t>Adult Chest</t>
   </si>
   <si>
-    <t>Pediatric body protocol CTDI is below ACR reference level of 15 mGy</t>
-  </si>
-  <si>
-    <t>Pediatric head protocol CTDI is below ACR reference level of 35 mGy</t>
-  </si>
-  <si>
     <t>Room Number</t>
   </si>
   <si>
@@ -1090,6 +1078,18 @@
   </si>
   <si>
     <t>Somatom Confidence</t>
+  </si>
+  <si>
+    <t>Routine head protocol CTDI is below ACR Pass/Fail level of 80 mGy</t>
+  </si>
+  <si>
+    <t>Routine body protocol CTDI is below ACR Pass/Fail level of 30 mGy</t>
+  </si>
+  <si>
+    <t>Pediatric body protocol CTDI is below ACR Pass/fail level of 20 mGy</t>
+  </si>
+  <si>
+    <t>Pediatric head protocol CTDI is below ACR Pass/Fail level of 40 mGy</t>
   </si>
 </sst>
 </file>
@@ -3043,6 +3043,12 @@
     <xf numFmtId="168" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3107,12 +3113,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3918,7 +3918,7 @@
       <c r="F1" s="216"/>
       <c r="G1" s="1"/>
       <c r="J1" s="245" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3930,7 +3930,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
       <c r="J2" s="245" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -3955,7 +3955,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="1"/>
       <c r="J4" s="245" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3967,77 +3967,77 @@
       <c r="F5" s="2"/>
       <c r="G5" s="1"/>
       <c r="J5" s="245" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="219" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="276" t="str">
+      <c r="B6" s="278" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="276"/>
+      <c r="C6" s="278"/>
       <c r="D6" s="220" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="276" t="str">
+      <c r="E6" s="278" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="276"/>
+      <c r="F6" s="278"/>
       <c r="G6" s="1"/>
       <c r="J6" s="245" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="219" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="274"/>
-      <c r="C7" s="274"/>
+      <c r="B7" s="276"/>
+      <c r="C7" s="276"/>
       <c r="D7" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="274" t="str">
+      <c r="E7" s="276" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="274"/>
+      <c r="F7" s="276"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="219" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="274"/>
-      <c r="C8" s="274"/>
+      <c r="B8" s="276"/>
+      <c r="C8" s="276"/>
       <c r="D8" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="274" t="str">
+      <c r="E8" s="276" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="274"/>
+      <c r="F8" s="276"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="219" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="274"/>
-      <c r="C9" s="274"/>
+      <c r="B9" s="276"/>
+      <c r="C9" s="276"/>
       <c r="D9" s="220" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="274" t="str">
+      <c r="E9" s="276" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="274"/>
+      <c r="F9" s="276"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4047,19 +4047,19 @@
       <c r="D10" s="220" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="275" t="str">
+      <c r="E10" s="277" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="275"/>
+      <c r="F10" s="277"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="219" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="276"/>
-      <c r="C11" s="276"/>
+      <c r="B11" s="278"/>
+      <c r="C11" s="278"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4082,10 +4082,10 @@
       <c r="A13" s="222" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="276" t="s">
+      <c r="B13" s="278" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="276"/>
+      <c r="C13" s="278"/>
       <c r="D13" s="220" t="s">
         <v>16</v>
       </c>
@@ -4451,7 +4451,7 @@
       <c r="L1" s="13"/>
       <c r="M1" s="14"/>
       <c r="O1" s="16" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
@@ -4482,7 +4482,7 @@
       </c>
       <c r="Y2" s="25"/>
       <c r="AA2" s="26" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4516,7 +4516,7 @@
         <v>44</v>
       </c>
       <c r="AB4" s="29" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4685,19 +4685,19 @@
       <c r="E10" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="289" t="str">
+      <c r="F10" s="291" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="289"/>
+      <c r="G10" s="291"/>
       <c r="J10" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="289" t="str">
+      <c r="K10" s="291" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="289"/>
+      <c r="L10" s="291"/>
       <c r="M10" s="23"/>
       <c r="O10" s="24"/>
       <c r="Q10" s="28" t="s">
@@ -4738,19 +4738,19 @@
       <c r="E11" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="292" t="str">
+      <c r="F11" s="294" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="292"/>
+      <c r="G11" s="294"/>
       <c r="J11" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="289" t="str">
+      <c r="K11" s="291" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="289"/>
+      <c r="L11" s="291"/>
       <c r="M11" s="23"/>
       <c r="O11" s="24"/>
       <c r="Q11" s="28" t="s">
@@ -4791,19 +4791,19 @@
       <c r="E12" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="292" t="str">
+      <c r="F12" s="294" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="292"/>
+      <c r="G12" s="294"/>
       <c r="J12" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="293" t="str">
+      <c r="K12" s="295" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="293"/>
+      <c r="L12" s="295"/>
       <c r="M12" s="23"/>
       <c r="O12" s="24"/>
       <c r="Q12" s="28" t="s">
@@ -4844,19 +4844,19 @@
       <c r="E13" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="292" t="str">
+      <c r="F13" s="294" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="292"/>
+      <c r="G13" s="294"/>
       <c r="J13" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="289" t="str">
+      <c r="K13" s="291" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="289"/>
+      <c r="L13" s="291"/>
       <c r="M13" s="23"/>
       <c r="O13" s="24"/>
       <c r="Q13" s="28" t="s">
@@ -4954,19 +4954,19 @@
       <c r="E16" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="289" t="str">
+      <c r="F16" s="291" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="289"/>
+      <c r="G16" s="291"/>
       <c r="J16" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="293" t="str">
+      <c r="K16" s="295" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="293"/>
+      <c r="L16" s="295"/>
       <c r="M16" s="23"/>
       <c r="O16" s="24"/>
       <c r="P16" s="56" t="s">
@@ -4994,19 +4994,19 @@
       <c r="E17" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="292" t="str">
+      <c r="F17" s="294" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="292"/>
+      <c r="G17" s="294"/>
       <c r="J17" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="289" t="str">
+      <c r="K17" s="291" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="289"/>
+      <c r="L17" s="291"/>
       <c r="M17" s="23"/>
       <c r="O17" s="24"/>
       <c r="Q17" s="28" t="s">
@@ -5047,11 +5047,11 @@
       <c r="J18" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="289" t="str">
+      <c r="K18" s="291" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="289"/>
+      <c r="L18" s="291"/>
       <c r="M18" s="23"/>
       <c r="O18" s="24"/>
       <c r="Q18" s="28" t="s">
@@ -5123,11 +5123,11 @@
       <c r="E20" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="289" t="str">
+      <c r="F20" s="291" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="289"/>
+      <c r="G20" s="291"/>
       <c r="I20" s="59" t="s">
         <v>76</v>
       </c>
@@ -5152,19 +5152,19 @@
       <c r="E21" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="291" t="str">
+      <c r="F21" s="293" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="291"/>
+      <c r="G21" s="293"/>
       <c r="J21" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="289" t="str">
+      <c r="K21" s="291" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="289"/>
+      <c r="L21" s="291"/>
       <c r="M21" s="23"/>
       <c r="O21" s="24"/>
       <c r="Q21" s="28" t="s">
@@ -5203,11 +5203,11 @@
       <c r="J22" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="289" t="str">
+      <c r="K22" s="291" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="289"/>
+      <c r="L22" s="291"/>
       <c r="M22" s="23"/>
       <c r="O22" s="24"/>
       <c r="Q22" s="28" t="s">
@@ -5248,19 +5248,19 @@
       <c r="E23" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="289" t="str">
+      <c r="F23" s="291" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="289"/>
+      <c r="G23" s="291"/>
       <c r="J23" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="289" t="str">
+      <c r="K23" s="291" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="289"/>
+      <c r="L23" s="291"/>
       <c r="M23" s="23"/>
       <c r="O23" s="24"/>
       <c r="P23" s="56" t="s">
@@ -5296,11 +5296,11 @@
       <c r="E24" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="289" t="str">
+      <c r="F24" s="291" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="289"/>
+      <c r="G24" s="291"/>
       <c r="M24" s="23"/>
       <c r="O24" s="24"/>
       <c r="Q24" s="28" t="s">
@@ -5341,11 +5341,11 @@
       <c r="E25" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="289" t="str">
+      <c r="F25" s="291" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="289"/>
+      <c r="G25" s="291"/>
       <c r="J25" s="55" t="s">
         <v>82</v>
       </c>
@@ -5385,11 +5385,11 @@
       <c r="J26" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="289" t="str">
+      <c r="K26" s="291" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="289"/>
+      <c r="L26" s="291"/>
       <c r="M26" s="23"/>
       <c r="O26" s="24"/>
       <c r="Q26" s="28" t="s">
@@ -5417,19 +5417,19 @@
       <c r="E27" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="289" t="str">
+      <c r="F27" s="291" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="289"/>
+      <c r="G27" s="291"/>
       <c r="J27" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="289" t="str">
+      <c r="K27" s="291" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="289"/>
+      <c r="L27" s="291"/>
       <c r="M27" s="23"/>
       <c r="O27" s="24"/>
       <c r="P27" s="56" t="s">
@@ -5456,11 +5456,11 @@
       <c r="E28" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="289" t="str">
+      <c r="F28" s="291" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="289"/>
+      <c r="G28" s="291"/>
       <c r="M28" s="23"/>
       <c r="O28" s="24"/>
       <c r="Q28" s="28" t="s">
@@ -5501,11 +5501,11 @@
       <c r="E29" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="289" t="str">
+      <c r="F29" s="291" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="289"/>
+      <c r="G29" s="291"/>
       <c r="M29" s="23"/>
       <c r="O29" s="24"/>
       <c r="Q29" s="28" t="s">
@@ -5615,10 +5615,10 @@
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
-      <c r="L32" s="290" t="s">
+      <c r="L32" s="292" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="290"/>
+      <c r="M32" s="292"/>
       <c r="AA32" s="28" t="s">
         <v>70</v>
       </c>
@@ -6378,7 +6378,7 @@
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="69" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E55" s="69" t="s">
         <v>133</v>
@@ -6415,7 +6415,7 @@
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="69" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E56" s="69" t="s">
         <v>135</v>
@@ -6452,10 +6452,10 @@
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="69" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E57" s="69" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="L57" s="66" t="str">
         <f t="shared" ref="L57" si="8">IF(O61="","TBD",IF(O61=1,"YES",IF(O61=3,"NA","")))</f>
@@ -6525,7 +6525,7 @@
       </c>
       <c r="Y59" s="25"/>
       <c r="AA59" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB59" s="39"/>
       <c r="AC59" s="40" t="str">
@@ -6544,7 +6544,7 @@
       <c r="B60" s="21"/>
       <c r="C60" s="69"/>
       <c r="E60" s="69" t="s">
-        <v>143</v>
+        <v>346</v>
       </c>
       <c r="L60" s="66" t="str">
         <f>IF(O63="","TBD",IF(O63=1,"YES",IF(O63=3,"NA","")))</f>
@@ -6560,7 +6560,7 @@
       </c>
       <c r="Y60" s="25"/>
       <c r="AA60" s="36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6570,7 +6570,7 @@
       <c r="B61" s="21"/>
       <c r="C61" s="69"/>
       <c r="E61" s="69" t="s">
-        <v>145</v>
+        <v>347</v>
       </c>
       <c r="L61" s="66" t="str">
         <f>IF(O64="","TBD",IF(O64=1,"YES",IF(O64=3,"NA","")))</f>
@@ -6582,7 +6582,7 @@
       </c>
       <c r="O61" s="71"/>
       <c r="P61" s="15" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="Y61" s="25"/>
       <c r="AA61" s="28" t="s">
@@ -6605,7 +6605,7 @@
       <c r="B62" s="21"/>
       <c r="C62" s="69"/>
       <c r="E62" s="69" t="s">
-        <v>147</v>
+        <v>348</v>
       </c>
       <c r="L62" s="66" t="str">
         <f>IF(O65="","TBD",IF(O65=1,"YES",IF(O65=3,"NA","")))</f>
@@ -6639,7 +6639,7 @@
       </c>
       <c r="B63" s="21"/>
       <c r="E63" s="69" t="s">
-        <v>148</v>
+        <v>349</v>
       </c>
       <c r="L63" s="66" t="str">
         <f>IF(O66="","TBD",IF(O66=1,"YES",IF(O66=3,"NA","")))</f>
@@ -6650,11 +6650,11 @@
         <v/>
       </c>
       <c r="O63" s="73">
-        <f>IF(S121="",3,IF(S121&lt;X120,1,2))</f>
+        <f>IF(S121="",3,IF(S121&lt;Y120,1,2))</f>
         <v>3</v>
       </c>
       <c r="P63" s="15" t="s">
-        <v>143</v>
+        <v>346</v>
       </c>
       <c r="Y63" s="25"/>
       <c r="AA63" s="28" t="s">
@@ -6687,11 +6687,11 @@
       <c r="L64" s="31"/>
       <c r="M64" s="32"/>
       <c r="O64" s="73">
-        <f>IF(Q121="",3,IF(Q121&lt;X119,1,2))</f>
+        <f>IF(Q121="",3,IF(Q121&lt;Y119,1,2))</f>
         <v>3</v>
       </c>
       <c r="P64" s="15" t="s">
-        <v>145</v>
+        <v>347</v>
       </c>
       <c r="Y64" s="25"/>
       <c r="AA64" s="28" t="s">
@@ -6726,11 +6726,11 @@
         <v>Eugene Mah</v>
       </c>
       <c r="O65" s="73">
-        <f>IF(T121="",3,IF(T121&lt;X122,1,2))</f>
+        <f>IF(T121="",3,IF(T121&lt;Y122,1,2))</f>
         <v>3</v>
       </c>
       <c r="P65" s="15" t="s">
-        <v>147</v>
+        <v>348</v>
       </c>
       <c r="Y65" s="25"/>
       <c r="AA65" s="28" t="s">
@@ -6751,7 +6751,7 @@
         <v>66</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D66" s="75" t="str">
         <f>IF($R$14="","",$R$14)</f>
@@ -6765,11 +6765,11 @@
         <v/>
       </c>
       <c r="O66" s="73">
-        <f>IF(U121="",3,IF(U121&lt;X123,1,2))</f>
+        <f>IF(U121="",3,IF(U121&lt;Y123,1,2))</f>
         <v>3</v>
       </c>
       <c r="P66" s="15" t="s">
-        <v>148</v>
+        <v>349</v>
       </c>
       <c r="Y66" s="25"/>
       <c r="AA66" s="28" t="s">
@@ -6881,27 +6881,27 @@
       </c>
       <c r="B70" s="21"/>
       <c r="E70" s="69"/>
-      <c r="F70" s="286" t="s">
-        <v>150</v>
-      </c>
-      <c r="G70" s="286"/>
-      <c r="H70" s="286"/>
-      <c r="I70" s="286" t="s">
-        <v>151</v>
-      </c>
-      <c r="J70" s="286"/>
+      <c r="F70" s="288" t="s">
+        <v>146</v>
+      </c>
+      <c r="G70" s="288"/>
+      <c r="H70" s="288"/>
+      <c r="I70" s="288" t="s">
+        <v>147</v>
+      </c>
+      <c r="J70" s="288"/>
       <c r="M70" s="23"/>
       <c r="O70" s="44"/>
       <c r="P70" s="17"/>
-      <c r="Q70" s="287" t="s">
-        <v>150</v>
-      </c>
-      <c r="R70" s="287"/>
-      <c r="S70" s="287"/>
-      <c r="T70" s="287" t="s">
-        <v>151</v>
-      </c>
-      <c r="U70" s="287"/>
+      <c r="Q70" s="289" t="s">
+        <v>146</v>
+      </c>
+      <c r="R70" s="289"/>
+      <c r="S70" s="289"/>
+      <c r="T70" s="289" t="s">
+        <v>147</v>
+      </c>
+      <c r="U70" s="289"/>
       <c r="V70" s="17"/>
       <c r="W70" s="17"/>
       <c r="X70" s="17"/>
@@ -6926,36 +6926,36 @@
       <c r="B71" s="21"/>
       <c r="E71" s="69"/>
       <c r="F71" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M71" s="23"/>
       <c r="O71" s="24"/>
       <c r="Q71" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="R71" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="S71" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="T71" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="U71" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Y71" s="25"/>
       <c r="AA71" s="28" t="s">
@@ -7361,7 +7361,7 @@
       </c>
       <c r="Y77" s="25"/>
       <c r="AA77" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB77" s="39"/>
       <c r="AC77" s="40" t="str">
@@ -7428,7 +7428,7 @@
       </c>
       <c r="Y78" s="25"/>
       <c r="AA78" s="36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="AB78" s="20"/>
       <c r="AC78" s="20"/>
@@ -8043,7 +8043,7 @@
       </c>
       <c r="B88" s="21"/>
       <c r="E88" s="48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F88" s="257" t="str">
         <f t="shared" si="12"/>
@@ -8068,7 +8068,7 @@
       <c r="M88" s="23"/>
       <c r="O88" s="24"/>
       <c r="P88" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q88" s="238" t="str">
         <f t="shared" si="17"/>
@@ -8122,15 +8122,15 @@
       <c r="M89" s="87"/>
       <c r="O89" s="24"/>
       <c r="P89" s="53"/>
-      <c r="Q89" s="288" t="s">
-        <v>150</v>
-      </c>
-      <c r="R89" s="288"/>
-      <c r="S89" s="288"/>
-      <c r="T89" s="288" t="s">
-        <v>151</v>
-      </c>
-      <c r="U89" s="288"/>
+      <c r="Q89" s="290" t="s">
+        <v>146</v>
+      </c>
+      <c r="R89" s="290"/>
+      <c r="S89" s="290"/>
+      <c r="T89" s="290" t="s">
+        <v>147</v>
+      </c>
+      <c r="U89" s="290"/>
       <c r="Y89" s="25"/>
       <c r="AA89" s="28" t="s">
         <v>129</v>
@@ -8151,24 +8151,24 @@
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="88" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="M90" s="23"/>
       <c r="O90" s="24"/>
       <c r="Q90" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="R90" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="S90" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="T90" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="U90" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Y90" s="25"/>
       <c r="AA90" s="28" t="s">
@@ -8190,14 +8190,14 @@
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="48" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D91" s="165" t="str">
         <f>IF(P112="","",P112)</f>
         <v>Piranha</v>
       </c>
       <c r="G91" s="264" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="H91" s="273" t="str">
         <f>IF(S112="","",S112)</f>
@@ -8233,14 +8233,14 @@
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="48" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D92" s="272" t="str">
         <f>IF(P113="","",P113)</f>
         <v/>
       </c>
       <c r="G92" s="264" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="H92" s="273" t="str">
         <f>IF(S113="","",S113)</f>
@@ -8317,15 +8317,15 @@
       </c>
       <c r="B94" s="21"/>
       <c r="E94" s="69"/>
-      <c r="F94" s="279" t="s">
-        <v>150</v>
-      </c>
-      <c r="G94" s="279"/>
-      <c r="H94" s="279"/>
-      <c r="I94" s="280" t="s">
-        <v>151</v>
-      </c>
-      <c r="J94" s="280"/>
+      <c r="F94" s="281" t="s">
+        <v>146</v>
+      </c>
+      <c r="G94" s="281"/>
+      <c r="H94" s="281"/>
+      <c r="I94" s="282" t="s">
+        <v>147</v>
+      </c>
+      <c r="J94" s="282"/>
       <c r="M94" s="23"/>
       <c r="O94" s="24"/>
       <c r="P94" s="28" t="s">
@@ -8357,22 +8357,22 @@
       <c r="B95" s="21"/>
       <c r="E95" s="69"/>
       <c r="F95" s="89" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G95" s="90" t="s">
+        <v>149</v>
+      </c>
+      <c r="H95" s="91" t="s">
+        <v>150</v>
+      </c>
+      <c r="I95" s="90" t="s">
+        <v>148</v>
+      </c>
+      <c r="J95" s="91" t="s">
+        <v>150</v>
+      </c>
+      <c r="K95" s="56" t="s">
         <v>153</v>
-      </c>
-      <c r="H95" s="91" t="s">
-        <v>154</v>
-      </c>
-      <c r="I95" s="90" t="s">
-        <v>152</v>
-      </c>
-      <c r="J95" s="91" t="s">
-        <v>154</v>
-      </c>
-      <c r="K95" s="56" t="s">
-        <v>157</v>
       </c>
       <c r="M95" s="23"/>
       <c r="O95" s="24"/>
@@ -8386,7 +8386,7 @@
       <c r="U95" s="240"/>
       <c r="Y95" s="25"/>
       <c r="AA95" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB95" s="39"/>
       <c r="AC95" s="40" t="str">
@@ -8405,7 +8405,7 @@
       <c r="B96" s="21"/>
       <c r="D96" s="53"/>
       <c r="E96" s="48" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F96" s="92" t="str">
         <f>IF(F88="","",F88)</f>
@@ -8428,7 +8428,7 @@
         <v/>
       </c>
       <c r="K96" s="15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="M96" s="23"/>
       <c r="O96" s="24"/>
@@ -8442,7 +8442,7 @@
       <c r="U96" s="240"/>
       <c r="Y96" s="25"/>
       <c r="AA96" s="36" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -8450,10 +8450,10 @@
         <v>31</v>
       </c>
       <c r="B97" s="21"/>
-      <c r="D97" s="284" t="s">
-        <v>160</v>
-      </c>
-      <c r="E97" s="285"/>
+      <c r="D97" s="286" t="s">
+        <v>156</v>
+      </c>
+      <c r="E97" s="287"/>
       <c r="F97" s="95" t="str">
         <f t="shared" ref="F97:J102" si="24">IF(Q118="","",Q118)</f>
         <v/>
@@ -8476,7 +8476,7 @@
       </c>
       <c r="K97" s="20"/>
       <c r="L97" s="98" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M97" s="99" t="s">
         <v>19</v>
@@ -8509,8 +8509,8 @@
         <v>32</v>
       </c>
       <c r="B98" s="21"/>
-      <c r="D98" s="284"/>
-      <c r="E98" s="285"/>
+      <c r="D98" s="286"/>
+      <c r="E98" s="287"/>
       <c r="F98" s="100" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -8533,10 +8533,10 @@
       </c>
       <c r="K98" s="20"/>
       <c r="L98" s="103" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="M98" s="104" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O98" s="24"/>
       <c r="P98" s="28" t="s">
@@ -8566,8 +8566,8 @@
         <v>33</v>
       </c>
       <c r="B99" s="21"/>
-      <c r="D99" s="284"/>
-      <c r="E99" s="285"/>
+      <c r="D99" s="286"/>
+      <c r="E99" s="287"/>
       <c r="F99" s="105" t="str">
         <f t="shared" si="24"/>
         <v/>
@@ -8627,7 +8627,7 @@
       <c r="B100" s="21"/>
       <c r="D100" s="53"/>
       <c r="E100" s="48" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F100" s="111" t="str">
         <f t="shared" si="24"/>
@@ -8650,7 +8650,7 @@
         <v/>
       </c>
       <c r="K100" s="116" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L100" s="117">
         <v>75</v>
@@ -8688,7 +8688,7 @@
       <c r="B101" s="21"/>
       <c r="D101" s="53"/>
       <c r="E101" s="48" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F101" s="77" t="str">
         <f t="shared" si="24"/>
@@ -8711,7 +8711,7 @@
         <v/>
       </c>
       <c r="K101" s="116" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L101" s="117">
         <v>15</v>
@@ -8748,7 +8748,7 @@
       </c>
       <c r="B102" s="21"/>
       <c r="E102" s="48" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F102" s="83" t="str">
         <f t="shared" si="24"/>
@@ -8771,7 +8771,7 @@
         <v/>
       </c>
       <c r="K102" s="116" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="L102" s="117">
         <v>7.5</v>
@@ -8814,7 +8814,7 @@
       </c>
       <c r="B103" s="21"/>
       <c r="E103" s="48" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F103" s="119" t="str">
         <f t="shared" ref="F103:J106" si="27">IF(Q125="","",Q125)</f>
@@ -8837,7 +8837,7 @@
         <v/>
       </c>
       <c r="K103" s="122" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L103" s="123">
         <v>35</v>
@@ -8874,7 +8874,7 @@
       </c>
       <c r="B104" s="21"/>
       <c r="E104" s="48" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F104" s="125" t="str">
         <f t="shared" si="27"/>
@@ -8928,7 +8928,7 @@
       <c r="C105" s="20"/>
       <c r="D105" s="20"/>
       <c r="E105" s="48" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F105" s="92" t="str">
         <f t="shared" si="27"/>
@@ -8982,7 +8982,7 @@
       <c r="C106" s="20"/>
       <c r="D106" s="20"/>
       <c r="E106" s="48" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F106" s="128" t="str">
         <f t="shared" si="27"/>
@@ -9050,7 +9050,7 @@
       <c r="M107" s="23"/>
       <c r="O107" s="24"/>
       <c r="P107" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q107" s="240"/>
       <c r="R107" s="240"/>
@@ -9138,7 +9138,7 @@
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="131" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J110" s="20"/>
       <c r="M110" s="23"/>
@@ -9164,7 +9164,7 @@
       </c>
       <c r="B111" s="21"/>
       <c r="D111" s="48" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E111" s="77" t="str">
         <f t="shared" ref="E111:H114" si="28">IF(Q133="","",Q133)</f>
@@ -9185,7 +9185,7 @@
       <c r="J111" s="20"/>
       <c r="M111" s="23"/>
       <c r="O111" s="132" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="P111" s="17"/>
       <c r="Q111" s="17"/>
@@ -9216,7 +9216,7 @@
       </c>
       <c r="B112" s="21"/>
       <c r="D112" s="48" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E112" s="80" t="str">
         <f t="shared" si="28"/>
@@ -9237,13 +9237,13 @@
       <c r="J112" s="20"/>
       <c r="M112" s="23"/>
       <c r="O112" s="266" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="P112" s="267" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="R112" s="265" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="S112" s="270"/>
       <c r="T112" s="269"/>
@@ -9267,7 +9267,7 @@
       </c>
       <c r="B113" s="21"/>
       <c r="D113" s="48" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E113" s="80" t="str">
         <f t="shared" si="28"/>
@@ -9288,17 +9288,17 @@
       <c r="J113" s="20"/>
       <c r="M113" s="23"/>
       <c r="O113" s="266" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="P113" s="268"/>
       <c r="R113" s="265" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="S113" s="271"/>
       <c r="T113" s="269"/>
       <c r="Y113" s="25"/>
       <c r="AA113" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB113" s="39"/>
       <c r="AC113" s="40" t="str">
@@ -9316,7 +9316,7 @@
       </c>
       <c r="B114" s="21"/>
       <c r="D114" s="48" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E114" s="80" t="str">
         <f t="shared" si="28"/>
@@ -9339,7 +9339,7 @@
       <c r="O114" s="24"/>
       <c r="Y114" s="25"/>
       <c r="AA114" s="36" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="115" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -9348,7 +9348,7 @@
       </c>
       <c r="B115" s="21"/>
       <c r="D115" s="48" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E115" s="242" t="str">
         <f>IF(Q140="","",Q140)</f>
@@ -9369,17 +9369,17 @@
       <c r="J115" s="20"/>
       <c r="M115" s="23"/>
       <c r="O115" s="24"/>
-      <c r="Q115" s="281" t="s">
-        <v>150</v>
-      </c>
-      <c r="R115" s="281"/>
-      <c r="S115" s="281"/>
-      <c r="T115" s="277" t="s">
-        <v>151</v>
-      </c>
-      <c r="U115" s="277"/>
+      <c r="Q115" s="283" t="s">
+        <v>146</v>
+      </c>
+      <c r="R115" s="283"/>
+      <c r="S115" s="283"/>
+      <c r="T115" s="279" t="s">
+        <v>147</v>
+      </c>
+      <c r="U115" s="279"/>
       <c r="W115" s="56" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="Y115" s="25"/>
       <c r="AA115" s="28" t="s">
@@ -9409,22 +9409,22 @@
       <c r="M116" s="23"/>
       <c r="O116" s="24"/>
       <c r="Q116" s="103" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="R116" s="133" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="S116" s="134" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="T116" s="133" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="U116" s="134" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="W116" s="15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="Y116" s="25"/>
       <c r="AA116" s="28" t="s">
@@ -9446,7 +9446,7 @@
       </c>
       <c r="B117" s="21"/>
       <c r="D117" s="48" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E117" s="92" t="str">
         <f>IF(Q141="","",Q141)</f>
@@ -9468,7 +9468,7 @@
       <c r="M117" s="23"/>
       <c r="O117" s="24"/>
       <c r="P117" s="28" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="Q117" s="135" t="str">
         <f>IF(Q88="","",Q88)</f>
@@ -9492,7 +9492,7 @@
       </c>
       <c r="W117" s="20"/>
       <c r="X117" s="98" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Y117" s="7" t="s">
         <v>19</v>
@@ -9516,7 +9516,7 @@
       </c>
       <c r="B118" s="21"/>
       <c r="E118" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F118" s="15" t="str">
         <f>V134</f>
@@ -9525,10 +9525,10 @@
       <c r="I118" s="20"/>
       <c r="J118" s="20"/>
       <c r="M118" s="23"/>
-      <c r="O118" s="283" t="s">
-        <v>160</v>
-      </c>
-      <c r="P118" s="282"/>
+      <c r="O118" s="285" t="s">
+        <v>156</v>
+      </c>
+      <c r="P118" s="284"/>
       <c r="Q118" s="138"/>
       <c r="R118" s="139"/>
       <c r="S118" s="140"/>
@@ -9536,10 +9536,10 @@
       <c r="U118" s="140"/>
       <c r="W118" s="20"/>
       <c r="X118" s="103" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="Y118" s="134" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="AA118" s="28" t="s">
         <v>112</v>
@@ -9566,8 +9566,8 @@
       <c r="I119" s="20"/>
       <c r="J119" s="20"/>
       <c r="M119" s="23"/>
-      <c r="O119" s="283"/>
-      <c r="P119" s="282"/>
+      <c r="O119" s="285"/>
+      <c r="P119" s="284"/>
       <c r="Q119" s="141"/>
       <c r="R119" s="142"/>
       <c r="S119" s="143"/>
@@ -9601,15 +9601,15 @@
       </c>
       <c r="B120" s="21"/>
       <c r="M120" s="23"/>
-      <c r="O120" s="283"/>
-      <c r="P120" s="282"/>
+      <c r="O120" s="285"/>
+      <c r="P120" s="284"/>
       <c r="Q120" s="145"/>
       <c r="R120" s="146"/>
       <c r="S120" s="147"/>
       <c r="T120" s="146"/>
       <c r="U120" s="147"/>
       <c r="W120" s="116" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="X120" s="117">
         <v>75</v>
@@ -9641,7 +9641,7 @@
       <c r="M121" s="23"/>
       <c r="O121" s="24"/>
       <c r="P121" s="28" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="Q121" s="149" t="str">
         <f>IF(OR(Q118="",Q119="",Q120=""),"",AVERAGE(Q118:Q120))</f>
@@ -9664,7 +9664,7 @@
         <v/>
       </c>
       <c r="W121" s="116" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="X121" s="117">
         <v>15</v>
@@ -9701,7 +9701,7 @@
       <c r="M122" s="23"/>
       <c r="O122" s="24"/>
       <c r="P122" s="28" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="Q122" s="138"/>
       <c r="R122" s="139"/>
@@ -9709,7 +9709,7 @@
       <c r="T122" s="139"/>
       <c r="U122" s="140"/>
       <c r="W122" s="116" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="X122" s="117">
         <v>7.5</v>
@@ -9738,7 +9738,7 @@
       <c r="M123" s="23"/>
       <c r="O123" s="24"/>
       <c r="P123" s="28" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Q123" s="145"/>
       <c r="R123" s="146"/>
@@ -9746,7 +9746,7 @@
       <c r="T123" s="146"/>
       <c r="U123" s="147"/>
       <c r="W123" s="122" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="X123" s="123">
         <v>35</v>
@@ -9773,12 +9773,12 @@
       </c>
       <c r="B124" s="21"/>
       <c r="C124" s="164" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="M124" s="23"/>
       <c r="O124" s="24"/>
       <c r="P124" s="28" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="Q124" s="153" t="str">
         <f>IF(AB133="","",AB133)</f>
@@ -9824,21 +9824,21 @@
         <v/>
       </c>
       <c r="D125" s="69" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F125" s="165" t="str">
         <f>IF(O207="","",O207)</f>
         <v/>
       </c>
       <c r="G125" s="166" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I125" s="20"/>
       <c r="J125" s="20"/>
       <c r="M125" s="23"/>
       <c r="O125" s="157"/>
       <c r="P125" s="28" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Q125" s="158" t="str">
         <f>IF(OR(Q124="",Q121=""),"",ABS(Q121-Q124)/Q124)</f>
@@ -9887,7 +9887,7 @@
         <v/>
       </c>
       <c r="D126" s="69" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E126" s="53"/>
       <c r="F126" s="165" t="str">
@@ -9895,7 +9895,7 @@
         <v/>
       </c>
       <c r="G126" s="166" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H126" s="53"/>
       <c r="I126" s="20"/>
@@ -9903,7 +9903,7 @@
       <c r="M126" s="23"/>
       <c r="O126" s="157"/>
       <c r="P126" s="28" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="Q126" s="161" t="str">
         <f>IF(OR(Q117="",Q121=""),"",ABS(Q121-Q117)/Q117)</f>
@@ -9952,19 +9952,19 @@
         <v/>
       </c>
       <c r="D127" s="69" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F127" s="167" t="str">
         <f>IF(T211="","",T211)</f>
         <v/>
       </c>
       <c r="G127" s="166" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M127" s="23"/>
       <c r="O127" s="24"/>
       <c r="P127" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q127" s="135" t="str">
         <f>IF(Q121="","",IF(AND(Q121&lt;=Y119,Q125&lt;=0.05,Q126&lt;=0.2),"Pass","Fail"))</f>
@@ -10010,7 +10010,7 @@
       <c r="M128" s="23"/>
       <c r="O128" s="24"/>
       <c r="P128" s="28" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="Q128" s="150" t="str">
         <f>IF(OR(Q121="",Q75=""),"",Q121/(Q75/100))</f>
@@ -10058,7 +10058,7 @@
       <c r="M129" s="23"/>
       <c r="O129" s="24"/>
       <c r="P129" s="28" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="Q129" s="154" t="str">
         <f>IF(AB139="","",AB139)</f>
@@ -10115,10 +10115,10 @@
       <c r="M130" s="32"/>
       <c r="O130" s="24"/>
       <c r="P130" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="Q130" s="20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="R130" s="20"/>
       <c r="S130" s="20"/>
@@ -10162,7 +10162,7 @@
       <c r="O131" s="24"/>
       <c r="P131" s="20"/>
       <c r="Q131" s="20" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="R131" s="20"/>
       <c r="S131" s="20"/>
@@ -10173,7 +10173,7 @@
       <c r="X131" s="20"/>
       <c r="Y131" s="25"/>
       <c r="AA131" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB131" s="39"/>
       <c r="AC131" s="40" t="str">
@@ -10190,7 +10190,7 @@
         <v>66</v>
       </c>
       <c r="C132" s="28" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D132" s="75" t="str">
         <f>IF($R$14="","",$R$14)</f>
@@ -10204,11 +10204,11 @@
         <v/>
       </c>
       <c r="O132" s="168" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="Y132" s="25"/>
       <c r="AA132" s="36" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="133" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10221,7 +10221,7 @@
       </c>
       <c r="O133" s="24"/>
       <c r="P133" s="28" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="Q133" s="169"/>
       <c r="R133" s="170"/>
@@ -10254,21 +10254,21 @@
       </c>
       <c r="O134" s="24"/>
       <c r="P134" s="28" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="Q134" s="172"/>
       <c r="R134" s="173"/>
       <c r="S134" s="173"/>
       <c r="T134" s="174"/>
       <c r="U134" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="V134" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="Y134" s="25"/>
       <c r="AA134" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AB134" s="39"/>
       <c r="AC134" s="40" t="str">
@@ -10286,7 +10286,7 @@
       </c>
       <c r="B135" s="12"/>
       <c r="C135" s="178" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
@@ -10300,7 +10300,7 @@
       <c r="M135" s="14"/>
       <c r="O135" s="24"/>
       <c r="P135" s="28" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="Q135" s="172"/>
       <c r="R135" s="173"/>
@@ -10308,7 +10308,7 @@
       <c r="T135" s="174"/>
       <c r="Y135" s="25"/>
       <c r="AA135" s="28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="AB135" s="39"/>
       <c r="AC135" s="40" t="str">
@@ -10327,30 +10327,30 @@
       <c r="B136" s="21"/>
       <c r="C136" s="53"/>
       <c r="D136" s="48" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E136" s="165">
         <f>IF(Q149="","",Q149)</f>
         <v>0</v>
       </c>
       <c r="F136" s="69" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G136" s="20"/>
       <c r="H136" s="48" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I136" s="165">
         <f>IF(T149="","",T149)</f>
         <v>1</v>
       </c>
       <c r="J136" s="69" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M136" s="23"/>
       <c r="O136" s="24"/>
       <c r="P136" s="28" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="Q136" s="175"/>
       <c r="R136" s="176"/>
@@ -10358,7 +10358,7 @@
       <c r="T136" s="177"/>
       <c r="Y136" s="25"/>
       <c r="AA136" s="28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AB136" s="39"/>
       <c r="AC136" s="40" t="str">
@@ -10378,8 +10378,8 @@
       <c r="C137" s="53"/>
       <c r="M137" s="23"/>
       <c r="O137" s="24"/>
-      <c r="P137" s="282" t="s">
-        <v>180</v>
+      <c r="P137" s="284" t="s">
+        <v>176</v>
       </c>
       <c r="Q137" s="172"/>
       <c r="R137" s="173"/>
@@ -10387,7 +10387,7 @@
       <c r="T137" s="174"/>
       <c r="Y137" s="25"/>
       <c r="AA137" s="28" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AB137" s="39"/>
       <c r="AC137" s="40" t="str">
@@ -10408,13 +10408,13 @@
       <c r="D138" s="20"/>
       <c r="E138" s="69"/>
       <c r="F138" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G138" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K138" s="48" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L138" s="165" t="str">
         <f>IF(V152="","",IF(V152=1,"Pass","Fail"))</f>
@@ -10422,14 +10422,14 @@
       </c>
       <c r="M138" s="23"/>
       <c r="O138" s="24"/>
-      <c r="P138" s="282"/>
+      <c r="P138" s="284"/>
       <c r="Q138" s="172"/>
       <c r="R138" s="173"/>
       <c r="S138" s="173"/>
       <c r="T138" s="174"/>
       <c r="Y138" s="25"/>
       <c r="AA138" s="36" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AB138" s="20"/>
       <c r="AC138" s="20"/>
@@ -10443,7 +10443,7 @@
       <c r="C139" s="53"/>
       <c r="D139" s="20"/>
       <c r="E139" s="48" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F139" s="81" t="str">
         <f>IF(Q152="","",Q152)</f>
@@ -10454,11 +10454,11 @@
         <v/>
       </c>
       <c r="H139" s="20" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J139" s="20"/>
       <c r="K139" s="48" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="L139" s="212" t="str">
         <f>IF(V153="","",IF(V153=1,"Pass","Fail"))</f>
@@ -10466,7 +10466,7 @@
       </c>
       <c r="M139" s="23"/>
       <c r="O139" s="24"/>
-      <c r="P139" s="282"/>
+      <c r="P139" s="284"/>
       <c r="Q139" s="175"/>
       <c r="R139" s="176"/>
       <c r="S139" s="176"/>
@@ -10489,7 +10489,7 @@
       <c r="C140" s="53"/>
       <c r="D140" s="20"/>
       <c r="E140" s="48" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F140" s="81" t="str">
         <f>IF(Q153="","",IF(Q153=1,"YES","NO"))</f>
@@ -10502,7 +10502,7 @@
       <c r="H140" s="20"/>
       <c r="J140" s="20"/>
       <c r="K140" s="48" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L140" s="212" t="str">
         <f>IF(V154="","",IF(V154=1,"Pass","Fail"))</f>
@@ -10511,7 +10511,7 @@
       <c r="M140" s="23"/>
       <c r="O140" s="24"/>
       <c r="P140" s="28" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="Q140" s="179" t="str">
         <f>IF(OR(Q139="",Q138="",Q137=""),"",AVERAGE(Q137:Q139))</f>
@@ -10531,7 +10531,7 @@
       </c>
       <c r="Y140" s="25"/>
       <c r="AA140" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AB140" s="39"/>
       <c r="AD140" s="47" t="str">
@@ -10551,7 +10551,7 @@
       <c r="H141" s="20"/>
       <c r="J141" s="20"/>
       <c r="K141" s="48" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L141" s="212" t="str">
         <f>IF(V155="","",IF(V155=1,"Pass","Fail"))</f>
@@ -10560,7 +10560,7 @@
       <c r="M141" s="23"/>
       <c r="O141" s="24"/>
       <c r="P141" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q141" s="135" t="str">
         <f>IF(Q140="","",IF(OR(ABS(Q136-Q140)&lt;=3,ABS(AVERAGE(Q137:Q139)-Q136)/Q136&lt;0.3),"Pass","Fail"))</f>
@@ -10580,7 +10580,7 @@
       </c>
       <c r="Y141" s="25"/>
       <c r="AA141" s="28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="AB141" s="39"/>
       <c r="AC141" s="20"/>
@@ -10608,7 +10608,7 @@
       <c r="X142" s="20"/>
       <c r="Y142" s="25"/>
       <c r="AA142" s="28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AB142" s="39"/>
       <c r="AC142" s="20"/>
@@ -10640,7 +10640,7 @@
       <c r="X143" s="20"/>
       <c r="Y143" s="25"/>
       <c r="AA143" s="28" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AB143" s="39"/>
       <c r="AC143" s="20"/>
@@ -10682,7 +10682,7 @@
       <c r="M144" s="23"/>
       <c r="O144" s="71"/>
       <c r="P144" s="20" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="Q144" s="20"/>
       <c r="R144" s="20"/>
@@ -10748,7 +10748,7 @@
       <c r="X145" s="34"/>
       <c r="Y145" s="35"/>
       <c r="AA145" s="36" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="AB145" s="182"/>
       <c r="AC145" s="40" t="str">
@@ -10767,7 +10767,7 @@
       <c r="B146" s="21"/>
       <c r="C146" s="53"/>
       <c r="D146" s="48" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E146" s="80" t="str">
         <f t="shared" si="32"/>
@@ -10810,7 +10810,7 @@
       <c r="B147" s="21"/>
       <c r="C147" s="53"/>
       <c r="D147" s="48" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E147" s="80" t="str">
         <f t="shared" si="32"/>
@@ -10862,7 +10862,7 @@
       <c r="B148" s="21"/>
       <c r="C148" s="53"/>
       <c r="D148" s="48" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E148" s="80" t="str">
         <f t="shared" si="32"/>
@@ -10894,7 +10894,7 @@
       </c>
       <c r="M148" s="23"/>
       <c r="O148" s="132" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="P148" s="17"/>
       <c r="Q148" s="17"/>
@@ -10918,7 +10918,7 @@
       <c r="B149" s="21"/>
       <c r="C149" s="53"/>
       <c r="D149" s="48" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E149" s="80" t="str">
         <f t="shared" si="32"/>
@@ -10951,22 +10951,22 @@
       <c r="M149" s="23"/>
       <c r="O149" s="24"/>
       <c r="P149" s="28" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="Q149" s="183">
         <v>0</v>
       </c>
       <c r="R149" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="S149" s="28" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="T149" s="183">
         <v>1</v>
       </c>
       <c r="U149" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Y149" s="25"/>
       <c r="AA149" s="28"/>
@@ -10987,7 +10987,7 @@
       <c r="B150" s="21"/>
       <c r="C150" s="53"/>
       <c r="D150" s="48" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E150" s="80" t="str">
         <f t="shared" si="32"/>
@@ -11031,7 +11031,7 @@
       <c r="B151" s="21"/>
       <c r="C151" s="53"/>
       <c r="D151" s="48" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E151" s="83" t="str">
         <f t="shared" si="32"/>
@@ -11064,14 +11064,14 @@
       <c r="M151" s="23"/>
       <c r="O151" s="24"/>
       <c r="Q151" s="262" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="R151" s="262" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="U151" s="20"/>
       <c r="V151" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="Y151" s="25"/>
       <c r="AA151" s="28"/>
@@ -11092,7 +11092,7 @@
       <c r="B152" s="21"/>
       <c r="C152" s="53"/>
       <c r="G152" s="48" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H152" s="185" t="str">
         <f>IF(S165="","",IF(S165=1,"Pass","Fail"))</f>
@@ -11101,16 +11101,16 @@
       <c r="M152" s="23"/>
       <c r="O152" s="24"/>
       <c r="P152" s="28" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="Q152" s="142"/>
       <c r="R152" s="142"/>
       <c r="S152" s="29" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="T152" s="20"/>
       <c r="U152" s="28" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="V152" s="183"/>
       <c r="Y152" s="25"/>
@@ -11125,7 +11125,7 @@
       <c r="B153" s="21"/>
       <c r="C153" s="53"/>
       <c r="E153" s="36" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F153" s="15" t="str">
         <f>Q166</f>
@@ -11135,14 +11135,14 @@
       <c r="M153" s="23"/>
       <c r="O153" s="24"/>
       <c r="P153" s="28" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q153" s="142"/>
       <c r="R153" s="142"/>
       <c r="S153" s="28"/>
       <c r="T153" s="20"/>
       <c r="U153" s="28" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="V153" s="183"/>
       <c r="Y153" s="25"/>
@@ -11174,7 +11174,7 @@
       <c r="Q154" s="20"/>
       <c r="T154" s="20"/>
       <c r="U154" s="28" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="V154" s="183"/>
       <c r="Y154" s="25"/>
@@ -11192,7 +11192,7 @@
       <c r="O155" s="24"/>
       <c r="T155" s="20"/>
       <c r="U155" s="28" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="V155" s="183"/>
       <c r="Y155" s="25"/>
@@ -11213,7 +11213,7 @@
       </c>
       <c r="B156" s="21"/>
       <c r="C156" s="164" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="M156" s="23"/>
       <c r="O156" s="168" t="s">
@@ -11231,7 +11231,7 @@
       <c r="B157" s="21"/>
       <c r="C157" s="53"/>
       <c r="E157" s="48" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F157" s="77" t="str">
         <f t="shared" ref="F157:J163" si="33">IF(Q170="","",Q170)</f>
@@ -11280,7 +11280,7 @@
       </c>
       <c r="W157" s="187"/>
       <c r="X157" s="261" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="Y157" s="261"/>
       <c r="AA157" s="28"/>
@@ -11301,7 +11301,7 @@
       <c r="B158" s="21"/>
       <c r="C158" s="53"/>
       <c r="E158" s="48" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F158" s="80" t="str">
         <f t="shared" si="33"/>
@@ -11336,10 +11336,10 @@
       <c r="V158" s="142"/>
       <c r="W158" s="187"/>
       <c r="X158" s="262" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="Y158" s="261" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="AA158" s="28"/>
       <c r="AB158" s="184"/>
@@ -11352,7 +11352,7 @@
       <c r="B159" s="21"/>
       <c r="C159" s="53"/>
       <c r="E159" s="48" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F159" s="80" t="str">
         <f t="shared" si="33"/>
@@ -11376,7 +11376,7 @@
       </c>
       <c r="M159" s="23"/>
       <c r="O159" s="186" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P159" s="142"/>
       <c r="Q159" s="142"/>
@@ -11386,7 +11386,7 @@
       <c r="U159" s="142"/>
       <c r="V159" s="142"/>
       <c r="W159" s="188" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="X159" s="117">
         <v>-107</v>
@@ -11412,7 +11412,7 @@
       <c r="B160" s="21"/>
       <c r="C160" s="53"/>
       <c r="E160" s="48" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F160" s="80" t="str">
         <f t="shared" si="33"/>
@@ -11436,7 +11436,7 @@
       </c>
       <c r="M160" s="23"/>
       <c r="O160" s="186" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="P160" s="142"/>
       <c r="Q160" s="142"/>
@@ -11446,7 +11446,7 @@
       <c r="U160" s="142"/>
       <c r="V160" s="142"/>
       <c r="W160" s="188" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="X160" s="117">
         <v>-7</v>
@@ -11465,7 +11465,7 @@
       <c r="B161" s="21"/>
       <c r="C161" s="53"/>
       <c r="E161" s="48" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F161" s="80" t="str">
         <f t="shared" si="33"/>
@@ -11489,7 +11489,7 @@
       </c>
       <c r="M161" s="23"/>
       <c r="O161" s="186" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="P161" s="142"/>
       <c r="Q161" s="142"/>
@@ -11499,7 +11499,7 @@
       <c r="U161" s="142"/>
       <c r="V161" s="142"/>
       <c r="W161" s="188" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="X161" s="117">
         <v>110</v>
@@ -11525,7 +11525,7 @@
       <c r="B162" s="21"/>
       <c r="C162" s="53"/>
       <c r="E162" s="48" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F162" s="83" t="str">
         <f t="shared" si="33"/>
@@ -11549,7 +11549,7 @@
       </c>
       <c r="M162" s="23"/>
       <c r="O162" s="186" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P162" s="142"/>
       <c r="Q162" s="142"/>
@@ -11559,7 +11559,7 @@
       <c r="U162" s="142"/>
       <c r="V162" s="142"/>
       <c r="W162" s="188" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="X162" s="117">
         <v>850</v>
@@ -11578,7 +11578,7 @@
       <c r="B163" s="21"/>
       <c r="C163" s="53"/>
       <c r="E163" s="48" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F163" s="92" t="str">
         <f t="shared" si="33"/>
@@ -11602,7 +11602,7 @@
       </c>
       <c r="M163" s="23"/>
       <c r="O163" s="186" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P163" s="142"/>
       <c r="Q163" s="142"/>
@@ -11612,7 +11612,7 @@
       <c r="U163" s="142"/>
       <c r="V163" s="142"/>
       <c r="W163" s="188" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="X163" s="117">
         <v>-1005</v>
@@ -11638,7 +11638,7 @@
       <c r="B164" s="21"/>
       <c r="C164" s="53"/>
       <c r="F164" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G164" s="15" t="str">
         <f>R177</f>
@@ -11646,7 +11646,7 @@
       </c>
       <c r="M164" s="23"/>
       <c r="O164" s="186" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="P164" s="142"/>
       <c r="Q164" s="142"/>
@@ -11674,11 +11674,11 @@
       <c r="M165" s="23"/>
       <c r="O165" s="24"/>
       <c r="R165" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="S165" s="189"/>
       <c r="T165" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="Y165" s="25"/>
       <c r="AA165" s="28"/>
@@ -11701,10 +11701,10 @@
       <c r="M166" s="23"/>
       <c r="O166" s="24"/>
       <c r="P166" s="36" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="Q166" s="15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Y166" s="25"/>
       <c r="AA166" s="28"/>
@@ -11717,12 +11717,12 @@
       </c>
       <c r="B167" s="21"/>
       <c r="C167" s="164" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M167" s="23"/>
       <c r="O167" s="24"/>
       <c r="Q167" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="Y167" s="25"/>
       <c r="AA167" s="28"/>
@@ -11743,14 +11743,14 @@
       <c r="B168" s="21"/>
       <c r="C168" s="53"/>
       <c r="D168" s="69"/>
-      <c r="E168" s="278" t="s">
-        <v>150</v>
-      </c>
-      <c r="F168" s="278"/>
-      <c r="G168" s="278" t="s">
-        <v>151</v>
-      </c>
-      <c r="H168" s="278"/>
+      <c r="E168" s="280" t="s">
+        <v>146</v>
+      </c>
+      <c r="F168" s="280"/>
+      <c r="G168" s="280" t="s">
+        <v>147</v>
+      </c>
+      <c r="H168" s="280"/>
       <c r="M168" s="23"/>
       <c r="O168" s="24"/>
       <c r="Y168" s="25"/>
@@ -11766,20 +11766,20 @@
       <c r="C169" s="53"/>
       <c r="D169" s="69"/>
       <c r="E169" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G169" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H169" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M169" s="23"/>
       <c r="O169" s="168" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="Y169" s="25"/>
       <c r="AA169" s="28"/>
@@ -11800,7 +11800,7 @@
       <c r="B170" s="21"/>
       <c r="C170" s="53"/>
       <c r="D170" s="48" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E170" s="77" t="str">
         <f t="shared" ref="E170:H174" si="34">IF(P183="","",P183)</f>
@@ -11819,7 +11819,7 @@
         <v/>
       </c>
       <c r="J170" s="48" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="K170" s="185" t="str">
         <f>IF(V183="","",IF(V183=3,"NA",IF(V183=1,"Pass","Fail")))</f>
@@ -11828,7 +11828,7 @@
       <c r="M170" s="23"/>
       <c r="O170" s="186"/>
       <c r="P170" s="28" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="Q170" s="138"/>
       <c r="R170" s="139"/>
@@ -11847,7 +11847,7 @@
       <c r="B171" s="21"/>
       <c r="C171" s="53"/>
       <c r="D171" s="48" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E171" s="80" t="str">
         <f t="shared" si="34"/>
@@ -11866,7 +11866,7 @@
         <v/>
       </c>
       <c r="J171" s="48" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K171" s="185" t="str">
         <f>IF(X183="","",X183)</f>
@@ -11875,7 +11875,7 @@
       <c r="M171" s="23"/>
       <c r="O171" s="186"/>
       <c r="P171" s="28" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="Q171" s="141"/>
       <c r="R171" s="142"/>
@@ -11901,7 +11901,7 @@
       <c r="B172" s="21"/>
       <c r="C172" s="53"/>
       <c r="D172" s="48" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E172" s="80" t="str">
         <f t="shared" si="34"/>
@@ -11922,7 +11922,7 @@
       <c r="M172" s="23"/>
       <c r="O172" s="186"/>
       <c r="P172" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="Q172" s="141"/>
       <c r="R172" s="142"/>
@@ -11941,7 +11941,7 @@
       <c r="B173" s="21"/>
       <c r="C173" s="53"/>
       <c r="D173" s="48" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E173" s="80" t="str">
         <f t="shared" si="34"/>
@@ -11962,7 +11962,7 @@
       <c r="M173" s="23"/>
       <c r="O173" s="186"/>
       <c r="P173" s="28" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="Q173" s="190" t="str">
         <f>IF(OR(Q171="",Q172=""),"",AVERAGE(Q171:Q172))</f>
@@ -12003,7 +12003,7 @@
       <c r="B174" s="21"/>
       <c r="C174" s="53"/>
       <c r="D174" s="48" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E174" s="105" t="str">
         <f t="shared" si="34"/>
@@ -12024,7 +12024,7 @@
       <c r="M174" s="23"/>
       <c r="O174" s="186"/>
       <c r="P174" s="28" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="Q174" s="141"/>
       <c r="R174" s="142"/>
@@ -12043,7 +12043,7 @@
       <c r="B175" s="21"/>
       <c r="C175" s="53"/>
       <c r="F175" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G175" s="29" t="str">
         <f>V184</f>
@@ -12052,7 +12052,7 @@
       <c r="M175" s="23"/>
       <c r="O175" s="186"/>
       <c r="P175" s="28" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="Q175" s="145"/>
       <c r="R175" s="146"/>
@@ -12084,7 +12084,7 @@
       <c r="M176" s="23"/>
       <c r="O176" s="24"/>
       <c r="P176" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q176" s="135" t="str">
         <f>IF(OR(Q173="",Q174=""),"",IF(AND(ABS(Q173-Q170)&lt;=1.5,ABS(Q174)&lt;=5),"Pass","Fail"))</f>
@@ -12124,10 +12124,10 @@
       <c r="M177" s="23"/>
       <c r="O177" s="24"/>
       <c r="Q177" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="R177" s="15" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="Y177" s="25"/>
       <c r="AA177" s="28"/>
@@ -12154,7 +12154,7 @@
       <c r="M178" s="23"/>
       <c r="O178" s="24"/>
       <c r="R178" s="15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="Y178" s="25"/>
       <c r="AA178" s="28"/>
@@ -12167,7 +12167,7 @@
       </c>
       <c r="B179" s="21"/>
       <c r="C179" s="164" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="M179" s="23"/>
       <c r="O179" s="24"/>
@@ -12191,10 +12191,10 @@
       </c>
       <c r="B180" s="21"/>
       <c r="D180" s="8" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E180" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F180" s="8" t="str">
         <f>R190</f>
@@ -12205,13 +12205,13 @@
         <v>Diff (Mean)</v>
       </c>
       <c r="H180" s="8" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I180" s="20"/>
       <c r="J180" s="20"/>
       <c r="M180" s="23"/>
       <c r="O180" s="168" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="Y180" s="25"/>
       <c r="AA180" s="28"/>
@@ -12224,7 +12224,7 @@
       </c>
       <c r="B181" s="21"/>
       <c r="C181" s="48" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D181" s="77" t="str">
         <f t="shared" ref="D181:H185" si="35">IF(P191="","",P191)</f>
@@ -12251,11 +12251,11 @@
       <c r="M181" s="23"/>
       <c r="O181" s="24"/>
       <c r="P181" s="262" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="Q181" s="262"/>
       <c r="R181" s="262" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="S181" s="262"/>
       <c r="Y181" s="25"/>
@@ -12276,7 +12276,7 @@
       </c>
       <c r="B182" s="21"/>
       <c r="C182" s="48" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D182" s="80" t="str">
         <f t="shared" si="35"/>
@@ -12305,19 +12305,19 @@
       <c r="M182" s="23"/>
       <c r="O182" s="24"/>
       <c r="P182" s="262" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="Q182" s="262" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="R182" s="262" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="S182" s="262" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="V182" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="X182" s="20"/>
       <c r="Y182" s="25"/>
@@ -12328,7 +12328,7 @@
       </c>
       <c r="B183" s="21"/>
       <c r="C183" s="48" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D183" s="80" t="str">
         <f t="shared" si="35"/>
@@ -12354,18 +12354,18 @@
       <c r="J183" s="20"/>
       <c r="M183" s="23"/>
       <c r="O183" s="186" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="P183" s="142"/>
       <c r="Q183" s="142"/>
       <c r="R183" s="142"/>
       <c r="S183" s="142"/>
       <c r="U183" s="28" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="V183" s="189"/>
       <c r="W183" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="X183" s="191" t="str">
         <f>IF(V183=3,"NA",IF(OR(P187="",Q187=""),"",IF(AND(P187&gt;=1,Q187&gt;=1),"Pass","Fail")))</f>
@@ -12379,7 +12379,7 @@
       </c>
       <c r="B184" s="21"/>
       <c r="C184" s="48" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D184" s="80" t="str">
         <f t="shared" si="35"/>
@@ -12405,17 +12405,17 @@
       <c r="J184" s="20"/>
       <c r="M184" s="23"/>
       <c r="O184" s="186" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="P184" s="142"/>
       <c r="Q184" s="142"/>
       <c r="R184" s="142"/>
       <c r="S184" s="142"/>
       <c r="U184" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="V184" s="29" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Y184" s="25"/>
     </row>
@@ -12425,7 +12425,7 @@
       </c>
       <c r="B185" s="21"/>
       <c r="C185" s="48" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D185" s="83" t="str">
         <f t="shared" si="35"/>
@@ -12451,14 +12451,14 @@
       <c r="J185" s="20"/>
       <c r="M185" s="23"/>
       <c r="O185" s="186" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P185" s="142"/>
       <c r="Q185" s="142"/>
       <c r="R185" s="142"/>
       <c r="S185" s="142"/>
       <c r="V185" s="15" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="Y185" s="25"/>
     </row>
@@ -12469,7 +12469,7 @@
       <c r="B186" s="21"/>
       <c r="C186" s="20"/>
       <c r="D186" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E186" s="15" t="str">
         <f>T196</f>
@@ -12482,7 +12482,7 @@
       <c r="J186" s="20"/>
       <c r="M186" s="23"/>
       <c r="O186" s="186" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="P186" s="117" t="str">
         <f>IF(OR(P183="",P184=""),"",P183-P184)</f>
@@ -12501,7 +12501,7 @@
         <v/>
       </c>
       <c r="V186" s="15" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Y186" s="25"/>
     </row>
@@ -12523,7 +12523,7 @@
       <c r="J187" s="20"/>
       <c r="M187" s="23"/>
       <c r="O187" s="186" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="P187" s="150" t="str">
         <f>IF(OR(P185="",P186=""),"",ABS(P186)/P185)</f>
@@ -12542,7 +12542,7 @@
         <v/>
       </c>
       <c r="V187" s="15" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="Y187" s="25"/>
     </row>
@@ -12562,11 +12562,11 @@
       </c>
       <c r="B189" s="21"/>
       <c r="C189" s="164" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="M189" s="23"/>
       <c r="O189" s="168" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="Y189" s="25"/>
     </row>
@@ -12577,27 +12577,27 @@
       <c r="B190" s="21"/>
       <c r="C190" s="53"/>
       <c r="E190" s="8" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="M190" s="23"/>
       <c r="O190" s="24"/>
       <c r="P190" s="262" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="Q190" s="262" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="R190" s="262" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="S190" s="262" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="T190" s="262" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="U190" s="20"/>
       <c r="V190" s="20"/>
@@ -12610,7 +12610,7 @@
       <c r="B191" s="21"/>
       <c r="C191" s="53"/>
       <c r="D191" s="48" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E191" s="77" t="str">
         <f>IF(P199="","",P199)</f>
@@ -12621,7 +12621,7 @@
         <v/>
       </c>
       <c r="H191" s="192" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I191" s="15" t="str">
         <f>T199</f>
@@ -12629,7 +12629,7 @@
       </c>
       <c r="M191" s="23"/>
       <c r="O191" s="186" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="P191" s="142"/>
       <c r="Q191" s="142"/>
@@ -12658,7 +12658,7 @@
       <c r="B192" s="21"/>
       <c r="C192" s="53"/>
       <c r="D192" s="48" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E192" s="83" t="str">
         <f>IF(P200="","",P200)</f>
@@ -12675,7 +12675,7 @@
       </c>
       <c r="M192" s="23"/>
       <c r="O192" s="186" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="P192" s="142"/>
       <c r="Q192" s="142"/>
@@ -12704,7 +12704,7 @@
       <c r="F193" s="192"/>
       <c r="M193" s="23"/>
       <c r="O193" s="186" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P193" s="142"/>
       <c r="Q193" s="142"/>
@@ -12733,7 +12733,7 @@
       <c r="F194" s="53"/>
       <c r="M194" s="23"/>
       <c r="O194" s="186" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="P194" s="142"/>
       <c r="Q194" s="142"/>
@@ -12768,7 +12768,7 @@
       <c r="J195" s="20"/>
       <c r="M195" s="23"/>
       <c r="O195" s="186" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="P195" s="142"/>
       <c r="Q195" s="142"/>
@@ -12806,13 +12806,13 @@
       <c r="M196" s="32"/>
       <c r="O196" s="71"/>
       <c r="P196" s="15" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="S196" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="T196" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="Y196" s="25"/>
     </row>
@@ -12835,7 +12835,7 @@
         <v>Eugene Mah</v>
       </c>
       <c r="O197" s="168" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="Y197" s="25"/>
     </row>
@@ -12844,7 +12844,7 @@
         <v>66</v>
       </c>
       <c r="C198" s="28" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D198" s="75" t="str">
         <f>IF($R$14="","",$R$14)</f>
@@ -12859,10 +12859,10 @@
       </c>
       <c r="O198" s="24"/>
       <c r="P198" s="262" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="Q198" s="262" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="R198" s="260"/>
       <c r="Y198" s="25"/>
@@ -12876,7 +12876,7 @@
         <v>Medical University of South Carolina</v>
       </c>
       <c r="O199" s="186" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="P199" s="142"/>
       <c r="Q199" s="117" t="str">
@@ -12885,10 +12885,10 @@
       </c>
       <c r="R199" s="260"/>
       <c r="S199" s="192" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="T199" s="15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="Y199" s="25"/>
     </row>
@@ -12897,14 +12897,14 @@
         <v>2</v>
       </c>
       <c r="H200" s="193" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="M200" s="36" t="str">
         <f>$H$5</f>
         <v>CT System Compliance Inspection</v>
       </c>
       <c r="O200" s="186" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="P200" s="142"/>
       <c r="Q200" s="117" t="str">
@@ -12914,7 +12914,7 @@
       <c r="R200" s="260"/>
       <c r="S200" s="53"/>
       <c r="T200" s="15" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Y200" s="25"/>
     </row>
@@ -12956,7 +12956,7 @@
       <c r="L202" s="195"/>
       <c r="M202" s="23"/>
       <c r="O202" s="168" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="Y202" s="25"/>
     </row>
@@ -12980,7 +12980,7 @@
       <c r="M203" s="23"/>
       <c r="O203" s="24"/>
       <c r="S203" s="20" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="U203" s="20"/>
       <c r="Y203" s="25"/>
@@ -13005,13 +13005,13 @@
       <c r="M204" s="23"/>
       <c r="O204" s="71"/>
       <c r="P204" s="15" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="R204" s="20"/>
       <c r="S204" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="T204" s="297"/>
+        <v>266</v>
+      </c>
+      <c r="T204" s="275"/>
       <c r="Y204" s="25"/>
     </row>
     <row r="205" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13034,13 +13034,13 @@
       <c r="M205" s="23"/>
       <c r="O205" s="71"/>
       <c r="P205" s="15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="R205" s="20"/>
       <c r="S205" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="T205" s="297"/>
+        <v>267</v>
+      </c>
+      <c r="T205" s="275"/>
       <c r="Y205" s="25"/>
     </row>
     <row r="206" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13063,13 +13063,13 @@
       <c r="M206" s="23"/>
       <c r="O206" s="71"/>
       <c r="P206" s="15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="R206" s="20"/>
       <c r="S206" s="28" t="s">
-        <v>250</v>
-      </c>
-      <c r="T206" s="297"/>
+        <v>246</v>
+      </c>
+      <c r="T206" s="275"/>
       <c r="Y206" s="25"/>
     </row>
     <row r="207" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13090,16 +13090,16 @@
       <c r="K207" s="197"/>
       <c r="L207" s="197"/>
       <c r="M207" s="23"/>
-      <c r="O207" s="296"/>
+      <c r="O207" s="274"/>
       <c r="P207" s="15" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="Q207" s="20"/>
       <c r="R207" s="20"/>
       <c r="S207" s="28" t="s">
-        <v>272</v>
-      </c>
-      <c r="T207" s="297"/>
+        <v>268</v>
+      </c>
+      <c r="T207" s="275"/>
       <c r="U207" s="20"/>
       <c r="V207" s="20"/>
       <c r="W207" s="20"/>
@@ -13124,16 +13124,16 @@
       <c r="K208" s="195"/>
       <c r="L208" s="195"/>
       <c r="M208" s="23"/>
-      <c r="O208" s="296"/>
+      <c r="O208" s="274"/>
       <c r="P208" s="15" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="Q208" s="20"/>
       <c r="R208" s="20"/>
       <c r="S208" s="28" t="s">
-        <v>273</v>
-      </c>
-      <c r="T208" s="297"/>
+        <v>269</v>
+      </c>
+      <c r="T208" s="275"/>
       <c r="U208" s="20"/>
       <c r="V208" s="20"/>
       <c r="W208" s="20"/>
@@ -13159,15 +13159,15 @@
       <c r="L209" s="197"/>
       <c r="M209" s="23"/>
       <c r="O209" s="198" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="P209" s="15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="Q209" s="20"/>
       <c r="R209" s="20"/>
       <c r="S209" s="28" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="T209" s="150" t="str">
         <f>IF(T204="","",AVERAGE(T204:T208))</f>
@@ -13199,12 +13199,12 @@
       <c r="M210" s="23"/>
       <c r="O210" s="157"/>
       <c r="P210" s="20" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="Q210" s="20"/>
       <c r="R210" s="20"/>
       <c r="S210" s="28" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="T210" s="180" t="str">
         <f>IF(T204="","",STDEV(T204:T208))</f>
@@ -13239,7 +13239,7 @@
       <c r="Q211" s="34"/>
       <c r="R211" s="34"/>
       <c r="S211" s="199" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="T211" s="200" t="str">
         <f>IF(T204="","",2*(MAX(T204:T208)-MIN(T204:T208))/(MAX(T204:T208)+MIN(T204:T208)))</f>
@@ -13289,7 +13289,7 @@
       <c r="L213" s="197"/>
       <c r="M213" s="23"/>
       <c r="T213" s="201" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="214" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13315,7 +13315,7 @@
       <c r="Q214" s="17"/>
       <c r="R214" s="17"/>
       <c r="S214" s="202" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="T214" s="17"/>
       <c r="U214" s="17"/>
@@ -13344,7 +13344,7 @@
       <c r="M215" s="23"/>
       <c r="O215" s="24"/>
       <c r="P215" s="28" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="Q215" s="203"/>
       <c r="R215" s="204"/>
@@ -13378,7 +13378,7 @@
       <c r="M216" s="23"/>
       <c r="O216" s="24"/>
       <c r="P216" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q216" s="208"/>
       <c r="R216" s="209">
@@ -13388,7 +13388,7 @@
       <c r="S216" s="210"/>
       <c r="T216" s="210"/>
       <c r="U216" s="211" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="V216" s="210"/>
       <c r="W216" s="210"/>
@@ -13415,7 +13415,7 @@
       <c r="M217" s="23"/>
       <c r="O217" s="24"/>
       <c r="P217" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q217" s="203"/>
       <c r="R217" s="204"/>
@@ -13449,7 +13449,7 @@
       <c r="M218" s="23"/>
       <c r="O218" s="24"/>
       <c r="P218" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q218" s="208"/>
       <c r="R218" s="209">
@@ -13459,7 +13459,7 @@
       <c r="S218" s="210"/>
       <c r="T218" s="210"/>
       <c r="U218" s="211" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="V218" s="210"/>
       <c r="W218" s="210"/>
@@ -13486,7 +13486,7 @@
       <c r="M219" s="23"/>
       <c r="O219" s="24"/>
       <c r="P219" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q219" s="203"/>
       <c r="R219" s="204"/>
@@ -13520,7 +13520,7 @@
       <c r="M220" s="23"/>
       <c r="O220" s="24"/>
       <c r="P220" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q220" s="208"/>
       <c r="R220" s="209">
@@ -13530,7 +13530,7 @@
       <c r="S220" s="210"/>
       <c r="T220" s="210"/>
       <c r="U220" s="211" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="V220" s="210"/>
       <c r="W220" s="210"/>
@@ -13557,7 +13557,7 @@
       <c r="M221" s="23"/>
       <c r="O221" s="24"/>
       <c r="P221" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q221" s="203"/>
       <c r="R221" s="204"/>
@@ -13591,7 +13591,7 @@
       <c r="M222" s="23"/>
       <c r="O222" s="24"/>
       <c r="P222" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q222" s="208"/>
       <c r="R222" s="209">
@@ -13601,7 +13601,7 @@
       <c r="S222" s="210"/>
       <c r="T222" s="210"/>
       <c r="U222" s="211" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="V222" s="210"/>
       <c r="W222" s="210"/>
@@ -13628,7 +13628,7 @@
       <c r="M223" s="23"/>
       <c r="O223" s="24"/>
       <c r="P223" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q223" s="203"/>
       <c r="R223" s="204"/>
@@ -13662,7 +13662,7 @@
       <c r="M224" s="23"/>
       <c r="O224" s="24"/>
       <c r="P224" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q224" s="208"/>
       <c r="R224" s="209">
@@ -13672,7 +13672,7 @@
       <c r="S224" s="210"/>
       <c r="T224" s="210"/>
       <c r="U224" s="211" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="V224" s="210"/>
       <c r="W224" s="210"/>
@@ -13699,7 +13699,7 @@
       <c r="M225" s="23"/>
       <c r="O225" s="24"/>
       <c r="P225" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q225" s="203"/>
       <c r="R225" s="204"/>
@@ -13733,7 +13733,7 @@
       <c r="M226" s="23"/>
       <c r="O226" s="24"/>
       <c r="P226" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q226" s="208"/>
       <c r="R226" s="209">
@@ -13768,7 +13768,7 @@
       <c r="M227" s="23"/>
       <c r="O227" s="24"/>
       <c r="P227" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q227" s="203"/>
       <c r="R227" s="204"/>
@@ -13802,7 +13802,7 @@
       <c r="M228" s="23"/>
       <c r="O228" s="24"/>
       <c r="P228" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q228" s="208"/>
       <c r="R228" s="209">
@@ -13837,7 +13837,7 @@
       <c r="M229" s="23"/>
       <c r="O229" s="24"/>
       <c r="P229" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q229" s="203"/>
       <c r="R229" s="204"/>
@@ -13871,7 +13871,7 @@
       <c r="M230" s="23"/>
       <c r="O230" s="24"/>
       <c r="P230" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q230" s="208"/>
       <c r="R230" s="209">
@@ -13906,7 +13906,7 @@
       <c r="M231" s="23"/>
       <c r="O231" s="24"/>
       <c r="P231" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q231" s="203"/>
       <c r="R231" s="204"/>
@@ -13940,7 +13940,7 @@
       <c r="M232" s="23"/>
       <c r="O232" s="24"/>
       <c r="P232" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q232" s="208"/>
       <c r="R232" s="209">
@@ -13975,7 +13975,7 @@
       <c r="M233" s="23"/>
       <c r="O233" s="24"/>
       <c r="P233" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q233" s="203"/>
       <c r="R233" s="204"/>
@@ -14009,7 +14009,7 @@
       <c r="M234" s="23"/>
       <c r="O234" s="24"/>
       <c r="P234" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q234" s="208"/>
       <c r="R234" s="209">
@@ -14044,7 +14044,7 @@
       <c r="M235" s="23"/>
       <c r="O235" s="24"/>
       <c r="P235" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q235" s="203"/>
       <c r="R235" s="204"/>
@@ -14078,7 +14078,7 @@
       <c r="M236" s="23"/>
       <c r="O236" s="24"/>
       <c r="P236" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q236" s="208"/>
       <c r="R236" s="209">
@@ -14113,7 +14113,7 @@
       <c r="M237" s="23"/>
       <c r="O237" s="24"/>
       <c r="P237" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q237" s="203"/>
       <c r="R237" s="204"/>
@@ -14147,7 +14147,7 @@
       <c r="M238" s="23"/>
       <c r="O238" s="24"/>
       <c r="P238" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q238" s="208"/>
       <c r="R238" s="209">
@@ -14182,7 +14182,7 @@
       <c r="M239" s="23"/>
       <c r="O239" s="24"/>
       <c r="P239" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q239" s="203"/>
       <c r="R239" s="204"/>
@@ -14216,7 +14216,7 @@
       <c r="M240" s="23"/>
       <c r="O240" s="24"/>
       <c r="P240" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q240" s="208"/>
       <c r="R240" s="209">
@@ -14251,7 +14251,7 @@
       <c r="M241" s="23"/>
       <c r="O241" s="24"/>
       <c r="P241" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q241" s="203"/>
       <c r="R241" s="204"/>
@@ -14285,7 +14285,7 @@
       <c r="M242" s="23"/>
       <c r="O242" s="24"/>
       <c r="P242" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q242" s="208"/>
       <c r="R242" s="209">
@@ -14320,7 +14320,7 @@
       <c r="M243" s="23"/>
       <c r="O243" s="24"/>
       <c r="P243" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q243" s="203"/>
       <c r="R243" s="204"/>
@@ -14354,7 +14354,7 @@
       <c r="M244" s="23"/>
       <c r="O244" s="24"/>
       <c r="P244" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q244" s="208"/>
       <c r="R244" s="209">
@@ -14389,7 +14389,7 @@
       <c r="M245" s="23"/>
       <c r="O245" s="24"/>
       <c r="P245" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q245" s="203"/>
       <c r="R245" s="204"/>
@@ -14423,7 +14423,7 @@
       <c r="M246" s="23"/>
       <c r="O246" s="24"/>
       <c r="P246" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q246" s="208"/>
       <c r="R246" s="209">
@@ -14458,7 +14458,7 @@
       <c r="M247" s="23"/>
       <c r="O247" s="24"/>
       <c r="P247" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q247" s="203"/>
       <c r="R247" s="204"/>
@@ -14492,7 +14492,7 @@
       <c r="M248" s="23"/>
       <c r="O248" s="24"/>
       <c r="P248" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q248" s="208"/>
       <c r="R248" s="209">
@@ -14527,7 +14527,7 @@
       <c r="M249" s="23"/>
       <c r="O249" s="24"/>
       <c r="P249" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q249" s="203"/>
       <c r="R249" s="204"/>
@@ -14561,7 +14561,7 @@
       <c r="M250" s="23"/>
       <c r="O250" s="24"/>
       <c r="P250" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q250" s="208"/>
       <c r="R250" s="209">
@@ -14596,7 +14596,7 @@
       <c r="M251" s="23"/>
       <c r="O251" s="24"/>
       <c r="P251" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q251" s="203"/>
       <c r="R251" s="204"/>
@@ -14630,7 +14630,7 @@
       <c r="M252" s="23"/>
       <c r="O252" s="24"/>
       <c r="P252" s="207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q252" s="210"/>
       <c r="R252" s="209">
@@ -14832,7 +14832,7 @@
         <v>66</v>
       </c>
       <c r="C264" s="28" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D264" s="75" t="str">
         <f>IF($R$14="","",$R$14)</f>
@@ -15089,45 +15089,45 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="295" t="s">
+      <c r="A4" s="297" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="297" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" s="297"/>
+      <c r="D4" s="297"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="297"/>
+      <c r="B5" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="B4" s="295" t="s">
-        <v>290</v>
-      </c>
-      <c r="C4" s="295"/>
-      <c r="D4" s="295"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="295"/>
-      <c r="B5" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C6" s="10">
         <v>3.5</v>
@@ -15138,10 +15138,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C7" s="10">
         <v>6</v>
@@ -15152,10 +15152,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C8" s="10">
         <v>10.5</v>
@@ -15166,10 +15166,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C9" s="10">
         <v>11.5</v>
@@ -15180,10 +15180,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C10" s="10">
         <v>11.1</v>
@@ -15194,10 +15194,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C11" s="10">
         <v>18.8</v>
@@ -15208,10 +15208,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C12" s="10">
         <v>19.399999999999999</v>
@@ -15222,10 +15222,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C13" s="10">
         <v>24.4</v>
@@ -15236,10 +15236,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C14" s="10">
         <v>27.4</v>
@@ -15250,10 +15250,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C15" s="10">
         <v>44</v>
@@ -15264,10 +15264,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C16" s="10">
         <v>45.5</v>
@@ -15283,33 +15283,33 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="295" t="s">
+      <c r="A18" s="297" t="s">
+        <v>285</v>
+      </c>
+      <c r="B18" s="297" t="s">
+        <v>302</v>
+      </c>
+      <c r="C18" s="297"/>
+      <c r="D18" s="297"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="297"/>
+      <c r="B19" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="B18" s="295" t="s">
-        <v>306</v>
-      </c>
-      <c r="C18" s="295"/>
-      <c r="D18" s="295"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="295"/>
-      <c r="B19" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C20" s="10">
         <v>4.7</v>
@@ -15320,10 +15320,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C21" s="10">
         <v>6.6</v>
@@ -15334,10 +15334,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C22" s="10">
         <v>11.2</v>
@@ -15348,10 +15348,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C23" s="10">
         <v>8.5</v>
@@ -15362,10 +15362,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C24" s="10">
         <v>11.6</v>
@@ -15376,10 +15376,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C25" s="10">
         <v>11.5</v>
@@ -15390,10 +15390,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C26" s="10">
         <v>11.8</v>
@@ -15404,10 +15404,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C27" s="10">
         <v>19.8</v>
@@ -15418,10 +15418,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C28" s="10">
         <v>41</v>
@@ -15432,10 +15432,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C29" s="10">
         <v>45.5</v>
@@ -15446,10 +15446,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C30" s="10">
         <v>43.5</v>
@@ -15460,10 +15460,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C31" s="10">
         <v>23.5</v>
@@ -15474,10 +15474,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C32" s="10">
         <v>28</v>
@@ -15488,10 +15488,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C33" s="10">
         <v>18</v>
@@ -15502,10 +15502,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C34" s="10">
         <v>25</v>
@@ -15516,10 +15516,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C35" s="10">
         <v>20</v>
@@ -15529,26 +15529,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="295" t="s">
+      <c r="A37" s="297" t="s">
+        <v>285</v>
+      </c>
+      <c r="B37" s="297" t="s">
+        <v>307</v>
+      </c>
+      <c r="C37" s="297"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="297"/>
+      <c r="B38" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="B37" s="295" t="s">
-        <v>311</v>
-      </c>
-      <c r="C37" s="295"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="295"/>
-      <c r="B38" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B39" s="10">
         <v>22.5</v>
@@ -15559,7 +15559,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B40" s="10">
         <v>33.5</v>
@@ -15570,7 +15570,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B41" s="10">
         <v>19.5</v>
@@ -15581,7 +15581,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B42" s="10">
         <v>11.5</v>
@@ -15592,7 +15592,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B43" s="10">
         <v>6.5</v>
@@ -15603,7 +15603,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B44" s="10">
         <v>4</v>
@@ -15614,7 +15614,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B45" s="10">
         <v>7</v>
@@ -15624,26 +15624,26 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="295" t="s">
+      <c r="A47" s="297" t="s">
+        <v>285</v>
+      </c>
+      <c r="B47" s="297" t="s">
+        <v>310</v>
+      </c>
+      <c r="C47" s="297"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="297"/>
+      <c r="B48" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="B47" s="295" t="s">
-        <v>314</v>
-      </c>
-      <c r="C47" s="295"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="295"/>
-      <c r="B48" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B49" s="10">
         <v>30.5</v>
@@ -15654,7 +15654,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B50" s="10">
         <v>18.5</v>
@@ -15665,7 +15665,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B51" s="10">
         <v>24.5</v>
@@ -15676,7 +15676,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B52" s="10">
         <v>15.5</v>
@@ -15687,7 +15687,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B53" s="10">
         <v>12.5</v>
@@ -15698,7 +15698,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B54" s="10">
         <v>3.5</v>
@@ -15709,7 +15709,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B55" s="10">
         <v>3</v>
@@ -15719,26 +15719,26 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="295" t="s">
+      <c r="A57" s="297" t="s">
+        <v>285</v>
+      </c>
+      <c r="B57" s="297" t="s">
+        <v>317</v>
+      </c>
+      <c r="C57" s="297"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="297"/>
+      <c r="B58" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="B57" s="295" t="s">
-        <v>321</v>
-      </c>
-      <c r="C57" s="295"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="295"/>
-      <c r="B58" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B59" s="10">
         <v>4.9000000000000004</v>
@@ -15749,7 +15749,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B60" s="10">
         <v>12.6</v>
@@ -15760,7 +15760,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B61" s="10">
         <v>14.5</v>
@@ -15771,7 +15771,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B62" s="10">
         <v>12.6</v>
@@ -15782,7 +15782,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B63" s="10">
         <v>18.5</v>
@@ -15793,7 +15793,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B64" s="10">
         <v>18.5</v>
@@ -15804,7 +15804,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B65" s="10">
         <v>24.2</v>
@@ -15814,26 +15814,26 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="295" t="s">
+      <c r="A67" s="297" t="s">
+        <v>285</v>
+      </c>
+      <c r="B67" s="297" t="s">
+        <v>322</v>
+      </c>
+      <c r="C67" s="297"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="297"/>
+      <c r="B68" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="B67" s="295" t="s">
-        <v>326</v>
-      </c>
-      <c r="C67" s="295"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="295"/>
-      <c r="B68" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B69" s="11">
         <v>3</v>
@@ -15844,7 +15844,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B70" s="11">
         <v>7</v>
@@ -15855,7 +15855,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B71" s="11">
         <v>7.5</v>
@@ -15866,7 +15866,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B72" s="11">
         <v>12</v>
@@ -15877,7 +15877,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B73" s="11">
         <v>24</v>
@@ -15888,7 +15888,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B74" s="11">
         <v>22.5</v>
@@ -15899,7 +15899,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B75" s="11">
         <v>24.5</v>
@@ -15910,7 +15910,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B76" s="11">
         <v>28.5</v>
@@ -15921,7 +15921,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B77" s="11">
         <v>47.5</v>
@@ -15932,7 +15932,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B78" s="11">
         <v>66</v>
@@ -15943,7 +15943,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B79" s="11">
         <v>67</v>
@@ -15953,25 +15953,25 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="294" t="s">
+      <c r="A81" s="296" t="s">
+        <v>285</v>
+      </c>
+      <c r="B81" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="296"/>
+      <c r="B82" t="s">
+        <v>288</v>
+      </c>
+      <c r="C82" t="s">
         <v>289</v>
-      </c>
-      <c r="B81" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="294"/>
-      <c r="B82" t="s">
-        <v>292</v>
-      </c>
-      <c r="C82" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B83">
         <v>18.8</v>
@@ -15982,7 +15982,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B84">
         <v>3.5</v>
@@ -15993,7 +15993,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B85">
         <v>19.8</v>
@@ -16004,7 +16004,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B86">
         <v>25</v>

</xml_diff>

<commit_message>
Fix page break and cell formatting
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maheug\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA06C11D-632A-41CD-ADF1-C3B3A55EC521}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD5F86D-F627-437D-909F-580FAAE63C06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <definedName name="CTDI">Sheet1!$B$67:$M$132</definedName>
     <definedName name="CTReport" localSheetId="1">"First,CTDI,ACRPhantom,Comments"</definedName>
     <definedName name="First">Sheet1!$B$1:$M$66</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$B$1:$M$198</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$B$1:$M$264</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$A$1:$F$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2579" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="350">
   <si>
     <t>Medical Physicist CT Survey Report</t>
   </si>
@@ -1046,9 +1046,6 @@
   </si>
   <si>
     <t>First,CTDI,ACRPhantom,Comments</t>
-  </si>
-  <si>
-    <t>First,CTDI,ACRPhantom</t>
   </si>
   <si>
     <t>Siemens CT Beam Profiles http://128.23.56.214/MPwiki/index.php?title=Siemens_CT_Beam_Profiles</t>
@@ -2232,7 +2229,7 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="299">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3053,13 +3050,37 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3095,32 +3116,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3981,19 +3981,19 @@
       <c r="A6" s="219" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="278" t="str">
+      <c r="B6" s="277" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="278"/>
+      <c r="C6" s="277"/>
       <c r="D6" s="220" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="278" t="str">
+      <c r="E6" s="277" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="278"/>
+      <c r="F6" s="277"/>
       <c r="G6" s="1"/>
       <c r="J6" s="245" t="s">
         <v>333</v>
@@ -4003,48 +4003,48 @@
       <c r="A7" s="219" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="276"/>
-      <c r="C7" s="276"/>
+      <c r="B7" s="278"/>
+      <c r="C7" s="278"/>
       <c r="D7" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="276" t="str">
+      <c r="E7" s="278" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="276"/>
+      <c r="F7" s="278"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="219" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="276"/>
-      <c r="C8" s="276"/>
+      <c r="B8" s="278"/>
+      <c r="C8" s="278"/>
       <c r="D8" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="276" t="str">
+      <c r="E8" s="278" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="276"/>
+      <c r="F8" s="278"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="219" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="276"/>
-      <c r="C9" s="276"/>
+      <c r="B9" s="278"/>
+      <c r="C9" s="278"/>
       <c r="D9" s="220" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="276" t="str">
+      <c r="E9" s="278" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="276"/>
+      <c r="F9" s="278"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4054,19 +4054,19 @@
       <c r="D10" s="220" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="277" t="str">
+      <c r="E10" s="279" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="277"/>
+      <c r="F10" s="279"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="219" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="278"/>
-      <c r="C11" s="278"/>
+      <c r="B11" s="277"/>
+      <c r="C11" s="277"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4089,10 +4089,10 @@
       <c r="A13" s="222" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="278" t="s">
+      <c r="B13" s="277" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="278"/>
+      <c r="C13" s="277"/>
       <c r="D13" s="220" t="s">
         <v>16</v>
       </c>
@@ -4395,17 +4395,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -4428,9 +4428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4491,7 +4489,7 @@
       </c>
       <c r="Y2" s="25"/>
       <c r="AA2" s="26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4608,7 +4606,7 @@
       </c>
       <c r="AD7" s="41" t="str">
         <f>IF(OR(AA2="",AA2=0),"",AA2)</f>
-        <v>First,CTDI,ACRPhantom</v>
+        <v>First,CTDI,ACRPhantom,Comments</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4694,19 +4692,19 @@
       <c r="E10" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="292" t="str">
+      <c r="F10" s="280" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="292"/>
+      <c r="G10" s="280"/>
       <c r="J10" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="292" t="str">
+      <c r="K10" s="280" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="292"/>
+      <c r="L10" s="280"/>
       <c r="M10" s="23"/>
       <c r="O10" s="24"/>
       <c r="Q10" s="28" t="s">
@@ -4747,19 +4745,19 @@
       <c r="E11" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="295" t="str">
+      <c r="F11" s="281" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="295"/>
+      <c r="G11" s="281"/>
       <c r="J11" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="292" t="str">
+      <c r="K11" s="280" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="292"/>
+      <c r="L11" s="280"/>
       <c r="M11" s="23"/>
       <c r="O11" s="24"/>
       <c r="Q11" s="28" t="s">
@@ -4800,19 +4798,19 @@
       <c r="E12" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="295" t="str">
+      <c r="F12" s="281" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="295"/>
+      <c r="G12" s="281"/>
       <c r="J12" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="296" t="str">
+      <c r="K12" s="282" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="296"/>
+      <c r="L12" s="282"/>
       <c r="M12" s="23"/>
       <c r="O12" s="24"/>
       <c r="Q12" s="28" t="s">
@@ -4853,19 +4851,19 @@
       <c r="E13" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="295" t="str">
+      <c r="F13" s="281" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="295"/>
+      <c r="G13" s="281"/>
       <c r="J13" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="292" t="str">
+      <c r="K13" s="280" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="292"/>
+      <c r="L13" s="280"/>
       <c r="M13" s="23"/>
       <c r="O13" s="24"/>
       <c r="Q13" s="28" t="s">
@@ -4963,19 +4961,19 @@
       <c r="E16" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="292" t="str">
+      <c r="F16" s="280" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="292"/>
+      <c r="G16" s="280"/>
       <c r="J16" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="296" t="str">
+      <c r="K16" s="282" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="296"/>
+      <c r="L16" s="282"/>
       <c r="M16" s="23"/>
       <c r="O16" s="24"/>
       <c r="P16" s="56" t="s">
@@ -5003,19 +5001,19 @@
       <c r="E17" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="295" t="str">
+      <c r="F17" s="281" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="295"/>
+      <c r="G17" s="281"/>
       <c r="J17" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="292" t="str">
+      <c r="K17" s="280" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="292"/>
+      <c r="L17" s="280"/>
       <c r="M17" s="23"/>
       <c r="O17" s="24"/>
       <c r="Q17" s="28" t="s">
@@ -5056,11 +5054,11 @@
       <c r="J18" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="292" t="str">
+      <c r="K18" s="280" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="292"/>
+      <c r="L18" s="280"/>
       <c r="M18" s="23"/>
       <c r="O18" s="24"/>
       <c r="Q18" s="28" t="s">
@@ -5132,11 +5130,11 @@
       <c r="E20" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="292" t="str">
+      <c r="F20" s="280" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="292"/>
+      <c r="G20" s="280"/>
       <c r="I20" s="59" t="s">
         <v>76</v>
       </c>
@@ -5161,19 +5159,19 @@
       <c r="E21" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="294" t="str">
+      <c r="F21" s="283" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="294"/>
+      <c r="G21" s="283"/>
       <c r="J21" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="292" t="str">
+      <c r="K21" s="280" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="292"/>
+      <c r="L21" s="280"/>
       <c r="M21" s="23"/>
       <c r="O21" s="24"/>
       <c r="Q21" s="28" t="s">
@@ -5212,11 +5210,11 @@
       <c r="J22" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="292" t="str">
+      <c r="K22" s="280" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="292"/>
+      <c r="L22" s="280"/>
       <c r="M22" s="23"/>
       <c r="O22" s="24"/>
       <c r="Q22" s="28" t="s">
@@ -5257,19 +5255,19 @@
       <c r="E23" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="292" t="str">
+      <c r="F23" s="280" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="292"/>
+      <c r="G23" s="280"/>
       <c r="J23" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="292" t="str">
+      <c r="K23" s="280" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="292"/>
+      <c r="L23" s="280"/>
       <c r="M23" s="23"/>
       <c r="O23" s="24"/>
       <c r="P23" s="56" t="s">
@@ -5305,11 +5303,11 @@
       <c r="E24" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="292" t="str">
+      <c r="F24" s="280" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="292"/>
+      <c r="G24" s="280"/>
       <c r="M24" s="23"/>
       <c r="O24" s="24"/>
       <c r="Q24" s="28" t="s">
@@ -5350,11 +5348,11 @@
       <c r="E25" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="292" t="str">
+      <c r="F25" s="280" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="292"/>
+      <c r="G25" s="280"/>
       <c r="J25" s="55" t="s">
         <v>82</v>
       </c>
@@ -5394,11 +5392,11 @@
       <c r="J26" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="292" t="str">
+      <c r="K26" s="280" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="292"/>
+      <c r="L26" s="280"/>
       <c r="M26" s="23"/>
       <c r="O26" s="24"/>
       <c r="Q26" s="28" t="s">
@@ -5426,19 +5424,19 @@
       <c r="E27" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="292" t="str">
+      <c r="F27" s="280" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="292"/>
+      <c r="G27" s="280"/>
       <c r="J27" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="292" t="str">
+      <c r="K27" s="280" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="292"/>
+      <c r="L27" s="280"/>
       <c r="M27" s="23"/>
       <c r="O27" s="24"/>
       <c r="P27" s="56" t="s">
@@ -5465,11 +5463,11 @@
       <c r="E28" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="292" t="str">
+      <c r="F28" s="280" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="292"/>
+      <c r="G28" s="280"/>
       <c r="M28" s="23"/>
       <c r="O28" s="24"/>
       <c r="Q28" s="28" t="s">
@@ -5510,11 +5508,11 @@
       <c r="E29" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="292" t="str">
+      <c r="F29" s="280" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="292"/>
+      <c r="G29" s="280"/>
       <c r="M29" s="23"/>
       <c r="O29" s="24"/>
       <c r="Q29" s="28" t="s">
@@ -5624,10 +5622,10 @@
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
-      <c r="L32" s="293" t="s">
+      <c r="L32" s="284" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="293"/>
+      <c r="M32" s="284"/>
       <c r="AA32" s="28" t="s">
         <v>70</v>
       </c>
@@ -5926,11 +5924,11 @@
         <v>102</v>
       </c>
       <c r="L41" s="66" t="str">
-        <f>IF(O44="","TBD",IF(O44=1,"YES",IF(O44=3,"NA","")))</f>
+        <f t="shared" ref="L41:L46" si="4">IF(O44="","TBD",IF(O44=1,"YES",IF(O44=3,"NA","")))</f>
         <v>TBD</v>
       </c>
       <c r="M41" s="67" t="str">
-        <f>IF(O44=2,"NO","")</f>
+        <f t="shared" ref="M41:M46" si="5">IF(O44=2,"NO","")</f>
         <v/>
       </c>
       <c r="O41" s="71"/>
@@ -5952,11 +5950,11 @@
         <v>104</v>
       </c>
       <c r="L42" s="66" t="str">
-        <f>IF(O45="","TBD",IF(O45=1,"YES",IF(O45=3,"NA","")))</f>
+        <f t="shared" si="4"/>
         <v>TBD</v>
       </c>
       <c r="M42" s="67" t="str">
-        <f>IF(O45=2,"NO","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O42" s="71"/>
@@ -5978,11 +5976,11 @@
         <v>106</v>
       </c>
       <c r="L43" s="66" t="str">
-        <f>IF(O46="","TBD",IF(O46=1,"YES",IF(O46=3,"NA","")))</f>
+        <f t="shared" si="4"/>
         <v>TBD</v>
       </c>
       <c r="M43" s="67" t="str">
-        <f>IF(O46=2,"NO","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O43" s="24"/>
@@ -5995,11 +5993,11 @@
       </c>
       <c r="AB43" s="39"/>
       <c r="AC43" s="40" t="str">
-        <f t="shared" ref="AC43:AC59" si="4">IF(AB43&lt;&gt;AD43,"Change","")</f>
+        <f t="shared" ref="AC43:AC59" si="6">IF(AB43&lt;&gt;AD43,"Change","")</f>
         <v/>
       </c>
       <c r="AD43" s="47" t="str">
-        <f t="shared" ref="AD43:AD59" si="5">IF(Q72="","",Q72)</f>
+        <f t="shared" ref="AD43:AD59" si="7">IF(Q72="","",Q72)</f>
         <v/>
       </c>
     </row>
@@ -6013,11 +6011,11 @@
         <v>108</v>
       </c>
       <c r="L44" s="66" t="str">
-        <f>IF(O47="","TBD",IF(O47=1,"YES",IF(O47=3,"NA","")))</f>
+        <f t="shared" si="4"/>
         <v>TBD</v>
       </c>
       <c r="M44" s="67" t="str">
-        <f>IF(O47=2,"NO","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O44" s="71"/>
@@ -6030,11 +6028,11 @@
       </c>
       <c r="AB44" s="39"/>
       <c r="AC44" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD44" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6048,11 +6046,11 @@
         <v>110</v>
       </c>
       <c r="L45" s="66" t="str">
-        <f>IF(O48="","TBD",IF(O48=1,"YES",IF(O48=3,"NA","")))</f>
+        <f t="shared" si="4"/>
         <v>TBD</v>
       </c>
       <c r="M45" s="67" t="str">
-        <f>IF(O48=2,"NO","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O45" s="71"/>
@@ -6065,11 +6063,11 @@
       </c>
       <c r="AB45" s="39"/>
       <c r="AC45" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD45" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6080,14 +6078,14 @@
       <c r="B46" s="21"/>
       <c r="C46" s="69"/>
       <c r="E46" s="69" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L46" s="66" t="str">
-        <f>IF(O49="","TBD",IF(O49=1,"YES",IF(O49=3,"NA","")))</f>
+        <f t="shared" si="4"/>
         <v>TBD</v>
       </c>
       <c r="M46" s="67" t="str">
-        <f>IF(O49=2,"NO","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O46" s="71"/>
@@ -6100,11 +6098,11 @@
       </c>
       <c r="AB46" s="39"/>
       <c r="AC46" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD46" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6118,11 +6116,11 @@
         <v>113</v>
       </c>
       <c r="L47" s="66" t="str">
-        <f t="shared" ref="L47:L56" si="6">IF(O51="","TBD",IF(O51=1,"YES",IF(O51=3,"NA","")))</f>
+        <f t="shared" ref="L47:L56" si="8">IF(O51="","TBD",IF(O51=1,"YES",IF(O51=3,"NA","")))</f>
         <v>TBD</v>
       </c>
       <c r="M47" s="67" t="str">
-        <f t="shared" ref="M47:M56" si="7">IF(O51=2,"NO","")</f>
+        <f t="shared" ref="M47:M56" si="9">IF(O51=2,"NO","")</f>
         <v/>
       </c>
       <c r="O47" s="71"/>
@@ -6135,11 +6133,11 @@
       </c>
       <c r="AB47" s="39"/>
       <c r="AC47" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD47" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6153,11 +6151,11 @@
         <v>115</v>
       </c>
       <c r="L48" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M48" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O48" s="71"/>
@@ -6170,11 +6168,11 @@
       </c>
       <c r="AB48" s="39"/>
       <c r="AC48" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD48" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6188,16 +6186,16 @@
         <v>117</v>
       </c>
       <c r="L49" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M49" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O49" s="71"/>
       <c r="P49" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Y49" s="25"/>
       <c r="AA49" s="28" t="s">
@@ -6205,11 +6203,11 @@
       </c>
       <c r="AB49" s="39"/>
       <c r="AC49" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD49" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6223,11 +6221,11 @@
         <v>119</v>
       </c>
       <c r="L50" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M50" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O50" s="263"/>
@@ -6237,11 +6235,11 @@
       </c>
       <c r="AB50" s="39"/>
       <c r="AC50" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD50" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6257,11 +6255,11 @@
         <v>122</v>
       </c>
       <c r="L51" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M51" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O51" s="71"/>
@@ -6274,11 +6272,11 @@
       </c>
       <c r="AB51" s="39"/>
       <c r="AC51" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD51" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6294,11 +6292,11 @@
         <v>125</v>
       </c>
       <c r="L52" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M52" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O52" s="71"/>
@@ -6311,11 +6309,11 @@
       </c>
       <c r="AB52" s="39"/>
       <c r="AC52" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD52" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6331,11 +6329,11 @@
         <v>128</v>
       </c>
       <c r="L53" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M53" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O53" s="71"/>
@@ -6348,11 +6346,11 @@
       </c>
       <c r="AB53" s="39"/>
       <c r="AC53" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD53" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6368,11 +6366,11 @@
         <v>131</v>
       </c>
       <c r="L54" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M54" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O54" s="71"/>
@@ -6385,11 +6383,11 @@
       </c>
       <c r="AB54" s="39"/>
       <c r="AC54" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD54" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6399,17 +6397,17 @@
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="69" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E55" s="69" t="s">
         <v>133</v>
       </c>
       <c r="L55" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M55" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O55" s="71"/>
@@ -6422,11 +6420,11 @@
       </c>
       <c r="AB55" s="39"/>
       <c r="AC55" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD55" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6436,17 +6434,17 @@
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="69" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E56" s="69" t="s">
         <v>135</v>
       </c>
       <c r="L56" s="66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TBD</v>
       </c>
       <c r="M56" s="67" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O56" s="71"/>
@@ -6459,11 +6457,11 @@
       </c>
       <c r="AB56" s="39"/>
       <c r="AC56" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD56" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6473,17 +6471,17 @@
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="69" t="s">
+        <v>337</v>
+      </c>
+      <c r="E57" s="69" t="s">
         <v>338</v>
       </c>
-      <c r="E57" s="69" t="s">
-        <v>339</v>
-      </c>
       <c r="L57" s="66" t="str">
-        <f t="shared" ref="L57" si="8">IF(O61="","TBD",IF(O61=1,"YES",IF(O61=3,"NA","")))</f>
+        <f t="shared" ref="L57" si="10">IF(O61="","TBD",IF(O61=1,"YES",IF(O61=3,"NA","")))</f>
         <v>TBD</v>
       </c>
       <c r="M57" s="67" t="str">
-        <f t="shared" ref="M57" si="9">IF(O61=2,"NO","")</f>
+        <f t="shared" ref="M57" si="11">IF(O61=2,"NO","")</f>
         <v/>
       </c>
       <c r="O57" s="71"/>
@@ -6496,11 +6494,11 @@
       </c>
       <c r="AB57" s="39"/>
       <c r="AC57" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD57" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6521,11 +6519,11 @@
       </c>
       <c r="AB58" s="39"/>
       <c r="AC58" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD58" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6550,11 +6548,11 @@
       </c>
       <c r="AB59" s="39"/>
       <c r="AC59" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD59" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6565,7 +6563,7 @@
       <c r="B60" s="21"/>
       <c r="C60" s="69"/>
       <c r="E60" s="69" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L60" s="66" t="str">
         <f>IF(O63="","TBD",IF(O63=1,"YES",IF(O63=3,"NA","")))</f>
@@ -6591,7 +6589,7 @@
       <c r="B61" s="21"/>
       <c r="C61" s="69"/>
       <c r="E61" s="69" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L61" s="66" t="str">
         <f>IF(O64="","TBD",IF(O64=1,"YES",IF(O64=3,"NA","")))</f>
@@ -6603,7 +6601,7 @@
       </c>
       <c r="O61" s="71"/>
       <c r="P61" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y61" s="25"/>
       <c r="AA61" s="28" t="s">
@@ -6611,11 +6609,11 @@
       </c>
       <c r="AB61" s="39"/>
       <c r="AC61" s="40" t="str">
-        <f t="shared" ref="AC61:AC77" si="10">IF(AB61&lt;&gt;AD61,"Change","")</f>
+        <f t="shared" ref="AC61:AC77" si="12">IF(AB61&lt;&gt;AD61,"Change","")</f>
         <v/>
       </c>
       <c r="AD61" s="47" t="str">
-        <f t="shared" ref="AD61:AD77" si="11">IF(R72="","",R72)</f>
+        <f t="shared" ref="AD61:AD77" si="13">IF(R72="","",R72)</f>
         <v/>
       </c>
     </row>
@@ -6626,7 +6624,7 @@
       <c r="B62" s="21"/>
       <c r="C62" s="69"/>
       <c r="E62" s="69" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L62" s="66" t="str">
         <f>IF(O65="","TBD",IF(O65=1,"YES",IF(O65=3,"NA","")))</f>
@@ -6646,11 +6644,11 @@
       </c>
       <c r="AB62" s="39"/>
       <c r="AC62" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD62" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6660,7 +6658,7 @@
       </c>
       <c r="B63" s="21"/>
       <c r="E63" s="69" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L63" s="66" t="str">
         <f>IF(O66="","TBD",IF(O66=1,"YES",IF(O66=3,"NA","")))</f>
@@ -6675,7 +6673,7 @@
         <v>3</v>
       </c>
       <c r="P63" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="Y63" s="25"/>
       <c r="AA63" s="28" t="s">
@@ -6683,11 +6681,11 @@
       </c>
       <c r="AB63" s="39"/>
       <c r="AC63" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD63" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6712,7 +6710,7 @@
         <v>3</v>
       </c>
       <c r="P64" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="Y64" s="25"/>
       <c r="AA64" s="28" t="s">
@@ -6720,11 +6718,11 @@
       </c>
       <c r="AB64" s="39"/>
       <c r="AC64" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD64" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6751,7 +6749,7 @@
         <v>3</v>
       </c>
       <c r="P65" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Y65" s="25"/>
       <c r="AA65" s="28" t="s">
@@ -6759,11 +6757,11 @@
       </c>
       <c r="AB65" s="39"/>
       <c r="AC65" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD65" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6790,7 +6788,7 @@
         <v>3</v>
       </c>
       <c r="P66" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Y66" s="25"/>
       <c r="AA66" s="28" t="s">
@@ -6798,11 +6796,11 @@
       </c>
       <c r="AB66" s="39"/>
       <c r="AC66" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD66" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6830,11 +6828,11 @@
       </c>
       <c r="AB67" s="39"/>
       <c r="AC67" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD67" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6854,11 +6852,11 @@
       </c>
       <c r="AB68" s="39"/>
       <c r="AC68" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD68" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6888,11 +6886,11 @@
       </c>
       <c r="AB69" s="39"/>
       <c r="AC69" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD69" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6902,27 +6900,27 @@
       </c>
       <c r="B70" s="21"/>
       <c r="E70" s="69"/>
-      <c r="F70" s="290" t="s">
+      <c r="F70" s="285" t="s">
         <v>146</v>
       </c>
-      <c r="G70" s="290"/>
-      <c r="H70" s="290"/>
-      <c r="I70" s="290" t="s">
+      <c r="G70" s="285"/>
+      <c r="H70" s="285"/>
+      <c r="I70" s="285" t="s">
         <v>147</v>
       </c>
-      <c r="J70" s="290"/>
+      <c r="J70" s="285"/>
       <c r="M70" s="23"/>
       <c r="O70" s="44"/>
       <c r="P70" s="17"/>
-      <c r="Q70" s="291" t="s">
+      <c r="Q70" s="286" t="s">
         <v>146</v>
       </c>
-      <c r="R70" s="291"/>
-      <c r="S70" s="291"/>
-      <c r="T70" s="291" t="s">
+      <c r="R70" s="286"/>
+      <c r="S70" s="286"/>
+      <c r="T70" s="286" t="s">
         <v>147</v>
       </c>
-      <c r="U70" s="291"/>
+      <c r="U70" s="286"/>
       <c r="V70" s="17"/>
       <c r="W70" s="17"/>
       <c r="X70" s="17"/>
@@ -6932,11 +6930,11 @@
       </c>
       <c r="AB70" s="39"/>
       <c r="AC70" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD70" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -6984,11 +6982,11 @@
       </c>
       <c r="AB71" s="39"/>
       <c r="AC71" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD71" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -7001,23 +6999,23 @@
         <v>107</v>
       </c>
       <c r="F72" s="251" t="str">
-        <f t="shared" ref="F72:F88" si="12">IF(Q72="","",Q72)</f>
+        <f t="shared" ref="F72:F88" si="14">IF(Q72="","",Q72)</f>
         <v/>
       </c>
       <c r="G72" s="252" t="str">
-        <f t="shared" ref="G72:G88" si="13">IF(R72="","",R72)</f>
+        <f t="shared" ref="G72:G88" si="15">IF(R72="","",R72)</f>
         <v/>
       </c>
       <c r="H72" s="252" t="str">
-        <f t="shared" ref="H72:H88" si="14">IF(S72="","",S72)</f>
+        <f t="shared" ref="H72:H88" si="16">IF(S72="","",S72)</f>
         <v/>
       </c>
       <c r="I72" s="252" t="str">
-        <f t="shared" ref="I72:I88" si="15">IF(T72="","",T72)</f>
+        <f t="shared" ref="I72:I88" si="17">IF(T72="","",T72)</f>
         <v/>
       </c>
       <c r="J72" s="253" t="str">
-        <f t="shared" ref="J72:J88" si="16">IF(U72="","",U72)</f>
+        <f t="shared" ref="J72:J88" si="18">IF(U72="","",U72)</f>
         <v/>
       </c>
       <c r="M72" s="23"/>
@@ -7026,23 +7024,23 @@
         <v>107</v>
       </c>
       <c r="Q72" s="238" t="str">
-        <f t="shared" ref="Q72:Q88" si="17">IF(Q91&lt;&gt;"",Q91,IF(AB43="","",AB43))</f>
+        <f t="shared" ref="Q72:Q88" si="19">IF(Q91&lt;&gt;"",Q91,IF(AB43="","",AB43))</f>
         <v/>
       </c>
       <c r="R72" s="238" t="str">
-        <f t="shared" ref="R72:R88" si="18">IF(R91&lt;&gt;"",R91,IF(AB61="","",AB61))</f>
+        <f t="shared" ref="R72:R88" si="20">IF(R91&lt;&gt;"",R91,IF(AB61="","",AB61))</f>
         <v/>
       </c>
       <c r="S72" s="238" t="str">
-        <f t="shared" ref="S72:S88" si="19">IF(S91&lt;&gt;"",S91,IF(AB79="","",AB79))</f>
+        <f t="shared" ref="S72:S88" si="21">IF(S91&lt;&gt;"",S91,IF(AB79="","",AB79))</f>
         <v/>
       </c>
       <c r="T72" s="238" t="str">
-        <f t="shared" ref="T72:T88" si="20">IF(T91&lt;&gt;"",T91,IF(AB97="","",AB97))</f>
+        <f t="shared" ref="T72:T88" si="22">IF(T91&lt;&gt;"",T91,IF(AB97="","",AB97))</f>
         <v/>
       </c>
       <c r="U72" s="238" t="str">
-        <f t="shared" ref="U72:U88" si="21">IF(U91&lt;&gt;"",U91,IF(AB115="","",AB115))</f>
+        <f t="shared" ref="U72:U88" si="23">IF(U91&lt;&gt;"",U91,IF(AB115="","",AB115))</f>
         <v/>
       </c>
       <c r="Y72" s="25"/>
@@ -7051,11 +7049,11 @@
       </c>
       <c r="AB72" s="39"/>
       <c r="AC72" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD72" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -7068,23 +7066,23 @@
         <v>109</v>
       </c>
       <c r="F73" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G73" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H73" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I73" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J73" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M73" s="23"/>
@@ -7093,23 +7091,23 @@
         <v>109</v>
       </c>
       <c r="Q73" s="239" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R73" s="239" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S73" s="239" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T73" s="239" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U73" s="239" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y73" s="25"/>
@@ -7118,11 +7116,11 @@
       </c>
       <c r="AB73" s="39"/>
       <c r="AC73" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD73" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -7135,23 +7133,23 @@
         <v>111</v>
       </c>
       <c r="F74" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G74" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H74" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I74" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J74" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M74" s="23"/>
@@ -7160,23 +7158,23 @@
         <v>111</v>
       </c>
       <c r="Q74" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R74" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S74" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T74" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U74" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y74" s="25"/>
@@ -7185,11 +7183,11 @@
       </c>
       <c r="AB74" s="39"/>
       <c r="AC74" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD74" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -7202,23 +7200,23 @@
         <v>112</v>
       </c>
       <c r="F75" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G75" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H75" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I75" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J75" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M75" s="23"/>
@@ -7227,23 +7225,23 @@
         <v>112</v>
       </c>
       <c r="Q75" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R75" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S75" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T75" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U75" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y75" s="25"/>
@@ -7252,11 +7250,11 @@
       </c>
       <c r="AB75" s="39"/>
       <c r="AC75" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD75" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -7269,23 +7267,23 @@
         <v>114</v>
       </c>
       <c r="F76" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G76" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H76" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I76" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J76" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M76" s="23"/>
@@ -7294,23 +7292,23 @@
         <v>114</v>
       </c>
       <c r="Q76" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R76" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S76" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T76" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U76" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y76" s="25"/>
@@ -7319,11 +7317,11 @@
       </c>
       <c r="AB76" s="39"/>
       <c r="AC76" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD76" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -7336,23 +7334,23 @@
         <v>116</v>
       </c>
       <c r="F77" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G77" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H77" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I77" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J77" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M77" s="23"/>
@@ -7361,23 +7359,23 @@
         <v>116</v>
       </c>
       <c r="Q77" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R77" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S77" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T77" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U77" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y77" s="25"/>
@@ -7386,11 +7384,11 @@
       </c>
       <c r="AB77" s="39"/>
       <c r="AC77" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD77" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -7403,23 +7401,23 @@
         <v>118</v>
       </c>
       <c r="F78" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G78" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H78" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I78" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J78" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M78" s="23"/>
@@ -7428,23 +7426,23 @@
         <v>118</v>
       </c>
       <c r="Q78" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R78" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S78" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T78" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U78" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y78" s="25"/>
@@ -7464,23 +7462,23 @@
         <v>120</v>
       </c>
       <c r="F79" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G79" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H79" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I79" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J79" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M79" s="23"/>
@@ -7489,23 +7487,23 @@
         <v>120</v>
       </c>
       <c r="Q79" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R79" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S79" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T79" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U79" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y79" s="25"/>
@@ -7514,11 +7512,11 @@
       </c>
       <c r="AB79" s="39"/>
       <c r="AC79" s="40" t="str">
-        <f t="shared" ref="AC79:AC95" si="22">IF(AB79&lt;&gt;AD79,"Change","")</f>
+        <f t="shared" ref="AC79:AC95" si="24">IF(AB79&lt;&gt;AD79,"Change","")</f>
         <v/>
       </c>
       <c r="AD79" s="47" t="str">
-        <f t="shared" ref="AD79:AD95" si="23">IF(S72="","",S72)</f>
+        <f t="shared" ref="AD79:AD95" si="25">IF(S72="","",S72)</f>
         <v/>
       </c>
     </row>
@@ -7531,23 +7529,23 @@
         <v>123</v>
       </c>
       <c r="F80" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G80" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H80" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I80" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J80" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M80" s="23"/>
@@ -7556,23 +7554,23 @@
         <v>123</v>
       </c>
       <c r="Q80" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R80" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S80" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T80" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U80" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y80" s="25"/>
@@ -7581,11 +7579,11 @@
       </c>
       <c r="AB80" s="39"/>
       <c r="AC80" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD80" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -7598,23 +7596,23 @@
         <v>126</v>
       </c>
       <c r="F81" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G81" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H81" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I81" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J81" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M81" s="23"/>
@@ -7623,23 +7621,23 @@
         <v>126</v>
       </c>
       <c r="Q81" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R81" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S81" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T81" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U81" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y81" s="25"/>
@@ -7648,11 +7646,11 @@
       </c>
       <c r="AB81" s="39"/>
       <c r="AC81" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD81" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -7665,23 +7663,23 @@
         <v>129</v>
       </c>
       <c r="F82" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G82" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H82" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I82" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J82" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M82" s="23"/>
@@ -7690,23 +7688,23 @@
         <v>129</v>
       </c>
       <c r="Q82" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R82" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S82" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T82" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U82" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y82" s="25"/>
@@ -7715,11 +7713,11 @@
       </c>
       <c r="AB82" s="39"/>
       <c r="AC82" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD82" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -7732,23 +7730,23 @@
         <v>132</v>
       </c>
       <c r="F83" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G83" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H83" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I83" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J83" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M83" s="23"/>
@@ -7757,23 +7755,23 @@
         <v>132</v>
       </c>
       <c r="Q83" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R83" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S83" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T83" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U83" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y83" s="25"/>
@@ -7782,11 +7780,11 @@
       </c>
       <c r="AB83" s="39"/>
       <c r="AC83" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD83" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -7799,23 +7797,23 @@
         <v>134</v>
       </c>
       <c r="F84" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G84" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H84" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I84" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J84" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M84" s="23"/>
@@ -7824,23 +7822,23 @@
         <v>134</v>
       </c>
       <c r="Q84" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R84" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S84" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T84" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U84" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y84" s="25"/>
@@ -7849,11 +7847,11 @@
       </c>
       <c r="AB84" s="39"/>
       <c r="AC84" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD84" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -7866,23 +7864,23 @@
         <v>137</v>
       </c>
       <c r="F85" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G85" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H85" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I85" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J85" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M85" s="23"/>
@@ -7891,23 +7889,23 @@
         <v>137</v>
       </c>
       <c r="Q85" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R85" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S85" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T85" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U85" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y85" s="25"/>
@@ -7916,11 +7914,11 @@
       </c>
       <c r="AB85" s="39"/>
       <c r="AC85" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD85" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -7933,23 +7931,23 @@
         <v>139</v>
       </c>
       <c r="F86" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G86" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H86" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I86" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J86" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M86" s="23"/>
@@ -7958,23 +7956,23 @@
         <v>139</v>
       </c>
       <c r="Q86" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R86" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S86" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T86" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U86" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y86" s="25"/>
@@ -7983,11 +7981,11 @@
       </c>
       <c r="AB86" s="39"/>
       <c r="AC86" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD86" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8000,23 +7998,23 @@
         <v>142</v>
       </c>
       <c r="F87" s="254" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G87" s="255" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H87" s="255" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I87" s="255" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J87" s="256" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M87" s="23"/>
@@ -8025,23 +8023,23 @@
         <v>142</v>
       </c>
       <c r="Q87" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R87" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S87" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T87" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U87" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y87" s="25"/>
@@ -8050,11 +8048,11 @@
       </c>
       <c r="AB87" s="39"/>
       <c r="AC87" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD87" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8067,23 +8065,23 @@
         <v>143</v>
       </c>
       <c r="F88" s="257" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G88" s="258" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H88" s="258" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I88" s="258" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J88" s="259" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M88" s="23"/>
@@ -8092,23 +8090,23 @@
         <v>143</v>
       </c>
       <c r="Q88" s="238" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="R88" s="238" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S88" s="238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="T88" s="238" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="U88" s="238" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Y88" s="25"/>
@@ -8117,11 +8115,11 @@
       </c>
       <c r="AB88" s="39"/>
       <c r="AC88" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD88" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8143,26 +8141,26 @@
       <c r="M89" s="87"/>
       <c r="O89" s="24"/>
       <c r="P89" s="53"/>
-      <c r="Q89" s="279" t="s">
+      <c r="Q89" s="287" t="s">
         <v>146</v>
       </c>
-      <c r="R89" s="279"/>
-      <c r="S89" s="279"/>
-      <c r="T89" s="279" t="s">
+      <c r="R89" s="287"/>
+      <c r="S89" s="287"/>
+      <c r="T89" s="287" t="s">
         <v>147</v>
       </c>
-      <c r="U89" s="279"/>
+      <c r="U89" s="287"/>
       <c r="Y89" s="25"/>
       <c r="AA89" s="28" t="s">
         <v>129</v>
       </c>
       <c r="AB89" s="39"/>
       <c r="AC89" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD89" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8197,11 +8195,11 @@
       </c>
       <c r="AB90" s="39"/>
       <c r="AC90" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD90" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8211,14 +8209,14 @@
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D91" s="165" t="str">
         <f>IF(P112="","",P112)</f>
         <v>Piranha</v>
       </c>
       <c r="G91" s="264" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H91" s="273" t="str">
         <f>IF(S112="","",S112)</f>
@@ -8240,11 +8238,11 @@
       </c>
       <c r="AB91" s="39"/>
       <c r="AC91" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD91" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8254,14 +8252,14 @@
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D92" s="272" t="str">
         <f>IF(P113="","",P113)</f>
         <v/>
       </c>
       <c r="G92" s="264" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H92" s="273" t="str">
         <f>IF(S113="","",S113)</f>
@@ -8272,9 +8270,18 @@
       <c r="P92" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="Q92" s="241"/>
-      <c r="R92" s="241"/>
-      <c r="S92" s="241"/>
+      <c r="Q92" s="241" t="str">
+        <f t="shared" ref="Q92:S92" si="26">IF(OR(Q93="",Q95=""),"",Q93/Q95)</f>
+        <v/>
+      </c>
+      <c r="R92" s="241" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="S92" s="241" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
       <c r="T92" s="241" t="str">
         <f>IF(OR(T93="",T95=""),"",T93/T95)</f>
         <v/>
@@ -8289,11 +8296,11 @@
       </c>
       <c r="AB92" s="39"/>
       <c r="AC92" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD92" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8307,9 +8314,18 @@
       <c r="P93" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="Q93" s="240"/>
-      <c r="R93" s="240"/>
-      <c r="S93" s="240"/>
+      <c r="Q93" s="240" t="str">
+        <f t="shared" ref="Q93:S93" si="27">IF(OR(Q94="",Q103=""),"",Q94*Q103)</f>
+        <v/>
+      </c>
+      <c r="R93" s="240" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="S93" s="240" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
       <c r="T93" s="240" t="str">
         <f>IF(OR(T94="",T103=""),"",T94*T103)</f>
         <v/>
@@ -8324,11 +8340,11 @@
       </c>
       <c r="AB93" s="39"/>
       <c r="AC93" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD93" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8338,15 +8354,15 @@
       </c>
       <c r="B94" s="21"/>
       <c r="E94" s="69"/>
-      <c r="F94" s="283" t="s">
+      <c r="F94" s="291" t="s">
         <v>146</v>
       </c>
-      <c r="G94" s="283"/>
-      <c r="H94" s="283"/>
-      <c r="I94" s="284" t="s">
+      <c r="G94" s="291"/>
+      <c r="H94" s="291"/>
+      <c r="I94" s="292" t="s">
         <v>147</v>
       </c>
-      <c r="J94" s="284"/>
+      <c r="J94" s="292"/>
       <c r="M94" s="23"/>
       <c r="O94" s="24"/>
       <c r="P94" s="28" t="s">
@@ -8363,11 +8379,11 @@
       </c>
       <c r="AB94" s="39"/>
       <c r="AC94" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD94" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8411,11 +8427,11 @@
       </c>
       <c r="AB95" s="39"/>
       <c r="AC95" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AD95" s="47" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
     </row>
@@ -8471,28 +8487,28 @@
         <v>31</v>
       </c>
       <c r="B97" s="21"/>
-      <c r="D97" s="288" t="s">
+      <c r="D97" s="296" t="s">
         <v>156</v>
       </c>
-      <c r="E97" s="289"/>
+      <c r="E97" s="297"/>
       <c r="F97" s="95" t="str">
-        <f t="shared" ref="F97:J102" si="24">IF(Q118="","",Q118)</f>
+        <f t="shared" ref="F97:J102" si="28">IF(Q118="","",Q118)</f>
         <v/>
       </c>
       <c r="G97" s="96" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H97" s="97" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="I97" s="96" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J97" s="97" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="K97" s="20"/>
@@ -8517,11 +8533,11 @@
       </c>
       <c r="AB97" s="39"/>
       <c r="AC97" s="40" t="str">
-        <f t="shared" ref="AC97:AC113" si="25">IF(AB97&lt;&gt;AD97,"Change","")</f>
+        <f t="shared" ref="AC97:AC113" si="29">IF(AB97&lt;&gt;AD97,"Change","")</f>
         <v/>
       </c>
       <c r="AD97" s="47" t="str">
-        <f t="shared" ref="AD97:AD113" si="26">IF(T72="","",T72)</f>
+        <f t="shared" ref="AD97:AD113" si="30">IF(T72="","",T72)</f>
         <v/>
       </c>
     </row>
@@ -8530,26 +8546,26 @@
         <v>32</v>
       </c>
       <c r="B98" s="21"/>
-      <c r="D98" s="288"/>
-      <c r="E98" s="289"/>
+      <c r="D98" s="296"/>
+      <c r="E98" s="297"/>
       <c r="F98" s="100" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G98" s="101" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H98" s="102" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="I98" s="101" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J98" s="102" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="K98" s="20"/>
@@ -8574,11 +8590,11 @@
       </c>
       <c r="AB98" s="39"/>
       <c r="AC98" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD98" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -8587,26 +8603,26 @@
         <v>33</v>
       </c>
       <c r="B99" s="21"/>
-      <c r="D99" s="288"/>
-      <c r="E99" s="289"/>
+      <c r="D99" s="296"/>
+      <c r="E99" s="297"/>
       <c r="F99" s="105" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G99" s="106" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H99" s="107" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="I99" s="106" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J99" s="107" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="K99" s="108" t="s">
@@ -8633,11 +8649,11 @@
       </c>
       <c r="AB99" s="39"/>
       <c r="AC99" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD99" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -8651,23 +8667,23 @@
         <v>160</v>
       </c>
       <c r="F100" s="111" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G100" s="112" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H100" s="113" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="I100" s="114" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J100" s="115" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="K100" s="116" t="s">
@@ -8694,11 +8710,11 @@
       </c>
       <c r="AB100" s="39"/>
       <c r="AC100" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD100" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -8712,23 +8728,23 @@
         <v>162</v>
       </c>
       <c r="F101" s="77" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G101" s="78" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H101" s="79" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="I101" s="78" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J101" s="79" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="K101" s="116" t="s">
@@ -8755,11 +8771,11 @@
       </c>
       <c r="AB101" s="39"/>
       <c r="AC101" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD101" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -8772,23 +8788,23 @@
         <v>164</v>
       </c>
       <c r="F102" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="G102" s="84" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="H102" s="85" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="I102" s="84" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J102" s="85" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="K102" s="116" t="s">
@@ -8804,9 +8820,18 @@
       <c r="P102" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="Q102" s="240"/>
-      <c r="R102" s="240"/>
-      <c r="S102" s="240"/>
+      <c r="Q102" s="240" t="str">
+        <f t="shared" ref="Q102:S102" si="31">IF(OR(Q100="",Q101="",Q103=""),"",(Q101*Q100)*Q103)</f>
+        <v/>
+      </c>
+      <c r="R102" s="240" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="S102" s="240" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
       <c r="T102" s="240" t="str">
         <f>IF(OR(T100="",T101="",T103=""),"",(T101*T100)*T103)</f>
         <v/>
@@ -8821,11 +8846,11 @@
       </c>
       <c r="AB102" s="39"/>
       <c r="AC102" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD102" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -8838,23 +8863,23 @@
         <v>166</v>
       </c>
       <c r="F103" s="119" t="str">
-        <f t="shared" ref="F103:J106" si="27">IF(Q125="","",Q125)</f>
+        <f t="shared" ref="F103:J106" si="32">IF(Q125="","",Q125)</f>
         <v/>
       </c>
       <c r="G103" s="120" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H103" s="121" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I103" s="120" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J103" s="121" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K103" s="122" t="s">
@@ -8881,11 +8906,11 @@
       </c>
       <c r="AB103" s="39"/>
       <c r="AC103" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD103" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -8898,23 +8923,23 @@
         <v>168</v>
       </c>
       <c r="F104" s="125" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G104" s="126" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H104" s="127" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I104" s="126" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J104" s="127" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M104" s="23"/>
@@ -8933,11 +8958,11 @@
       </c>
       <c r="AB104" s="39"/>
       <c r="AC104" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD104" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -8952,23 +8977,23 @@
         <v>169</v>
       </c>
       <c r="F105" s="92" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G105" s="93" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H105" s="94" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I105" s="93" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J105" s="94" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M105" s="23"/>
@@ -8987,11 +9012,11 @@
       </c>
       <c r="AB105" s="39"/>
       <c r="AC105" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD105" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9006,23 +9031,23 @@
         <v>170</v>
       </c>
       <c r="F106" s="128" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G106" s="129" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H106" s="130" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I106" s="129" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J106" s="130" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M106" s="23"/>
@@ -9041,11 +9066,11 @@
       </c>
       <c r="AB106" s="39"/>
       <c r="AC106" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD106" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9084,11 +9109,11 @@
       </c>
       <c r="AB107" s="39"/>
       <c r="AC107" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD107" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9125,11 +9150,11 @@
       </c>
       <c r="AB108" s="39"/>
       <c r="AC108" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD108" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9145,11 +9170,11 @@
       </c>
       <c r="AB109" s="39"/>
       <c r="AC109" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD109" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9171,11 +9196,11 @@
       </c>
       <c r="AB110" s="39"/>
       <c r="AC110" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD110" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9188,19 +9213,19 @@
         <v>172</v>
       </c>
       <c r="E111" s="77" t="str">
-        <f t="shared" ref="E111:H114" si="28">IF(Q133="","",Q133)</f>
+        <f t="shared" ref="E111:H114" si="33">IF(Q133="","",Q133)</f>
         <v/>
       </c>
       <c r="F111" s="78" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G111" s="78" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H111" s="79" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J111" s="20"/>
@@ -9223,11 +9248,11 @@
       </c>
       <c r="AB111" s="39"/>
       <c r="AC111" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD111" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9240,31 +9265,31 @@
         <v>173</v>
       </c>
       <c r="E112" s="80" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="F112" s="81" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G112" s="81" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H112" s="82" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J112" s="20"/>
       <c r="M112" s="23"/>
       <c r="O112" s="266" t="s">
+        <v>339</v>
+      </c>
+      <c r="P112" s="267" t="s">
         <v>340</v>
       </c>
-      <c r="P112" s="267" t="s">
-        <v>341</v>
-      </c>
       <c r="R112" s="265" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="S112" s="270"/>
       <c r="T112" s="269"/>
@@ -9274,11 +9299,11 @@
       </c>
       <c r="AB112" s="39"/>
       <c r="AC112" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD112" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9291,29 +9316,29 @@
         <v>174</v>
       </c>
       <c r="E113" s="80" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="F113" s="81" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G113" s="81" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H113" s="82" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J113" s="20"/>
       <c r="M113" s="23"/>
       <c r="O113" s="266" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="P113" s="268"/>
       <c r="R113" s="265" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="S113" s="271"/>
       <c r="T113" s="269"/>
@@ -9323,11 +9348,11 @@
       </c>
       <c r="AB113" s="39"/>
       <c r="AC113" s="40" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AD113" s="47" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -9340,19 +9365,19 @@
         <v>175</v>
       </c>
       <c r="E114" s="80" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="F114" s="81" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G114" s="81" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H114" s="82" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J114" s="20"/>
@@ -9390,15 +9415,15 @@
       <c r="J115" s="20"/>
       <c r="M115" s="23"/>
       <c r="O115" s="24"/>
-      <c r="Q115" s="285" t="s">
+      <c r="Q115" s="293" t="s">
         <v>146</v>
       </c>
-      <c r="R115" s="285"/>
-      <c r="S115" s="285"/>
-      <c r="T115" s="281" t="s">
+      <c r="R115" s="293"/>
+      <c r="S115" s="293"/>
+      <c r="T115" s="289" t="s">
         <v>147</v>
       </c>
-      <c r="U115" s="281"/>
+      <c r="U115" s="289"/>
       <c r="W115" s="56" t="s">
         <v>153</v>
       </c>
@@ -9408,11 +9433,11 @@
       </c>
       <c r="AB115" s="39"/>
       <c r="AC115" s="40" t="str">
-        <f t="shared" ref="AC115:AC131" si="29">IF(AB115&lt;&gt;AD115,"Change","")</f>
+        <f t="shared" ref="AC115:AC131" si="34">IF(AB115&lt;&gt;AD115,"Change","")</f>
         <v/>
       </c>
       <c r="AD115" s="47" t="str">
-        <f t="shared" ref="AD115:AD131" si="30">IF(U72="","",U72)</f>
+        <f t="shared" ref="AD115:AD131" si="35">IF(U72="","",U72)</f>
         <v/>
       </c>
     </row>
@@ -9453,11 +9478,11 @@
       </c>
       <c r="AB116" s="39"/>
       <c r="AC116" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD116" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9523,11 +9548,11 @@
       </c>
       <c r="AB117" s="39"/>
       <c r="AC117" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD117" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9546,10 +9571,10 @@
       <c r="I118" s="20"/>
       <c r="J118" s="20"/>
       <c r="M118" s="23"/>
-      <c r="O118" s="287" t="s">
+      <c r="O118" s="295" t="s">
         <v>156</v>
       </c>
-      <c r="P118" s="286"/>
+      <c r="P118" s="294"/>
       <c r="Q118" s="138"/>
       <c r="R118" s="139"/>
       <c r="S118" s="140"/>
@@ -9567,11 +9592,11 @@
       </c>
       <c r="AB118" s="39"/>
       <c r="AC118" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD118" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9587,8 +9612,8 @@
       <c r="I119" s="20"/>
       <c r="J119" s="20"/>
       <c r="M119" s="23"/>
-      <c r="O119" s="287"/>
-      <c r="P119" s="286"/>
+      <c r="O119" s="295"/>
+      <c r="P119" s="294"/>
       <c r="Q119" s="141"/>
       <c r="R119" s="142"/>
       <c r="S119" s="143"/>
@@ -9608,11 +9633,11 @@
       </c>
       <c r="AB119" s="39"/>
       <c r="AC119" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD119" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9622,8 +9647,8 @@
       </c>
       <c r="B120" s="21"/>
       <c r="M120" s="23"/>
-      <c r="O120" s="287"/>
-      <c r="P120" s="286"/>
+      <c r="O120" s="295"/>
+      <c r="P120" s="294"/>
       <c r="Q120" s="145"/>
       <c r="R120" s="146"/>
       <c r="S120" s="147"/>
@@ -9643,11 +9668,11 @@
       </c>
       <c r="AB120" s="39"/>
       <c r="AC120" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD120" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9698,11 +9723,11 @@
       </c>
       <c r="AB121" s="39"/>
       <c r="AC121" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD121" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9743,11 +9768,11 @@
       </c>
       <c r="AB122" s="39"/>
       <c r="AC122" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD122" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9780,11 +9805,11 @@
       </c>
       <c r="AB123" s="39"/>
       <c r="AC123" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD123" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9827,11 +9852,11 @@
       </c>
       <c r="AB124" s="39"/>
       <c r="AC124" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD124" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9847,7 +9872,7 @@
       <c r="D125" s="69" t="s">
         <v>185</v>
       </c>
-      <c r="F125" s="165" t="str">
+      <c r="F125" s="276" t="str">
         <f>IF(O207="","",O207)</f>
         <v/>
       </c>
@@ -9890,11 +9915,11 @@
       </c>
       <c r="AB125" s="39"/>
       <c r="AC125" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD125" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -9911,7 +9936,7 @@
         <v>188</v>
       </c>
       <c r="E126" s="53"/>
-      <c r="F126" s="165" t="str">
+      <c r="F126" s="276" t="str">
         <f>IF(O208="","",O208)</f>
         <v/>
       </c>
@@ -9955,11 +9980,11 @@
       </c>
       <c r="AB126" s="39"/>
       <c r="AC126" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD126" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -10015,11 +10040,11 @@
       </c>
       <c r="AB127" s="39"/>
       <c r="AC127" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD127" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -10061,11 +10086,11 @@
       </c>
       <c r="AB128" s="39"/>
       <c r="AC128" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD128" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -10110,11 +10135,11 @@
       </c>
       <c r="AB129" s="39"/>
       <c r="AC129" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD129" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -10154,11 +10179,11 @@
       </c>
       <c r="AB130" s="39"/>
       <c r="AC130" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD130" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -10198,11 +10223,11 @@
       </c>
       <c r="AB131" s="39"/>
       <c r="AC131" s="40" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AD131" s="47" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -10399,7 +10424,7 @@
       <c r="C137" s="53"/>
       <c r="M137" s="23"/>
       <c r="O137" s="24"/>
-      <c r="P137" s="286" t="s">
+      <c r="P137" s="294" t="s">
         <v>176</v>
       </c>
       <c r="Q137" s="172"/>
@@ -10443,7 +10468,7 @@
       </c>
       <c r="M138" s="23"/>
       <c r="O138" s="24"/>
-      <c r="P138" s="286"/>
+      <c r="P138" s="294"/>
       <c r="Q138" s="172"/>
       <c r="R138" s="173"/>
       <c r="S138" s="173"/>
@@ -10487,7 +10512,7 @@
       </c>
       <c r="M139" s="23"/>
       <c r="O139" s="24"/>
-      <c r="P139" s="286"/>
+      <c r="P139" s="294"/>
       <c r="Q139" s="175"/>
       <c r="R139" s="176"/>
       <c r="S139" s="176"/>
@@ -10588,15 +10613,15 @@
         <v/>
       </c>
       <c r="R141" s="136" t="str">
-        <f t="shared" ref="R141:T141" si="31">IF(R140="","",IF(OR(ABS(R136-R140)&lt;=3,ABS(AVERAGE(R137:R139)-R136)/R136&lt;0.3),"Pass","Fail"))</f>
+        <f t="shared" ref="R141:T141" si="36">IF(R140="","",IF(OR(ABS(R136-R140)&lt;=3,ABS(AVERAGE(R137:R139)-R136)/R136&lt;0.3),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="S141" s="136" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="T141" s="137" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="Y141" s="25"/>
@@ -10729,31 +10754,31 @@
         <v>111</v>
       </c>
       <c r="E145" s="80" t="str">
-        <f t="shared" ref="E145:K151" si="32">IF(P158="","",P158)</f>
+        <f t="shared" ref="E145:K151" si="37">IF(P158="","",P158)</f>
         <v/>
       </c>
       <c r="F145" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="G145" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="H145" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="I145" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="J145" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="K145" s="82" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="M145" s="23"/>
@@ -10791,31 +10816,31 @@
         <v>211</v>
       </c>
       <c r="E146" s="80" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="F146" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="G146" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="H146" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="I146" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="J146" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="K146" s="82" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="M146" s="23"/>
@@ -10834,31 +10859,31 @@
         <v>213</v>
       </c>
       <c r="E147" s="80" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="F147" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="G147" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="H147" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="I147" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="J147" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="K147" s="82" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="M147" s="23"/>
@@ -10886,31 +10911,31 @@
         <v>214</v>
       </c>
       <c r="E148" s="80" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="F148" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="G148" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="H148" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="I148" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="J148" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="K148" s="82" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="M148" s="23"/>
@@ -10942,31 +10967,31 @@
         <v>216</v>
       </c>
       <c r="E149" s="80" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="F149" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="G149" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="H149" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="I149" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="J149" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="K149" s="82" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="M149" s="23"/>
@@ -11011,31 +11036,31 @@
         <v>217</v>
       </c>
       <c r="E150" s="80" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="F150" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="G150" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="H150" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="I150" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="J150" s="81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="K150" s="82" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="M150" s="23"/>
@@ -11055,31 +11080,31 @@
         <v>219</v>
       </c>
       <c r="E151" s="83" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="F151" s="84" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="G151" s="84" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="H151" s="84" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="I151" s="84" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="J151" s="84" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="K151" s="85" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="M151" s="23"/>
@@ -11255,23 +11280,23 @@
         <v>225</v>
       </c>
       <c r="F157" s="77" t="str">
-        <f t="shared" ref="F157:J163" si="33">IF(Q170="","",Q170)</f>
+        <f t="shared" ref="F157:J163" si="38">IF(Q170="","",Q170)</f>
         <v/>
       </c>
       <c r="G157" s="78" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="H157" s="78" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="I157" s="78" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="J157" s="79" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="M157" s="23"/>
@@ -11300,10 +11325,10 @@
         <v>150</v>
       </c>
       <c r="W157" s="187"/>
-      <c r="X157" s="279" t="s">
+      <c r="X157" s="287" t="s">
         <v>221</v>
       </c>
-      <c r="Y157" s="280"/>
+      <c r="Y157" s="288"/>
       <c r="AA157" s="28"/>
       <c r="AB157" s="182"/>
       <c r="AC157" s="40" t="str">
@@ -11325,23 +11350,23 @@
         <v>226</v>
       </c>
       <c r="F158" s="80" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="G158" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="H158" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="I158" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="J158" s="82" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="M158" s="23"/>
@@ -11376,23 +11401,23 @@
         <v>227</v>
       </c>
       <c r="F159" s="80" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="G159" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="H159" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="I159" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="J159" s="82" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="M159" s="23"/>
@@ -11436,23 +11461,23 @@
         <v>200</v>
       </c>
       <c r="F160" s="80" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="G160" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="H160" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="I160" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="J160" s="82" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="M160" s="23"/>
@@ -11489,23 +11514,23 @@
         <v>228</v>
       </c>
       <c r="F161" s="80" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="G161" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="H161" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="I161" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="J161" s="82" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="M161" s="23"/>
@@ -11549,23 +11574,23 @@
         <v>229</v>
       </c>
       <c r="F162" s="83" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="G162" s="84" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="H162" s="84" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="I162" s="84" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="J162" s="85" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="M162" s="23"/>
@@ -11602,23 +11627,23 @@
         <v>169</v>
       </c>
       <c r="F163" s="92" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="G163" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="H163" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="I163" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="J163" s="94" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="M163" s="23"/>
@@ -11764,14 +11789,14 @@
       <c r="B168" s="21"/>
       <c r="C168" s="53"/>
       <c r="D168" s="69"/>
-      <c r="E168" s="282" t="s">
+      <c r="E168" s="290" t="s">
         <v>146</v>
       </c>
-      <c r="F168" s="282"/>
-      <c r="G168" s="282" t="s">
+      <c r="F168" s="290"/>
+      <c r="G168" s="290" t="s">
         <v>147</v>
       </c>
-      <c r="H168" s="282"/>
+      <c r="H168" s="290"/>
       <c r="M168" s="23"/>
       <c r="O168" s="24"/>
       <c r="Y168" s="25"/>
@@ -11824,19 +11849,19 @@
         <v>233</v>
       </c>
       <c r="E170" s="77" t="str">
-        <f t="shared" ref="E170:H174" si="34">IF(P183="","",P183)</f>
+        <f t="shared" ref="E170:H174" si="39">IF(P183="","",P183)</f>
         <v/>
       </c>
       <c r="F170" s="78" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="G170" s="78" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="H170" s="79" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="J170" s="48" t="s">
@@ -11871,19 +11896,19 @@
         <v>235</v>
       </c>
       <c r="E171" s="80" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="F171" s="81" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="G171" s="81" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="H171" s="82" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="J171" s="48" t="s">
@@ -11925,19 +11950,19 @@
         <v>236</v>
       </c>
       <c r="E172" s="80" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="F172" s="81" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="G172" s="81" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="H172" s="82" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="M172" s="23"/>
@@ -11965,19 +11990,19 @@
         <v>237</v>
       </c>
       <c r="E173" s="80" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="F173" s="81" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="G173" s="81" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="H173" s="82" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="M173" s="23"/>
@@ -12027,19 +12052,19 @@
         <v>238</v>
       </c>
       <c r="E174" s="105" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="F174" s="106" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="G174" s="106" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="H174" s="107" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="M174" s="23"/>
@@ -12248,23 +12273,23 @@
         <v>246</v>
       </c>
       <c r="D181" s="77" t="str">
-        <f t="shared" ref="D181:H185" si="35">IF(P191="","",P191)</f>
+        <f t="shared" ref="D181:H185" si="40">IF(P191="","",P191)</f>
         <v/>
       </c>
       <c r="E181" s="79" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="F181" s="77" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="G181" s="78" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="H181" s="79" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I181" s="20"/>
@@ -12300,23 +12325,23 @@
         <v>248</v>
       </c>
       <c r="D182" s="80" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="E182" s="82" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="F182" s="80" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="G182" s="81" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="H182" s="82" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I182" s="20"/>
@@ -12352,23 +12377,23 @@
         <v>251</v>
       </c>
       <c r="D183" s="80" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="E183" s="82" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="F183" s="80" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="G183" s="81" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="H183" s="82" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I183" s="20"/>
@@ -12403,23 +12428,23 @@
         <v>253</v>
       </c>
       <c r="D184" s="80" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="E184" s="82" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="F184" s="80" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="G184" s="81" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="H184" s="82" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I184" s="20"/>
@@ -12449,23 +12474,23 @@
         <v>255</v>
       </c>
       <c r="D185" s="83" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="E185" s="85" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="F185" s="83" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="G185" s="84" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="H185" s="85" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I185" s="20"/>
@@ -14869,39 +14894,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="T70:U70"/>
-    <mergeCell ref="Q89:S89"/>
-    <mergeCell ref="T89:U89"/>
     <mergeCell ref="X157:Y157"/>
     <mergeCell ref="T115:U115"/>
     <mergeCell ref="E168:F168"/>
@@ -14912,6 +14904,39 @@
     <mergeCell ref="P137:P139"/>
     <mergeCell ref="O118:P120"/>
     <mergeCell ref="D97:E99"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="Q89:S89"/>
+    <mergeCell ref="T89:U89"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <conditionalFormatting sqref="L33:L38 L60:L63 L41:L57">
     <cfRule type="cellIs" dxfId="36" priority="46" operator="equal">
@@ -15086,9 +15111,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Arial,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <rowBreaks count="2" manualBreakCount="2">
+  <rowBreaks count="3" manualBreakCount="3">
     <brk id="66" min="1" max="12" man="1"/>
     <brk id="132" min="1" max="12" man="1"/>
+    <brk id="198" min="1" max="12" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="13" max="1048575" man="1"/>
@@ -15111,7 +15137,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -15975,15 +16001,15 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="297" t="s">
+      <c r="A81" s="299" t="s">
         <v>285</v>
       </c>
       <c r="B81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="297"/>
+      <c r="A82" s="299"/>
       <c r="B82" t="s">
         <v>288</v>
       </c>
@@ -16037,12 +16063,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:C37"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:C47"/>
@@ -16050,6 +16070,12 @@
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="69" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Add data section for monitor eval
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="358">
   <si>
     <t>Medical Physicist CT Survey Report</t>
   </si>
@@ -1098,6 +1098,27 @@
   </si>
   <si>
     <t>DHEC form SC-RHA-20 “Notice to Employees” posted or referenced</t>
+  </si>
+  <si>
+    <t>Measurements</t>
+  </si>
+  <si>
+    <t>Set text</t>
+  </si>
+  <si>
+    <t>Light_x000D_(cd/m²)</t>
+  </si>
+  <si>
+    <t>LN01</t>
+  </si>
+  <si>
+    <t>LN18</t>
+  </si>
+  <si>
+    <t>UNL10</t>
+  </si>
+  <si>
+    <t>UNL80</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1134,7 @@
     <numFmt numFmtId="169" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="170" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
@@ -1250,8 +1271,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1298,6 +1326,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2245,7 +2279,7 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="299">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3069,13 +3103,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3099,41 +3154,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3994,19 +4031,19 @@
       <c r="A6" s="218" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="279" t="str">
+      <c r="B6" s="277" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="279"/>
+      <c r="C6" s="277"/>
       <c r="D6" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="279" t="str">
+      <c r="E6" s="277" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="279"/>
+      <c r="F6" s="277"/>
       <c r="G6" s="1"/>
       <c r="J6" s="244" t="s">
         <v>331</v>
@@ -4016,48 +4053,48 @@
       <c r="A7" s="218" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="277"/>
-      <c r="C7" s="277"/>
+      <c r="B7" s="278"/>
+      <c r="C7" s="278"/>
       <c r="D7" s="219" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="277" t="str">
+      <c r="E7" s="278" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="277"/>
+      <c r="F7" s="278"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="218" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="277"/>
-      <c r="C8" s="277"/>
+      <c r="B8" s="278"/>
+      <c r="C8" s="278"/>
       <c r="D8" s="219" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="277" t="str">
+      <c r="E8" s="278" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="277"/>
+      <c r="F8" s="278"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="218" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="277"/>
-      <c r="C9" s="277"/>
+      <c r="B9" s="278"/>
+      <c r="C9" s="278"/>
       <c r="D9" s="219" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="277" t="str">
+      <c r="E9" s="278" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="277"/>
+      <c r="F9" s="278"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4067,19 +4104,19 @@
       <c r="D10" s="219" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="278" t="str">
+      <c r="E10" s="279" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="278"/>
+      <c r="F10" s="279"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="218" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="279"/>
-      <c r="C11" s="279"/>
+      <c r="B11" s="277"/>
+      <c r="C11" s="277"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4102,10 +4139,10 @@
       <c r="A13" s="221" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="279" t="s">
+      <c r="B13" s="277" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="279"/>
+      <c r="C13" s="277"/>
       <c r="D13" s="219" t="s">
         <v>16</v>
       </c>
@@ -4418,17 +4455,17 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29">
@@ -4449,7 +4486,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD264"/>
+  <dimension ref="A1:AH264"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4464,7 +4501,7 @@
     <col min="33" max="16384" width="9.33203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8">
         <v>1</v>
       </c>
@@ -4496,8 +4533,11 @@
       <c r="AA1" s="18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG1" s="55" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>2</v>
       </c>
@@ -4515,7 +4555,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -4533,8 +4573,14 @@
         <f>IF(AB7="","",AB7)</f>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG3" s="299" t="s">
+        <v>352</v>
+      </c>
+      <c r="AH3" s="299" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>4</v>
       </c>
@@ -4548,8 +4594,12 @@
       <c r="AB4" s="28" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG4" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="AH4" s="14"/>
+    </row>
+    <row r="5" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>5</v>
       </c>
@@ -4563,8 +4613,12 @@
         <v>45</v>
       </c>
       <c r="Y5" s="24"/>
-    </row>
-    <row r="6" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG5" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="AH5" s="14"/>
+    </row>
+    <row r="6" spans="1:34" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>6</v>
       </c>
@@ -4600,8 +4654,12 @@
       <c r="AD6" s="14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="AG6" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH6" s="14"/>
+    </row>
+    <row r="7" spans="1:34" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>7</v>
       </c>
@@ -4631,8 +4689,12 @@
         <f>IF(OR(AA2="",AA2=0),"",AA2)</f>
         <v>First,CTDI,ACRPhantom,Comments</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG7" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH7" s="14"/>
+    </row>
+    <row r="8" spans="1:34" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>8</v>
       </c>
@@ -4658,8 +4720,12 @@
         <f>IF(P7="","",P7)</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="AG8" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH8" s="14"/>
+    </row>
+    <row r="9" spans="1:34" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>9</v>
       </c>
@@ -4706,8 +4772,12 @@
         <f>IF(X7="","",X7)</f>
         <v>Eugene Mah</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG9" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH9" s="14"/>
+    </row>
+    <row r="10" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>10</v>
       </c>
@@ -4715,19 +4785,19 @@
       <c r="E10" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="290" t="str">
+      <c r="F10" s="280" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="290"/>
+      <c r="G10" s="280"/>
       <c r="J10" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="290" t="str">
+      <c r="K10" s="280" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="290"/>
+      <c r="L10" s="280"/>
       <c r="M10" s="22"/>
       <c r="O10" s="23"/>
       <c r="Q10" s="27" t="s">
@@ -4759,8 +4829,12 @@
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG10" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH10" s="14"/>
+    </row>
+    <row r="11" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>11</v>
       </c>
@@ -4768,19 +4842,19 @@
       <c r="E11" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="295" t="str">
+      <c r="F11" s="282" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="295"/>
+      <c r="G11" s="282"/>
       <c r="J11" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="290" t="str">
+      <c r="K11" s="280" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="290"/>
+      <c r="L11" s="280"/>
       <c r="M11" s="22"/>
       <c r="O11" s="23"/>
       <c r="Q11" s="27" t="s">
@@ -4812,8 +4886,12 @@
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG11" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH11" s="14"/>
+    </row>
+    <row r="12" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>12</v>
       </c>
@@ -4821,19 +4899,19 @@
       <c r="E12" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="295" t="str">
+      <c r="F12" s="282" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="295"/>
+      <c r="G12" s="282"/>
       <c r="J12" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="296" t="str">
+      <c r="K12" s="283" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="296"/>
+      <c r="L12" s="283"/>
       <c r="M12" s="22"/>
       <c r="O12" s="23"/>
       <c r="Q12" s="27" t="s">
@@ -4865,8 +4943,12 @@
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG12" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH12" s="14"/>
+    </row>
+    <row r="13" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>13</v>
       </c>
@@ -4874,19 +4956,19 @@
       <c r="E13" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="295" t="str">
+      <c r="F13" s="282" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="295"/>
+      <c r="G13" s="282"/>
       <c r="J13" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="290" t="str">
+      <c r="K13" s="280" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="290"/>
+      <c r="L13" s="280"/>
       <c r="M13" s="22"/>
       <c r="O13" s="23"/>
       <c r="Q13" s="27" t="s">
@@ -4918,8 +5000,12 @@
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG13" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH13" s="14"/>
+    </row>
+    <row r="14" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>14</v>
       </c>
@@ -4951,8 +5037,12 @@
         <f>IF(R14="","",R14)</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG14" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH14" s="14"/>
+    </row>
+    <row r="15" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>15</v>
       </c>
@@ -4975,8 +5065,12 @@
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG15" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH15" s="14"/>
+    </row>
+    <row r="16" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>16</v>
       </c>
@@ -4984,19 +5078,19 @@
       <c r="E16" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="290" t="str">
+      <c r="F16" s="280" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="290"/>
+      <c r="G16" s="280"/>
       <c r="J16" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="296" t="str">
+      <c r="K16" s="283" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="296"/>
+      <c r="L16" s="283"/>
       <c r="M16" s="22"/>
       <c r="O16" s="23"/>
       <c r="P16" s="55" t="s">
@@ -5015,8 +5109,12 @@
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG16" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH16" s="14"/>
+    </row>
+    <row r="17" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>17</v>
       </c>
@@ -5024,19 +5122,19 @@
       <c r="E17" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="295" t="str">
+      <c r="F17" s="282" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="295"/>
+      <c r="G17" s="282"/>
       <c r="J17" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="290" t="str">
+      <c r="K17" s="280" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="290"/>
+      <c r="L17" s="280"/>
       <c r="M17" s="22"/>
       <c r="O17" s="23"/>
       <c r="Q17" s="27" t="s">
@@ -5068,8 +5166,12 @@
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG17" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH17" s="14"/>
+    </row>
+    <row r="18" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>18</v>
       </c>
@@ -5077,11 +5179,11 @@
       <c r="J18" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="290" t="str">
+      <c r="K18" s="280" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="290"/>
+      <c r="L18" s="280"/>
       <c r="M18" s="22"/>
       <c r="O18" s="23"/>
       <c r="Q18" s="27" t="s">
@@ -5113,8 +5215,12 @@
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG18" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH18" s="14"/>
+    </row>
+    <row r="19" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>19</v>
       </c>
@@ -5144,8 +5250,12 @@
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="19"/>
-    </row>
-    <row r="20" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG19" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH19" s="14"/>
+    </row>
+    <row r="20" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>20</v>
       </c>
@@ -5153,11 +5263,11 @@
       <c r="E20" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="290" t="str">
+      <c r="F20" s="280" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="290"/>
+      <c r="G20" s="280"/>
       <c r="I20" s="58" t="s">
         <v>76</v>
       </c>
@@ -5173,8 +5283,12 @@
       <c r="AA20" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG20" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH20" s="14"/>
+    </row>
+    <row r="21" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>21</v>
       </c>
@@ -5182,19 +5296,19 @@
       <c r="E21" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="293" t="str">
+      <c r="F21" s="284" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="293"/>
+      <c r="G21" s="284"/>
       <c r="J21" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="290" t="str">
+      <c r="K21" s="280" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="290"/>
+      <c r="L21" s="280"/>
       <c r="M21" s="22"/>
       <c r="O21" s="23"/>
       <c r="Q21" s="27" t="s">
@@ -5221,8 +5335,12 @@
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG21" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH21" s="14"/>
+    </row>
+    <row r="22" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>22</v>
       </c>
@@ -5233,11 +5351,11 @@
       <c r="J22" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="290" t="str">
+      <c r="K22" s="280" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="290"/>
+      <c r="L22" s="280"/>
       <c r="M22" s="22"/>
       <c r="O22" s="23"/>
       <c r="Q22" s="27" t="s">
@@ -5269,8 +5387,12 @@
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG22" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH22" s="14"/>
+    </row>
+    <row r="23" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>23</v>
       </c>
@@ -5278,19 +5400,19 @@
       <c r="E23" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="290" t="str">
+      <c r="F23" s="280" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="290"/>
+      <c r="G23" s="280"/>
       <c r="J23" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="290" t="str">
+      <c r="K23" s="280" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="290"/>
+      <c r="L23" s="280"/>
       <c r="M23" s="22"/>
       <c r="O23" s="23"/>
       <c r="P23" s="55" t="s">
@@ -5317,8 +5439,12 @@
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG23" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH23" s="14"/>
+    </row>
+    <row r="24" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>24</v>
       </c>
@@ -5326,11 +5452,11 @@
       <c r="E24" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="290" t="str">
+      <c r="F24" s="280" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="290"/>
+      <c r="G24" s="280"/>
       <c r="M24" s="22"/>
       <c r="O24" s="23"/>
       <c r="Q24" s="27" t="s">
@@ -5362,8 +5488,12 @@
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG24" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH24" s="14"/>
+    </row>
+    <row r="25" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>25</v>
       </c>
@@ -5371,11 +5501,11 @@
       <c r="E25" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="290" t="str">
+      <c r="F25" s="280" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="290"/>
+      <c r="G25" s="280"/>
       <c r="J25" s="54" t="s">
         <v>82</v>
       </c>
@@ -5402,8 +5532,12 @@
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG25" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH25" s="14"/>
+    </row>
+    <row r="26" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>26</v>
       </c>
@@ -5415,11 +5549,11 @@
       <c r="J26" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="290" t="str">
+      <c r="K26" s="280" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="290"/>
+      <c r="L26" s="280"/>
       <c r="M26" s="22"/>
       <c r="O26" s="23"/>
       <c r="Q26" s="27" t="s">
@@ -5439,7 +5573,7 @@
       <c r="AC26" s="19"/>
       <c r="AD26" s="19"/>
     </row>
-    <row r="27" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>27</v>
       </c>
@@ -5447,19 +5581,19 @@
       <c r="E27" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="290" t="str">
+      <c r="F27" s="280" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="290"/>
+      <c r="G27" s="280"/>
       <c r="J27" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="290" t="str">
+      <c r="K27" s="280" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="290"/>
+      <c r="L27" s="280"/>
       <c r="M27" s="22"/>
       <c r="O27" s="23"/>
       <c r="P27" s="55" t="s">
@@ -5478,7 +5612,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>28</v>
       </c>
@@ -5486,11 +5620,11 @@
       <c r="E28" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="290" t="str">
+      <c r="F28" s="280" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="290"/>
+      <c r="G28" s="280"/>
       <c r="M28" s="22"/>
       <c r="O28" s="23"/>
       <c r="Q28" s="27" t="s">
@@ -5523,7 +5657,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>29</v>
       </c>
@@ -5531,11 +5665,11 @@
       <c r="E29" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="290" t="str">
+      <c r="F29" s="280" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="290"/>
+      <c r="G29" s="280"/>
       <c r="M29" s="22"/>
       <c r="O29" s="23"/>
       <c r="Q29" s="27" t="s">
@@ -5560,7 +5694,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>30</v>
       </c>
@@ -5599,7 +5733,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>31</v>
       </c>
@@ -5627,7 +5761,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>32</v>
       </c>
@@ -5645,10 +5779,10 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="291" t="s">
+      <c r="L32" s="285" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="291"/>
+      <c r="M32" s="285"/>
       <c r="AA32" s="27" t="s">
         <v>70</v>
       </c>
@@ -6923,27 +7057,27 @@
       </c>
       <c r="B70" s="20"/>
       <c r="E70" s="68"/>
-      <c r="F70" s="292" t="s">
+      <c r="F70" s="286" t="s">
         <v>145</v>
       </c>
-      <c r="G70" s="292"/>
-      <c r="H70" s="292"/>
-      <c r="I70" s="292" t="s">
+      <c r="G70" s="286"/>
+      <c r="H70" s="286"/>
+      <c r="I70" s="286" t="s">
         <v>146</v>
       </c>
-      <c r="J70" s="292"/>
+      <c r="J70" s="286"/>
       <c r="M70" s="22"/>
       <c r="O70" s="43"/>
       <c r="P70" s="16"/>
-      <c r="Q70" s="280" t="s">
+      <c r="Q70" s="287" t="s">
         <v>145</v>
       </c>
-      <c r="R70" s="280"/>
-      <c r="S70" s="280"/>
-      <c r="T70" s="280" t="s">
+      <c r="R70" s="287"/>
+      <c r="S70" s="287"/>
+      <c r="T70" s="287" t="s">
         <v>146</v>
       </c>
-      <c r="U70" s="280"/>
+      <c r="U70" s="287"/>
       <c r="V70" s="16"/>
       <c r="W70" s="16"/>
       <c r="X70" s="16"/>
@@ -8211,15 +8345,15 @@
       <c r="M90" s="22"/>
       <c r="O90" s="23"/>
       <c r="P90" s="52"/>
-      <c r="Q90" s="294" t="s">
+      <c r="Q90" s="296" t="s">
         <v>145</v>
       </c>
-      <c r="R90" s="294"/>
-      <c r="S90" s="294"/>
-      <c r="T90" s="294" t="s">
+      <c r="R90" s="296"/>
+      <c r="S90" s="296"/>
+      <c r="T90" s="296" t="s">
         <v>146</v>
       </c>
-      <c r="U90" s="294"/>
+      <c r="U90" s="296"/>
       <c r="Y90" s="24"/>
       <c r="AA90" s="27" t="s">
         <v>122</v>
@@ -8362,15 +8496,15 @@
       </c>
       <c r="B94" s="20"/>
       <c r="E94" s="68"/>
-      <c r="F94" s="282" t="s">
+      <c r="F94" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="G94" s="282"/>
-      <c r="H94" s="282"/>
-      <c r="I94" s="283" t="s">
+      <c r="G94" s="289"/>
+      <c r="H94" s="289"/>
+      <c r="I94" s="290" t="s">
         <v>146</v>
       </c>
-      <c r="J94" s="283"/>
+      <c r="J94" s="290"/>
       <c r="M94" s="22"/>
       <c r="O94" s="23"/>
       <c r="P94" s="27" t="s">
@@ -8534,10 +8668,10 @@
         <v>31</v>
       </c>
       <c r="B97" s="20"/>
-      <c r="D97" s="284" t="s">
+      <c r="D97" s="291" t="s">
         <v>155</v>
       </c>
-      <c r="E97" s="285"/>
+      <c r="E97" s="292"/>
       <c r="F97" s="94" t="str">
         <f t="shared" ref="F97:J102" si="31">IF(Q122="","",Q122)</f>
         <v/>
@@ -8593,8 +8727,8 @@
         <v>32</v>
       </c>
       <c r="B98" s="20"/>
-      <c r="D98" s="284"/>
-      <c r="E98" s="285"/>
+      <c r="D98" s="291"/>
+      <c r="E98" s="292"/>
       <c r="F98" s="99" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -8650,8 +8784,8 @@
         <v>33</v>
       </c>
       <c r="B99" s="20"/>
-      <c r="D99" s="284"/>
-      <c r="E99" s="285"/>
+      <c r="D99" s="291"/>
+      <c r="E99" s="292"/>
       <c r="F99" s="104" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -9594,15 +9728,15 @@
       <c r="J119" s="19"/>
       <c r="M119" s="22"/>
       <c r="O119" s="23"/>
-      <c r="Q119" s="288" t="s">
+      <c r="Q119" s="294" t="s">
         <v>145</v>
       </c>
-      <c r="R119" s="280"/>
-      <c r="S119" s="289"/>
-      <c r="T119" s="288" t="s">
+      <c r="R119" s="287"/>
+      <c r="S119" s="295"/>
+      <c r="T119" s="294" t="s">
         <v>146</v>
       </c>
-      <c r="U119" s="289"/>
+      <c r="U119" s="295"/>
       <c r="W119" s="55" t="s">
         <v>152</v>
       </c>
@@ -9726,10 +9860,10 @@
         <v>Water phantom is free from rings, streaks, lines, cupping artifacts</v>
       </c>
       <c r="M122" s="22"/>
-      <c r="O122" s="286" t="s">
+      <c r="O122" s="293" t="s">
         <v>155</v>
       </c>
-      <c r="P122" s="287"/>
+      <c r="P122" s="281"/>
       <c r="Q122" s="137"/>
       <c r="R122" s="138"/>
       <c r="S122" s="139"/>
@@ -9761,8 +9895,8 @@
       </c>
       <c r="B123" s="20"/>
       <c r="M123" s="22"/>
-      <c r="O123" s="286"/>
-      <c r="P123" s="287"/>
+      <c r="O123" s="293"/>
+      <c r="P123" s="281"/>
       <c r="Q123" s="140"/>
       <c r="R123" s="141"/>
       <c r="S123" s="142"/>
@@ -9799,8 +9933,8 @@
         <v>183</v>
       </c>
       <c r="M124" s="22"/>
-      <c r="O124" s="286"/>
-      <c r="P124" s="287"/>
+      <c r="O124" s="293"/>
+      <c r="P124" s="281"/>
       <c r="Q124" s="144"/>
       <c r="R124" s="145"/>
       <c r="S124" s="146"/>
@@ -9840,9 +9974,9 @@
       <c r="D125" s="68" t="s">
         <v>184</v>
       </c>
-      <c r="F125" s="272" t="str">
+      <c r="F125" s="272">
         <f>IF(O211="","",O211)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G125" s="165" t="s">
         <v>185</v>
@@ -9909,9 +10043,9 @@
         <v>187</v>
       </c>
       <c r="E126" s="52"/>
-      <c r="F126" s="272" t="str">
+      <c r="F126" s="272">
         <f>IF(O212="","",O212)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G126" s="165" t="s">
         <v>188</v>
@@ -9963,9 +10097,9 @@
       <c r="D127" s="68" t="s">
         <v>190</v>
       </c>
-      <c r="F127" s="166" t="str">
+      <c r="F127" s="166" t="e">
         <f>IF(T215="","",T215)</f>
-        <v/>
+        <v>#DIV/0!</v>
       </c>
       <c r="G127" s="165" t="s">
         <v>191</v>
@@ -10637,7 +10771,7 @@
       </c>
       <c r="M141" s="22"/>
       <c r="O141" s="23"/>
-      <c r="P141" s="287" t="s">
+      <c r="P141" s="281" t="s">
         <v>175</v>
       </c>
       <c r="Q141" s="171"/>
@@ -10666,7 +10800,7 @@
       <c r="C142" s="52"/>
       <c r="M142" s="22"/>
       <c r="O142" s="23"/>
-      <c r="P142" s="287"/>
+      <c r="P142" s="281"/>
       <c r="Q142" s="171"/>
       <c r="R142" s="172"/>
       <c r="S142" s="172"/>
@@ -10695,7 +10829,7 @@
       </c>
       <c r="M143" s="22"/>
       <c r="O143" s="23"/>
-      <c r="P143" s="287"/>
+      <c r="P143" s="281"/>
       <c r="Q143" s="174"/>
       <c r="R143" s="175"/>
       <c r="S143" s="175"/>
@@ -11841,14 +11975,14 @@
       <c r="B168" s="20"/>
       <c r="C168" s="52"/>
       <c r="D168" s="68"/>
-      <c r="E168" s="281" t="s">
+      <c r="E168" s="288" t="s">
         <v>145</v>
       </c>
-      <c r="F168" s="281"/>
-      <c r="G168" s="281" t="s">
+      <c r="F168" s="288"/>
+      <c r="G168" s="288" t="s">
         <v>146</v>
       </c>
-      <c r="H168" s="281"/>
+      <c r="H168" s="288"/>
       <c r="M168" s="22"/>
       <c r="O168" s="185" t="s">
         <v>218</v>
@@ -13255,7 +13389,10 @@
       <c r="S208" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="T208" s="271"/>
+      <c r="T208" s="271">
+        <f>AH16</f>
+        <v>0</v>
+      </c>
       <c r="Y208" s="24"/>
     </row>
     <row r="209" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13284,7 +13421,10 @@
       <c r="S209" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="T209" s="271"/>
+      <c r="T209" s="271">
+        <f t="shared" ref="T209:T212" si="46">AH17</f>
+        <v>0</v>
+      </c>
       <c r="Y209" s="24"/>
     </row>
     <row r="210" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13313,7 +13453,10 @@
       <c r="S210" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="T210" s="271"/>
+      <c r="T210" s="271">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
       <c r="Y210" s="24"/>
     </row>
     <row r="211" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13334,7 +13477,10 @@
       <c r="K211" s="194"/>
       <c r="L211" s="194"/>
       <c r="M211" s="22"/>
-      <c r="O211" s="270"/>
+      <c r="O211" s="270">
+        <f>AH4</f>
+        <v>0</v>
+      </c>
       <c r="P211" s="14" t="s">
         <v>185</v>
       </c>
@@ -13343,7 +13489,10 @@
       <c r="S211" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="T211" s="271"/>
+      <c r="T211" s="271">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
       <c r="U211" s="19"/>
       <c r="V211" s="19"/>
       <c r="W211" s="19"/>
@@ -13368,7 +13517,10 @@
       <c r="K212" s="196"/>
       <c r="L212" s="196"/>
       <c r="M212" s="22"/>
-      <c r="O212" s="270"/>
+      <c r="O212" s="270">
+        <f>AH5</f>
+        <v>0</v>
+      </c>
       <c r="P212" s="14" t="s">
         <v>188</v>
       </c>
@@ -13377,7 +13529,10 @@
       <c r="S212" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="T212" s="271"/>
+      <c r="T212" s="271">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
       <c r="U212" s="19"/>
       <c r="V212" s="19"/>
       <c r="W212" s="19"/>
@@ -13413,9 +13568,9 @@
       <c r="S213" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="T213" s="149" t="str">
+      <c r="T213" s="149">
         <f>IF(T208="","",AVERAGE(T208:T212))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="U213" s="19"/>
       <c r="V213" s="19"/>
@@ -13450,9 +13605,9 @@
       <c r="S214" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="T214" s="179" t="str">
+      <c r="T214" s="179">
         <f>IF(T208="","",STDEV(T208:T212))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="U214" s="19"/>
       <c r="V214" s="19"/>
@@ -13485,9 +13640,9 @@
       <c r="S215" s="198" t="s">
         <v>273</v>
       </c>
-      <c r="T215" s="199" t="str">
+      <c r="T215" s="199" t="e">
         <f>IF(T208="","",2*(MAX(T208:T212)-MIN(T208:T212))/(MAX(T208:T212)+MIN(T208:T212)))</f>
-        <v/>
+        <v>#DIV/0!</v>
       </c>
       <c r="U215" s="33"/>
       <c r="V215" s="33"/>
@@ -15033,6 +15188,32 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="42">
+    <mergeCell ref="O122:P124"/>
+    <mergeCell ref="Q119:S119"/>
+    <mergeCell ref="T119:U119"/>
+    <mergeCell ref="Q90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="E168:F168"/>
+    <mergeCell ref="G168:H168"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="D97:E99"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="P141:P143"/>
@@ -15042,12 +15223,6 @@
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K22:L22"/>
@@ -15055,26 +15230,6 @@
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F25:G25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="T70:U70"/>
-    <mergeCell ref="E168:F168"/>
-    <mergeCell ref="G168:H168"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="I94:J94"/>
-    <mergeCell ref="D97:E99"/>
-    <mergeCell ref="O122:P124"/>
-    <mergeCell ref="Q119:S119"/>
-    <mergeCell ref="T119:U119"/>
-    <mergeCell ref="Q90:S90"/>
-    <mergeCell ref="T90:U90"/>
   </mergeCells>
   <conditionalFormatting sqref="L33:L38 L60:L63 L41:L57">
     <cfRule type="cellIs" dxfId="36" priority="46" operator="equal">
@@ -15287,17 +15442,17 @@
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="298" t="s">
+      <c r="A4" s="297" t="s">
         <v>284</v>
       </c>
-      <c r="B4" s="298" t="s">
+      <c r="B4" s="297" t="s">
         <v>285</v>
       </c>
-      <c r="C4" s="298"/>
-      <c r="D4" s="298"/>
+      <c r="C4" s="297"/>
+      <c r="D4" s="297"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="298"/>
+      <c r="A5" s="297"/>
       <c r="B5" s="5" t="s">
         <v>286</v>
       </c>
@@ -15469,17 +15624,17 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="298" t="s">
+      <c r="A18" s="297" t="s">
         <v>284</v>
       </c>
-      <c r="B18" s="298" t="s">
+      <c r="B18" s="297" t="s">
         <v>301</v>
       </c>
-      <c r="C18" s="298"/>
-      <c r="D18" s="298"/>
+      <c r="C18" s="297"/>
+      <c r="D18" s="297"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="298"/>
+      <c r="A19" s="297"/>
       <c r="B19" s="5" t="s">
         <v>286</v>
       </c>
@@ -15715,16 +15870,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="298" t="s">
+      <c r="A37" s="297" t="s">
         <v>284</v>
       </c>
-      <c r="B37" s="298" t="s">
+      <c r="B37" s="297" t="s">
         <v>306</v>
       </c>
-      <c r="C37" s="298"/>
+      <c r="C37" s="297"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="298"/>
+      <c r="A38" s="297"/>
       <c r="B38" s="5" t="s">
         <v>287</v>
       </c>
@@ -15810,16 +15965,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="298" t="s">
+      <c r="A47" s="297" t="s">
         <v>284</v>
       </c>
-      <c r="B47" s="298" t="s">
+      <c r="B47" s="297" t="s">
         <v>309</v>
       </c>
-      <c r="C47" s="298"/>
+      <c r="C47" s="297"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="298"/>
+      <c r="A48" s="297"/>
       <c r="B48" s="5" t="s">
         <v>287</v>
       </c>
@@ -15905,16 +16060,16 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="298" t="s">
+      <c r="A57" s="297" t="s">
         <v>284</v>
       </c>
-      <c r="B57" s="298" t="s">
+      <c r="B57" s="297" t="s">
         <v>316</v>
       </c>
-      <c r="C57" s="298"/>
+      <c r="C57" s="297"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="298"/>
+      <c r="A58" s="297"/>
       <c r="B58" s="5" t="s">
         <v>287</v>
       </c>
@@ -16000,16 +16155,16 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="298" t="s">
+      <c r="A67" s="297" t="s">
         <v>284</v>
       </c>
-      <c r="B67" s="298" t="s">
+      <c r="B67" s="297" t="s">
         <v>321</v>
       </c>
-      <c r="C67" s="298"/>
+      <c r="C67" s="297"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="298"/>
+      <c r="A68" s="297"/>
       <c r="B68" s="5" t="s">
         <v>287</v>
       </c>
@@ -16139,7 +16294,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="297" t="s">
+      <c r="A81" s="298" t="s">
         <v>284</v>
       </c>
       <c r="B81" t="s">
@@ -16147,7 +16302,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="297"/>
+      <c r="A82" s="298"/>
       <c r="B82" t="s">
         <v>287</v>
       </c>
@@ -16211,12 +16366,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="13">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:C37"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:C47"/>
@@ -16224,6 +16373,12 @@
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="69" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fix references to CTDI pass/fail criteria
References were pointing to the wrong cells
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7317BC6D-F9EF-4EA1-9A92-E31FCC743D7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
     <definedName name="Z_25C83B95_F566_493A_A3D1_2FC57CA3E0EA_.wvu.PrintArea" localSheetId="1" hidden="1">Sheet1!$B$1:$M$264</definedName>
     <definedName name="Z_25C83B95_F566_493A_A3D1_2FC57CA3E0EA_.wvu.PrintArea" localSheetId="0" hidden="1">Summary!$A$1:$F$40</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Eugene Mah - Personal View" guid="{25C83B95-F566-493A-A3D1-2FC57CA3E0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="784" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
@@ -35,6 +36,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1163,7 +1167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
@@ -3153,6 +3157,45 @@
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="77" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3210,6 +3253,12 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3219,63 +3268,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="77" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Fail" xfId="6"/>
-    <cellStyle name="Heading" xfId="3"/>
-    <cellStyle name="Heading1" xfId="4"/>
+    <cellStyle name="Fail" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Heading1" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pass" xfId="5"/>
+    <cellStyle name="Pass" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Percent" xfId="7" builtinId="5"/>
-    <cellStyle name="Result" xfId="1"/>
-    <cellStyle name="Result2" xfId="2"/>
+    <cellStyle name="Result" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="148">
+  <dxfs count="37">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3563,1116 +3567,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5147,7 +4041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5234,19 +4128,19 @@
       <c r="A6" s="216" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="278" t="str">
+      <c r="B6" s="291" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="278"/>
+      <c r="C6" s="291"/>
       <c r="D6" s="217" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="278" t="str">
+      <c r="E6" s="291" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="278"/>
+      <c r="F6" s="291"/>
       <c r="G6" s="1"/>
       <c r="J6" s="242" t="s">
         <v>326</v>
@@ -5256,48 +4150,48 @@
       <c r="A7" s="216" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="276"/>
-      <c r="C7" s="276"/>
+      <c r="B7" s="289"/>
+      <c r="C7" s="289"/>
       <c r="D7" s="217" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="276" t="str">
+      <c r="E7" s="289" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="276"/>
+      <c r="F7" s="289"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="216" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="276"/>
-      <c r="C8" s="276"/>
+      <c r="B8" s="289"/>
+      <c r="C8" s="289"/>
       <c r="D8" s="217" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="276" t="str">
+      <c r="E8" s="289" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="276"/>
+      <c r="F8" s="289"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="216" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="276"/>
-      <c r="C9" s="276"/>
+      <c r="B9" s="289"/>
+      <c r="C9" s="289"/>
       <c r="D9" s="217" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="276" t="str">
+      <c r="E9" s="289" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="276"/>
+      <c r="F9" s="289"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5307,19 +4201,19 @@
       <c r="D10" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="277" t="str">
+      <c r="E10" s="290" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="277"/>
+      <c r="F10" s="290"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="216" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="278"/>
-      <c r="C11" s="278"/>
+      <c r="B11" s="291"/>
+      <c r="C11" s="291"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -5342,10 +4236,10 @@
       <c r="A13" s="219" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="278" t="s">
+      <c r="B13" s="291" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="278"/>
+      <c r="C13" s="291"/>
       <c r="D13" s="217" t="s">
         <v>16</v>
       </c>
@@ -5671,10 +4565,10 @@
     <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$J$1:$J$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$J$4:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -5688,11 +4582,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="M112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V131" sqref="V131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5741,7 +4635,7 @@
       <c r="AG1" s="55" t="s">
         <v>345</v>
       </c>
-      <c r="AH1" s="298"/>
+      <c r="AH1" s="276"/>
     </row>
     <row r="2" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
@@ -5760,8 +4654,8 @@
       <c r="AA2" s="25" t="s">
         <v>327</v>
       </c>
-      <c r="AG2" s="298"/>
-      <c r="AH2" s="298"/>
+      <c r="AG2" s="276"/>
+      <c r="AH2" s="276"/>
     </row>
     <row r="3" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -5802,10 +4696,10 @@
       <c r="AB4" s="28" t="s">
         <v>327</v>
       </c>
-      <c r="AG4" s="298" t="s">
+      <c r="AG4" s="276" t="s">
         <v>352</v>
       </c>
-      <c r="AH4" s="298"/>
+      <c r="AH4" s="276"/>
     </row>
     <row r="5" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
@@ -5821,7 +4715,7 @@
         <v>45</v>
       </c>
       <c r="Y5" s="24"/>
-      <c r="AG5" s="298" t="s">
+      <c r="AG5" s="276" t="s">
         <v>348</v>
       </c>
       <c r="AH5" s="14"/>
@@ -5862,7 +4756,7 @@
       <c r="AD6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AG6" s="298" t="s">
+      <c r="AG6" s="276" t="s">
         <v>348</v>
       </c>
       <c r="AH6" s="14"/>
@@ -5897,7 +4791,7 @@
         <f>IF(OR(AA2="",AA2=0),"",AA2)</f>
         <v>First,CTDI,ACRPhantom,Comments</v>
       </c>
-      <c r="AG7" s="298" t="s">
+      <c r="AG7" s="276" t="s">
         <v>349</v>
       </c>
       <c r="AH7" s="14"/>
@@ -5928,7 +4822,7 @@
         <f>IF(P7="","",P7)</f>
         <v/>
       </c>
-      <c r="AG8" s="298" t="s">
+      <c r="AG8" s="276" t="s">
         <v>349</v>
       </c>
       <c r="AH8" s="14"/>
@@ -5980,7 +4874,7 @@
         <f>IF(X7="","",X7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="AG9" s="298" t="s">
+      <c r="AG9" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH9" s="14"/>
@@ -5993,19 +4887,19 @@
       <c r="E10" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="292" t="str">
+      <c r="F10" s="305" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="292"/>
+      <c r="G10" s="305"/>
       <c r="J10" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="292" t="str">
+      <c r="K10" s="305" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="292"/>
+      <c r="L10" s="305"/>
       <c r="M10" s="22"/>
       <c r="O10" s="23"/>
       <c r="Q10" s="27" t="s">
@@ -6037,7 +4931,7 @@
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="AG10" s="298" t="s">
+      <c r="AG10" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH10" s="14"/>
@@ -6050,19 +4944,19 @@
       <c r="E11" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="293" t="str">
+      <c r="F11" s="306" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="293"/>
+      <c r="G11" s="306"/>
       <c r="J11" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="292" t="str">
+      <c r="K11" s="305" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="292"/>
+      <c r="L11" s="305"/>
       <c r="M11" s="22"/>
       <c r="O11" s="23"/>
       <c r="Q11" s="27" t="s">
@@ -6094,7 +4988,7 @@
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="AG11" s="298" t="s">
+      <c r="AG11" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH11" s="14"/>
@@ -6107,19 +5001,19 @@
       <c r="E12" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="293" t="str">
+      <c r="F12" s="306" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="293"/>
+      <c r="G12" s="306"/>
       <c r="J12" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="294" t="str">
+      <c r="K12" s="307" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="294"/>
+      <c r="L12" s="307"/>
       <c r="M12" s="22"/>
       <c r="O12" s="23"/>
       <c r="Q12" s="27" t="s">
@@ -6151,7 +5045,7 @@
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="AG12" s="298" t="s">
+      <c r="AG12" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH12" s="14"/>
@@ -6164,19 +5058,19 @@
       <c r="E13" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="293" t="str">
+      <c r="F13" s="306" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="293"/>
+      <c r="G13" s="306"/>
       <c r="J13" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="292" t="str">
+      <c r="K13" s="305" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="292"/>
+      <c r="L13" s="305"/>
       <c r="M13" s="22"/>
       <c r="O13" s="23"/>
       <c r="Q13" s="27" t="s">
@@ -6208,7 +5102,7 @@
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="AG13" s="298" t="s">
+      <c r="AG13" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH13" s="14"/>
@@ -6245,7 +5139,7 @@
         <f>IF(R14="","",R14)</f>
         <v/>
       </c>
-      <c r="AG14" s="298" t="s">
+      <c r="AG14" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH14" s="14"/>
@@ -6273,7 +5167,7 @@
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="AG15" s="298" t="s">
+      <c r="AG15" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH15" s="14"/>
@@ -6286,19 +5180,19 @@
       <c r="E16" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="292" t="str">
+      <c r="F16" s="305" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="292"/>
+      <c r="G16" s="305"/>
       <c r="J16" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="294" t="str">
+      <c r="K16" s="307" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="294"/>
+      <c r="L16" s="307"/>
       <c r="M16" s="22"/>
       <c r="O16" s="23"/>
       <c r="P16" s="55" t="s">
@@ -6317,7 +5211,7 @@
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="AG16" s="298" t="s">
+      <c r="AG16" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH16" s="14"/>
@@ -6330,19 +5224,19 @@
       <c r="E17" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="293" t="str">
+      <c r="F17" s="306" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="293"/>
+      <c r="G17" s="306"/>
       <c r="J17" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="292" t="str">
+      <c r="K17" s="305" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="292"/>
+      <c r="L17" s="305"/>
       <c r="M17" s="22"/>
       <c r="O17" s="23"/>
       <c r="Q17" s="27" t="s">
@@ -6374,7 +5268,7 @@
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="AG17" s="298" t="s">
+      <c r="AG17" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH17" s="14"/>
@@ -6387,11 +5281,11 @@
       <c r="J18" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="292" t="str">
+      <c r="K18" s="305" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="292"/>
+      <c r="L18" s="305"/>
       <c r="M18" s="22"/>
       <c r="O18" s="23"/>
       <c r="Q18" s="27" t="s">
@@ -6423,7 +5317,7 @@
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="AG18" s="298" t="s">
+      <c r="AG18" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH18" s="14"/>
@@ -6458,7 +5352,7 @@
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="19"/>
-      <c r="AG19" s="298" t="s">
+      <c r="AG19" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH19" s="14"/>
@@ -6471,11 +5365,11 @@
       <c r="E20" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="292" t="str">
+      <c r="F20" s="305" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="292"/>
+      <c r="G20" s="305"/>
       <c r="I20" s="58" t="s">
         <v>76</v>
       </c>
@@ -6491,7 +5385,7 @@
       <c r="AA20" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="AG20" s="298" t="s">
+      <c r="AG20" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH20" s="14"/>
@@ -6504,19 +5398,19 @@
       <c r="E21" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="295" t="str">
+      <c r="F21" s="310" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="295"/>
+      <c r="G21" s="310"/>
       <c r="J21" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="292" t="str">
+      <c r="K21" s="305" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="292"/>
+      <c r="L21" s="305"/>
       <c r="M21" s="22"/>
       <c r="O21" s="23"/>
       <c r="Q21" s="27" t="s">
@@ -6543,7 +5437,7 @@
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="AG21" s="298" t="s">
+      <c r="AG21" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH21" s="14"/>
@@ -6559,11 +5453,11 @@
       <c r="J22" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="292" t="str">
+      <c r="K22" s="305" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="292"/>
+      <c r="L22" s="305"/>
       <c r="M22" s="22"/>
       <c r="O22" s="23"/>
       <c r="Q22" s="27" t="s">
@@ -6595,7 +5489,7 @@
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="AG22" s="298" t="s">
+      <c r="AG22" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH22" s="14"/>
@@ -6608,19 +5502,19 @@
       <c r="E23" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="292" t="str">
+      <c r="F23" s="305" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="292"/>
+      <c r="G23" s="305"/>
       <c r="J23" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="292" t="str">
+      <c r="K23" s="305" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="292"/>
+      <c r="L23" s="305"/>
       <c r="M23" s="22"/>
       <c r="O23" s="23"/>
       <c r="P23" s="55" t="s">
@@ -6647,7 +5541,7 @@
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="AG23" s="298" t="s">
+      <c r="AG23" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH23" s="14"/>
@@ -6660,11 +5554,11 @@
       <c r="E24" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="292" t="str">
+      <c r="F24" s="305" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="292"/>
+      <c r="G24" s="305"/>
       <c r="M24" s="22"/>
       <c r="O24" s="23"/>
       <c r="Q24" s="27" t="s">
@@ -6696,7 +5590,7 @@
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="AG24" s="298" t="s">
+      <c r="AG24" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH24" s="14"/>
@@ -6709,11 +5603,11 @@
       <c r="E25" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="292" t="str">
+      <c r="F25" s="305" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="292"/>
+      <c r="G25" s="305"/>
       <c r="J25" s="54" t="s">
         <v>82</v>
       </c>
@@ -6740,7 +5634,7 @@
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="AG25" s="298" t="s">
+      <c r="AG25" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH25" s="14"/>
@@ -6757,11 +5651,11 @@
       <c r="J26" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="292" t="str">
+      <c r="K26" s="305" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="292"/>
+      <c r="L26" s="305"/>
       <c r="M26" s="22"/>
       <c r="O26" s="23"/>
       <c r="Q26" s="27" t="s">
@@ -6780,7 +5674,7 @@
       <c r="AB26" s="19"/>
       <c r="AC26" s="19"/>
       <c r="AD26" s="19"/>
-      <c r="AG26" s="298" t="s">
+      <c r="AG26" s="276" t="s">
         <v>350</v>
       </c>
       <c r="AH26" s="14"/>
@@ -6793,19 +5687,19 @@
       <c r="E27" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="292" t="str">
+      <c r="F27" s="305" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="292"/>
+      <c r="G27" s="305"/>
       <c r="J27" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="292" t="str">
+      <c r="K27" s="305" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="292"/>
+      <c r="L27" s="305"/>
       <c r="M27" s="22"/>
       <c r="O27" s="23"/>
       <c r="P27" s="55" t="s">
@@ -6823,7 +5717,7 @@
       <c r="AA27" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AG27" s="298" t="s">
+      <c r="AG27" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH27" s="14"/>
@@ -6836,11 +5730,11 @@
       <c r="E28" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="292" t="str">
+      <c r="F28" s="305" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="292"/>
+      <c r="G28" s="305"/>
       <c r="M28" s="22"/>
       <c r="O28" s="23"/>
       <c r="Q28" s="27" t="s">
@@ -6872,7 +5766,7 @@
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="AG28" s="298" t="s">
+      <c r="AG28" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH28" s="14"/>
@@ -6885,11 +5779,11 @@
       <c r="E29" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="292" t="str">
+      <c r="F29" s="305" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="292"/>
+      <c r="G29" s="305"/>
       <c r="M29" s="22"/>
       <c r="O29" s="23"/>
       <c r="Q29" s="27" t="s">
@@ -6913,7 +5807,7 @@
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="AG29" s="298" t="s">
+      <c r="AG29" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH29" s="14"/>
@@ -6956,7 +5850,7 @@
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="AG30" s="298" t="s">
+      <c r="AG30" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH30" s="14"/>
@@ -6988,7 +5882,7 @@
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="AG31" s="298" t="s">
+      <c r="AG31" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH31" s="14"/>
@@ -7011,10 +5905,10 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="290" t="s">
+      <c r="L32" s="303" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="290"/>
+      <c r="M32" s="303"/>
       <c r="AA32" s="27" t="s">
         <v>70</v>
       </c>
@@ -7027,7 +5921,7 @@
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="AG32" s="298" t="s">
+      <c r="AG32" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH32" s="14"/>
@@ -7067,7 +5961,7 @@
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="AG33" s="298" t="s">
+      <c r="AG33" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH33" s="14"/>
@@ -7116,7 +6010,7 @@
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="AG34" s="298" t="s">
+      <c r="AG34" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH34" s="14"/>
@@ -7152,7 +6046,7 @@
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="AG35" s="298" t="s">
+      <c r="AG35" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH35" s="14"/>
@@ -7193,7 +6087,7 @@
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="AG36" s="298" t="s">
+      <c r="AG36" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH36" s="14"/>
@@ -7232,7 +6126,7 @@
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="AG37" s="298" t="s">
+      <c r="AG37" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH37" s="14"/>
@@ -7271,7 +6165,7 @@
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="AG38" s="298" t="s">
+      <c r="AG38" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH38" s="14"/>
@@ -7301,7 +6195,7 @@
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="AG39" s="298" t="s">
+      <c r="AG39" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH39" s="14"/>
@@ -7334,7 +6228,7 @@
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="AG40" s="298" t="s">
+      <c r="AG40" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH40" s="14"/>
@@ -7364,7 +6258,7 @@
       <c r="AA41" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="AG41" s="298" t="s">
+      <c r="AG41" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH41" s="14"/>
@@ -7394,7 +6288,7 @@
       <c r="AA42" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="AG42" s="298" t="s">
+      <c r="AG42" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH42" s="14"/>
@@ -7433,7 +6327,7 @@
         <f t="shared" ref="AD43:AD60" si="7">IF(Q72="","",Q72)</f>
         <v/>
       </c>
-      <c r="AG43" s="298" t="s">
+      <c r="AG43" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH43" s="14"/>
@@ -7472,7 +6366,7 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AG44" s="298" t="s">
+      <c r="AG44" s="276" t="s">
         <v>351</v>
       </c>
       <c r="AH44" s="14"/>
@@ -7511,10 +6405,10 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AG45" s="298" t="s">
+      <c r="AG45" s="276" t="s">
         <v>351</v>
       </c>
-      <c r="AH45" s="298"/>
+      <c r="AH45" s="276"/>
     </row>
     <row r="46" spans="1:34" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
@@ -8345,27 +7239,27 @@
       </c>
       <c r="B70" s="20"/>
       <c r="E70" s="68"/>
-      <c r="F70" s="291" t="s">
+      <c r="F70" s="304" t="s">
         <v>145</v>
       </c>
-      <c r="G70" s="291"/>
-      <c r="H70" s="291"/>
-      <c r="I70" s="291" t="s">
+      <c r="G70" s="304"/>
+      <c r="H70" s="304"/>
+      <c r="I70" s="304" t="s">
         <v>146</v>
       </c>
-      <c r="J70" s="291"/>
+      <c r="J70" s="304"/>
       <c r="M70" s="22"/>
       <c r="O70" s="43"/>
       <c r="P70" s="16"/>
-      <c r="Q70" s="282" t="s">
+      <c r="Q70" s="295" t="s">
         <v>145</v>
       </c>
-      <c r="R70" s="282"/>
-      <c r="S70" s="282"/>
-      <c r="T70" s="282" t="s">
+      <c r="R70" s="295"/>
+      <c r="S70" s="295"/>
+      <c r="T70" s="295" t="s">
         <v>146</v>
       </c>
-      <c r="U70" s="282"/>
+      <c r="U70" s="295"/>
       <c r="V70" s="16"/>
       <c r="W70" s="16"/>
       <c r="X70" s="16"/>
@@ -9633,15 +8527,15 @@
       <c r="M90" s="22"/>
       <c r="O90" s="23"/>
       <c r="P90" s="52"/>
-      <c r="Q90" s="284" t="s">
+      <c r="Q90" s="297" t="s">
         <v>145</v>
       </c>
-      <c r="R90" s="284"/>
-      <c r="S90" s="284"/>
-      <c r="T90" s="284" t="s">
+      <c r="R90" s="297"/>
+      <c r="S90" s="297"/>
+      <c r="T90" s="297" t="s">
         <v>146</v>
       </c>
-      <c r="U90" s="284"/>
+      <c r="U90" s="297"/>
       <c r="Y90" s="24"/>
       <c r="AA90" s="27" t="s">
         <v>122</v>
@@ -9784,15 +8678,15 @@
       </c>
       <c r="B94" s="20"/>
       <c r="E94" s="68"/>
-      <c r="F94" s="286" t="s">
+      <c r="F94" s="299" t="s">
         <v>145</v>
       </c>
-      <c r="G94" s="286"/>
-      <c r="H94" s="286"/>
-      <c r="I94" s="287" t="s">
+      <c r="G94" s="299"/>
+      <c r="H94" s="299"/>
+      <c r="I94" s="300" t="s">
         <v>146</v>
       </c>
-      <c r="J94" s="287"/>
+      <c r="J94" s="300"/>
       <c r="M94" s="22"/>
       <c r="O94" s="23"/>
       <c r="P94" s="27" t="s">
@@ -9956,10 +8850,10 @@
         <v>31</v>
       </c>
       <c r="B97" s="20"/>
-      <c r="D97" s="288" t="s">
+      <c r="D97" s="301" t="s">
         <v>155</v>
       </c>
-      <c r="E97" s="289"/>
+      <c r="E97" s="302"/>
       <c r="F97" s="94" t="str">
         <f t="shared" ref="F97:J102" si="31">IF(Q122="","",Q122)</f>
         <v/>
@@ -10015,8 +8909,8 @@
         <v>32</v>
       </c>
       <c r="B98" s="20"/>
-      <c r="D98" s="288"/>
-      <c r="E98" s="289"/>
+      <c r="D98" s="301"/>
+      <c r="E98" s="302"/>
       <c r="F98" s="99" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -10072,8 +8966,8 @@
         <v>33</v>
       </c>
       <c r="B99" s="20"/>
-      <c r="D99" s="288"/>
-      <c r="E99" s="289"/>
+      <c r="D99" s="301"/>
+      <c r="E99" s="302"/>
       <c r="F99" s="104" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -10964,7 +9858,7 @@
       </c>
       <c r="P117" s="262"/>
       <c r="R117" s="259" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="S117" s="265"/>
       <c r="T117" s="263"/>
@@ -11016,15 +9910,15 @@
       <c r="J119" s="19"/>
       <c r="M119" s="22"/>
       <c r="O119" s="23"/>
-      <c r="Q119" s="281" t="s">
+      <c r="Q119" s="294" t="s">
         <v>145</v>
       </c>
-      <c r="R119" s="282"/>
-      <c r="S119" s="283"/>
-      <c r="T119" s="281" t="s">
+      <c r="R119" s="295"/>
+      <c r="S119" s="296"/>
+      <c r="T119" s="294" t="s">
         <v>146</v>
       </c>
-      <c r="U119" s="283"/>
+      <c r="U119" s="296"/>
       <c r="W119" s="55" t="s">
         <v>152</v>
       </c>
@@ -11148,10 +10042,10 @@
         <v>Water phantom is free from rings, streaks, lines, cupping artifacts</v>
       </c>
       <c r="M122" s="22"/>
-      <c r="O122" s="279" t="s">
+      <c r="O122" s="292" t="s">
         <v>155</v>
       </c>
-      <c r="P122" s="280"/>
+      <c r="P122" s="293"/>
       <c r="Q122" s="137"/>
       <c r="R122" s="138"/>
       <c r="S122" s="139"/>
@@ -11183,8 +10077,8 @@
       </c>
       <c r="B123" s="20"/>
       <c r="M123" s="22"/>
-      <c r="O123" s="279"/>
-      <c r="P123" s="280"/>
+      <c r="O123" s="292"/>
+      <c r="P123" s="293"/>
       <c r="Q123" s="140"/>
       <c r="R123" s="141"/>
       <c r="S123" s="142"/>
@@ -11221,8 +10115,8 @@
         <v>183</v>
       </c>
       <c r="M124" s="22"/>
-      <c r="O124" s="279"/>
-      <c r="P124" s="280"/>
+      <c r="O124" s="292"/>
+      <c r="P124" s="293"/>
       <c r="Q124" s="144"/>
       <c r="R124" s="145"/>
       <c r="S124" s="146"/>
@@ -11345,7 +10239,7 @@
       </c>
       <c r="H126" s="52"/>
       <c r="I126" s="19"/>
-      <c r="J126" s="312"/>
+      <c r="J126" s="288"/>
       <c r="K126" s="14" t="s">
         <v>369</v>
       </c>
@@ -11400,7 +10294,7 @@
       <c r="G127" s="165" t="s">
         <v>191</v>
       </c>
-      <c r="J127" s="312"/>
+      <c r="J127" s="288"/>
       <c r="K127" s="14" t="s">
         <v>368</v>
       </c>
@@ -11616,23 +10510,23 @@
         <v>168</v>
       </c>
       <c r="Q131" s="134" t="str">
-        <f>IF(Q125="","",IF(AND(Q125&lt;=Y123,Q129&lt;=0.05,Q130&lt;=0.2),"Pass","Fail"))</f>
+        <f>IF(Q125="","",IF(AND(Q125&lt;=X123,Q130&lt;=0.2),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="R131" s="135" t="str">
-        <f>IF(R125="","",IF(AND(R125&lt;=Y123,R130&lt;=0.2),"Pass","Fail"))</f>
+        <f>IF(R125="","",IF(AND(R125&lt;=X123,R130&lt;=0.2),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="S131" s="136" t="str">
-        <f>IF(S125="","",IF(AND(S125&lt;=Y124,S130&lt;=0.2),"Pass","Fail"))</f>
+        <f>IF(S125="","",IF(AND(S125&lt;=X124,S130&lt;=0.2),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="T131" s="135" t="str">
-        <f>IF(T125="","",IF(AND(T125&lt;=Y126,T129&lt;=0.05,T130&lt;=0.2),"Pass","Fail"))</f>
+        <f>IF(T125="","",IF(AND(T125&lt;=X126,T130&lt;=0.2),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="U131" s="136" t="str">
-        <f>IF(U125="","",IF(AND(U125&lt;=Y127,U129&lt;=0.05,U130&lt;=0.2),"Pass","Fail"))</f>
+        <f>IF(U125="","",IF(AND(U125&lt;=X127,U130&lt;=0.2),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="V131" s="19"/>
@@ -12078,7 +10972,7 @@
       </c>
       <c r="M141" s="22"/>
       <c r="O141" s="23"/>
-      <c r="P141" s="280" t="s">
+      <c r="P141" s="293" t="s">
         <v>175</v>
       </c>
       <c r="Q141" s="171"/>
@@ -12107,7 +11001,7 @@
       <c r="C142" s="52"/>
       <c r="M142" s="22"/>
       <c r="O142" s="23"/>
-      <c r="P142" s="280"/>
+      <c r="P142" s="293"/>
       <c r="Q142" s="171"/>
       <c r="R142" s="172"/>
       <c r="S142" s="172"/>
@@ -12136,7 +11030,7 @@
       </c>
       <c r="M143" s="22"/>
       <c r="O143" s="23"/>
-      <c r="P143" s="280"/>
+      <c r="P143" s="293"/>
       <c r="Q143" s="174"/>
       <c r="R143" s="175"/>
       <c r="S143" s="175"/>
@@ -13282,14 +12176,14 @@
       <c r="B168" s="20"/>
       <c r="C168" s="52"/>
       <c r="D168" s="68"/>
-      <c r="E168" s="285" t="s">
+      <c r="E168" s="298" t="s">
         <v>145</v>
       </c>
-      <c r="F168" s="285"/>
-      <c r="G168" s="285" t="s">
+      <c r="F168" s="298"/>
+      <c r="G168" s="298" t="s">
         <v>146</v>
       </c>
-      <c r="H168" s="285"/>
+      <c r="H168" s="298"/>
       <c r="M168" s="22"/>
       <c r="O168" s="185" t="s">
         <v>218</v>
@@ -14646,7 +13540,7 @@
       <c r="T206" s="274" t="s">
         <v>362</v>
       </c>
-      <c r="U206" s="304" t="s">
+      <c r="U206" s="308" t="s">
         <v>363</v>
       </c>
       <c r="Y206" s="24"/>
@@ -14670,13 +13564,13 @@
       <c r="L207" s="196"/>
       <c r="M207" s="22"/>
       <c r="O207" s="23"/>
-      <c r="S207" s="301" t="s">
+      <c r="S207" s="279" t="s">
         <v>190</v>
       </c>
       <c r="T207" s="274" t="s">
         <v>365</v>
       </c>
-      <c r="U207" s="305"/>
+      <c r="U207" s="309"/>
       <c r="Y207" s="24"/>
     </row>
     <row r="208" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -14702,14 +13596,14 @@
         <v>184</v>
       </c>
       <c r="R208" s="19"/>
-      <c r="S208" s="299" t="s">
+      <c r="S208" s="277" t="s">
         <v>353</v>
       </c>
-      <c r="T208" s="302">
+      <c r="T208" s="280">
         <f>AH27</f>
         <v>0</v>
       </c>
-      <c r="U208" s="303" t="e">
+      <c r="U208" s="281" t="e">
         <f>(T208-MEDIAN($T$208:$T$216))/MEDIAN($T$208:$T$216)</f>
         <v>#DIV/0!</v>
       </c>
@@ -14738,14 +13632,14 @@
         <v>187</v>
       </c>
       <c r="R209" s="19"/>
-      <c r="S209" s="299" t="s">
+      <c r="S209" s="277" t="s">
         <v>354</v>
       </c>
-      <c r="T209" s="302">
+      <c r="T209" s="280">
         <f t="shared" ref="T209:T216" si="46">AH28</f>
         <v>0</v>
       </c>
-      <c r="U209" s="303" t="e">
+      <c r="U209" s="281" t="e">
         <f t="shared" ref="U209:U216" si="47">(T209-MEDIAN($T$208:$T$216))/MEDIAN($T$208:$T$216)</f>
         <v>#DIV/0!</v>
       </c>
@@ -14774,14 +13668,14 @@
         <v>190</v>
       </c>
       <c r="R210" s="19"/>
-      <c r="S210" s="299" t="s">
+      <c r="S210" s="277" t="s">
         <v>355</v>
       </c>
-      <c r="T210" s="302">
+      <c r="T210" s="280">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="U210" s="303" t="e">
+      <c r="U210" s="281" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
@@ -14814,14 +13708,14 @@
       </c>
       <c r="Q211" s="19"/>
       <c r="R211" s="19"/>
-      <c r="S211" s="299" t="s">
+      <c r="S211" s="277" t="s">
         <v>356</v>
       </c>
-      <c r="T211" s="302">
+      <c r="T211" s="280">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="U211" s="303" t="e">
+      <c r="U211" s="281" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
@@ -14857,14 +13751,14 @@
       </c>
       <c r="Q212" s="19"/>
       <c r="R212" s="19"/>
-      <c r="S212" s="299" t="s">
+      <c r="S212" s="277" t="s">
         <v>357</v>
       </c>
-      <c r="T212" s="302">
+      <c r="T212" s="280">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="U212" s="303" t="e">
+      <c r="U212" s="281" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
@@ -14899,14 +13793,14 @@
       </c>
       <c r="Q213" s="19"/>
       <c r="R213" s="19"/>
-      <c r="S213" s="299" t="s">
+      <c r="S213" s="277" t="s">
         <v>358</v>
       </c>
-      <c r="T213" s="302">
+      <c r="T213" s="280">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="U213" s="303" t="e">
+      <c r="U213" s="281" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
@@ -14934,19 +13828,19 @@
       <c r="L214" s="194"/>
       <c r="M214" s="22"/>
       <c r="O214" s="156"/>
-      <c r="P214" s="298" t="s">
+      <c r="P214" s="276" t="s">
         <v>366</v>
       </c>
       <c r="Q214" s="19"/>
       <c r="R214" s="19"/>
-      <c r="S214" s="299" t="s">
+      <c r="S214" s="277" t="s">
         <v>359</v>
       </c>
-      <c r="T214" s="302">
+      <c r="T214" s="280">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="U214" s="303" t="e">
+      <c r="U214" s="281" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
@@ -14974,17 +13868,17 @@
       <c r="L215" s="196"/>
       <c r="M215" s="22"/>
       <c r="O215" s="156"/>
-      <c r="P215" s="298" t="s">
+      <c r="P215" s="276" t="s">
         <v>367</v>
       </c>
-      <c r="S215" s="299" t="s">
+      <c r="S215" s="277" t="s">
         <v>360</v>
       </c>
-      <c r="T215" s="302">
+      <c r="T215" s="280">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="U215" s="303" t="e">
+      <c r="U215" s="281" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
@@ -15009,14 +13903,14 @@
       <c r="L216" s="196"/>
       <c r="M216" s="22"/>
       <c r="O216" s="156"/>
-      <c r="S216" s="299" t="s">
+      <c r="S216" s="277" t="s">
         <v>361</v>
       </c>
-      <c r="T216" s="306">
+      <c r="T216" s="282">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="U216" s="310" t="e">
+      <c r="U216" s="286" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
@@ -15044,11 +13938,11 @@
       <c r="S217" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="T217" s="307">
+      <c r="T217" s="283">
         <f>IF(T208="","",AVERAGE(T208:T212))</f>
         <v>0</v>
       </c>
-      <c r="U217" s="311" t="e">
+      <c r="U217" s="287" t="e">
         <f>MAX(U208:U216)</f>
         <v>#DIV/0!</v>
       </c>
@@ -15079,7 +13973,7 @@
       <c r="S218" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="T218" s="308">
+      <c r="T218" s="284">
         <f>IF(T208="","",STDEV(T208:T212))</f>
         <v>0</v>
       </c>
@@ -15104,10 +13998,10 @@
       <c r="L219" s="196"/>
       <c r="M219" s="22"/>
       <c r="O219" s="156"/>
-      <c r="S219" s="300" t="s">
+      <c r="S219" s="278" t="s">
         <v>268</v>
       </c>
-      <c r="T219" s="309" t="e">
+      <c r="T219" s="285" t="e">
         <f>IF(T208="","",2*(MAX(T208:T212)-MIN(T208:T212))/(MAX(T208:T212)+MIN(T208:T212)))</f>
         <v>#DIV/0!</v>
       </c>
@@ -16633,164 +15527,164 @@
     <mergeCell ref="T90:U90"/>
   </mergeCells>
   <conditionalFormatting sqref="L33:L38 L60:L63 L41:L57">
-    <cfRule type="cellIs" dxfId="73" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="47" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q131:U131 F105:J105">
-    <cfRule type="cellIs" dxfId="72" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="45" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q145:T145 E117:H117">
-    <cfRule type="cellIs" dxfId="71" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122">
-    <cfRule type="cellIs" dxfId="70" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C125:C127">
-    <cfRule type="cellIs" dxfId="68" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H152">
-    <cfRule type="cellIs" dxfId="67" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="37" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F163:J163 Q180:U180 K170:K171 F191:F192 Q203:Q204">
-    <cfRule type="cellIs" dxfId="66" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q130:U130">
-    <cfRule type="cellIs" dxfId="65" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="lessThan">
       <formula>0.2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="32" operator="greaterThan">
       <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q129:U129">
-    <cfRule type="cellIs" dxfId="63" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M33:M38 M60:M63 M41:M57">
-    <cfRule type="cellIs" dxfId="61" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L138:L141">
-    <cfRule type="cellIs" dxfId="60" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q203:Q204">
-    <cfRule type="cellIs" dxfId="59" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R195:S199">
-    <cfRule type="cellIs" dxfId="57" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H181:H185">
-    <cfRule type="cellIs" dxfId="55" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T195:T199">
-    <cfRule type="cellIs" dxfId="54" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P164:V164">
-    <cfRule type="cellIs" dxfId="52" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
       <formula>-5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X187">
-    <cfRule type="cellIs" dxfId="50" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P191:Q191">
-    <cfRule type="cellIs" dxfId="48" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R191">
-    <cfRule type="cellIs" dxfId="46" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S191">
-    <cfRule type="cellIs" dxfId="44" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R163:T163">
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
       <formula>$X$163</formula>
       <formula>$Y$163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R164:T164">
-    <cfRule type="cellIs" dxfId="41" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>$X$164</formula>
       <formula>$Y$164</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R166:T166">
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>$X$165</formula>
       <formula>$Y$165</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R167:T167">
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>$X$166</formula>
       <formula>$Y$166</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R168:T168">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>$X$167</formula>
       <formula>$Y$167</formula>
     </cfRule>
@@ -16817,7 +15711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView topLeftCell="A51" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
@@ -16843,17 +15737,17 @@
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="297" t="s">
+      <c r="A4" s="312" t="s">
         <v>279</v>
       </c>
-      <c r="B4" s="297" t="s">
+      <c r="B4" s="312" t="s">
         <v>280</v>
       </c>
-      <c r="C4" s="297"/>
-      <c r="D4" s="297"/>
+      <c r="C4" s="312"/>
+      <c r="D4" s="312"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="297"/>
+      <c r="A5" s="312"/>
       <c r="B5" s="5" t="s">
         <v>281</v>
       </c>
@@ -17025,17 +15919,17 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="297" t="s">
+      <c r="A18" s="312" t="s">
         <v>279</v>
       </c>
-      <c r="B18" s="297" t="s">
+      <c r="B18" s="312" t="s">
         <v>296</v>
       </c>
-      <c r="C18" s="297"/>
-      <c r="D18" s="297"/>
+      <c r="C18" s="312"/>
+      <c r="D18" s="312"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="297"/>
+      <c r="A19" s="312"/>
       <c r="B19" s="5" t="s">
         <v>281</v>
       </c>
@@ -17271,16 +16165,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="297" t="s">
+      <c r="A37" s="312" t="s">
         <v>279</v>
       </c>
-      <c r="B37" s="297" t="s">
+      <c r="B37" s="312" t="s">
         <v>301</v>
       </c>
-      <c r="C37" s="297"/>
+      <c r="C37" s="312"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="297"/>
+      <c r="A38" s="312"/>
       <c r="B38" s="5" t="s">
         <v>282</v>
       </c>
@@ -17366,16 +16260,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="297" t="s">
+      <c r="A47" s="312" t="s">
         <v>279</v>
       </c>
-      <c r="B47" s="297" t="s">
+      <c r="B47" s="312" t="s">
         <v>304</v>
       </c>
-      <c r="C47" s="297"/>
+      <c r="C47" s="312"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="297"/>
+      <c r="A48" s="312"/>
       <c r="B48" s="5" t="s">
         <v>282</v>
       </c>
@@ -17461,16 +16355,16 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="297" t="s">
+      <c r="A57" s="312" t="s">
         <v>279</v>
       </c>
-      <c r="B57" s="297" t="s">
+      <c r="B57" s="312" t="s">
         <v>311</v>
       </c>
-      <c r="C57" s="297"/>
+      <c r="C57" s="312"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="297"/>
+      <c r="A58" s="312"/>
       <c r="B58" s="5" t="s">
         <v>282</v>
       </c>
@@ -17556,16 +16450,16 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="297" t="s">
+      <c r="A67" s="312" t="s">
         <v>279</v>
       </c>
-      <c r="B67" s="297" t="s">
+      <c r="B67" s="312" t="s">
         <v>316</v>
       </c>
-      <c r="C67" s="297"/>
+      <c r="C67" s="312"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="297"/>
+      <c r="A68" s="312"/>
       <c r="B68" s="5" t="s">
         <v>282</v>
       </c>
@@ -17695,7 +16589,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="296" t="s">
+      <c r="A81" s="311" t="s">
         <v>279</v>
       </c>
       <c r="B81" t="s">
@@ -17703,7 +16597,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="296"/>
+      <c r="A82" s="311"/>
       <c r="B82" t="s">
         <v>282</v>
       </c>

</xml_diff>

<commit_message>
Changes that I've forgotten
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47798AA5-B0D3-4205-B2C9-5FE63992C5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAE33A4-60E2-477D-A333-BDF60B18F9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="Z_25C83B95_F566_493A_A3D1_2FC57CA3E0EA_.wvu.PrintArea" localSheetId="1" hidden="1">Sheet1!$B$1:$M$264</definedName>
     <definedName name="Z_25C83B95_F566_493A_A3D1_2FC57CA3E0EA_.wvu.PrintArea" localSheetId="0" hidden="1">Summary!$A$1:$F$40</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="1" iterateDelta="1E-4"/>
   <customWorkbookViews>
     <customWorkbookView name="Eugene Mah - Personal View" guid="{25C83B95-F566-493A-A3D1-2FC57CA3E0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="784" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="373">
   <si>
     <t>Medical Physicist CT Survey Report</t>
   </si>
@@ -3138,74 +3138,74 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -3219,16 +3219,6 @@
     <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="38">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3416,6 +3406,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3685,15 +3685,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>77400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>3060</xdr:rowOff>
+      <xdr:colOff>54540</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>277560</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>95700</xdr:rowOff>
+      <xdr:colOff>254700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>118560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3712,8 +3712,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1649520" y="2540520"/>
-          <a:ext cx="974160" cy="290520"/>
+          <a:off x="1753800" y="2761500"/>
+          <a:ext cx="1030740" cy="290760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3993,8 +3993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4076,19 +4076,19 @@
       <c r="A6" s="203" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="269" t="str">
+      <c r="B6" s="267" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="269"/>
+      <c r="C6" s="267"/>
       <c r="D6" s="203" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="269" t="str">
+      <c r="E6" s="267" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="269"/>
+      <c r="F6" s="267"/>
       <c r="G6" s="1"/>
       <c r="J6" s="228" t="s">
         <v>320</v>
@@ -4098,48 +4098,48 @@
       <c r="A7" s="203" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="267"/>
-      <c r="C7" s="267"/>
+      <c r="B7" s="268"/>
+      <c r="C7" s="268"/>
       <c r="D7" s="203" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="267" t="str">
+      <c r="E7" s="268" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="267"/>
+      <c r="F7" s="268"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="203" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="267"/>
-      <c r="C8" s="267"/>
+      <c r="B8" s="268"/>
+      <c r="C8" s="268"/>
       <c r="D8" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="267" t="str">
+      <c r="E8" s="268" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="267"/>
+      <c r="F8" s="268"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="203" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="267"/>
-      <c r="C9" s="267"/>
+      <c r="B9" s="268"/>
+      <c r="C9" s="268"/>
       <c r="D9" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="267" t="str">
+      <c r="E9" s="268" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="267"/>
+      <c r="F9" s="268"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4149,19 +4149,19 @@
       <c r="D10" s="203" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="268" t="str">
+      <c r="E10" s="269" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="268"/>
+      <c r="F10" s="269"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="269"/>
-      <c r="C11" s="269"/>
+      <c r="B11" s="267"/>
+      <c r="C11" s="267"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4184,10 +4184,10 @@
       <c r="A13" s="205" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="269" t="s">
+      <c r="B13" s="267" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="269"/>
+      <c r="C13" s="267"/>
       <c r="D13" s="203" t="s">
         <v>16</v>
       </c>
@@ -4276,7 +4276,9 @@
       <c r="E20" s="211" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="210"/>
+      <c r="F20" s="210" t="s">
+        <v>320</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4301,7 +4303,9 @@
       <c r="E22" s="211" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="210"/>
+      <c r="F22" s="210" t="s">
+        <v>320</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4500,17 +4504,17 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -4533,7 +4537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -4829,19 +4833,19 @@
       <c r="E10" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="282" t="str">
+      <c r="F10" s="272" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="282"/>
+      <c r="G10" s="272"/>
       <c r="J10" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="282" t="str">
+      <c r="K10" s="272" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="282"/>
+      <c r="L10" s="272"/>
       <c r="M10" s="18"/>
       <c r="O10" s="19"/>
       <c r="Q10" s="23" t="s">
@@ -4885,19 +4889,19 @@
       <c r="E11" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="283" t="str">
+      <c r="F11" s="274" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="283"/>
+      <c r="G11" s="274"/>
       <c r="J11" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="282" t="str">
+      <c r="K11" s="272" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="282"/>
+      <c r="L11" s="272"/>
       <c r="M11" s="18"/>
       <c r="O11" s="19"/>
       <c r="Q11" s="23" t="s">
@@ -4941,19 +4945,19 @@
       <c r="E12" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="283" t="str">
+      <c r="F12" s="274" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="283"/>
+      <c r="G12" s="274"/>
       <c r="J12" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="284" t="str">
+      <c r="K12" s="275" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="284"/>
+      <c r="L12" s="275"/>
       <c r="M12" s="18"/>
       <c r="O12" s="19"/>
       <c r="Q12" s="23" t="s">
@@ -4997,19 +5001,19 @@
       <c r="E13" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="283" t="str">
+      <c r="F13" s="274" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="283"/>
+      <c r="G13" s="274"/>
       <c r="J13" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="282" t="str">
+      <c r="K13" s="272" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="282"/>
+      <c r="L13" s="272"/>
       <c r="M13" s="18"/>
       <c r="O13" s="19"/>
       <c r="Q13" s="23" t="s">
@@ -5115,19 +5119,19 @@
       <c r="E16" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="282" t="str">
+      <c r="F16" s="272" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="282"/>
+      <c r="G16" s="272"/>
       <c r="J16" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="284" t="str">
+      <c r="K16" s="275" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="284"/>
+      <c r="L16" s="275"/>
       <c r="M16" s="18"/>
       <c r="O16" s="19"/>
       <c r="P16" s="50" t="s">
@@ -5158,19 +5162,19 @@
       <c r="E17" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="283" t="str">
+      <c r="F17" s="274" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="283"/>
+      <c r="G17" s="274"/>
       <c r="J17" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="282" t="str">
+      <c r="K17" s="272" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="282"/>
+      <c r="L17" s="272"/>
       <c r="M17" s="18"/>
       <c r="O17" s="19"/>
       <c r="Q17" s="23" t="s">
@@ -5214,11 +5218,11 @@
       <c r="J18" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="282" t="str">
+      <c r="K18" s="272" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="282"/>
+      <c r="L18" s="272"/>
       <c r="M18" s="18"/>
       <c r="O18" s="19"/>
       <c r="Q18" s="23" t="s">
@@ -5286,11 +5290,11 @@
       <c r="E20" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="282" t="str">
+      <c r="F20" s="272" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="282"/>
+      <c r="G20" s="272"/>
       <c r="I20" s="53" t="s">
         <v>76</v>
       </c>
@@ -5315,19 +5319,19 @@
       <c r="E21" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="287" t="str">
+      <c r="F21" s="276" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="287"/>
+      <c r="G21" s="276"/>
       <c r="J21" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="282" t="str">
+      <c r="K21" s="272" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="282"/>
+      <c r="L21" s="272"/>
       <c r="M21" s="18"/>
       <c r="O21" s="19"/>
       <c r="Q21" s="23" t="s">
@@ -5369,11 +5373,11 @@
       <c r="J22" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="282" t="str">
+      <c r="K22" s="272" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="282"/>
+      <c r="L22" s="272"/>
       <c r="M22" s="18"/>
       <c r="O22" s="19"/>
       <c r="Q22" s="23" t="s">
@@ -5417,19 +5421,19 @@
       <c r="E23" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="282" t="str">
+      <c r="F23" s="272" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="282"/>
+      <c r="G23" s="272"/>
       <c r="J23" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="282" t="str">
+      <c r="K23" s="272" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="282"/>
+      <c r="L23" s="272"/>
       <c r="M23" s="18"/>
       <c r="O23" s="19"/>
       <c r="P23" s="50" t="s">
@@ -5468,11 +5472,11 @@
       <c r="E24" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="282" t="str">
+      <c r="F24" s="272" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="282"/>
+      <c r="G24" s="272"/>
       <c r="M24" s="18"/>
       <c r="O24" s="19"/>
       <c r="Q24" s="23" t="s">
@@ -5516,11 +5520,11 @@
       <c r="E25" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="282" t="str">
+      <c r="F25" s="272" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="282"/>
+      <c r="G25" s="272"/>
       <c r="J25" s="49" t="s">
         <v>82</v>
       </c>
@@ -5562,11 +5566,11 @@
       <c r="J26" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="282" t="str">
+      <c r="K26" s="272" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="282"/>
+      <c r="L26" s="272"/>
       <c r="M26" s="18"/>
       <c r="O26" s="19"/>
       <c r="Q26" s="23" t="s">
@@ -5593,19 +5597,19 @@
       <c r="E27" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="282" t="str">
+      <c r="F27" s="272" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="282"/>
+      <c r="G27" s="272"/>
       <c r="J27" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="282" t="str">
+      <c r="K27" s="272" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="282"/>
+      <c r="L27" s="272"/>
       <c r="M27" s="18"/>
       <c r="O27" s="19"/>
       <c r="P27" s="50" t="s">
@@ -5635,11 +5639,11 @@
       <c r="E28" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="282" t="str">
+      <c r="F28" s="272" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="282"/>
+      <c r="G28" s="272"/>
       <c r="M28" s="18"/>
       <c r="O28" s="19"/>
       <c r="Q28" s="23" t="s">
@@ -5683,11 +5687,11 @@
       <c r="E29" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="282" t="str">
+      <c r="F29" s="272" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="282"/>
+      <c r="G29" s="272"/>
       <c r="M29" s="18"/>
       <c r="O29" s="19"/>
       <c r="Q29" s="23" t="s">
@@ -5806,10 +5810,10 @@
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
-      <c r="L32" s="281" t="s">
+      <c r="L32" s="277" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="281"/>
+      <c r="M32" s="277"/>
       <c r="AA32" s="23" t="s">
         <v>70</v>
       </c>
@@ -7121,27 +7125,27 @@
       </c>
       <c r="B70" s="16"/>
       <c r="E70" s="61"/>
-      <c r="F70" s="276" t="s">
+      <c r="F70" s="278" t="s">
         <v>139</v>
       </c>
-      <c r="G70" s="276"/>
-      <c r="H70" s="276"/>
-      <c r="I70" s="276" t="s">
+      <c r="G70" s="278"/>
+      <c r="H70" s="278"/>
+      <c r="I70" s="278" t="s">
         <v>140</v>
       </c>
-      <c r="J70" s="276"/>
+      <c r="J70" s="278"/>
       <c r="M70" s="18"/>
       <c r="O70" s="39"/>
       <c r="P70" s="13"/>
-      <c r="Q70" s="273" t="s">
+      <c r="Q70" s="279" t="s">
         <v>139</v>
       </c>
-      <c r="R70" s="273"/>
-      <c r="S70" s="273"/>
-      <c r="T70" s="273" t="s">
+      <c r="R70" s="279"/>
+      <c r="S70" s="279"/>
+      <c r="T70" s="279" t="s">
         <v>140</v>
       </c>
-      <c r="U70" s="273"/>
+      <c r="U70" s="279"/>
       <c r="V70" s="13"/>
       <c r="W70" s="13"/>
       <c r="X70" s="13"/>
@@ -8405,15 +8409,15 @@
       </c>
       <c r="M90" s="18"/>
       <c r="O90" s="19"/>
-      <c r="Q90" s="275" t="s">
+      <c r="Q90" s="287" t="s">
         <v>139</v>
       </c>
-      <c r="R90" s="275"/>
-      <c r="S90" s="275"/>
-      <c r="T90" s="275" t="s">
+      <c r="R90" s="287"/>
+      <c r="S90" s="287"/>
+      <c r="T90" s="287" t="s">
         <v>140</v>
       </c>
-      <c r="U90" s="275"/>
+      <c r="U90" s="287"/>
       <c r="Y90" s="20"/>
       <c r="AA90" s="23" t="s">
         <v>120</v>
@@ -8556,15 +8560,15 @@
       </c>
       <c r="B94" s="16"/>
       <c r="E94" s="61"/>
-      <c r="F94" s="277" t="s">
+      <c r="F94" s="280" t="s">
         <v>139</v>
       </c>
-      <c r="G94" s="277"/>
-      <c r="H94" s="277"/>
-      <c r="I94" s="278" t="s">
+      <c r="G94" s="280"/>
+      <c r="H94" s="280"/>
+      <c r="I94" s="281" t="s">
         <v>140</v>
       </c>
-      <c r="J94" s="278"/>
+      <c r="J94" s="281"/>
       <c r="M94" s="18"/>
       <c r="O94" s="19"/>
       <c r="P94" s="23" t="s">
@@ -8727,10 +8731,10 @@
         <v>31</v>
       </c>
       <c r="B97" s="16"/>
-      <c r="D97" s="279" t="s">
+      <c r="D97" s="282" t="s">
         <v>149</v>
       </c>
-      <c r="E97" s="280"/>
+      <c r="E97" s="283"/>
       <c r="F97" s="87" t="str">
         <f t="shared" ref="F97:J102" si="31">IF(Q122="","",Q122)</f>
         <v/>
@@ -8785,8 +8789,8 @@
         <v>32</v>
       </c>
       <c r="B98" s="16"/>
-      <c r="D98" s="279"/>
-      <c r="E98" s="280"/>
+      <c r="D98" s="282"/>
+      <c r="E98" s="283"/>
       <c r="F98" s="92" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -8841,8 +8845,8 @@
         <v>33</v>
       </c>
       <c r="B99" s="16"/>
-      <c r="D99" s="279"/>
-      <c r="E99" s="280"/>
+      <c r="D99" s="282"/>
+      <c r="E99" s="283"/>
       <c r="F99" s="97" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -9749,15 +9753,15 @@
       <c r="B119" s="16"/>
       <c r="M119" s="18"/>
       <c r="O119" s="19"/>
-      <c r="Q119" s="272" t="s">
+      <c r="Q119" s="285" t="s">
         <v>139</v>
       </c>
-      <c r="R119" s="273"/>
-      <c r="S119" s="274"/>
-      <c r="T119" s="272" t="s">
+      <c r="R119" s="279"/>
+      <c r="S119" s="286"/>
+      <c r="T119" s="285" t="s">
         <v>140</v>
       </c>
-      <c r="U119" s="274"/>
+      <c r="U119" s="286"/>
       <c r="W119" s="50" t="s">
         <v>146</v>
       </c>
@@ -9880,10 +9884,10 @@
         <v>Water phantom is free from rings, streaks, lines, cupping artifacts</v>
       </c>
       <c r="M122" s="18"/>
-      <c r="O122" s="270" t="s">
+      <c r="O122" s="284" t="s">
         <v>149</v>
       </c>
-      <c r="P122" s="271"/>
+      <c r="P122" s="273"/>
       <c r="Q122" s="130"/>
       <c r="R122" s="131"/>
       <c r="S122" s="132"/>
@@ -9914,8 +9918,8 @@
       </c>
       <c r="B123" s="16"/>
       <c r="M123" s="18"/>
-      <c r="O123" s="270"/>
-      <c r="P123" s="271"/>
+      <c r="O123" s="284"/>
+      <c r="P123" s="273"/>
       <c r="Q123" s="133"/>
       <c r="R123" s="134"/>
       <c r="S123" s="135"/>
@@ -9952,8 +9956,8 @@
         <v>177</v>
       </c>
       <c r="M124" s="18"/>
-      <c r="O124" s="270"/>
-      <c r="P124" s="271"/>
+      <c r="O124" s="284"/>
+      <c r="P124" s="273"/>
       <c r="Q124" s="137"/>
       <c r="R124" s="138"/>
       <c r="S124" s="139"/>
@@ -10755,7 +10759,7 @@
       </c>
       <c r="M141" s="18"/>
       <c r="O141" s="19"/>
-      <c r="P141" s="271" t="s">
+      <c r="P141" s="273" t="s">
         <v>169</v>
       </c>
       <c r="Q141" s="161"/>
@@ -10783,7 +10787,7 @@
       <c r="B142" s="16"/>
       <c r="M142" s="18"/>
       <c r="O142" s="19"/>
-      <c r="P142" s="271"/>
+      <c r="P142" s="273"/>
       <c r="Q142" s="161"/>
       <c r="R142" s="162"/>
       <c r="S142" s="162"/>
@@ -10812,7 +10816,7 @@
       </c>
       <c r="M143" s="18"/>
       <c r="O143" s="19"/>
-      <c r="P143" s="271"/>
+      <c r="P143" s="273"/>
       <c r="Q143" s="164"/>
       <c r="R143" s="165"/>
       <c r="S143" s="165"/>
@@ -11888,14 +11892,14 @@
       </c>
       <c r="B168" s="16"/>
       <c r="D168" s="61"/>
-      <c r="E168" s="276" t="s">
+      <c r="E168" s="278" t="s">
         <v>139</v>
       </c>
-      <c r="F168" s="276"/>
-      <c r="G168" s="276" t="s">
+      <c r="F168" s="278"/>
+      <c r="G168" s="278" t="s">
         <v>140</v>
       </c>
-      <c r="H168" s="276"/>
+      <c r="H168" s="278"/>
       <c r="M168" s="18"/>
       <c r="O168" s="174" t="s">
         <v>212</v>
@@ -13185,7 +13189,7 @@
       <c r="T206" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="U206" s="285" t="s">
+      <c r="U206" s="270" t="s">
         <v>357</v>
       </c>
       <c r="Y206" s="20"/>
@@ -13215,7 +13219,7 @@
       <c r="T207" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="U207" s="286"/>
+      <c r="U207" s="271"/>
       <c r="Y207" s="20"/>
     </row>
     <row r="208" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15085,6 +15089,33 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="43">
+    <mergeCell ref="O122:P124"/>
+    <mergeCell ref="Q119:S119"/>
+    <mergeCell ref="T119:U119"/>
+    <mergeCell ref="Q90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="E168:F168"/>
+    <mergeCell ref="G168:H168"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="D97:E99"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
     <mergeCell ref="U206:U207"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="F20:G20"/>
@@ -15101,33 +15132,6 @@
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="T70:U70"/>
-    <mergeCell ref="E168:F168"/>
-    <mergeCell ref="G168:H168"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="I94:J94"/>
-    <mergeCell ref="D97:E99"/>
-    <mergeCell ref="O122:P124"/>
-    <mergeCell ref="Q119:S119"/>
-    <mergeCell ref="T119:U119"/>
-    <mergeCell ref="Q90:S90"/>
-    <mergeCell ref="T90:U90"/>
   </mergeCells>
   <conditionalFormatting sqref="C122">
     <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
@@ -15211,94 +15215,94 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Q145:T145">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Q129:U129">
-    <cfRule type="cellIs" dxfId="19" priority="30" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="30" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="31" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q130:U130">
-    <cfRule type="cellIs" dxfId="17" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="29" operator="lessThan">
       <formula>0.2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="33" operator="greaterThan">
       <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R191">
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R195:S199">
-    <cfRule type="cellIs" dxfId="13" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="23" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="24" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R163:T163">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="between">
       <formula>$X$163</formula>
       <formula>$Y$163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R164:T164">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="between">
       <formula>$X$164</formula>
       <formula>$Y$164</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R166:T166">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="between">
       <formula>$X$165</formula>
       <formula>$Y$165</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R167:T167">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="between">
       <formula>$X$166</formula>
       <formula>$Y$166</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R168:T168">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="between">
       <formula>$X$167</formula>
       <formula>$Y$167</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S191">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T195:T199">
-    <cfRule type="cellIs" dxfId="4" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="20" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X187">
-    <cfRule type="cellIs" dxfId="2" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q145:T145">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15342,17 +15346,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="289" t="s">
+      <c r="A4" s="288" t="s">
         <v>273</v>
       </c>
-      <c r="B4" s="289" t="s">
+      <c r="B4" s="288" t="s">
         <v>274</v>
       </c>
-      <c r="C4" s="289"/>
-      <c r="D4" s="289"/>
+      <c r="C4" s="288"/>
+      <c r="D4" s="288"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="289"/>
+      <c r="A5" s="288"/>
       <c r="B5" s="4" t="s">
         <v>275</v>
       </c>
@@ -15524,17 +15528,17 @@
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="289" t="s">
+      <c r="A18" s="288" t="s">
         <v>273</v>
       </c>
-      <c r="B18" s="289" t="s">
+      <c r="B18" s="288" t="s">
         <v>290</v>
       </c>
-      <c r="C18" s="289"/>
-      <c r="D18" s="289"/>
+      <c r="C18" s="288"/>
+      <c r="D18" s="288"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="289"/>
+      <c r="A19" s="288"/>
       <c r="B19" s="4" t="s">
         <v>275</v>
       </c>
@@ -15770,16 +15774,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="289" t="s">
+      <c r="A37" s="288" t="s">
         <v>273</v>
       </c>
-      <c r="B37" s="289" t="s">
+      <c r="B37" s="288" t="s">
         <v>295</v>
       </c>
-      <c r="C37" s="289"/>
+      <c r="C37" s="288"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="289"/>
+      <c r="A38" s="288"/>
       <c r="B38" s="4" t="s">
         <v>276</v>
       </c>
@@ -15865,16 +15869,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="289" t="s">
+      <c r="A47" s="288" t="s">
         <v>273</v>
       </c>
-      <c r="B47" s="289" t="s">
+      <c r="B47" s="288" t="s">
         <v>298</v>
       </c>
-      <c r="C47" s="289"/>
+      <c r="C47" s="288"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="289"/>
+      <c r="A48" s="288"/>
       <c r="B48" s="4" t="s">
         <v>276</v>
       </c>
@@ -15960,16 +15964,16 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="289" t="s">
+      <c r="A57" s="288" t="s">
         <v>273</v>
       </c>
-      <c r="B57" s="289" t="s">
+      <c r="B57" s="288" t="s">
         <v>305</v>
       </c>
-      <c r="C57" s="289"/>
+      <c r="C57" s="288"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="289"/>
+      <c r="A58" s="288"/>
       <c r="B58" s="4" t="s">
         <v>276</v>
       </c>
@@ -16055,16 +16059,16 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="289" t="s">
+      <c r="A67" s="288" t="s">
         <v>273</v>
       </c>
-      <c r="B67" s="289" t="s">
+      <c r="B67" s="288" t="s">
         <v>310</v>
       </c>
-      <c r="C67" s="289"/>
+      <c r="C67" s="288"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="289"/>
+      <c r="A68" s="288"/>
       <c r="B68" s="4" t="s">
         <v>276</v>
       </c>
@@ -16194,7 +16198,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="288" t="s">
+      <c r="A81" s="289" t="s">
         <v>273</v>
       </c>
       <c r="B81" t="s">
@@ -16202,7 +16206,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="288"/>
+      <c r="A82" s="289"/>
       <c r="B82" t="s">
         <v>276</v>
       </c>
@@ -16266,12 +16270,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="13">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:C37"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:C47"/>
@@ -16279,6 +16277,12 @@
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="69" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Update formula for beam profile acceptability
</commit_message>
<xml_diff>
--- a/MUSCCT.xlsx
+++ b/MUSCCT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAE33A4-60E2-477D-A333-BDF60B18F9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC7E37B-62E9-4A98-9E1B-E3592CD6C000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -3138,14 +3138,59 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3153,59 +3198,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -3993,7 +3993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -4076,19 +4076,19 @@
       <c r="A6" s="203" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="267" t="str">
+      <c r="B6" s="269" t="str">
         <f>Sheet1!F10</f>
         <v/>
       </c>
-      <c r="C6" s="267"/>
+      <c r="C6" s="269"/>
       <c r="D6" s="203" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="267" t="str">
+      <c r="E6" s="269" t="str">
         <f>Sheet1!R14</f>
         <v/>
       </c>
-      <c r="F6" s="267"/>
+      <c r="F6" s="269"/>
       <c r="G6" s="1"/>
       <c r="J6" s="228" t="s">
         <v>320</v>
@@ -4098,48 +4098,48 @@
       <c r="A7" s="203" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="268"/>
-      <c r="C7" s="268"/>
+      <c r="B7" s="267"/>
+      <c r="C7" s="267"/>
       <c r="D7" s="203" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="268" t="str">
+      <c r="E7" s="267" t="str">
         <f>Sheet1!F16</f>
         <v/>
       </c>
-      <c r="F7" s="268"/>
+      <c r="F7" s="267"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="203" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="268"/>
-      <c r="C8" s="268"/>
+      <c r="B8" s="267"/>
+      <c r="C8" s="267"/>
       <c r="D8" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="268" t="str">
+      <c r="E8" s="267" t="str">
         <f>Sheet1!F17</f>
         <v/>
       </c>
-      <c r="F8" s="268"/>
+      <c r="F8" s="267"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="203" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="268"/>
-      <c r="C9" s="268"/>
+      <c r="B9" s="267"/>
+      <c r="C9" s="267"/>
       <c r="D9" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="268" t="str">
+      <c r="E9" s="267" t="str">
         <f>Sheet1!K17</f>
         <v/>
       </c>
-      <c r="F9" s="268"/>
+      <c r="F9" s="267"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4149,19 +4149,19 @@
       <c r="D10" s="203" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="269" t="str">
+      <c r="E10" s="268" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="F10" s="269"/>
+      <c r="F10" s="268"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="267"/>
-      <c r="C11" s="267"/>
+      <c r="B11" s="269"/>
+      <c r="C11" s="269"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4184,10 +4184,10 @@
       <c r="A13" s="205" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="267" t="s">
+      <c r="B13" s="269" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="267"/>
+      <c r="C13" s="269"/>
       <c r="D13" s="203" t="s">
         <v>16</v>
       </c>
@@ -4504,17 +4504,17 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C29" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -4537,8 +4537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH264"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="J127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R145" sqref="Q145:S145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4833,19 +4833,19 @@
       <c r="E10" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="272" t="str">
+      <c r="F10" s="282" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="272"/>
+      <c r="G10" s="282"/>
       <c r="J10" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="272" t="str">
+      <c r="K10" s="282" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="272"/>
+      <c r="L10" s="282"/>
       <c r="M10" s="18"/>
       <c r="O10" s="19"/>
       <c r="Q10" s="23" t="s">
@@ -4889,19 +4889,19 @@
       <c r="E11" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="274" t="str">
+      <c r="F11" s="283" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="274"/>
+      <c r="G11" s="283"/>
       <c r="J11" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="272" t="str">
+      <c r="K11" s="282" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="272"/>
+      <c r="L11" s="282"/>
       <c r="M11" s="18"/>
       <c r="O11" s="19"/>
       <c r="Q11" s="23" t="s">
@@ -4945,19 +4945,19 @@
       <c r="E12" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="274" t="str">
+      <c r="F12" s="283" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="274"/>
+      <c r="G12" s="283"/>
       <c r="J12" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="275" t="str">
+      <c r="K12" s="284" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="275"/>
+      <c r="L12" s="284"/>
       <c r="M12" s="18"/>
       <c r="O12" s="19"/>
       <c r="Q12" s="23" t="s">
@@ -5001,19 +5001,19 @@
       <c r="E13" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="274" t="str">
+      <c r="F13" s="283" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="274"/>
+      <c r="G13" s="283"/>
       <c r="J13" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="272" t="str">
+      <c r="K13" s="282" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="272"/>
+      <c r="L13" s="282"/>
       <c r="M13" s="18"/>
       <c r="O13" s="19"/>
       <c r="Q13" s="23" t="s">
@@ -5119,19 +5119,19 @@
       <c r="E16" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="272" t="str">
+      <c r="F16" s="282" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="272"/>
+      <c r="G16" s="282"/>
       <c r="J16" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="275" t="str">
+      <c r="K16" s="284" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="275"/>
+      <c r="L16" s="284"/>
       <c r="M16" s="18"/>
       <c r="O16" s="19"/>
       <c r="P16" s="50" t="s">
@@ -5162,19 +5162,19 @@
       <c r="E17" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="274" t="str">
+      <c r="F17" s="283" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="274"/>
+      <c r="G17" s="283"/>
       <c r="J17" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="272" t="str">
+      <c r="K17" s="282" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="272"/>
+      <c r="L17" s="282"/>
       <c r="M17" s="18"/>
       <c r="O17" s="19"/>
       <c r="Q17" s="23" t="s">
@@ -5218,11 +5218,11 @@
       <c r="J18" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="272" t="str">
+      <c r="K18" s="282" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="272"/>
+      <c r="L18" s="282"/>
       <c r="M18" s="18"/>
       <c r="O18" s="19"/>
       <c r="Q18" s="23" t="s">
@@ -5290,11 +5290,11 @@
       <c r="E20" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="272" t="str">
+      <c r="F20" s="282" t="str">
         <f>IF(R21="","",R21)</f>
         <v/>
       </c>
-      <c r="G20" s="272"/>
+      <c r="G20" s="282"/>
       <c r="I20" s="53" t="s">
         <v>76</v>
       </c>
@@ -5319,19 +5319,19 @@
       <c r="E21" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="276" t="str">
+      <c r="F21" s="287" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="276"/>
+      <c r="G21" s="287"/>
       <c r="J21" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="272" t="str">
+      <c r="K21" s="282" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="272"/>
+      <c r="L21" s="282"/>
       <c r="M21" s="18"/>
       <c r="O21" s="19"/>
       <c r="Q21" s="23" t="s">
@@ -5373,11 +5373,11 @@
       <c r="J22" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="272" t="str">
+      <c r="K22" s="282" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="272"/>
+      <c r="L22" s="282"/>
       <c r="M22" s="18"/>
       <c r="O22" s="19"/>
       <c r="Q22" s="23" t="s">
@@ -5421,19 +5421,19 @@
       <c r="E23" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="272" t="str">
+      <c r="F23" s="282" t="str">
         <f>IF(R24="","",R24)</f>
         <v/>
       </c>
-      <c r="G23" s="272"/>
+      <c r="G23" s="282"/>
       <c r="J23" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="272" t="str">
+      <c r="K23" s="282" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="272"/>
+      <c r="L23" s="282"/>
       <c r="M23" s="18"/>
       <c r="O23" s="19"/>
       <c r="P23" s="50" t="s">
@@ -5472,11 +5472,11 @@
       <c r="E24" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="272" t="str">
+      <c r="F24" s="282" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="272"/>
+      <c r="G24" s="282"/>
       <c r="M24" s="18"/>
       <c r="O24" s="19"/>
       <c r="Q24" s="23" t="s">
@@ -5520,11 +5520,11 @@
       <c r="E25" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="272" t="str">
+      <c r="F25" s="282" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="272"/>
+      <c r="G25" s="282"/>
       <c r="J25" s="49" t="s">
         <v>82</v>
       </c>
@@ -5566,11 +5566,11 @@
       <c r="J26" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="272" t="str">
+      <c r="K26" s="282" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="272"/>
+      <c r="L26" s="282"/>
       <c r="M26" s="18"/>
       <c r="O26" s="19"/>
       <c r="Q26" s="23" t="s">
@@ -5597,19 +5597,19 @@
       <c r="E27" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="272" t="str">
+      <c r="F27" s="282" t="str">
         <f>IF(R28="","",R28)</f>
         <v/>
       </c>
-      <c r="G27" s="272"/>
+      <c r="G27" s="282"/>
       <c r="J27" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="272" t="str">
+      <c r="K27" s="282" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="272"/>
+      <c r="L27" s="282"/>
       <c r="M27" s="18"/>
       <c r="O27" s="19"/>
       <c r="P27" s="50" t="s">
@@ -5639,11 +5639,11 @@
       <c r="E28" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="272" t="str">
+      <c r="F28" s="282" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="272"/>
+      <c r="G28" s="282"/>
       <c r="M28" s="18"/>
       <c r="O28" s="19"/>
       <c r="Q28" s="23" t="s">
@@ -5687,11 +5687,11 @@
       <c r="E29" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="272" t="str">
+      <c r="F29" s="282" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="272"/>
+      <c r="G29" s="282"/>
       <c r="M29" s="18"/>
       <c r="O29" s="19"/>
       <c r="Q29" s="23" t="s">
@@ -5810,10 +5810,10 @@
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
-      <c r="L32" s="277" t="s">
+      <c r="L32" s="281" t="s">
         <v>89</v>
       </c>
-      <c r="M32" s="277"/>
+      <c r="M32" s="281"/>
       <c r="AA32" s="23" t="s">
         <v>70</v>
       </c>
@@ -7125,27 +7125,27 @@
       </c>
       <c r="B70" s="16"/>
       <c r="E70" s="61"/>
-      <c r="F70" s="278" t="s">
+      <c r="F70" s="276" t="s">
         <v>139</v>
       </c>
-      <c r="G70" s="278"/>
-      <c r="H70" s="278"/>
-      <c r="I70" s="278" t="s">
+      <c r="G70" s="276"/>
+      <c r="H70" s="276"/>
+      <c r="I70" s="276" t="s">
         <v>140</v>
       </c>
-      <c r="J70" s="278"/>
+      <c r="J70" s="276"/>
       <c r="M70" s="18"/>
       <c r="O70" s="39"/>
       <c r="P70" s="13"/>
-      <c r="Q70" s="279" t="s">
+      <c r="Q70" s="273" t="s">
         <v>139</v>
       </c>
-      <c r="R70" s="279"/>
-      <c r="S70" s="279"/>
-      <c r="T70" s="279" t="s">
+      <c r="R70" s="273"/>
+      <c r="S70" s="273"/>
+      <c r="T70" s="273" t="s">
         <v>140</v>
       </c>
-      <c r="U70" s="279"/>
+      <c r="U70" s="273"/>
       <c r="V70" s="13"/>
       <c r="W70" s="13"/>
       <c r="X70" s="13"/>
@@ -8409,15 +8409,15 @@
       </c>
       <c r="M90" s="18"/>
       <c r="O90" s="19"/>
-      <c r="Q90" s="287" t="s">
+      <c r="Q90" s="275" t="s">
         <v>139</v>
       </c>
-      <c r="R90" s="287"/>
-      <c r="S90" s="287"/>
-      <c r="T90" s="287" t="s">
+      <c r="R90" s="275"/>
+      <c r="S90" s="275"/>
+      <c r="T90" s="275" t="s">
         <v>140</v>
       </c>
-      <c r="U90" s="287"/>
+      <c r="U90" s="275"/>
       <c r="Y90" s="20"/>
       <c r="AA90" s="23" t="s">
         <v>120</v>
@@ -8560,15 +8560,15 @@
       </c>
       <c r="B94" s="16"/>
       <c r="E94" s="61"/>
-      <c r="F94" s="280" t="s">
+      <c r="F94" s="277" t="s">
         <v>139</v>
       </c>
-      <c r="G94" s="280"/>
-      <c r="H94" s="280"/>
-      <c r="I94" s="281" t="s">
+      <c r="G94" s="277"/>
+      <c r="H94" s="277"/>
+      <c r="I94" s="278" t="s">
         <v>140</v>
       </c>
-      <c r="J94" s="281"/>
+      <c r="J94" s="278"/>
       <c r="M94" s="18"/>
       <c r="O94" s="19"/>
       <c r="P94" s="23" t="s">
@@ -8731,10 +8731,10 @@
         <v>31</v>
       </c>
       <c r="B97" s="16"/>
-      <c r="D97" s="282" t="s">
+      <c r="D97" s="279" t="s">
         <v>149</v>
       </c>
-      <c r="E97" s="283"/>
+      <c r="E97" s="280"/>
       <c r="F97" s="87" t="str">
         <f t="shared" ref="F97:J102" si="31">IF(Q122="","",Q122)</f>
         <v/>
@@ -8789,8 +8789,8 @@
         <v>32</v>
       </c>
       <c r="B98" s="16"/>
-      <c r="D98" s="282"/>
-      <c r="E98" s="283"/>
+      <c r="D98" s="279"/>
+      <c r="E98" s="280"/>
       <c r="F98" s="92" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -8845,8 +8845,8 @@
         <v>33</v>
       </c>
       <c r="B99" s="16"/>
-      <c r="D99" s="282"/>
-      <c r="E99" s="283"/>
+      <c r="D99" s="279"/>
+      <c r="E99" s="280"/>
       <c r="F99" s="97" t="str">
         <f t="shared" si="31"/>
         <v/>
@@ -9753,15 +9753,15 @@
       <c r="B119" s="16"/>
       <c r="M119" s="18"/>
       <c r="O119" s="19"/>
-      <c r="Q119" s="285" t="s">
+      <c r="Q119" s="272" t="s">
         <v>139</v>
       </c>
-      <c r="R119" s="279"/>
-      <c r="S119" s="286"/>
-      <c r="T119" s="285" t="s">
+      <c r="R119" s="273"/>
+      <c r="S119" s="274"/>
+      <c r="T119" s="272" t="s">
         <v>140</v>
       </c>
-      <c r="U119" s="286"/>
+      <c r="U119" s="274"/>
       <c r="W119" s="50" t="s">
         <v>146</v>
       </c>
@@ -9884,10 +9884,10 @@
         <v>Water phantom is free from rings, streaks, lines, cupping artifacts</v>
       </c>
       <c r="M122" s="18"/>
-      <c r="O122" s="284" t="s">
+      <c r="O122" s="270" t="s">
         <v>149</v>
       </c>
-      <c r="P122" s="273"/>
+      <c r="P122" s="271"/>
       <c r="Q122" s="130"/>
       <c r="R122" s="131"/>
       <c r="S122" s="132"/>
@@ -9918,8 +9918,8 @@
       </c>
       <c r="B123" s="16"/>
       <c r="M123" s="18"/>
-      <c r="O123" s="284"/>
-      <c r="P123" s="273"/>
+      <c r="O123" s="270"/>
+      <c r="P123" s="271"/>
       <c r="Q123" s="133"/>
       <c r="R123" s="134"/>
       <c r="S123" s="135"/>
@@ -9956,8 +9956,8 @@
         <v>177</v>
       </c>
       <c r="M124" s="18"/>
-      <c r="O124" s="284"/>
-      <c r="P124" s="273"/>
+      <c r="O124" s="270"/>
+      <c r="P124" s="271"/>
       <c r="Q124" s="137"/>
       <c r="R124" s="138"/>
       <c r="S124" s="139"/>
@@ -10759,7 +10759,7 @@
       </c>
       <c r="M141" s="18"/>
       <c r="O141" s="19"/>
-      <c r="P141" s="273" t="s">
+      <c r="P141" s="271" t="s">
         <v>169</v>
       </c>
       <c r="Q141" s="161"/>
@@ -10787,7 +10787,7 @@
       <c r="B142" s="16"/>
       <c r="M142" s="18"/>
       <c r="O142" s="19"/>
-      <c r="P142" s="273"/>
+      <c r="P142" s="271"/>
       <c r="Q142" s="161"/>
       <c r="R142" s="162"/>
       <c r="S142" s="162"/>
@@ -10816,7 +10816,7 @@
       </c>
       <c r="M143" s="18"/>
       <c r="O143" s="19"/>
-      <c r="P143" s="273"/>
+      <c r="P143" s="271"/>
       <c r="Q143" s="164"/>
       <c r="R143" s="165"/>
       <c r="S143" s="165"/>
@@ -10928,15 +10928,15 @@
         <v>162</v>
       </c>
       <c r="Q145" s="127" t="str">
-        <f t="shared" ref="Q145:S145" si="42">IF(Q144="","",IF(OR(ABS(Q144-Q140)&lt;=3,ABS(Q144-Q140)&lt;=Q140*0.3),"Pass","Fail"))</f>
+        <f>IF(Q144="","",IF(OR(ABS(Q144-Q140)&lt;=3,ABS(Q144-Q140)&lt;=Q140*0.3,ABS(Q144-Q139)&lt;=3,ABS(Q144-Q139)&lt;=Q139*0.3),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="R145" s="128" t="str">
-        <f t="shared" si="42"/>
+        <f>IF(R144="","",IF(OR(ABS(R144-R140)&lt;=3,ABS(R144-R140)&lt;=R140*0.3,ABS(R144-R139)&lt;=3,ABS(R144-R139)&lt;=R139*0.3),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="S145" s="128" t="str">
-        <f t="shared" si="42"/>
+        <f>IF(S144="","",IF(OR(ABS(S144-S140)&lt;=3,ABS(S144-S140)&lt;=S140*0.3,ABS(S144-S139)&lt;=3,ABS(S144-S139)&lt;=S139*0.3),"Pass","Fail"))</f>
         <v/>
       </c>
       <c r="T145" s="129" t="str">
@@ -11406,23 +11406,23 @@
         <v>218</v>
       </c>
       <c r="F157" s="69" t="str">
-        <f t="shared" ref="F157:J163" si="43">IF(Q174="","",Q174)</f>
+        <f t="shared" ref="F157:J163" si="42">IF(Q174="","",Q174)</f>
         <v/>
       </c>
       <c r="G157" s="70" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="H157" s="70" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="I157" s="70" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="J157" s="71" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="M157" s="18"/>
@@ -11451,23 +11451,23 @@
         <v>219</v>
       </c>
       <c r="F158" s="72" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="G158" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="H158" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="I158" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="J158" s="74" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="M158" s="18"/>
@@ -11497,23 +11497,23 @@
         <v>220</v>
       </c>
       <c r="F159" s="72" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="G159" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="H159" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="I159" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="J159" s="74" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="M159" s="18"/>
@@ -11536,23 +11536,23 @@
         <v>193</v>
       </c>
       <c r="F160" s="72" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="G160" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="H160" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="I160" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="J160" s="74" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="M160" s="18"/>
@@ -11580,23 +11580,23 @@
         <v>221</v>
       </c>
       <c r="F161" s="72" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="G161" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="H161" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="I161" s="73" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="J161" s="74" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="M161" s="18"/>
@@ -11642,23 +11642,23 @@
         <v>222</v>
       </c>
       <c r="F162" s="75" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="G162" s="76" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="H162" s="76" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="I162" s="76" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="J162" s="77" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="M162" s="18"/>
@@ -11699,23 +11699,23 @@
         <v>162</v>
       </c>
       <c r="F163" s="84" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="G163" s="85" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="H163" s="85" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="I163" s="85" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="J163" s="86" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="M163" s="18"/>
@@ -11892,14 +11892,14 @@
       </c>
       <c r="B168" s="16"/>
       <c r="D168" s="61"/>
-      <c r="E168" s="278" t="s">
+      <c r="E168" s="276" t="s">
         <v>139</v>
       </c>
-      <c r="F168" s="278"/>
-      <c r="G168" s="278" t="s">
+      <c r="F168" s="276"/>
+      <c r="G168" s="276" t="s">
         <v>140</v>
       </c>
-      <c r="H168" s="278"/>
+      <c r="H168" s="276"/>
       <c r="M168" s="18"/>
       <c r="O168" s="174" t="s">
         <v>212</v>
@@ -11965,19 +11965,19 @@
         <v>226</v>
       </c>
       <c r="E170" s="69" t="str">
-        <f t="shared" ref="E170:H174" si="44">IF(P187="","",P187)</f>
+        <f t="shared" ref="E170:H174" si="43">IF(P187="","",P187)</f>
         <v/>
       </c>
       <c r="F170" s="70" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="G170" s="70" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="H170" s="71" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="J170" s="43" t="s">
@@ -12016,19 +12016,19 @@
         <v>228</v>
       </c>
       <c r="E171" s="72" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="F171" s="73" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="G171" s="73" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="H171" s="74" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="J171" s="43" t="s">
@@ -12057,19 +12057,19 @@
         <v>229</v>
       </c>
       <c r="E172" s="72" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="F172" s="73" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="G172" s="73" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="H172" s="74" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="M172" s="18"/>
@@ -12095,19 +12095,19 @@
         <v>230</v>
       </c>
       <c r="E173" s="72" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="F173" s="73" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="G173" s="73" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="H173" s="74" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="M173" s="18"/>
@@ -12128,19 +12128,19 @@
         <v>231</v>
       </c>
       <c r="E174" s="97" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="F174" s="98" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="G174" s="98" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="H174" s="99" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="M174" s="18"/>
@@ -12384,23 +12384,23 @@
         <v>239</v>
       </c>
       <c r="D181" s="69" t="str">
-        <f t="shared" ref="D181:H185" si="45">IF(P195="","",P195)</f>
+        <f t="shared" ref="D181:H185" si="44">IF(P195="","",P195)</f>
         <v/>
       </c>
       <c r="E181" s="71" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="F181" s="69" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="G181" s="70" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="H181" s="71" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="M181" s="18"/>
@@ -12425,23 +12425,23 @@
         <v>241</v>
       </c>
       <c r="D182" s="72" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="E182" s="74" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="F182" s="72" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="G182" s="73" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="H182" s="74" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="M182" s="18"/>
@@ -12470,23 +12470,23 @@
         <v>244</v>
       </c>
       <c r="D183" s="72" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="E183" s="74" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="F183" s="72" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="G183" s="73" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="H183" s="74" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="M183" s="18"/>
@@ -12505,23 +12505,23 @@
         <v>246</v>
       </c>
       <c r="D184" s="72" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="E184" s="74" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="F184" s="72" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="G184" s="73" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="H184" s="74" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="M184" s="18"/>
@@ -12549,23 +12549,23 @@
         <v>248</v>
       </c>
       <c r="D185" s="75" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="E185" s="77" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="F185" s="75" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="G185" s="76" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="H185" s="77" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="M185" s="18"/>
@@ -13189,7 +13189,7 @@
       <c r="T206" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="U206" s="270" t="s">
+      <c r="U206" s="285" t="s">
         <v>357</v>
       </c>
       <c r="Y206" s="20"/>
@@ -13219,7 +13219,7 @@
       <c r="T207" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="U207" s="271"/>
+      <c r="U207" s="286"/>
       <c r="Y207" s="20"/>
     </row>
     <row r="208" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -13283,11 +13283,11 @@
         <v>348</v>
       </c>
       <c r="T209" s="142">
-        <f t="shared" ref="T209:T216" si="46">AH28</f>
+        <f t="shared" ref="T209:T216" si="45">AH28</f>
         <v>0</v>
       </c>
       <c r="U209" s="260" t="e">
-        <f t="shared" ref="U209:U216" si="47">(T209-MEDIAN($T$208:$T$216))/MEDIAN($T$208:$T$216)</f>
+        <f t="shared" ref="U209:U216" si="46">(T209-MEDIAN($T$208:$T$216))/MEDIAN($T$208:$T$216)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Y209" s="20"/>
@@ -13318,11 +13318,11 @@
         <v>349</v>
       </c>
       <c r="T210" s="142">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U210" s="260" t="e">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="U210" s="260" t="e">
-        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y210" s="20"/>
@@ -13356,11 +13356,11 @@
         <v>350</v>
       </c>
       <c r="T211" s="142">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U211" s="260" t="e">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="U211" s="260" t="e">
-        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y211" s="20"/>
@@ -13394,11 +13394,11 @@
         <v>351</v>
       </c>
       <c r="T212" s="142">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U212" s="260" t="e">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="U212" s="260" t="e">
-        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y212" s="20"/>
@@ -13431,11 +13431,11 @@
         <v>352</v>
       </c>
       <c r="T213" s="142">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U213" s="260" t="e">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="U213" s="260" t="e">
-        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y213" s="20"/>
@@ -13466,11 +13466,11 @@
         <v>353</v>
       </c>
       <c r="T214" s="142">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U214" s="260" t="e">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="U214" s="260" t="e">
-        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y214" s="20"/>
@@ -13501,11 +13501,11 @@
         <v>354</v>
       </c>
       <c r="T215" s="142">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U215" s="260" t="e">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="U215" s="260" t="e">
-        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y215" s="20"/>
@@ -13533,11 +13533,11 @@
         <v>355</v>
       </c>
       <c r="T216" s="261">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="U216" s="265" t="e">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="U216" s="265" t="e">
-        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y216" s="20"/>
@@ -15089,33 +15089,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="43">
-    <mergeCell ref="O122:P124"/>
-    <mergeCell ref="Q119:S119"/>
-    <mergeCell ref="T119:U119"/>
-    <mergeCell ref="Q90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="E168:F168"/>
-    <mergeCell ref="G168:H168"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="I94:J94"/>
-    <mergeCell ref="D97:E99"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="T70:U70"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
     <mergeCell ref="U206:U207"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="F20:G20"/>
@@ -15132,6 +15105,33 @@
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="E168:F168"/>
+    <mergeCell ref="G168:H168"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="D97:E99"/>
+    <mergeCell ref="O122:P124"/>
+    <mergeCell ref="Q119:S119"/>
+    <mergeCell ref="T119:U119"/>
+    <mergeCell ref="Q90:S90"/>
+    <mergeCell ref="T90:U90"/>
   </mergeCells>
   <conditionalFormatting sqref="C122">
     <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
@@ -15346,17 +15346,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="288" t="s">
+      <c r="A4" s="289" t="s">
         <v>273</v>
       </c>
-      <c r="B4" s="288" t="s">
+      <c r="B4" s="289" t="s">
         <v>274</v>
       </c>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288"/>
+      <c r="C4" s="289"/>
+      <c r="D4" s="289"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="288"/>
+      <c r="A5" s="289"/>
       <c r="B5" s="4" t="s">
         <v>275</v>
       </c>
@@ -15528,17 +15528,17 @@
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="288" t="s">
+      <c r="A18" s="289" t="s">
         <v>273</v>
       </c>
-      <c r="B18" s="288" t="s">
+      <c r="B18" s="289" t="s">
         <v>290</v>
       </c>
-      <c r="C18" s="288"/>
-      <c r="D18" s="288"/>
+      <c r="C18" s="289"/>
+      <c r="D18" s="289"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="288"/>
+      <c r="A19" s="289"/>
       <c r="B19" s="4" t="s">
         <v>275</v>
       </c>
@@ -15774,16 +15774,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="288" t="s">
+      <c r="A37" s="289" t="s">
         <v>273</v>
       </c>
-      <c r="B37" s="288" t="s">
+      <c r="B37" s="289" t="s">
         <v>295</v>
       </c>
-      <c r="C37" s="288"/>
+      <c r="C37" s="289"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="288"/>
+      <c r="A38" s="289"/>
       <c r="B38" s="4" t="s">
         <v>276</v>
       </c>
@@ -15869,16 +15869,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="288" t="s">
+      <c r="A47" s="289" t="s">
         <v>273</v>
       </c>
-      <c r="B47" s="288" t="s">
+      <c r="B47" s="289" t="s">
         <v>298</v>
       </c>
-      <c r="C47" s="288"/>
+      <c r="C47" s="289"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="288"/>
+      <c r="A48" s="289"/>
       <c r="B48" s="4" t="s">
         <v>276</v>
       </c>
@@ -15964,16 +15964,16 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="288" t="s">
+      <c r="A57" s="289" t="s">
         <v>273</v>
       </c>
-      <c r="B57" s="288" t="s">
+      <c r="B57" s="289" t="s">
         <v>305</v>
       </c>
-      <c r="C57" s="288"/>
+      <c r="C57" s="289"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="288"/>
+      <c r="A58" s="289"/>
       <c r="B58" s="4" t="s">
         <v>276</v>
       </c>
@@ -16059,16 +16059,16 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="288" t="s">
+      <c r="A67" s="289" t="s">
         <v>273</v>
       </c>
-      <c r="B67" s="288" t="s">
+      <c r="B67" s="289" t="s">
         <v>310</v>
       </c>
-      <c r="C67" s="288"/>
+      <c r="C67" s="289"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="288"/>
+      <c r="A68" s="289"/>
       <c r="B68" s="4" t="s">
         <v>276</v>
       </c>
@@ -16198,7 +16198,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="289" t="s">
+      <c r="A81" s="288" t="s">
         <v>273</v>
       </c>
       <c r="B81" t="s">
@@ -16206,7 +16206,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="289"/>
+      <c r="A82" s="288"/>
       <c r="B82" t="s">
         <v>276</v>
       </c>
@@ -16270,6 +16270,12 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="13">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:C47"/>
@@ -16277,12 +16283,6 @@
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="B67:C67"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="69" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>